<commit_message>
Add HospitalType to drop down list
</commit_message>
<xml_diff>
--- a/Source Code/HospitalF Import Template - Ho Chi Minh.xlsx
+++ b/Source Code/HospitalF Import Template - Ho Chi Minh.xlsx
@@ -19,6 +19,7 @@
     <sheet name="Speciality" sheetId="5" r:id="rId5"/>
     <sheet name="Service" sheetId="6" r:id="rId6"/>
     <sheet name="Facility" sheetId="7" r:id="rId7"/>
+    <sheet name="HospitalType" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">City!$A$1:$A$2</definedName>
@@ -28,6 +29,7 @@
     <definedName name="CityList">City!$A$2</definedName>
     <definedName name="FacilityList">Facility!$A$2:$A$23</definedName>
     <definedName name="Hồ_Chí_Minh_List">District!$A$2:$A$25</definedName>
+    <definedName name="HospitalTypeList">HospitalType!$A$2:$A$9</definedName>
     <definedName name="ServiceList">Service!$A$2:$A$33</definedName>
     <definedName name="SG_1_List">Ward!$A$2:$A$11</definedName>
     <definedName name="SG_10_List">Ward!$S$2:$S$16</definedName>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="502">
   <si>
     <t>Tên bệnh viện</t>
   </si>
@@ -1544,6 +1546,33 @@
   </si>
   <si>
     <t>WardID</t>
+  </si>
+  <si>
+    <t>Bệnh viện công</t>
+  </si>
+  <si>
+    <t>Bệnh viện quốc tế</t>
+  </si>
+  <si>
+    <t>Bệnh viện thẩm mỹ</t>
+  </si>
+  <si>
+    <t>Bệnh viện thú y</t>
+  </si>
+  <si>
+    <t>Bệnh viện tư nhân</t>
+  </si>
+  <si>
+    <t>Nhà thuốc</t>
+  </si>
+  <si>
+    <t>Phòng khám tư nhân</t>
+  </si>
+  <si>
+    <t>Trung tâm y tế</t>
+  </si>
+  <si>
+    <t>HospitalTypeId</t>
   </si>
 </sst>
 </file>
@@ -2090,11 +2119,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:W200"/>
+  <dimension ref="A1:X200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2114,10 +2141,13 @@
     <col min="14" max="15" width="20.5703125" customWidth="1"/>
     <col min="16" max="17" width="32.85546875" customWidth="1"/>
     <col min="18" max="20" width="46.7109375" customWidth="1"/>
-    <col min="21" max="23" width="0" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="6.28515625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="7.7109375" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="8.28515625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -2187,8 +2217,11 @@
       <c r="W1" s="27" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" s="27" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2221,8 +2254,12 @@
         <f>IF(K2 &lt;&gt; "", VLOOKUP(K2, IF(J2="1", Ward!$A$2:$B$11, IF(J2="2", Ward!$C$2:$D$12, IF(J2="3", Ward!$E$2:$F$15, IF(J2="4", Ward!$G$2:$H$16, IF(J2="5", Ward!$I$2:$J$16, IF(J2="6", Ward!$K$2:$L$15, IF(J2="7", Ward!$M$2:$N$11, IF(J2="8", Ward!$O$2:$P$17, IF(J2="9", Ward!$Q$2:$R$14, IF(J2="10", Ward!$S$2:$T$16, IF(J2="11", Ward!$U$2:$V$17, IF(J2="12", Ward!$W$2:$X$12, IF(J2="Bình Chánh", Ward!$Y$2:$Z$17, IF(J2="Bình Tân", Ward!$AA$2:$AB$11, IF(J2="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J2="Cần Giờ", Ward!$AE$2:$AF$8, IF(J2="Củ Chi", Ward!$AG$2:$AH$22, IF(J2="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J2="Hóc Môn", Ward!$AK$2:$AL$13, IF(J2="Nhà Bè", Ward!$AM$2:$AN$8, IF(J2="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J2="Tân Bình", Ward!$AQ$2:$AR$16, IF(J2="Tân Phú", Ward!$AS$2:$AT$12, IF(J2="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X2" t="str">
+        <f>IF(B2 &lt;&gt; "", VLOOKUP(B2, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -2255,8 +2292,12 @@
         <f>IF(K3 &lt;&gt; "", VLOOKUP(K3, IF(J3="1", Ward!$A$2:$B$11, IF(J3="2", Ward!$C$2:$D$12, IF(J3="3", Ward!$E$2:$F$15, IF(J3="4", Ward!$G$2:$H$16, IF(J3="5", Ward!$I$2:$J$16, IF(J3="6", Ward!$K$2:$L$15, IF(J3="7", Ward!$M$2:$N$11, IF(J3="8", Ward!$O$2:$P$17, IF(J3="9", Ward!$Q$2:$R$14, IF(J3="10", Ward!$S$2:$T$16, IF(J3="11", Ward!$U$2:$V$17, IF(J3="12", Ward!$W$2:$X$12, IF(J3="Bình Chánh", Ward!$Y$2:$Z$17, IF(J3="Bình Tân", Ward!$AA$2:$AB$11, IF(J3="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J3="Cần Giờ", Ward!$AE$2:$AF$8, IF(J3="Củ Chi", Ward!$AG$2:$AH$22, IF(J3="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J3="Hóc Môn", Ward!$AK$2:$AL$13, IF(J3="Nhà Bè", Ward!$AM$2:$AN$8, IF(J3="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J3="Tân Bình", Ward!$AQ$2:$AR$16, IF(J3="Tân Phú", Ward!$AS$2:$AT$12, IF(J3="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X3" t="str">
+        <f>IF(B3 &lt;&gt; "", VLOOKUP(B3, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -2289,8 +2330,12 @@
         <f>IF(K4 &lt;&gt; "", VLOOKUP(K4, IF(J4="1", Ward!$A$2:$B$11, IF(J4="2", Ward!$C$2:$D$12, IF(J4="3", Ward!$E$2:$F$15, IF(J4="4", Ward!$G$2:$H$16, IF(J4="5", Ward!$I$2:$J$16, IF(J4="6", Ward!$K$2:$L$15, IF(J4="7", Ward!$M$2:$N$11, IF(J4="8", Ward!$O$2:$P$17, IF(J4="9", Ward!$Q$2:$R$14, IF(J4="10", Ward!$S$2:$T$16, IF(J4="11", Ward!$U$2:$V$17, IF(J4="12", Ward!$W$2:$X$12, IF(J4="Bình Chánh", Ward!$Y$2:$Z$17, IF(J4="Bình Tân", Ward!$AA$2:$AB$11, IF(J4="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J4="Cần Giờ", Ward!$AE$2:$AF$8, IF(J4="Củ Chi", Ward!$AG$2:$AH$22, IF(J4="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J4="Hóc Môn", Ward!$AK$2:$AL$13, IF(J4="Nhà Bè", Ward!$AM$2:$AN$8, IF(J4="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J4="Tân Bình", Ward!$AQ$2:$AR$16, IF(J4="Tân Phú", Ward!$AS$2:$AT$12, IF(J4="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X4" t="str">
+        <f>IF(B4 &lt;&gt; "", VLOOKUP(B4, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -2323,8 +2368,12 @@
         <f>IF(K5 &lt;&gt; "", VLOOKUP(K5, IF(J5="1", Ward!$A$2:$B$11, IF(J5="2", Ward!$C$2:$D$12, IF(J5="3", Ward!$E$2:$F$15, IF(J5="4", Ward!$G$2:$H$16, IF(J5="5", Ward!$I$2:$J$16, IF(J5="6", Ward!$K$2:$L$15, IF(J5="7", Ward!$M$2:$N$11, IF(J5="8", Ward!$O$2:$P$17, IF(J5="9", Ward!$Q$2:$R$14, IF(J5="10", Ward!$S$2:$T$16, IF(J5="11", Ward!$U$2:$V$17, IF(J5="12", Ward!$W$2:$X$12, IF(J5="Bình Chánh", Ward!$Y$2:$Z$17, IF(J5="Bình Tân", Ward!$AA$2:$AB$11, IF(J5="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J5="Cần Giờ", Ward!$AE$2:$AF$8, IF(J5="Củ Chi", Ward!$AG$2:$AH$22, IF(J5="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J5="Hóc Môn", Ward!$AK$2:$AL$13, IF(J5="Nhà Bè", Ward!$AM$2:$AN$8, IF(J5="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J5="Tân Bình", Ward!$AQ$2:$AR$16, IF(J5="Tân Phú", Ward!$AS$2:$AT$12, IF(J5="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X5" t="str">
+        <f>IF(B5 &lt;&gt; "", VLOOKUP(B5, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
@@ -2357,8 +2406,12 @@
         <f>IF(K6 &lt;&gt; "", VLOOKUP(K6, IF(J6="1", Ward!$A$2:$B$11, IF(J6="2", Ward!$C$2:$D$12, IF(J6="3", Ward!$E$2:$F$15, IF(J6="4", Ward!$G$2:$H$16, IF(J6="5", Ward!$I$2:$J$16, IF(J6="6", Ward!$K$2:$L$15, IF(J6="7", Ward!$M$2:$N$11, IF(J6="8", Ward!$O$2:$P$17, IF(J6="9", Ward!$Q$2:$R$14, IF(J6="10", Ward!$S$2:$T$16, IF(J6="11", Ward!$U$2:$V$17, IF(J6="12", Ward!$W$2:$X$12, IF(J6="Bình Chánh", Ward!$Y$2:$Z$17, IF(J6="Bình Tân", Ward!$AA$2:$AB$11, IF(J6="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J6="Cần Giờ", Ward!$AE$2:$AF$8, IF(J6="Củ Chi", Ward!$AG$2:$AH$22, IF(J6="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J6="Hóc Môn", Ward!$AK$2:$AL$13, IF(J6="Nhà Bè", Ward!$AM$2:$AN$8, IF(J6="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J6="Tân Bình", Ward!$AQ$2:$AR$16, IF(J6="Tân Phú", Ward!$AS$2:$AT$12, IF(J6="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X6" t="str">
+        <f>IF(B6 &lt;&gt; "", VLOOKUP(B6, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -2391,8 +2444,12 @@
         <f>IF(K7 &lt;&gt; "", VLOOKUP(K7, IF(J7="1", Ward!$A$2:$B$11, IF(J7="2", Ward!$C$2:$D$12, IF(J7="3", Ward!$E$2:$F$15, IF(J7="4", Ward!$G$2:$H$16, IF(J7="5", Ward!$I$2:$J$16, IF(J7="6", Ward!$K$2:$L$15, IF(J7="7", Ward!$M$2:$N$11, IF(J7="8", Ward!$O$2:$P$17, IF(J7="9", Ward!$Q$2:$R$14, IF(J7="10", Ward!$S$2:$T$16, IF(J7="11", Ward!$U$2:$V$17, IF(J7="12", Ward!$W$2:$X$12, IF(J7="Bình Chánh", Ward!$Y$2:$Z$17, IF(J7="Bình Tân", Ward!$AA$2:$AB$11, IF(J7="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J7="Cần Giờ", Ward!$AE$2:$AF$8, IF(J7="Củ Chi", Ward!$AG$2:$AH$22, IF(J7="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J7="Hóc Môn", Ward!$AK$2:$AL$13, IF(J7="Nhà Bè", Ward!$AM$2:$AN$8, IF(J7="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J7="Tân Bình", Ward!$AQ$2:$AR$16, IF(J7="Tân Phú", Ward!$AS$2:$AT$12, IF(J7="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X7" t="str">
+        <f>IF(B7 &lt;&gt; "", VLOOKUP(B7, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -2425,8 +2482,12 @@
         <f>IF(K8 &lt;&gt; "", VLOOKUP(K8, IF(J8="1", Ward!$A$2:$B$11, IF(J8="2", Ward!$C$2:$D$12, IF(J8="3", Ward!$E$2:$F$15, IF(J8="4", Ward!$G$2:$H$16, IF(J8="5", Ward!$I$2:$J$16, IF(J8="6", Ward!$K$2:$L$15, IF(J8="7", Ward!$M$2:$N$11, IF(J8="8", Ward!$O$2:$P$17, IF(J8="9", Ward!$Q$2:$R$14, IF(J8="10", Ward!$S$2:$T$16, IF(J8="11", Ward!$U$2:$V$17, IF(J8="12", Ward!$W$2:$X$12, IF(J8="Bình Chánh", Ward!$Y$2:$Z$17, IF(J8="Bình Tân", Ward!$AA$2:$AB$11, IF(J8="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J8="Cần Giờ", Ward!$AE$2:$AF$8, IF(J8="Củ Chi", Ward!$AG$2:$AH$22, IF(J8="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J8="Hóc Môn", Ward!$AK$2:$AL$13, IF(J8="Nhà Bè", Ward!$AM$2:$AN$8, IF(J8="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J8="Tân Bình", Ward!$AQ$2:$AR$16, IF(J8="Tân Phú", Ward!$AS$2:$AT$12, IF(J8="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X8" t="str">
+        <f>IF(B8 &lt;&gt; "", VLOOKUP(B8, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -2459,8 +2520,12 @@
         <f>IF(K9 &lt;&gt; "", VLOOKUP(K9, IF(J9="1", Ward!$A$2:$B$11, IF(J9="2", Ward!$C$2:$D$12, IF(J9="3", Ward!$E$2:$F$15, IF(J9="4", Ward!$G$2:$H$16, IF(J9="5", Ward!$I$2:$J$16, IF(J9="6", Ward!$K$2:$L$15, IF(J9="7", Ward!$M$2:$N$11, IF(J9="8", Ward!$O$2:$P$17, IF(J9="9", Ward!$Q$2:$R$14, IF(J9="10", Ward!$S$2:$T$16, IF(J9="11", Ward!$U$2:$V$17, IF(J9="12", Ward!$W$2:$X$12, IF(J9="Bình Chánh", Ward!$Y$2:$Z$17, IF(J9="Bình Tân", Ward!$AA$2:$AB$11, IF(J9="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J9="Cần Giờ", Ward!$AE$2:$AF$8, IF(J9="Củ Chi", Ward!$AG$2:$AH$22, IF(J9="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J9="Hóc Môn", Ward!$AK$2:$AL$13, IF(J9="Nhà Bè", Ward!$AM$2:$AN$8, IF(J9="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J9="Tân Bình", Ward!$AQ$2:$AR$16, IF(J9="Tân Phú", Ward!$AS$2:$AT$12, IF(J9="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X9" t="str">
+        <f>IF(B9 &lt;&gt; "", VLOOKUP(B9, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -2493,8 +2558,12 @@
         <f>IF(K10 &lt;&gt; "", VLOOKUP(K10, IF(J10="1", Ward!$A$2:$B$11, IF(J10="2", Ward!$C$2:$D$12, IF(J10="3", Ward!$E$2:$F$15, IF(J10="4", Ward!$G$2:$H$16, IF(J10="5", Ward!$I$2:$J$16, IF(J10="6", Ward!$K$2:$L$15, IF(J10="7", Ward!$M$2:$N$11, IF(J10="8", Ward!$O$2:$P$17, IF(J10="9", Ward!$Q$2:$R$14, IF(J10="10", Ward!$S$2:$T$16, IF(J10="11", Ward!$U$2:$V$17, IF(J10="12", Ward!$W$2:$X$12, IF(J10="Bình Chánh", Ward!$Y$2:$Z$17, IF(J10="Bình Tân", Ward!$AA$2:$AB$11, IF(J10="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J10="Cần Giờ", Ward!$AE$2:$AF$8, IF(J10="Củ Chi", Ward!$AG$2:$AH$22, IF(J10="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J10="Hóc Môn", Ward!$AK$2:$AL$13, IF(J10="Nhà Bè", Ward!$AM$2:$AN$8, IF(J10="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J10="Tân Bình", Ward!$AQ$2:$AR$16, IF(J10="Tân Phú", Ward!$AS$2:$AT$12, IF(J10="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X10" t="str">
+        <f>IF(B10 &lt;&gt; "", VLOOKUP(B10, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -2527,8 +2596,12 @@
         <f>IF(K11 &lt;&gt; "", VLOOKUP(K11, IF(J11="1", Ward!$A$2:$B$11, IF(J11="2", Ward!$C$2:$D$12, IF(J11="3", Ward!$E$2:$F$15, IF(J11="4", Ward!$G$2:$H$16, IF(J11="5", Ward!$I$2:$J$16, IF(J11="6", Ward!$K$2:$L$15, IF(J11="7", Ward!$M$2:$N$11, IF(J11="8", Ward!$O$2:$P$17, IF(J11="9", Ward!$Q$2:$R$14, IF(J11="10", Ward!$S$2:$T$16, IF(J11="11", Ward!$U$2:$V$17, IF(J11="12", Ward!$W$2:$X$12, IF(J11="Bình Chánh", Ward!$Y$2:$Z$17, IF(J11="Bình Tân", Ward!$AA$2:$AB$11, IF(J11="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J11="Cần Giờ", Ward!$AE$2:$AF$8, IF(J11="Củ Chi", Ward!$AG$2:$AH$22, IF(J11="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J11="Hóc Môn", Ward!$AK$2:$AL$13, IF(J11="Nhà Bè", Ward!$AM$2:$AN$8, IF(J11="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J11="Tân Bình", Ward!$AQ$2:$AR$16, IF(J11="Tân Phú", Ward!$AS$2:$AT$12, IF(J11="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X11" t="str">
+        <f>IF(B11 &lt;&gt; "", VLOOKUP(B11, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -2561,8 +2634,12 @@
         <f>IF(K12 &lt;&gt; "", VLOOKUP(K12, IF(J12="1", Ward!$A$2:$B$11, IF(J12="2", Ward!$C$2:$D$12, IF(J12="3", Ward!$E$2:$F$15, IF(J12="4", Ward!$G$2:$H$16, IF(J12="5", Ward!$I$2:$J$16, IF(J12="6", Ward!$K$2:$L$15, IF(J12="7", Ward!$M$2:$N$11, IF(J12="8", Ward!$O$2:$P$17, IF(J12="9", Ward!$Q$2:$R$14, IF(J12="10", Ward!$S$2:$T$16, IF(J12="11", Ward!$U$2:$V$17, IF(J12="12", Ward!$W$2:$X$12, IF(J12="Bình Chánh", Ward!$Y$2:$Z$17, IF(J12="Bình Tân", Ward!$AA$2:$AB$11, IF(J12="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J12="Cần Giờ", Ward!$AE$2:$AF$8, IF(J12="Củ Chi", Ward!$AG$2:$AH$22, IF(J12="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J12="Hóc Môn", Ward!$AK$2:$AL$13, IF(J12="Nhà Bè", Ward!$AM$2:$AN$8, IF(J12="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J12="Tân Bình", Ward!$AQ$2:$AR$16, IF(J12="Tân Phú", Ward!$AS$2:$AT$12, IF(J12="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X12" t="str">
+        <f>IF(B12 &lt;&gt; "", VLOOKUP(B12, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -2595,8 +2672,12 @@
         <f>IF(K13 &lt;&gt; "", VLOOKUP(K13, IF(J13="1", Ward!$A$2:$B$11, IF(J13="2", Ward!$C$2:$D$12, IF(J13="3", Ward!$E$2:$F$15, IF(J13="4", Ward!$G$2:$H$16, IF(J13="5", Ward!$I$2:$J$16, IF(J13="6", Ward!$K$2:$L$15, IF(J13="7", Ward!$M$2:$N$11, IF(J13="8", Ward!$O$2:$P$17, IF(J13="9", Ward!$Q$2:$R$14, IF(J13="10", Ward!$S$2:$T$16, IF(J13="11", Ward!$U$2:$V$17, IF(J13="12", Ward!$W$2:$X$12, IF(J13="Bình Chánh", Ward!$Y$2:$Z$17, IF(J13="Bình Tân", Ward!$AA$2:$AB$11, IF(J13="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J13="Cần Giờ", Ward!$AE$2:$AF$8, IF(J13="Củ Chi", Ward!$AG$2:$AH$22, IF(J13="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J13="Hóc Môn", Ward!$AK$2:$AL$13, IF(J13="Nhà Bè", Ward!$AM$2:$AN$8, IF(J13="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J13="Tân Bình", Ward!$AQ$2:$AR$16, IF(J13="Tân Phú", Ward!$AS$2:$AT$12, IF(J13="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X13" t="str">
+        <f>IF(B13 &lt;&gt; "", VLOOKUP(B13, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -2629,8 +2710,12 @@
         <f>IF(K14 &lt;&gt; "", VLOOKUP(K14, IF(J14="1", Ward!$A$2:$B$11, IF(J14="2", Ward!$C$2:$D$12, IF(J14="3", Ward!$E$2:$F$15, IF(J14="4", Ward!$G$2:$H$16, IF(J14="5", Ward!$I$2:$J$16, IF(J14="6", Ward!$K$2:$L$15, IF(J14="7", Ward!$M$2:$N$11, IF(J14="8", Ward!$O$2:$P$17, IF(J14="9", Ward!$Q$2:$R$14, IF(J14="10", Ward!$S$2:$T$16, IF(J14="11", Ward!$U$2:$V$17, IF(J14="12", Ward!$W$2:$X$12, IF(J14="Bình Chánh", Ward!$Y$2:$Z$17, IF(J14="Bình Tân", Ward!$AA$2:$AB$11, IF(J14="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J14="Cần Giờ", Ward!$AE$2:$AF$8, IF(J14="Củ Chi", Ward!$AG$2:$AH$22, IF(J14="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J14="Hóc Môn", Ward!$AK$2:$AL$13, IF(J14="Nhà Bè", Ward!$AM$2:$AN$8, IF(J14="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J14="Tân Bình", Ward!$AQ$2:$AR$16, IF(J14="Tân Phú", Ward!$AS$2:$AT$12, IF(J14="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X14" t="str">
+        <f>IF(B14 &lt;&gt; "", VLOOKUP(B14, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -2663,8 +2748,12 @@
         <f>IF(K15 &lt;&gt; "", VLOOKUP(K15, IF(J15="1", Ward!$A$2:$B$11, IF(J15="2", Ward!$C$2:$D$12, IF(J15="3", Ward!$E$2:$F$15, IF(J15="4", Ward!$G$2:$H$16, IF(J15="5", Ward!$I$2:$J$16, IF(J15="6", Ward!$K$2:$L$15, IF(J15="7", Ward!$M$2:$N$11, IF(J15="8", Ward!$O$2:$P$17, IF(J15="9", Ward!$Q$2:$R$14, IF(J15="10", Ward!$S$2:$T$16, IF(J15="11", Ward!$U$2:$V$17, IF(J15="12", Ward!$W$2:$X$12, IF(J15="Bình Chánh", Ward!$Y$2:$Z$17, IF(J15="Bình Tân", Ward!$AA$2:$AB$11, IF(J15="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J15="Cần Giờ", Ward!$AE$2:$AF$8, IF(J15="Củ Chi", Ward!$AG$2:$AH$22, IF(J15="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J15="Hóc Môn", Ward!$AK$2:$AL$13, IF(J15="Nhà Bè", Ward!$AM$2:$AN$8, IF(J15="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J15="Tân Bình", Ward!$AQ$2:$AR$16, IF(J15="Tân Phú", Ward!$AS$2:$AT$12, IF(J15="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X15" t="str">
+        <f>IF(B15 &lt;&gt; "", VLOOKUP(B15, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -2697,8 +2786,12 @@
         <f>IF(K16 &lt;&gt; "", VLOOKUP(K16, IF(J16="1", Ward!$A$2:$B$11, IF(J16="2", Ward!$C$2:$D$12, IF(J16="3", Ward!$E$2:$F$15, IF(J16="4", Ward!$G$2:$H$16, IF(J16="5", Ward!$I$2:$J$16, IF(J16="6", Ward!$K$2:$L$15, IF(J16="7", Ward!$M$2:$N$11, IF(J16="8", Ward!$O$2:$P$17, IF(J16="9", Ward!$Q$2:$R$14, IF(J16="10", Ward!$S$2:$T$16, IF(J16="11", Ward!$U$2:$V$17, IF(J16="12", Ward!$W$2:$X$12, IF(J16="Bình Chánh", Ward!$Y$2:$Z$17, IF(J16="Bình Tân", Ward!$AA$2:$AB$11, IF(J16="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J16="Cần Giờ", Ward!$AE$2:$AF$8, IF(J16="Củ Chi", Ward!$AG$2:$AH$22, IF(J16="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J16="Hóc Môn", Ward!$AK$2:$AL$13, IF(J16="Nhà Bè", Ward!$AM$2:$AN$8, IF(J16="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J16="Tân Bình", Ward!$AQ$2:$AR$16, IF(J16="Tân Phú", Ward!$AS$2:$AT$12, IF(J16="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X16" t="str">
+        <f>IF(B16 &lt;&gt; "", VLOOKUP(B16, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -2731,8 +2824,12 @@
         <f>IF(K17 &lt;&gt; "", VLOOKUP(K17, IF(J17="1", Ward!$A$2:$B$11, IF(J17="2", Ward!$C$2:$D$12, IF(J17="3", Ward!$E$2:$F$15, IF(J17="4", Ward!$G$2:$H$16, IF(J17="5", Ward!$I$2:$J$16, IF(J17="6", Ward!$K$2:$L$15, IF(J17="7", Ward!$M$2:$N$11, IF(J17="8", Ward!$O$2:$P$17, IF(J17="9", Ward!$Q$2:$R$14, IF(J17="10", Ward!$S$2:$T$16, IF(J17="11", Ward!$U$2:$V$17, IF(J17="12", Ward!$W$2:$X$12, IF(J17="Bình Chánh", Ward!$Y$2:$Z$17, IF(J17="Bình Tân", Ward!$AA$2:$AB$11, IF(J17="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J17="Cần Giờ", Ward!$AE$2:$AF$8, IF(J17="Củ Chi", Ward!$AG$2:$AH$22, IF(J17="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J17="Hóc Môn", Ward!$AK$2:$AL$13, IF(J17="Nhà Bè", Ward!$AM$2:$AN$8, IF(J17="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J17="Tân Bình", Ward!$AQ$2:$AR$16, IF(J17="Tân Phú", Ward!$AS$2:$AT$12, IF(J17="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X17" t="str">
+        <f>IF(B17 &lt;&gt; "", VLOOKUP(B17, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -2765,8 +2862,12 @@
         <f>IF(K18 &lt;&gt; "", VLOOKUP(K18, IF(J18="1", Ward!$A$2:$B$11, IF(J18="2", Ward!$C$2:$D$12, IF(J18="3", Ward!$E$2:$F$15, IF(J18="4", Ward!$G$2:$H$16, IF(J18="5", Ward!$I$2:$J$16, IF(J18="6", Ward!$K$2:$L$15, IF(J18="7", Ward!$M$2:$N$11, IF(J18="8", Ward!$O$2:$P$17, IF(J18="9", Ward!$Q$2:$R$14, IF(J18="10", Ward!$S$2:$T$16, IF(J18="11", Ward!$U$2:$V$17, IF(J18="12", Ward!$W$2:$X$12, IF(J18="Bình Chánh", Ward!$Y$2:$Z$17, IF(J18="Bình Tân", Ward!$AA$2:$AB$11, IF(J18="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J18="Cần Giờ", Ward!$AE$2:$AF$8, IF(J18="Củ Chi", Ward!$AG$2:$AH$22, IF(J18="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J18="Hóc Môn", Ward!$AK$2:$AL$13, IF(J18="Nhà Bè", Ward!$AM$2:$AN$8, IF(J18="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J18="Tân Bình", Ward!$AQ$2:$AR$16, IF(J18="Tân Phú", Ward!$AS$2:$AT$12, IF(J18="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X18" t="str">
+        <f>IF(B18 &lt;&gt; "", VLOOKUP(B18, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -2799,8 +2900,12 @@
         <f>IF(K19 &lt;&gt; "", VLOOKUP(K19, IF(J19="1", Ward!$A$2:$B$11, IF(J19="2", Ward!$C$2:$D$12, IF(J19="3", Ward!$E$2:$F$15, IF(J19="4", Ward!$G$2:$H$16, IF(J19="5", Ward!$I$2:$J$16, IF(J19="6", Ward!$K$2:$L$15, IF(J19="7", Ward!$M$2:$N$11, IF(J19="8", Ward!$O$2:$P$17, IF(J19="9", Ward!$Q$2:$R$14, IF(J19="10", Ward!$S$2:$T$16, IF(J19="11", Ward!$U$2:$V$17, IF(J19="12", Ward!$W$2:$X$12, IF(J19="Bình Chánh", Ward!$Y$2:$Z$17, IF(J19="Bình Tân", Ward!$AA$2:$AB$11, IF(J19="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J19="Cần Giờ", Ward!$AE$2:$AF$8, IF(J19="Củ Chi", Ward!$AG$2:$AH$22, IF(J19="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J19="Hóc Môn", Ward!$AK$2:$AL$13, IF(J19="Nhà Bè", Ward!$AM$2:$AN$8, IF(J19="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J19="Tân Bình", Ward!$AQ$2:$AR$16, IF(J19="Tân Phú", Ward!$AS$2:$AT$12, IF(J19="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X19" t="str">
+        <f>IF(B19 &lt;&gt; "", VLOOKUP(B19, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -2833,8 +2938,12 @@
         <f>IF(K20 &lt;&gt; "", VLOOKUP(K20, IF(J20="1", Ward!$A$2:$B$11, IF(J20="2", Ward!$C$2:$D$12, IF(J20="3", Ward!$E$2:$F$15, IF(J20="4", Ward!$G$2:$H$16, IF(J20="5", Ward!$I$2:$J$16, IF(J20="6", Ward!$K$2:$L$15, IF(J20="7", Ward!$M$2:$N$11, IF(J20="8", Ward!$O$2:$P$17, IF(J20="9", Ward!$Q$2:$R$14, IF(J20="10", Ward!$S$2:$T$16, IF(J20="11", Ward!$U$2:$V$17, IF(J20="12", Ward!$W$2:$X$12, IF(J20="Bình Chánh", Ward!$Y$2:$Z$17, IF(J20="Bình Tân", Ward!$AA$2:$AB$11, IF(J20="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J20="Cần Giờ", Ward!$AE$2:$AF$8, IF(J20="Củ Chi", Ward!$AG$2:$AH$22, IF(J20="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J20="Hóc Môn", Ward!$AK$2:$AL$13, IF(J20="Nhà Bè", Ward!$AM$2:$AN$8, IF(J20="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J20="Tân Bình", Ward!$AQ$2:$AR$16, IF(J20="Tân Phú", Ward!$AS$2:$AT$12, IF(J20="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X20" t="str">
+        <f>IF(B20 &lt;&gt; "", VLOOKUP(B20, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -2867,8 +2976,12 @@
         <f>IF(K21 &lt;&gt; "", VLOOKUP(K21, IF(J21="1", Ward!$A$2:$B$11, IF(J21="2", Ward!$C$2:$D$12, IF(J21="3", Ward!$E$2:$F$15, IF(J21="4", Ward!$G$2:$H$16, IF(J21="5", Ward!$I$2:$J$16, IF(J21="6", Ward!$K$2:$L$15, IF(J21="7", Ward!$M$2:$N$11, IF(J21="8", Ward!$O$2:$P$17, IF(J21="9", Ward!$Q$2:$R$14, IF(J21="10", Ward!$S$2:$T$16, IF(J21="11", Ward!$U$2:$V$17, IF(J21="12", Ward!$W$2:$X$12, IF(J21="Bình Chánh", Ward!$Y$2:$Z$17, IF(J21="Bình Tân", Ward!$AA$2:$AB$11, IF(J21="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J21="Cần Giờ", Ward!$AE$2:$AF$8, IF(J21="Củ Chi", Ward!$AG$2:$AH$22, IF(J21="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J21="Hóc Môn", Ward!$AK$2:$AL$13, IF(J21="Nhà Bè", Ward!$AM$2:$AN$8, IF(J21="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J21="Tân Bình", Ward!$AQ$2:$AR$16, IF(J21="Tân Phú", Ward!$AS$2:$AT$12, IF(J21="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X21" t="str">
+        <f>IF(B21 &lt;&gt; "", VLOOKUP(B21, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -2901,8 +3014,12 @@
         <f>IF(K22 &lt;&gt; "", VLOOKUP(K22, IF(J22="1", Ward!$A$2:$B$11, IF(J22="2", Ward!$C$2:$D$12, IF(J22="3", Ward!$E$2:$F$15, IF(J22="4", Ward!$G$2:$H$16, IF(J22="5", Ward!$I$2:$J$16, IF(J22="6", Ward!$K$2:$L$15, IF(J22="7", Ward!$M$2:$N$11, IF(J22="8", Ward!$O$2:$P$17, IF(J22="9", Ward!$Q$2:$R$14, IF(J22="10", Ward!$S$2:$T$16, IF(J22="11", Ward!$U$2:$V$17, IF(J22="12", Ward!$W$2:$X$12, IF(J22="Bình Chánh", Ward!$Y$2:$Z$17, IF(J22="Bình Tân", Ward!$AA$2:$AB$11, IF(J22="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J22="Cần Giờ", Ward!$AE$2:$AF$8, IF(J22="Củ Chi", Ward!$AG$2:$AH$22, IF(J22="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J22="Hóc Môn", Ward!$AK$2:$AL$13, IF(J22="Nhà Bè", Ward!$AM$2:$AN$8, IF(J22="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J22="Tân Bình", Ward!$AQ$2:$AR$16, IF(J22="Tân Phú", Ward!$AS$2:$AT$12, IF(J22="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X22" t="str">
+        <f>IF(B22 &lt;&gt; "", VLOOKUP(B22, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -2935,8 +3052,12 @@
         <f>IF(K23 &lt;&gt; "", VLOOKUP(K23, IF(J23="1", Ward!$A$2:$B$11, IF(J23="2", Ward!$C$2:$D$12, IF(J23="3", Ward!$E$2:$F$15, IF(J23="4", Ward!$G$2:$H$16, IF(J23="5", Ward!$I$2:$J$16, IF(J23="6", Ward!$K$2:$L$15, IF(J23="7", Ward!$M$2:$N$11, IF(J23="8", Ward!$O$2:$P$17, IF(J23="9", Ward!$Q$2:$R$14, IF(J23="10", Ward!$S$2:$T$16, IF(J23="11", Ward!$U$2:$V$17, IF(J23="12", Ward!$W$2:$X$12, IF(J23="Bình Chánh", Ward!$Y$2:$Z$17, IF(J23="Bình Tân", Ward!$AA$2:$AB$11, IF(J23="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J23="Cần Giờ", Ward!$AE$2:$AF$8, IF(J23="Củ Chi", Ward!$AG$2:$AH$22, IF(J23="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J23="Hóc Môn", Ward!$AK$2:$AL$13, IF(J23="Nhà Bè", Ward!$AM$2:$AN$8, IF(J23="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J23="Tân Bình", Ward!$AQ$2:$AR$16, IF(J23="Tân Phú", Ward!$AS$2:$AT$12, IF(J23="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X23" t="str">
+        <f>IF(B23 &lt;&gt; "", VLOOKUP(B23, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -2969,8 +3090,12 @@
         <f>IF(K24 &lt;&gt; "", VLOOKUP(K24, IF(J24="1", Ward!$A$2:$B$11, IF(J24="2", Ward!$C$2:$D$12, IF(J24="3", Ward!$E$2:$F$15, IF(J24="4", Ward!$G$2:$H$16, IF(J24="5", Ward!$I$2:$J$16, IF(J24="6", Ward!$K$2:$L$15, IF(J24="7", Ward!$M$2:$N$11, IF(J24="8", Ward!$O$2:$P$17, IF(J24="9", Ward!$Q$2:$R$14, IF(J24="10", Ward!$S$2:$T$16, IF(J24="11", Ward!$U$2:$V$17, IF(J24="12", Ward!$W$2:$X$12, IF(J24="Bình Chánh", Ward!$Y$2:$Z$17, IF(J24="Bình Tân", Ward!$AA$2:$AB$11, IF(J24="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J24="Cần Giờ", Ward!$AE$2:$AF$8, IF(J24="Củ Chi", Ward!$AG$2:$AH$22, IF(J24="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J24="Hóc Môn", Ward!$AK$2:$AL$13, IF(J24="Nhà Bè", Ward!$AM$2:$AN$8, IF(J24="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J24="Tân Bình", Ward!$AQ$2:$AR$16, IF(J24="Tân Phú", Ward!$AS$2:$AT$12, IF(J24="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X24" t="str">
+        <f>IF(B24 &lt;&gt; "", VLOOKUP(B24, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -3003,8 +3128,12 @@
         <f>IF(K25 &lt;&gt; "", VLOOKUP(K25, IF(J25="1", Ward!$A$2:$B$11, IF(J25="2", Ward!$C$2:$D$12, IF(J25="3", Ward!$E$2:$F$15, IF(J25="4", Ward!$G$2:$H$16, IF(J25="5", Ward!$I$2:$J$16, IF(J25="6", Ward!$K$2:$L$15, IF(J25="7", Ward!$M$2:$N$11, IF(J25="8", Ward!$O$2:$P$17, IF(J25="9", Ward!$Q$2:$R$14, IF(J25="10", Ward!$S$2:$T$16, IF(J25="11", Ward!$U$2:$V$17, IF(J25="12", Ward!$W$2:$X$12, IF(J25="Bình Chánh", Ward!$Y$2:$Z$17, IF(J25="Bình Tân", Ward!$AA$2:$AB$11, IF(J25="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J25="Cần Giờ", Ward!$AE$2:$AF$8, IF(J25="Củ Chi", Ward!$AG$2:$AH$22, IF(J25="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J25="Hóc Môn", Ward!$AK$2:$AL$13, IF(J25="Nhà Bè", Ward!$AM$2:$AN$8, IF(J25="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J25="Tân Bình", Ward!$AQ$2:$AR$16, IF(J25="Tân Phú", Ward!$AS$2:$AT$12, IF(J25="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X25" t="str">
+        <f>IF(B25 &lt;&gt; "", VLOOKUP(B25, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -3037,8 +3166,12 @@
         <f>IF(K26 &lt;&gt; "", VLOOKUP(K26, IF(J26="1", Ward!$A$2:$B$11, IF(J26="2", Ward!$C$2:$D$12, IF(J26="3", Ward!$E$2:$F$15, IF(J26="4", Ward!$G$2:$H$16, IF(J26="5", Ward!$I$2:$J$16, IF(J26="6", Ward!$K$2:$L$15, IF(J26="7", Ward!$M$2:$N$11, IF(J26="8", Ward!$O$2:$P$17, IF(J26="9", Ward!$Q$2:$R$14, IF(J26="10", Ward!$S$2:$T$16, IF(J26="11", Ward!$U$2:$V$17, IF(J26="12", Ward!$W$2:$X$12, IF(J26="Bình Chánh", Ward!$Y$2:$Z$17, IF(J26="Bình Tân", Ward!$AA$2:$AB$11, IF(J26="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J26="Cần Giờ", Ward!$AE$2:$AF$8, IF(J26="Củ Chi", Ward!$AG$2:$AH$22, IF(J26="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J26="Hóc Môn", Ward!$AK$2:$AL$13, IF(J26="Nhà Bè", Ward!$AM$2:$AN$8, IF(J26="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J26="Tân Bình", Ward!$AQ$2:$AR$16, IF(J26="Tân Phú", Ward!$AS$2:$AT$12, IF(J26="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X26" t="str">
+        <f>IF(B26 &lt;&gt; "", VLOOKUP(B26, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -3071,8 +3204,12 @@
         <f>IF(K27 &lt;&gt; "", VLOOKUP(K27, IF(J27="1", Ward!$A$2:$B$11, IF(J27="2", Ward!$C$2:$D$12, IF(J27="3", Ward!$E$2:$F$15, IF(J27="4", Ward!$G$2:$H$16, IF(J27="5", Ward!$I$2:$J$16, IF(J27="6", Ward!$K$2:$L$15, IF(J27="7", Ward!$M$2:$N$11, IF(J27="8", Ward!$O$2:$P$17, IF(J27="9", Ward!$Q$2:$R$14, IF(J27="10", Ward!$S$2:$T$16, IF(J27="11", Ward!$U$2:$V$17, IF(J27="12", Ward!$W$2:$X$12, IF(J27="Bình Chánh", Ward!$Y$2:$Z$17, IF(J27="Bình Tân", Ward!$AA$2:$AB$11, IF(J27="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J27="Cần Giờ", Ward!$AE$2:$AF$8, IF(J27="Củ Chi", Ward!$AG$2:$AH$22, IF(J27="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J27="Hóc Môn", Ward!$AK$2:$AL$13, IF(J27="Nhà Bè", Ward!$AM$2:$AN$8, IF(J27="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J27="Tân Bình", Ward!$AQ$2:$AR$16, IF(J27="Tân Phú", Ward!$AS$2:$AT$12, IF(J27="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X27" t="str">
+        <f>IF(B27 &lt;&gt; "", VLOOKUP(B27, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -3105,8 +3242,12 @@
         <f>IF(K28 &lt;&gt; "", VLOOKUP(K28, IF(J28="1", Ward!$A$2:$B$11, IF(J28="2", Ward!$C$2:$D$12, IF(J28="3", Ward!$E$2:$F$15, IF(J28="4", Ward!$G$2:$H$16, IF(J28="5", Ward!$I$2:$J$16, IF(J28="6", Ward!$K$2:$L$15, IF(J28="7", Ward!$M$2:$N$11, IF(J28="8", Ward!$O$2:$P$17, IF(J28="9", Ward!$Q$2:$R$14, IF(J28="10", Ward!$S$2:$T$16, IF(J28="11", Ward!$U$2:$V$17, IF(J28="12", Ward!$W$2:$X$12, IF(J28="Bình Chánh", Ward!$Y$2:$Z$17, IF(J28="Bình Tân", Ward!$AA$2:$AB$11, IF(J28="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J28="Cần Giờ", Ward!$AE$2:$AF$8, IF(J28="Củ Chi", Ward!$AG$2:$AH$22, IF(J28="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J28="Hóc Môn", Ward!$AK$2:$AL$13, IF(J28="Nhà Bè", Ward!$AM$2:$AN$8, IF(J28="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J28="Tân Bình", Ward!$AQ$2:$AR$16, IF(J28="Tân Phú", Ward!$AS$2:$AT$12, IF(J28="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X28" t="str">
+        <f>IF(B28 &lt;&gt; "", VLOOKUP(B28, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -3139,8 +3280,12 @@
         <f>IF(K29 &lt;&gt; "", VLOOKUP(K29, IF(J29="1", Ward!$A$2:$B$11, IF(J29="2", Ward!$C$2:$D$12, IF(J29="3", Ward!$E$2:$F$15, IF(J29="4", Ward!$G$2:$H$16, IF(J29="5", Ward!$I$2:$J$16, IF(J29="6", Ward!$K$2:$L$15, IF(J29="7", Ward!$M$2:$N$11, IF(J29="8", Ward!$O$2:$P$17, IF(J29="9", Ward!$Q$2:$R$14, IF(J29="10", Ward!$S$2:$T$16, IF(J29="11", Ward!$U$2:$V$17, IF(J29="12", Ward!$W$2:$X$12, IF(J29="Bình Chánh", Ward!$Y$2:$Z$17, IF(J29="Bình Tân", Ward!$AA$2:$AB$11, IF(J29="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J29="Cần Giờ", Ward!$AE$2:$AF$8, IF(J29="Củ Chi", Ward!$AG$2:$AH$22, IF(J29="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J29="Hóc Môn", Ward!$AK$2:$AL$13, IF(J29="Nhà Bè", Ward!$AM$2:$AN$8, IF(J29="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J29="Tân Bình", Ward!$AQ$2:$AR$16, IF(J29="Tân Phú", Ward!$AS$2:$AT$12, IF(J29="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X29" t="str">
+        <f>IF(B29 &lt;&gt; "", VLOOKUP(B29, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -3173,8 +3318,12 @@
         <f>IF(K30 &lt;&gt; "", VLOOKUP(K30, IF(J30="1", Ward!$A$2:$B$11, IF(J30="2", Ward!$C$2:$D$12, IF(J30="3", Ward!$E$2:$F$15, IF(J30="4", Ward!$G$2:$H$16, IF(J30="5", Ward!$I$2:$J$16, IF(J30="6", Ward!$K$2:$L$15, IF(J30="7", Ward!$M$2:$N$11, IF(J30="8", Ward!$O$2:$P$17, IF(J30="9", Ward!$Q$2:$R$14, IF(J30="10", Ward!$S$2:$T$16, IF(J30="11", Ward!$U$2:$V$17, IF(J30="12", Ward!$W$2:$X$12, IF(J30="Bình Chánh", Ward!$Y$2:$Z$17, IF(J30="Bình Tân", Ward!$AA$2:$AB$11, IF(J30="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J30="Cần Giờ", Ward!$AE$2:$AF$8, IF(J30="Củ Chi", Ward!$AG$2:$AH$22, IF(J30="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J30="Hóc Môn", Ward!$AK$2:$AL$13, IF(J30="Nhà Bè", Ward!$AM$2:$AN$8, IF(J30="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J30="Tân Bình", Ward!$AQ$2:$AR$16, IF(J30="Tân Phú", Ward!$AS$2:$AT$12, IF(J30="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X30" t="str">
+        <f>IF(B30 &lt;&gt; "", VLOOKUP(B30, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -3207,8 +3356,12 @@
         <f>IF(K31 &lt;&gt; "", VLOOKUP(K31, IF(J31="1", Ward!$A$2:$B$11, IF(J31="2", Ward!$C$2:$D$12, IF(J31="3", Ward!$E$2:$F$15, IF(J31="4", Ward!$G$2:$H$16, IF(J31="5", Ward!$I$2:$J$16, IF(J31="6", Ward!$K$2:$L$15, IF(J31="7", Ward!$M$2:$N$11, IF(J31="8", Ward!$O$2:$P$17, IF(J31="9", Ward!$Q$2:$R$14, IF(J31="10", Ward!$S$2:$T$16, IF(J31="11", Ward!$U$2:$V$17, IF(J31="12", Ward!$W$2:$X$12, IF(J31="Bình Chánh", Ward!$Y$2:$Z$17, IF(J31="Bình Tân", Ward!$AA$2:$AB$11, IF(J31="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J31="Cần Giờ", Ward!$AE$2:$AF$8, IF(J31="Củ Chi", Ward!$AG$2:$AH$22, IF(J31="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J31="Hóc Môn", Ward!$AK$2:$AL$13, IF(J31="Nhà Bè", Ward!$AM$2:$AN$8, IF(J31="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J31="Tân Bình", Ward!$AQ$2:$AR$16, IF(J31="Tân Phú", Ward!$AS$2:$AT$12, IF(J31="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X31" t="str">
+        <f>IF(B31 &lt;&gt; "", VLOOKUP(B31, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -3241,8 +3394,12 @@
         <f>IF(K32 &lt;&gt; "", VLOOKUP(K32, IF(J32="1", Ward!$A$2:$B$11, IF(J32="2", Ward!$C$2:$D$12, IF(J32="3", Ward!$E$2:$F$15, IF(J32="4", Ward!$G$2:$H$16, IF(J32="5", Ward!$I$2:$J$16, IF(J32="6", Ward!$K$2:$L$15, IF(J32="7", Ward!$M$2:$N$11, IF(J32="8", Ward!$O$2:$P$17, IF(J32="9", Ward!$Q$2:$R$14, IF(J32="10", Ward!$S$2:$T$16, IF(J32="11", Ward!$U$2:$V$17, IF(J32="12", Ward!$W$2:$X$12, IF(J32="Bình Chánh", Ward!$Y$2:$Z$17, IF(J32="Bình Tân", Ward!$AA$2:$AB$11, IF(J32="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J32="Cần Giờ", Ward!$AE$2:$AF$8, IF(J32="Củ Chi", Ward!$AG$2:$AH$22, IF(J32="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J32="Hóc Môn", Ward!$AK$2:$AL$13, IF(J32="Nhà Bè", Ward!$AM$2:$AN$8, IF(J32="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J32="Tân Bình", Ward!$AQ$2:$AR$16, IF(J32="Tân Phú", Ward!$AS$2:$AT$12, IF(J32="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X32" t="str">
+        <f>IF(B32 &lt;&gt; "", VLOOKUP(B32, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -3275,8 +3432,12 @@
         <f>IF(K33 &lt;&gt; "", VLOOKUP(K33, IF(J33="1", Ward!$A$2:$B$11, IF(J33="2", Ward!$C$2:$D$12, IF(J33="3", Ward!$E$2:$F$15, IF(J33="4", Ward!$G$2:$H$16, IF(J33="5", Ward!$I$2:$J$16, IF(J33="6", Ward!$K$2:$L$15, IF(J33="7", Ward!$M$2:$N$11, IF(J33="8", Ward!$O$2:$P$17, IF(J33="9", Ward!$Q$2:$R$14, IF(J33="10", Ward!$S$2:$T$16, IF(J33="11", Ward!$U$2:$V$17, IF(J33="12", Ward!$W$2:$X$12, IF(J33="Bình Chánh", Ward!$Y$2:$Z$17, IF(J33="Bình Tân", Ward!$AA$2:$AB$11, IF(J33="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J33="Cần Giờ", Ward!$AE$2:$AF$8, IF(J33="Củ Chi", Ward!$AG$2:$AH$22, IF(J33="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J33="Hóc Môn", Ward!$AK$2:$AL$13, IF(J33="Nhà Bè", Ward!$AM$2:$AN$8, IF(J33="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J33="Tân Bình", Ward!$AQ$2:$AR$16, IF(J33="Tân Phú", Ward!$AS$2:$AT$12, IF(J33="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X33" t="str">
+        <f>IF(B33 &lt;&gt; "", VLOOKUP(B33, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -3309,8 +3470,12 @@
         <f>IF(K34 &lt;&gt; "", VLOOKUP(K34, IF(J34="1", Ward!$A$2:$B$11, IF(J34="2", Ward!$C$2:$D$12, IF(J34="3", Ward!$E$2:$F$15, IF(J34="4", Ward!$G$2:$H$16, IF(J34="5", Ward!$I$2:$J$16, IF(J34="6", Ward!$K$2:$L$15, IF(J34="7", Ward!$M$2:$N$11, IF(J34="8", Ward!$O$2:$P$17, IF(J34="9", Ward!$Q$2:$R$14, IF(J34="10", Ward!$S$2:$T$16, IF(J34="11", Ward!$U$2:$V$17, IF(J34="12", Ward!$W$2:$X$12, IF(J34="Bình Chánh", Ward!$Y$2:$Z$17, IF(J34="Bình Tân", Ward!$AA$2:$AB$11, IF(J34="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J34="Cần Giờ", Ward!$AE$2:$AF$8, IF(J34="Củ Chi", Ward!$AG$2:$AH$22, IF(J34="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J34="Hóc Môn", Ward!$AK$2:$AL$13, IF(J34="Nhà Bè", Ward!$AM$2:$AN$8, IF(J34="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J34="Tân Bình", Ward!$AQ$2:$AR$16, IF(J34="Tân Phú", Ward!$AS$2:$AT$12, IF(J34="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X34" t="str">
+        <f>IF(B34 &lt;&gt; "", VLOOKUP(B34, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -3343,8 +3508,12 @@
         <f>IF(K35 &lt;&gt; "", VLOOKUP(K35, IF(J35="1", Ward!$A$2:$B$11, IF(J35="2", Ward!$C$2:$D$12, IF(J35="3", Ward!$E$2:$F$15, IF(J35="4", Ward!$G$2:$H$16, IF(J35="5", Ward!$I$2:$J$16, IF(J35="6", Ward!$K$2:$L$15, IF(J35="7", Ward!$M$2:$N$11, IF(J35="8", Ward!$O$2:$P$17, IF(J35="9", Ward!$Q$2:$R$14, IF(J35="10", Ward!$S$2:$T$16, IF(J35="11", Ward!$U$2:$V$17, IF(J35="12", Ward!$W$2:$X$12, IF(J35="Bình Chánh", Ward!$Y$2:$Z$17, IF(J35="Bình Tân", Ward!$AA$2:$AB$11, IF(J35="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J35="Cần Giờ", Ward!$AE$2:$AF$8, IF(J35="Củ Chi", Ward!$AG$2:$AH$22, IF(J35="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J35="Hóc Môn", Ward!$AK$2:$AL$13, IF(J35="Nhà Bè", Ward!$AM$2:$AN$8, IF(J35="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J35="Tân Bình", Ward!$AQ$2:$AR$16, IF(J35="Tân Phú", Ward!$AS$2:$AT$12, IF(J35="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X35" t="str">
+        <f>IF(B35 &lt;&gt; "", VLOOKUP(B35, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -3377,8 +3546,12 @@
         <f>IF(K36 &lt;&gt; "", VLOOKUP(K36, IF(J36="1", Ward!$A$2:$B$11, IF(J36="2", Ward!$C$2:$D$12, IF(J36="3", Ward!$E$2:$F$15, IF(J36="4", Ward!$G$2:$H$16, IF(J36="5", Ward!$I$2:$J$16, IF(J36="6", Ward!$K$2:$L$15, IF(J36="7", Ward!$M$2:$N$11, IF(J36="8", Ward!$O$2:$P$17, IF(J36="9", Ward!$Q$2:$R$14, IF(J36="10", Ward!$S$2:$T$16, IF(J36="11", Ward!$U$2:$V$17, IF(J36="12", Ward!$W$2:$X$12, IF(J36="Bình Chánh", Ward!$Y$2:$Z$17, IF(J36="Bình Tân", Ward!$AA$2:$AB$11, IF(J36="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J36="Cần Giờ", Ward!$AE$2:$AF$8, IF(J36="Củ Chi", Ward!$AG$2:$AH$22, IF(J36="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J36="Hóc Môn", Ward!$AK$2:$AL$13, IF(J36="Nhà Bè", Ward!$AM$2:$AN$8, IF(J36="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J36="Tân Bình", Ward!$AQ$2:$AR$16, IF(J36="Tân Phú", Ward!$AS$2:$AT$12, IF(J36="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X36" t="str">
+        <f>IF(B36 &lt;&gt; "", VLOOKUP(B36, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -3411,8 +3584,12 @@
         <f>IF(K37 &lt;&gt; "", VLOOKUP(K37, IF(J37="1", Ward!$A$2:$B$11, IF(J37="2", Ward!$C$2:$D$12, IF(J37="3", Ward!$E$2:$F$15, IF(J37="4", Ward!$G$2:$H$16, IF(J37="5", Ward!$I$2:$J$16, IF(J37="6", Ward!$K$2:$L$15, IF(J37="7", Ward!$M$2:$N$11, IF(J37="8", Ward!$O$2:$P$17, IF(J37="9", Ward!$Q$2:$R$14, IF(J37="10", Ward!$S$2:$T$16, IF(J37="11", Ward!$U$2:$V$17, IF(J37="12", Ward!$W$2:$X$12, IF(J37="Bình Chánh", Ward!$Y$2:$Z$17, IF(J37="Bình Tân", Ward!$AA$2:$AB$11, IF(J37="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J37="Cần Giờ", Ward!$AE$2:$AF$8, IF(J37="Củ Chi", Ward!$AG$2:$AH$22, IF(J37="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J37="Hóc Môn", Ward!$AK$2:$AL$13, IF(J37="Nhà Bè", Ward!$AM$2:$AN$8, IF(J37="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J37="Tân Bình", Ward!$AQ$2:$AR$16, IF(J37="Tân Phú", Ward!$AS$2:$AT$12, IF(J37="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X37" t="str">
+        <f>IF(B37 &lt;&gt; "", VLOOKUP(B37, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -3445,8 +3622,12 @@
         <f>IF(K38 &lt;&gt; "", VLOOKUP(K38, IF(J38="1", Ward!$A$2:$B$11, IF(J38="2", Ward!$C$2:$D$12, IF(J38="3", Ward!$E$2:$F$15, IF(J38="4", Ward!$G$2:$H$16, IF(J38="5", Ward!$I$2:$J$16, IF(J38="6", Ward!$K$2:$L$15, IF(J38="7", Ward!$M$2:$N$11, IF(J38="8", Ward!$O$2:$P$17, IF(J38="9", Ward!$Q$2:$R$14, IF(J38="10", Ward!$S$2:$T$16, IF(J38="11", Ward!$U$2:$V$17, IF(J38="12", Ward!$W$2:$X$12, IF(J38="Bình Chánh", Ward!$Y$2:$Z$17, IF(J38="Bình Tân", Ward!$AA$2:$AB$11, IF(J38="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J38="Cần Giờ", Ward!$AE$2:$AF$8, IF(J38="Củ Chi", Ward!$AG$2:$AH$22, IF(J38="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J38="Hóc Môn", Ward!$AK$2:$AL$13, IF(J38="Nhà Bè", Ward!$AM$2:$AN$8, IF(J38="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J38="Tân Bình", Ward!$AQ$2:$AR$16, IF(J38="Tân Phú", Ward!$AS$2:$AT$12, IF(J38="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X38" t="str">
+        <f>IF(B38 &lt;&gt; "", VLOOKUP(B38, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -3479,8 +3660,12 @@
         <f>IF(K39 &lt;&gt; "", VLOOKUP(K39, IF(J39="1", Ward!$A$2:$B$11, IF(J39="2", Ward!$C$2:$D$12, IF(J39="3", Ward!$E$2:$F$15, IF(J39="4", Ward!$G$2:$H$16, IF(J39="5", Ward!$I$2:$J$16, IF(J39="6", Ward!$K$2:$L$15, IF(J39="7", Ward!$M$2:$N$11, IF(J39="8", Ward!$O$2:$P$17, IF(J39="9", Ward!$Q$2:$R$14, IF(J39="10", Ward!$S$2:$T$16, IF(J39="11", Ward!$U$2:$V$17, IF(J39="12", Ward!$W$2:$X$12, IF(J39="Bình Chánh", Ward!$Y$2:$Z$17, IF(J39="Bình Tân", Ward!$AA$2:$AB$11, IF(J39="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J39="Cần Giờ", Ward!$AE$2:$AF$8, IF(J39="Củ Chi", Ward!$AG$2:$AH$22, IF(J39="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J39="Hóc Môn", Ward!$AK$2:$AL$13, IF(J39="Nhà Bè", Ward!$AM$2:$AN$8, IF(J39="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J39="Tân Bình", Ward!$AQ$2:$AR$16, IF(J39="Tân Phú", Ward!$AS$2:$AT$12, IF(J39="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X39" t="str">
+        <f>IF(B39 &lt;&gt; "", VLOOKUP(B39, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -3513,8 +3698,12 @@
         <f>IF(K40 &lt;&gt; "", VLOOKUP(K40, IF(J40="1", Ward!$A$2:$B$11, IF(J40="2", Ward!$C$2:$D$12, IF(J40="3", Ward!$E$2:$F$15, IF(J40="4", Ward!$G$2:$H$16, IF(J40="5", Ward!$I$2:$J$16, IF(J40="6", Ward!$K$2:$L$15, IF(J40="7", Ward!$M$2:$N$11, IF(J40="8", Ward!$O$2:$P$17, IF(J40="9", Ward!$Q$2:$R$14, IF(J40="10", Ward!$S$2:$T$16, IF(J40="11", Ward!$U$2:$V$17, IF(J40="12", Ward!$W$2:$X$12, IF(J40="Bình Chánh", Ward!$Y$2:$Z$17, IF(J40="Bình Tân", Ward!$AA$2:$AB$11, IF(J40="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J40="Cần Giờ", Ward!$AE$2:$AF$8, IF(J40="Củ Chi", Ward!$AG$2:$AH$22, IF(J40="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J40="Hóc Môn", Ward!$AK$2:$AL$13, IF(J40="Nhà Bè", Ward!$AM$2:$AN$8, IF(J40="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J40="Tân Bình", Ward!$AQ$2:$AR$16, IF(J40="Tân Phú", Ward!$AS$2:$AT$12, IF(J40="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X40" t="str">
+        <f>IF(B40 &lt;&gt; "", VLOOKUP(B40, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -3547,8 +3736,12 @@
         <f>IF(K41 &lt;&gt; "", VLOOKUP(K41, IF(J41="1", Ward!$A$2:$B$11, IF(J41="2", Ward!$C$2:$D$12, IF(J41="3", Ward!$E$2:$F$15, IF(J41="4", Ward!$G$2:$H$16, IF(J41="5", Ward!$I$2:$J$16, IF(J41="6", Ward!$K$2:$L$15, IF(J41="7", Ward!$M$2:$N$11, IF(J41="8", Ward!$O$2:$P$17, IF(J41="9", Ward!$Q$2:$R$14, IF(J41="10", Ward!$S$2:$T$16, IF(J41="11", Ward!$U$2:$V$17, IF(J41="12", Ward!$W$2:$X$12, IF(J41="Bình Chánh", Ward!$Y$2:$Z$17, IF(J41="Bình Tân", Ward!$AA$2:$AB$11, IF(J41="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J41="Cần Giờ", Ward!$AE$2:$AF$8, IF(J41="Củ Chi", Ward!$AG$2:$AH$22, IF(J41="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J41="Hóc Môn", Ward!$AK$2:$AL$13, IF(J41="Nhà Bè", Ward!$AM$2:$AN$8, IF(J41="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J41="Tân Bình", Ward!$AQ$2:$AR$16, IF(J41="Tân Phú", Ward!$AS$2:$AT$12, IF(J41="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X41" t="str">
+        <f>IF(B41 &lt;&gt; "", VLOOKUP(B41, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -3581,8 +3774,12 @@
         <f>IF(K42 &lt;&gt; "", VLOOKUP(K42, IF(J42="1", Ward!$A$2:$B$11, IF(J42="2", Ward!$C$2:$D$12, IF(J42="3", Ward!$E$2:$F$15, IF(J42="4", Ward!$G$2:$H$16, IF(J42="5", Ward!$I$2:$J$16, IF(J42="6", Ward!$K$2:$L$15, IF(J42="7", Ward!$M$2:$N$11, IF(J42="8", Ward!$O$2:$P$17, IF(J42="9", Ward!$Q$2:$R$14, IF(J42="10", Ward!$S$2:$T$16, IF(J42="11", Ward!$U$2:$V$17, IF(J42="12", Ward!$W$2:$X$12, IF(J42="Bình Chánh", Ward!$Y$2:$Z$17, IF(J42="Bình Tân", Ward!$AA$2:$AB$11, IF(J42="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J42="Cần Giờ", Ward!$AE$2:$AF$8, IF(J42="Củ Chi", Ward!$AG$2:$AH$22, IF(J42="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J42="Hóc Môn", Ward!$AK$2:$AL$13, IF(J42="Nhà Bè", Ward!$AM$2:$AN$8, IF(J42="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J42="Tân Bình", Ward!$AQ$2:$AR$16, IF(J42="Tân Phú", Ward!$AS$2:$AT$12, IF(J42="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X42" t="str">
+        <f>IF(B42 &lt;&gt; "", VLOOKUP(B42, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -3615,8 +3812,12 @@
         <f>IF(K43 &lt;&gt; "", VLOOKUP(K43, IF(J43="1", Ward!$A$2:$B$11, IF(J43="2", Ward!$C$2:$D$12, IF(J43="3", Ward!$E$2:$F$15, IF(J43="4", Ward!$G$2:$H$16, IF(J43="5", Ward!$I$2:$J$16, IF(J43="6", Ward!$K$2:$L$15, IF(J43="7", Ward!$M$2:$N$11, IF(J43="8", Ward!$O$2:$P$17, IF(J43="9", Ward!$Q$2:$R$14, IF(J43="10", Ward!$S$2:$T$16, IF(J43="11", Ward!$U$2:$V$17, IF(J43="12", Ward!$W$2:$X$12, IF(J43="Bình Chánh", Ward!$Y$2:$Z$17, IF(J43="Bình Tân", Ward!$AA$2:$AB$11, IF(J43="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J43="Cần Giờ", Ward!$AE$2:$AF$8, IF(J43="Củ Chi", Ward!$AG$2:$AH$22, IF(J43="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J43="Hóc Môn", Ward!$AK$2:$AL$13, IF(J43="Nhà Bè", Ward!$AM$2:$AN$8, IF(J43="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J43="Tân Bình", Ward!$AQ$2:$AR$16, IF(J43="Tân Phú", Ward!$AS$2:$AT$12, IF(J43="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X43" t="str">
+        <f>IF(B43 &lt;&gt; "", VLOOKUP(B43, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -3649,8 +3850,12 @@
         <f>IF(K44 &lt;&gt; "", VLOOKUP(K44, IF(J44="1", Ward!$A$2:$B$11, IF(J44="2", Ward!$C$2:$D$12, IF(J44="3", Ward!$E$2:$F$15, IF(J44="4", Ward!$G$2:$H$16, IF(J44="5", Ward!$I$2:$J$16, IF(J44="6", Ward!$K$2:$L$15, IF(J44="7", Ward!$M$2:$N$11, IF(J44="8", Ward!$O$2:$P$17, IF(J44="9", Ward!$Q$2:$R$14, IF(J44="10", Ward!$S$2:$T$16, IF(J44="11", Ward!$U$2:$V$17, IF(J44="12", Ward!$W$2:$X$12, IF(J44="Bình Chánh", Ward!$Y$2:$Z$17, IF(J44="Bình Tân", Ward!$AA$2:$AB$11, IF(J44="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J44="Cần Giờ", Ward!$AE$2:$AF$8, IF(J44="Củ Chi", Ward!$AG$2:$AH$22, IF(J44="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J44="Hóc Môn", Ward!$AK$2:$AL$13, IF(J44="Nhà Bè", Ward!$AM$2:$AN$8, IF(J44="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J44="Tân Bình", Ward!$AQ$2:$AR$16, IF(J44="Tân Phú", Ward!$AS$2:$AT$12, IF(J44="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X44" t="str">
+        <f>IF(B44 &lt;&gt; "", VLOOKUP(B44, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
@@ -3683,8 +3888,12 @@
         <f>IF(K45 &lt;&gt; "", VLOOKUP(K45, IF(J45="1", Ward!$A$2:$B$11, IF(J45="2", Ward!$C$2:$D$12, IF(J45="3", Ward!$E$2:$F$15, IF(J45="4", Ward!$G$2:$H$16, IF(J45="5", Ward!$I$2:$J$16, IF(J45="6", Ward!$K$2:$L$15, IF(J45="7", Ward!$M$2:$N$11, IF(J45="8", Ward!$O$2:$P$17, IF(J45="9", Ward!$Q$2:$R$14, IF(J45="10", Ward!$S$2:$T$16, IF(J45="11", Ward!$U$2:$V$17, IF(J45="12", Ward!$W$2:$X$12, IF(J45="Bình Chánh", Ward!$Y$2:$Z$17, IF(J45="Bình Tân", Ward!$AA$2:$AB$11, IF(J45="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J45="Cần Giờ", Ward!$AE$2:$AF$8, IF(J45="Củ Chi", Ward!$AG$2:$AH$22, IF(J45="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J45="Hóc Môn", Ward!$AK$2:$AL$13, IF(J45="Nhà Bè", Ward!$AM$2:$AN$8, IF(J45="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J45="Tân Bình", Ward!$AQ$2:$AR$16, IF(J45="Tân Phú", Ward!$AS$2:$AT$12, IF(J45="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X45" t="str">
+        <f>IF(B45 &lt;&gt; "", VLOOKUP(B45, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
@@ -3717,8 +3926,12 @@
         <f>IF(K46 &lt;&gt; "", VLOOKUP(K46, IF(J46="1", Ward!$A$2:$B$11, IF(J46="2", Ward!$C$2:$D$12, IF(J46="3", Ward!$E$2:$F$15, IF(J46="4", Ward!$G$2:$H$16, IF(J46="5", Ward!$I$2:$J$16, IF(J46="6", Ward!$K$2:$L$15, IF(J46="7", Ward!$M$2:$N$11, IF(J46="8", Ward!$O$2:$P$17, IF(J46="9", Ward!$Q$2:$R$14, IF(J46="10", Ward!$S$2:$T$16, IF(J46="11", Ward!$U$2:$V$17, IF(J46="12", Ward!$W$2:$X$12, IF(J46="Bình Chánh", Ward!$Y$2:$Z$17, IF(J46="Bình Tân", Ward!$AA$2:$AB$11, IF(J46="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J46="Cần Giờ", Ward!$AE$2:$AF$8, IF(J46="Củ Chi", Ward!$AG$2:$AH$22, IF(J46="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J46="Hóc Môn", Ward!$AK$2:$AL$13, IF(J46="Nhà Bè", Ward!$AM$2:$AN$8, IF(J46="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J46="Tân Bình", Ward!$AQ$2:$AR$16, IF(J46="Tân Phú", Ward!$AS$2:$AT$12, IF(J46="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X46" t="str">
+        <f>IF(B46 &lt;&gt; "", VLOOKUP(B46, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
@@ -3751,8 +3964,12 @@
         <f>IF(K47 &lt;&gt; "", VLOOKUP(K47, IF(J47="1", Ward!$A$2:$B$11, IF(J47="2", Ward!$C$2:$D$12, IF(J47="3", Ward!$E$2:$F$15, IF(J47="4", Ward!$G$2:$H$16, IF(J47="5", Ward!$I$2:$J$16, IF(J47="6", Ward!$K$2:$L$15, IF(J47="7", Ward!$M$2:$N$11, IF(J47="8", Ward!$O$2:$P$17, IF(J47="9", Ward!$Q$2:$R$14, IF(J47="10", Ward!$S$2:$T$16, IF(J47="11", Ward!$U$2:$V$17, IF(J47="12", Ward!$W$2:$X$12, IF(J47="Bình Chánh", Ward!$Y$2:$Z$17, IF(J47="Bình Tân", Ward!$AA$2:$AB$11, IF(J47="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J47="Cần Giờ", Ward!$AE$2:$AF$8, IF(J47="Củ Chi", Ward!$AG$2:$AH$22, IF(J47="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J47="Hóc Môn", Ward!$AK$2:$AL$13, IF(J47="Nhà Bè", Ward!$AM$2:$AN$8, IF(J47="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J47="Tân Bình", Ward!$AQ$2:$AR$16, IF(J47="Tân Phú", Ward!$AS$2:$AT$12, IF(J47="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X47" t="str">
+        <f>IF(B47 &lt;&gt; "", VLOOKUP(B47, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="16"/>
       <c r="C48" s="16"/>
@@ -3785,8 +4002,12 @@
         <f>IF(K48 &lt;&gt; "", VLOOKUP(K48, IF(J48="1", Ward!$A$2:$B$11, IF(J48="2", Ward!$C$2:$D$12, IF(J48="3", Ward!$E$2:$F$15, IF(J48="4", Ward!$G$2:$H$16, IF(J48="5", Ward!$I$2:$J$16, IF(J48="6", Ward!$K$2:$L$15, IF(J48="7", Ward!$M$2:$N$11, IF(J48="8", Ward!$O$2:$P$17, IF(J48="9", Ward!$Q$2:$R$14, IF(J48="10", Ward!$S$2:$T$16, IF(J48="11", Ward!$U$2:$V$17, IF(J48="12", Ward!$W$2:$X$12, IF(J48="Bình Chánh", Ward!$Y$2:$Z$17, IF(J48="Bình Tân", Ward!$AA$2:$AB$11, IF(J48="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J48="Cần Giờ", Ward!$AE$2:$AF$8, IF(J48="Củ Chi", Ward!$AG$2:$AH$22, IF(J48="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J48="Hóc Môn", Ward!$AK$2:$AL$13, IF(J48="Nhà Bè", Ward!$AM$2:$AN$8, IF(J48="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J48="Tân Bình", Ward!$AQ$2:$AR$16, IF(J48="Tân Phú", Ward!$AS$2:$AT$12, IF(J48="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X48" t="str">
+        <f>IF(B48 &lt;&gt; "", VLOOKUP(B48, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="16"/>
       <c r="C49" s="16"/>
@@ -3819,8 +4040,12 @@
         <f>IF(K49 &lt;&gt; "", VLOOKUP(K49, IF(J49="1", Ward!$A$2:$B$11, IF(J49="2", Ward!$C$2:$D$12, IF(J49="3", Ward!$E$2:$F$15, IF(J49="4", Ward!$G$2:$H$16, IF(J49="5", Ward!$I$2:$J$16, IF(J49="6", Ward!$K$2:$L$15, IF(J49="7", Ward!$M$2:$N$11, IF(J49="8", Ward!$O$2:$P$17, IF(J49="9", Ward!$Q$2:$R$14, IF(J49="10", Ward!$S$2:$T$16, IF(J49="11", Ward!$U$2:$V$17, IF(J49="12", Ward!$W$2:$X$12, IF(J49="Bình Chánh", Ward!$Y$2:$Z$17, IF(J49="Bình Tân", Ward!$AA$2:$AB$11, IF(J49="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J49="Cần Giờ", Ward!$AE$2:$AF$8, IF(J49="Củ Chi", Ward!$AG$2:$AH$22, IF(J49="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J49="Hóc Môn", Ward!$AK$2:$AL$13, IF(J49="Nhà Bè", Ward!$AM$2:$AN$8, IF(J49="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J49="Tân Bình", Ward!$AQ$2:$AR$16, IF(J49="Tân Phú", Ward!$AS$2:$AT$12, IF(J49="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X49" t="str">
+        <f>IF(B49 &lt;&gt; "", VLOOKUP(B49, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="16"/>
       <c r="C50" s="16"/>
@@ -3853,8 +4078,12 @@
         <f>IF(K50 &lt;&gt; "", VLOOKUP(K50, IF(J50="1", Ward!$A$2:$B$11, IF(J50="2", Ward!$C$2:$D$12, IF(J50="3", Ward!$E$2:$F$15, IF(J50="4", Ward!$G$2:$H$16, IF(J50="5", Ward!$I$2:$J$16, IF(J50="6", Ward!$K$2:$L$15, IF(J50="7", Ward!$M$2:$N$11, IF(J50="8", Ward!$O$2:$P$17, IF(J50="9", Ward!$Q$2:$R$14, IF(J50="10", Ward!$S$2:$T$16, IF(J50="11", Ward!$U$2:$V$17, IF(J50="12", Ward!$W$2:$X$12, IF(J50="Bình Chánh", Ward!$Y$2:$Z$17, IF(J50="Bình Tân", Ward!$AA$2:$AB$11, IF(J50="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J50="Cần Giờ", Ward!$AE$2:$AF$8, IF(J50="Củ Chi", Ward!$AG$2:$AH$22, IF(J50="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J50="Hóc Môn", Ward!$AK$2:$AL$13, IF(J50="Nhà Bè", Ward!$AM$2:$AN$8, IF(J50="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J50="Tân Bình", Ward!$AQ$2:$AR$16, IF(J50="Tân Phú", Ward!$AS$2:$AT$12, IF(J50="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X50" t="str">
+        <f>IF(B50 &lt;&gt; "", VLOOKUP(B50, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="16"/>
       <c r="C51" s="16"/>
@@ -3887,8 +4116,12 @@
         <f>IF(K51 &lt;&gt; "", VLOOKUP(K51, IF(J51="1", Ward!$A$2:$B$11, IF(J51="2", Ward!$C$2:$D$12, IF(J51="3", Ward!$E$2:$F$15, IF(J51="4", Ward!$G$2:$H$16, IF(J51="5", Ward!$I$2:$J$16, IF(J51="6", Ward!$K$2:$L$15, IF(J51="7", Ward!$M$2:$N$11, IF(J51="8", Ward!$O$2:$P$17, IF(J51="9", Ward!$Q$2:$R$14, IF(J51="10", Ward!$S$2:$T$16, IF(J51="11", Ward!$U$2:$V$17, IF(J51="12", Ward!$W$2:$X$12, IF(J51="Bình Chánh", Ward!$Y$2:$Z$17, IF(J51="Bình Tân", Ward!$AA$2:$AB$11, IF(J51="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J51="Cần Giờ", Ward!$AE$2:$AF$8, IF(J51="Củ Chi", Ward!$AG$2:$AH$22, IF(J51="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J51="Hóc Môn", Ward!$AK$2:$AL$13, IF(J51="Nhà Bè", Ward!$AM$2:$AN$8, IF(J51="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J51="Tân Bình", Ward!$AQ$2:$AR$16, IF(J51="Tân Phú", Ward!$AS$2:$AT$12, IF(J51="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X51" t="str">
+        <f>IF(B51 &lt;&gt; "", VLOOKUP(B51, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="16"/>
       <c r="C52" s="16"/>
@@ -3921,8 +4154,12 @@
         <f>IF(K52 &lt;&gt; "", VLOOKUP(K52, IF(J52="1", Ward!$A$2:$B$11, IF(J52="2", Ward!$C$2:$D$12, IF(J52="3", Ward!$E$2:$F$15, IF(J52="4", Ward!$G$2:$H$16, IF(J52="5", Ward!$I$2:$J$16, IF(J52="6", Ward!$K$2:$L$15, IF(J52="7", Ward!$M$2:$N$11, IF(J52="8", Ward!$O$2:$P$17, IF(J52="9", Ward!$Q$2:$R$14, IF(J52="10", Ward!$S$2:$T$16, IF(J52="11", Ward!$U$2:$V$17, IF(J52="12", Ward!$W$2:$X$12, IF(J52="Bình Chánh", Ward!$Y$2:$Z$17, IF(J52="Bình Tân", Ward!$AA$2:$AB$11, IF(J52="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J52="Cần Giờ", Ward!$AE$2:$AF$8, IF(J52="Củ Chi", Ward!$AG$2:$AH$22, IF(J52="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J52="Hóc Môn", Ward!$AK$2:$AL$13, IF(J52="Nhà Bè", Ward!$AM$2:$AN$8, IF(J52="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J52="Tân Bình", Ward!$AQ$2:$AR$16, IF(J52="Tân Phú", Ward!$AS$2:$AT$12, IF(J52="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X52" t="str">
+        <f>IF(B52 &lt;&gt; "", VLOOKUP(B52, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="16"/>
       <c r="C53" s="16"/>
@@ -3955,8 +4192,12 @@
         <f>IF(K53 &lt;&gt; "", VLOOKUP(K53, IF(J53="1", Ward!$A$2:$B$11, IF(J53="2", Ward!$C$2:$D$12, IF(J53="3", Ward!$E$2:$F$15, IF(J53="4", Ward!$G$2:$H$16, IF(J53="5", Ward!$I$2:$J$16, IF(J53="6", Ward!$K$2:$L$15, IF(J53="7", Ward!$M$2:$N$11, IF(J53="8", Ward!$O$2:$P$17, IF(J53="9", Ward!$Q$2:$R$14, IF(J53="10", Ward!$S$2:$T$16, IF(J53="11", Ward!$U$2:$V$17, IF(J53="12", Ward!$W$2:$X$12, IF(J53="Bình Chánh", Ward!$Y$2:$Z$17, IF(J53="Bình Tân", Ward!$AA$2:$AB$11, IF(J53="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J53="Cần Giờ", Ward!$AE$2:$AF$8, IF(J53="Củ Chi", Ward!$AG$2:$AH$22, IF(J53="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J53="Hóc Môn", Ward!$AK$2:$AL$13, IF(J53="Nhà Bè", Ward!$AM$2:$AN$8, IF(J53="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J53="Tân Bình", Ward!$AQ$2:$AR$16, IF(J53="Tân Phú", Ward!$AS$2:$AT$12, IF(J53="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X53" t="str">
+        <f>IF(B53 &lt;&gt; "", VLOOKUP(B53, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="16"/>
       <c r="C54" s="16"/>
@@ -3989,8 +4230,12 @@
         <f>IF(K54 &lt;&gt; "", VLOOKUP(K54, IF(J54="1", Ward!$A$2:$B$11, IF(J54="2", Ward!$C$2:$D$12, IF(J54="3", Ward!$E$2:$F$15, IF(J54="4", Ward!$G$2:$H$16, IF(J54="5", Ward!$I$2:$J$16, IF(J54="6", Ward!$K$2:$L$15, IF(J54="7", Ward!$M$2:$N$11, IF(J54="8", Ward!$O$2:$P$17, IF(J54="9", Ward!$Q$2:$R$14, IF(J54="10", Ward!$S$2:$T$16, IF(J54="11", Ward!$U$2:$V$17, IF(J54="12", Ward!$W$2:$X$12, IF(J54="Bình Chánh", Ward!$Y$2:$Z$17, IF(J54="Bình Tân", Ward!$AA$2:$AB$11, IF(J54="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J54="Cần Giờ", Ward!$AE$2:$AF$8, IF(J54="Củ Chi", Ward!$AG$2:$AH$22, IF(J54="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J54="Hóc Môn", Ward!$AK$2:$AL$13, IF(J54="Nhà Bè", Ward!$AM$2:$AN$8, IF(J54="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J54="Tân Bình", Ward!$AQ$2:$AR$16, IF(J54="Tân Phú", Ward!$AS$2:$AT$12, IF(J54="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X54" t="str">
+        <f>IF(B54 &lt;&gt; "", VLOOKUP(B54, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="16"/>
       <c r="C55" s="16"/>
@@ -4023,8 +4268,12 @@
         <f>IF(K55 &lt;&gt; "", VLOOKUP(K55, IF(J55="1", Ward!$A$2:$B$11, IF(J55="2", Ward!$C$2:$D$12, IF(J55="3", Ward!$E$2:$F$15, IF(J55="4", Ward!$G$2:$H$16, IF(J55="5", Ward!$I$2:$J$16, IF(J55="6", Ward!$K$2:$L$15, IF(J55="7", Ward!$M$2:$N$11, IF(J55="8", Ward!$O$2:$P$17, IF(J55="9", Ward!$Q$2:$R$14, IF(J55="10", Ward!$S$2:$T$16, IF(J55="11", Ward!$U$2:$V$17, IF(J55="12", Ward!$W$2:$X$12, IF(J55="Bình Chánh", Ward!$Y$2:$Z$17, IF(J55="Bình Tân", Ward!$AA$2:$AB$11, IF(J55="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J55="Cần Giờ", Ward!$AE$2:$AF$8, IF(J55="Củ Chi", Ward!$AG$2:$AH$22, IF(J55="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J55="Hóc Môn", Ward!$AK$2:$AL$13, IF(J55="Nhà Bè", Ward!$AM$2:$AN$8, IF(J55="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J55="Tân Bình", Ward!$AQ$2:$AR$16, IF(J55="Tân Phú", Ward!$AS$2:$AT$12, IF(J55="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X55" t="str">
+        <f>IF(B55 &lt;&gt; "", VLOOKUP(B55, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="16"/>
       <c r="C56" s="16"/>
@@ -4057,8 +4306,12 @@
         <f>IF(K56 &lt;&gt; "", VLOOKUP(K56, IF(J56="1", Ward!$A$2:$B$11, IF(J56="2", Ward!$C$2:$D$12, IF(J56="3", Ward!$E$2:$F$15, IF(J56="4", Ward!$G$2:$H$16, IF(J56="5", Ward!$I$2:$J$16, IF(J56="6", Ward!$K$2:$L$15, IF(J56="7", Ward!$M$2:$N$11, IF(J56="8", Ward!$O$2:$P$17, IF(J56="9", Ward!$Q$2:$R$14, IF(J56="10", Ward!$S$2:$T$16, IF(J56="11", Ward!$U$2:$V$17, IF(J56="12", Ward!$W$2:$X$12, IF(J56="Bình Chánh", Ward!$Y$2:$Z$17, IF(J56="Bình Tân", Ward!$AA$2:$AB$11, IF(J56="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J56="Cần Giờ", Ward!$AE$2:$AF$8, IF(J56="Củ Chi", Ward!$AG$2:$AH$22, IF(J56="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J56="Hóc Môn", Ward!$AK$2:$AL$13, IF(J56="Nhà Bè", Ward!$AM$2:$AN$8, IF(J56="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J56="Tân Bình", Ward!$AQ$2:$AR$16, IF(J56="Tân Phú", Ward!$AS$2:$AT$12, IF(J56="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X56" t="str">
+        <f>IF(B56 &lt;&gt; "", VLOOKUP(B56, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="16"/>
       <c r="C57" s="16"/>
@@ -4091,8 +4344,12 @@
         <f>IF(K57 &lt;&gt; "", VLOOKUP(K57, IF(J57="1", Ward!$A$2:$B$11, IF(J57="2", Ward!$C$2:$D$12, IF(J57="3", Ward!$E$2:$F$15, IF(J57="4", Ward!$G$2:$H$16, IF(J57="5", Ward!$I$2:$J$16, IF(J57="6", Ward!$K$2:$L$15, IF(J57="7", Ward!$M$2:$N$11, IF(J57="8", Ward!$O$2:$P$17, IF(J57="9", Ward!$Q$2:$R$14, IF(J57="10", Ward!$S$2:$T$16, IF(J57="11", Ward!$U$2:$V$17, IF(J57="12", Ward!$W$2:$X$12, IF(J57="Bình Chánh", Ward!$Y$2:$Z$17, IF(J57="Bình Tân", Ward!$AA$2:$AB$11, IF(J57="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J57="Cần Giờ", Ward!$AE$2:$AF$8, IF(J57="Củ Chi", Ward!$AG$2:$AH$22, IF(J57="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J57="Hóc Môn", Ward!$AK$2:$AL$13, IF(J57="Nhà Bè", Ward!$AM$2:$AN$8, IF(J57="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J57="Tân Bình", Ward!$AQ$2:$AR$16, IF(J57="Tân Phú", Ward!$AS$2:$AT$12, IF(J57="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X57" t="str">
+        <f>IF(B57 &lt;&gt; "", VLOOKUP(B57, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="16"/>
       <c r="C58" s="16"/>
@@ -4125,8 +4382,12 @@
         <f>IF(K58 &lt;&gt; "", VLOOKUP(K58, IF(J58="1", Ward!$A$2:$B$11, IF(J58="2", Ward!$C$2:$D$12, IF(J58="3", Ward!$E$2:$F$15, IF(J58="4", Ward!$G$2:$H$16, IF(J58="5", Ward!$I$2:$J$16, IF(J58="6", Ward!$K$2:$L$15, IF(J58="7", Ward!$M$2:$N$11, IF(J58="8", Ward!$O$2:$P$17, IF(J58="9", Ward!$Q$2:$R$14, IF(J58="10", Ward!$S$2:$T$16, IF(J58="11", Ward!$U$2:$V$17, IF(J58="12", Ward!$W$2:$X$12, IF(J58="Bình Chánh", Ward!$Y$2:$Z$17, IF(J58="Bình Tân", Ward!$AA$2:$AB$11, IF(J58="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J58="Cần Giờ", Ward!$AE$2:$AF$8, IF(J58="Củ Chi", Ward!$AG$2:$AH$22, IF(J58="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J58="Hóc Môn", Ward!$AK$2:$AL$13, IF(J58="Nhà Bè", Ward!$AM$2:$AN$8, IF(J58="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J58="Tân Bình", Ward!$AQ$2:$AR$16, IF(J58="Tân Phú", Ward!$AS$2:$AT$12, IF(J58="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X58" t="str">
+        <f>IF(B58 &lt;&gt; "", VLOOKUP(B58, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="16"/>
       <c r="C59" s="16"/>
@@ -4159,8 +4420,12 @@
         <f>IF(K59 &lt;&gt; "", VLOOKUP(K59, IF(J59="1", Ward!$A$2:$B$11, IF(J59="2", Ward!$C$2:$D$12, IF(J59="3", Ward!$E$2:$F$15, IF(J59="4", Ward!$G$2:$H$16, IF(J59="5", Ward!$I$2:$J$16, IF(J59="6", Ward!$K$2:$L$15, IF(J59="7", Ward!$M$2:$N$11, IF(J59="8", Ward!$O$2:$P$17, IF(J59="9", Ward!$Q$2:$R$14, IF(J59="10", Ward!$S$2:$T$16, IF(J59="11", Ward!$U$2:$V$17, IF(J59="12", Ward!$W$2:$X$12, IF(J59="Bình Chánh", Ward!$Y$2:$Z$17, IF(J59="Bình Tân", Ward!$AA$2:$AB$11, IF(J59="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J59="Cần Giờ", Ward!$AE$2:$AF$8, IF(J59="Củ Chi", Ward!$AG$2:$AH$22, IF(J59="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J59="Hóc Môn", Ward!$AK$2:$AL$13, IF(J59="Nhà Bè", Ward!$AM$2:$AN$8, IF(J59="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J59="Tân Bình", Ward!$AQ$2:$AR$16, IF(J59="Tân Phú", Ward!$AS$2:$AT$12, IF(J59="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X59" t="str">
+        <f>IF(B59 &lt;&gt; "", VLOOKUP(B59, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="16"/>
       <c r="C60" s="16"/>
@@ -4193,8 +4458,12 @@
         <f>IF(K60 &lt;&gt; "", VLOOKUP(K60, IF(J60="1", Ward!$A$2:$B$11, IF(J60="2", Ward!$C$2:$D$12, IF(J60="3", Ward!$E$2:$F$15, IF(J60="4", Ward!$G$2:$H$16, IF(J60="5", Ward!$I$2:$J$16, IF(J60="6", Ward!$K$2:$L$15, IF(J60="7", Ward!$M$2:$N$11, IF(J60="8", Ward!$O$2:$P$17, IF(J60="9", Ward!$Q$2:$R$14, IF(J60="10", Ward!$S$2:$T$16, IF(J60="11", Ward!$U$2:$V$17, IF(J60="12", Ward!$W$2:$X$12, IF(J60="Bình Chánh", Ward!$Y$2:$Z$17, IF(J60="Bình Tân", Ward!$AA$2:$AB$11, IF(J60="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J60="Cần Giờ", Ward!$AE$2:$AF$8, IF(J60="Củ Chi", Ward!$AG$2:$AH$22, IF(J60="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J60="Hóc Môn", Ward!$AK$2:$AL$13, IF(J60="Nhà Bè", Ward!$AM$2:$AN$8, IF(J60="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J60="Tân Bình", Ward!$AQ$2:$AR$16, IF(J60="Tân Phú", Ward!$AS$2:$AT$12, IF(J60="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X60" t="str">
+        <f>IF(B60 &lt;&gt; "", VLOOKUP(B60, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="16"/>
       <c r="C61" s="16"/>
@@ -4227,8 +4496,12 @@
         <f>IF(K61 &lt;&gt; "", VLOOKUP(K61, IF(J61="1", Ward!$A$2:$B$11, IF(J61="2", Ward!$C$2:$D$12, IF(J61="3", Ward!$E$2:$F$15, IF(J61="4", Ward!$G$2:$H$16, IF(J61="5", Ward!$I$2:$J$16, IF(J61="6", Ward!$K$2:$L$15, IF(J61="7", Ward!$M$2:$N$11, IF(J61="8", Ward!$O$2:$P$17, IF(J61="9", Ward!$Q$2:$R$14, IF(J61="10", Ward!$S$2:$T$16, IF(J61="11", Ward!$U$2:$V$17, IF(J61="12", Ward!$W$2:$X$12, IF(J61="Bình Chánh", Ward!$Y$2:$Z$17, IF(J61="Bình Tân", Ward!$AA$2:$AB$11, IF(J61="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J61="Cần Giờ", Ward!$AE$2:$AF$8, IF(J61="Củ Chi", Ward!$AG$2:$AH$22, IF(J61="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J61="Hóc Môn", Ward!$AK$2:$AL$13, IF(J61="Nhà Bè", Ward!$AM$2:$AN$8, IF(J61="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J61="Tân Bình", Ward!$AQ$2:$AR$16, IF(J61="Tân Phú", Ward!$AS$2:$AT$12, IF(J61="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X61" t="str">
+        <f>IF(B61 &lt;&gt; "", VLOOKUP(B61, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="16"/>
       <c r="C62" s="16"/>
@@ -4261,8 +4534,12 @@
         <f>IF(K62 &lt;&gt; "", VLOOKUP(K62, IF(J62="1", Ward!$A$2:$B$11, IF(J62="2", Ward!$C$2:$D$12, IF(J62="3", Ward!$E$2:$F$15, IF(J62="4", Ward!$G$2:$H$16, IF(J62="5", Ward!$I$2:$J$16, IF(J62="6", Ward!$K$2:$L$15, IF(J62="7", Ward!$M$2:$N$11, IF(J62="8", Ward!$O$2:$P$17, IF(J62="9", Ward!$Q$2:$R$14, IF(J62="10", Ward!$S$2:$T$16, IF(J62="11", Ward!$U$2:$V$17, IF(J62="12", Ward!$W$2:$X$12, IF(J62="Bình Chánh", Ward!$Y$2:$Z$17, IF(J62="Bình Tân", Ward!$AA$2:$AB$11, IF(J62="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J62="Cần Giờ", Ward!$AE$2:$AF$8, IF(J62="Củ Chi", Ward!$AG$2:$AH$22, IF(J62="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J62="Hóc Môn", Ward!$AK$2:$AL$13, IF(J62="Nhà Bè", Ward!$AM$2:$AN$8, IF(J62="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J62="Tân Bình", Ward!$AQ$2:$AR$16, IF(J62="Tân Phú", Ward!$AS$2:$AT$12, IF(J62="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X62" t="str">
+        <f>IF(B62 &lt;&gt; "", VLOOKUP(B62, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="16"/>
       <c r="C63" s="16"/>
@@ -4295,8 +4572,12 @@
         <f>IF(K63 &lt;&gt; "", VLOOKUP(K63, IF(J63="1", Ward!$A$2:$B$11, IF(J63="2", Ward!$C$2:$D$12, IF(J63="3", Ward!$E$2:$F$15, IF(J63="4", Ward!$G$2:$H$16, IF(J63="5", Ward!$I$2:$J$16, IF(J63="6", Ward!$K$2:$L$15, IF(J63="7", Ward!$M$2:$N$11, IF(J63="8", Ward!$O$2:$P$17, IF(J63="9", Ward!$Q$2:$R$14, IF(J63="10", Ward!$S$2:$T$16, IF(J63="11", Ward!$U$2:$V$17, IF(J63="12", Ward!$W$2:$X$12, IF(J63="Bình Chánh", Ward!$Y$2:$Z$17, IF(J63="Bình Tân", Ward!$AA$2:$AB$11, IF(J63="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J63="Cần Giờ", Ward!$AE$2:$AF$8, IF(J63="Củ Chi", Ward!$AG$2:$AH$22, IF(J63="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J63="Hóc Môn", Ward!$AK$2:$AL$13, IF(J63="Nhà Bè", Ward!$AM$2:$AN$8, IF(J63="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J63="Tân Bình", Ward!$AQ$2:$AR$16, IF(J63="Tân Phú", Ward!$AS$2:$AT$12, IF(J63="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X63" t="str">
+        <f>IF(B63 &lt;&gt; "", VLOOKUP(B63, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="16"/>
       <c r="C64" s="16"/>
@@ -4329,8 +4610,12 @@
         <f>IF(K64 &lt;&gt; "", VLOOKUP(K64, IF(J64="1", Ward!$A$2:$B$11, IF(J64="2", Ward!$C$2:$D$12, IF(J64="3", Ward!$E$2:$F$15, IF(J64="4", Ward!$G$2:$H$16, IF(J64="5", Ward!$I$2:$J$16, IF(J64="6", Ward!$K$2:$L$15, IF(J64="7", Ward!$M$2:$N$11, IF(J64="8", Ward!$O$2:$P$17, IF(J64="9", Ward!$Q$2:$R$14, IF(J64="10", Ward!$S$2:$T$16, IF(J64="11", Ward!$U$2:$V$17, IF(J64="12", Ward!$W$2:$X$12, IF(J64="Bình Chánh", Ward!$Y$2:$Z$17, IF(J64="Bình Tân", Ward!$AA$2:$AB$11, IF(J64="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J64="Cần Giờ", Ward!$AE$2:$AF$8, IF(J64="Củ Chi", Ward!$AG$2:$AH$22, IF(J64="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J64="Hóc Môn", Ward!$AK$2:$AL$13, IF(J64="Nhà Bè", Ward!$AM$2:$AN$8, IF(J64="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J64="Tân Bình", Ward!$AQ$2:$AR$16, IF(J64="Tân Phú", Ward!$AS$2:$AT$12, IF(J64="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X64" t="str">
+        <f>IF(B64 &lt;&gt; "", VLOOKUP(B64, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="16"/>
       <c r="C65" s="16"/>
@@ -4363,8 +4648,12 @@
         <f>IF(K65 &lt;&gt; "", VLOOKUP(K65, IF(J65="1", Ward!$A$2:$B$11, IF(J65="2", Ward!$C$2:$D$12, IF(J65="3", Ward!$E$2:$F$15, IF(J65="4", Ward!$G$2:$H$16, IF(J65="5", Ward!$I$2:$J$16, IF(J65="6", Ward!$K$2:$L$15, IF(J65="7", Ward!$M$2:$N$11, IF(J65="8", Ward!$O$2:$P$17, IF(J65="9", Ward!$Q$2:$R$14, IF(J65="10", Ward!$S$2:$T$16, IF(J65="11", Ward!$U$2:$V$17, IF(J65="12", Ward!$W$2:$X$12, IF(J65="Bình Chánh", Ward!$Y$2:$Z$17, IF(J65="Bình Tân", Ward!$AA$2:$AB$11, IF(J65="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J65="Cần Giờ", Ward!$AE$2:$AF$8, IF(J65="Củ Chi", Ward!$AG$2:$AH$22, IF(J65="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J65="Hóc Môn", Ward!$AK$2:$AL$13, IF(J65="Nhà Bè", Ward!$AM$2:$AN$8, IF(J65="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J65="Tân Bình", Ward!$AQ$2:$AR$16, IF(J65="Tân Phú", Ward!$AS$2:$AT$12, IF(J65="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X65" t="str">
+        <f>IF(B65 &lt;&gt; "", VLOOKUP(B65, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="16"/>
       <c r="C66" s="16"/>
@@ -4397,8 +4686,12 @@
         <f>IF(K66 &lt;&gt; "", VLOOKUP(K66, IF(J66="1", Ward!$A$2:$B$11, IF(J66="2", Ward!$C$2:$D$12, IF(J66="3", Ward!$E$2:$F$15, IF(J66="4", Ward!$G$2:$H$16, IF(J66="5", Ward!$I$2:$J$16, IF(J66="6", Ward!$K$2:$L$15, IF(J66="7", Ward!$M$2:$N$11, IF(J66="8", Ward!$O$2:$P$17, IF(J66="9", Ward!$Q$2:$R$14, IF(J66="10", Ward!$S$2:$T$16, IF(J66="11", Ward!$U$2:$V$17, IF(J66="12", Ward!$W$2:$X$12, IF(J66="Bình Chánh", Ward!$Y$2:$Z$17, IF(J66="Bình Tân", Ward!$AA$2:$AB$11, IF(J66="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J66="Cần Giờ", Ward!$AE$2:$AF$8, IF(J66="Củ Chi", Ward!$AG$2:$AH$22, IF(J66="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J66="Hóc Môn", Ward!$AK$2:$AL$13, IF(J66="Nhà Bè", Ward!$AM$2:$AN$8, IF(J66="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J66="Tân Bình", Ward!$AQ$2:$AR$16, IF(J66="Tân Phú", Ward!$AS$2:$AT$12, IF(J66="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X66" t="str">
+        <f>IF(B66 &lt;&gt; "", VLOOKUP(B66, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="16"/>
       <c r="C67" s="16"/>
@@ -4431,8 +4724,12 @@
         <f>IF(K67 &lt;&gt; "", VLOOKUP(K67, IF(J67="1", Ward!$A$2:$B$11, IF(J67="2", Ward!$C$2:$D$12, IF(J67="3", Ward!$E$2:$F$15, IF(J67="4", Ward!$G$2:$H$16, IF(J67="5", Ward!$I$2:$J$16, IF(J67="6", Ward!$K$2:$L$15, IF(J67="7", Ward!$M$2:$N$11, IF(J67="8", Ward!$O$2:$P$17, IF(J67="9", Ward!$Q$2:$R$14, IF(J67="10", Ward!$S$2:$T$16, IF(J67="11", Ward!$U$2:$V$17, IF(J67="12", Ward!$W$2:$X$12, IF(J67="Bình Chánh", Ward!$Y$2:$Z$17, IF(J67="Bình Tân", Ward!$AA$2:$AB$11, IF(J67="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J67="Cần Giờ", Ward!$AE$2:$AF$8, IF(J67="Củ Chi", Ward!$AG$2:$AH$22, IF(J67="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J67="Hóc Môn", Ward!$AK$2:$AL$13, IF(J67="Nhà Bè", Ward!$AM$2:$AN$8, IF(J67="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J67="Tân Bình", Ward!$AQ$2:$AR$16, IF(J67="Tân Phú", Ward!$AS$2:$AT$12, IF(J67="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X67" t="str">
+        <f>IF(B67 &lt;&gt; "", VLOOKUP(B67, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="16"/>
       <c r="C68" s="16"/>
@@ -4465,8 +4762,12 @@
         <f>IF(K68 &lt;&gt; "", VLOOKUP(K68, IF(J68="1", Ward!$A$2:$B$11, IF(J68="2", Ward!$C$2:$D$12, IF(J68="3", Ward!$E$2:$F$15, IF(J68="4", Ward!$G$2:$H$16, IF(J68="5", Ward!$I$2:$J$16, IF(J68="6", Ward!$K$2:$L$15, IF(J68="7", Ward!$M$2:$N$11, IF(J68="8", Ward!$O$2:$P$17, IF(J68="9", Ward!$Q$2:$R$14, IF(J68="10", Ward!$S$2:$T$16, IF(J68="11", Ward!$U$2:$V$17, IF(J68="12", Ward!$W$2:$X$12, IF(J68="Bình Chánh", Ward!$Y$2:$Z$17, IF(J68="Bình Tân", Ward!$AA$2:$AB$11, IF(J68="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J68="Cần Giờ", Ward!$AE$2:$AF$8, IF(J68="Củ Chi", Ward!$AG$2:$AH$22, IF(J68="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J68="Hóc Môn", Ward!$AK$2:$AL$13, IF(J68="Nhà Bè", Ward!$AM$2:$AN$8, IF(J68="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J68="Tân Bình", Ward!$AQ$2:$AR$16, IF(J68="Tân Phú", Ward!$AS$2:$AT$12, IF(J68="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X68" t="str">
+        <f>IF(B68 &lt;&gt; "", VLOOKUP(B68, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="16"/>
       <c r="C69" s="16"/>
@@ -4499,8 +4800,12 @@
         <f>IF(K69 &lt;&gt; "", VLOOKUP(K69, IF(J69="1", Ward!$A$2:$B$11, IF(J69="2", Ward!$C$2:$D$12, IF(J69="3", Ward!$E$2:$F$15, IF(J69="4", Ward!$G$2:$H$16, IF(J69="5", Ward!$I$2:$J$16, IF(J69="6", Ward!$K$2:$L$15, IF(J69="7", Ward!$M$2:$N$11, IF(J69="8", Ward!$O$2:$P$17, IF(J69="9", Ward!$Q$2:$R$14, IF(J69="10", Ward!$S$2:$T$16, IF(J69="11", Ward!$U$2:$V$17, IF(J69="12", Ward!$W$2:$X$12, IF(J69="Bình Chánh", Ward!$Y$2:$Z$17, IF(J69="Bình Tân", Ward!$AA$2:$AB$11, IF(J69="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J69="Cần Giờ", Ward!$AE$2:$AF$8, IF(J69="Củ Chi", Ward!$AG$2:$AH$22, IF(J69="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J69="Hóc Môn", Ward!$AK$2:$AL$13, IF(J69="Nhà Bè", Ward!$AM$2:$AN$8, IF(J69="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J69="Tân Bình", Ward!$AQ$2:$AR$16, IF(J69="Tân Phú", Ward!$AS$2:$AT$12, IF(J69="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X69" t="str">
+        <f>IF(B69 &lt;&gt; "", VLOOKUP(B69, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="16"/>
       <c r="C70" s="16"/>
@@ -4533,8 +4838,12 @@
         <f>IF(K70 &lt;&gt; "", VLOOKUP(K70, IF(J70="1", Ward!$A$2:$B$11, IF(J70="2", Ward!$C$2:$D$12, IF(J70="3", Ward!$E$2:$F$15, IF(J70="4", Ward!$G$2:$H$16, IF(J70="5", Ward!$I$2:$J$16, IF(J70="6", Ward!$K$2:$L$15, IF(J70="7", Ward!$M$2:$N$11, IF(J70="8", Ward!$O$2:$P$17, IF(J70="9", Ward!$Q$2:$R$14, IF(J70="10", Ward!$S$2:$T$16, IF(J70="11", Ward!$U$2:$V$17, IF(J70="12", Ward!$W$2:$X$12, IF(J70="Bình Chánh", Ward!$Y$2:$Z$17, IF(J70="Bình Tân", Ward!$AA$2:$AB$11, IF(J70="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J70="Cần Giờ", Ward!$AE$2:$AF$8, IF(J70="Củ Chi", Ward!$AG$2:$AH$22, IF(J70="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J70="Hóc Môn", Ward!$AK$2:$AL$13, IF(J70="Nhà Bè", Ward!$AM$2:$AN$8, IF(J70="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J70="Tân Bình", Ward!$AQ$2:$AR$16, IF(J70="Tân Phú", Ward!$AS$2:$AT$12, IF(J70="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X70" t="str">
+        <f>IF(B70 &lt;&gt; "", VLOOKUP(B70, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="16"/>
       <c r="C71" s="16"/>
@@ -4567,8 +4876,12 @@
         <f>IF(K71 &lt;&gt; "", VLOOKUP(K71, IF(J71="1", Ward!$A$2:$B$11, IF(J71="2", Ward!$C$2:$D$12, IF(J71="3", Ward!$E$2:$F$15, IF(J71="4", Ward!$G$2:$H$16, IF(J71="5", Ward!$I$2:$J$16, IF(J71="6", Ward!$K$2:$L$15, IF(J71="7", Ward!$M$2:$N$11, IF(J71="8", Ward!$O$2:$P$17, IF(J71="9", Ward!$Q$2:$R$14, IF(J71="10", Ward!$S$2:$T$16, IF(J71="11", Ward!$U$2:$V$17, IF(J71="12", Ward!$W$2:$X$12, IF(J71="Bình Chánh", Ward!$Y$2:$Z$17, IF(J71="Bình Tân", Ward!$AA$2:$AB$11, IF(J71="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J71="Cần Giờ", Ward!$AE$2:$AF$8, IF(J71="Củ Chi", Ward!$AG$2:$AH$22, IF(J71="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J71="Hóc Môn", Ward!$AK$2:$AL$13, IF(J71="Nhà Bè", Ward!$AM$2:$AN$8, IF(J71="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J71="Tân Bình", Ward!$AQ$2:$AR$16, IF(J71="Tân Phú", Ward!$AS$2:$AT$12, IF(J71="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X71" t="str">
+        <f>IF(B71 &lt;&gt; "", VLOOKUP(B71, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="16"/>
       <c r="C72" s="16"/>
@@ -4601,8 +4914,12 @@
         <f>IF(K72 &lt;&gt; "", VLOOKUP(K72, IF(J72="1", Ward!$A$2:$B$11, IF(J72="2", Ward!$C$2:$D$12, IF(J72="3", Ward!$E$2:$F$15, IF(J72="4", Ward!$G$2:$H$16, IF(J72="5", Ward!$I$2:$J$16, IF(J72="6", Ward!$K$2:$L$15, IF(J72="7", Ward!$M$2:$N$11, IF(J72="8", Ward!$O$2:$P$17, IF(J72="9", Ward!$Q$2:$R$14, IF(J72="10", Ward!$S$2:$T$16, IF(J72="11", Ward!$U$2:$V$17, IF(J72="12", Ward!$W$2:$X$12, IF(J72="Bình Chánh", Ward!$Y$2:$Z$17, IF(J72="Bình Tân", Ward!$AA$2:$AB$11, IF(J72="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J72="Cần Giờ", Ward!$AE$2:$AF$8, IF(J72="Củ Chi", Ward!$AG$2:$AH$22, IF(J72="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J72="Hóc Môn", Ward!$AK$2:$AL$13, IF(J72="Nhà Bè", Ward!$AM$2:$AN$8, IF(J72="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J72="Tân Bình", Ward!$AQ$2:$AR$16, IF(J72="Tân Phú", Ward!$AS$2:$AT$12, IF(J72="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X72" t="str">
+        <f>IF(B72 &lt;&gt; "", VLOOKUP(B72, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="16"/>
       <c r="C73" s="16"/>
@@ -4635,8 +4952,12 @@
         <f>IF(K73 &lt;&gt; "", VLOOKUP(K73, IF(J73="1", Ward!$A$2:$B$11, IF(J73="2", Ward!$C$2:$D$12, IF(J73="3", Ward!$E$2:$F$15, IF(J73="4", Ward!$G$2:$H$16, IF(J73="5", Ward!$I$2:$J$16, IF(J73="6", Ward!$K$2:$L$15, IF(J73="7", Ward!$M$2:$N$11, IF(J73="8", Ward!$O$2:$P$17, IF(J73="9", Ward!$Q$2:$R$14, IF(J73="10", Ward!$S$2:$T$16, IF(J73="11", Ward!$U$2:$V$17, IF(J73="12", Ward!$W$2:$X$12, IF(J73="Bình Chánh", Ward!$Y$2:$Z$17, IF(J73="Bình Tân", Ward!$AA$2:$AB$11, IF(J73="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J73="Cần Giờ", Ward!$AE$2:$AF$8, IF(J73="Củ Chi", Ward!$AG$2:$AH$22, IF(J73="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J73="Hóc Môn", Ward!$AK$2:$AL$13, IF(J73="Nhà Bè", Ward!$AM$2:$AN$8, IF(J73="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J73="Tân Bình", Ward!$AQ$2:$AR$16, IF(J73="Tân Phú", Ward!$AS$2:$AT$12, IF(J73="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X73" t="str">
+        <f>IF(B73 &lt;&gt; "", VLOOKUP(B73, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="16"/>
       <c r="C74" s="16"/>
@@ -4669,8 +4990,12 @@
         <f>IF(K74 &lt;&gt; "", VLOOKUP(K74, IF(J74="1", Ward!$A$2:$B$11, IF(J74="2", Ward!$C$2:$D$12, IF(J74="3", Ward!$E$2:$F$15, IF(J74="4", Ward!$G$2:$H$16, IF(J74="5", Ward!$I$2:$J$16, IF(J74="6", Ward!$K$2:$L$15, IF(J74="7", Ward!$M$2:$N$11, IF(J74="8", Ward!$O$2:$P$17, IF(J74="9", Ward!$Q$2:$R$14, IF(J74="10", Ward!$S$2:$T$16, IF(J74="11", Ward!$U$2:$V$17, IF(J74="12", Ward!$W$2:$X$12, IF(J74="Bình Chánh", Ward!$Y$2:$Z$17, IF(J74="Bình Tân", Ward!$AA$2:$AB$11, IF(J74="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J74="Cần Giờ", Ward!$AE$2:$AF$8, IF(J74="Củ Chi", Ward!$AG$2:$AH$22, IF(J74="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J74="Hóc Môn", Ward!$AK$2:$AL$13, IF(J74="Nhà Bè", Ward!$AM$2:$AN$8, IF(J74="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J74="Tân Bình", Ward!$AQ$2:$AR$16, IF(J74="Tân Phú", Ward!$AS$2:$AT$12, IF(J74="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X74" t="str">
+        <f>IF(B74 &lt;&gt; "", VLOOKUP(B74, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="16"/>
       <c r="C75" s="16"/>
@@ -4703,8 +5028,12 @@
         <f>IF(K75 &lt;&gt; "", VLOOKUP(K75, IF(J75="1", Ward!$A$2:$B$11, IF(J75="2", Ward!$C$2:$D$12, IF(J75="3", Ward!$E$2:$F$15, IF(J75="4", Ward!$G$2:$H$16, IF(J75="5", Ward!$I$2:$J$16, IF(J75="6", Ward!$K$2:$L$15, IF(J75="7", Ward!$M$2:$N$11, IF(J75="8", Ward!$O$2:$P$17, IF(J75="9", Ward!$Q$2:$R$14, IF(J75="10", Ward!$S$2:$T$16, IF(J75="11", Ward!$U$2:$V$17, IF(J75="12", Ward!$W$2:$X$12, IF(J75="Bình Chánh", Ward!$Y$2:$Z$17, IF(J75="Bình Tân", Ward!$AA$2:$AB$11, IF(J75="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J75="Cần Giờ", Ward!$AE$2:$AF$8, IF(J75="Củ Chi", Ward!$AG$2:$AH$22, IF(J75="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J75="Hóc Môn", Ward!$AK$2:$AL$13, IF(J75="Nhà Bè", Ward!$AM$2:$AN$8, IF(J75="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J75="Tân Bình", Ward!$AQ$2:$AR$16, IF(J75="Tân Phú", Ward!$AS$2:$AT$12, IF(J75="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X75" t="str">
+        <f>IF(B75 &lt;&gt; "", VLOOKUP(B75, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="16"/>
       <c r="C76" s="16"/>
@@ -4737,8 +5066,12 @@
         <f>IF(K76 &lt;&gt; "", VLOOKUP(K76, IF(J76="1", Ward!$A$2:$B$11, IF(J76="2", Ward!$C$2:$D$12, IF(J76="3", Ward!$E$2:$F$15, IF(J76="4", Ward!$G$2:$H$16, IF(J76="5", Ward!$I$2:$J$16, IF(J76="6", Ward!$K$2:$L$15, IF(J76="7", Ward!$M$2:$N$11, IF(J76="8", Ward!$O$2:$P$17, IF(J76="9", Ward!$Q$2:$R$14, IF(J76="10", Ward!$S$2:$T$16, IF(J76="11", Ward!$U$2:$V$17, IF(J76="12", Ward!$W$2:$X$12, IF(J76="Bình Chánh", Ward!$Y$2:$Z$17, IF(J76="Bình Tân", Ward!$AA$2:$AB$11, IF(J76="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J76="Cần Giờ", Ward!$AE$2:$AF$8, IF(J76="Củ Chi", Ward!$AG$2:$AH$22, IF(J76="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J76="Hóc Môn", Ward!$AK$2:$AL$13, IF(J76="Nhà Bè", Ward!$AM$2:$AN$8, IF(J76="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J76="Tân Bình", Ward!$AQ$2:$AR$16, IF(J76="Tân Phú", Ward!$AS$2:$AT$12, IF(J76="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X76" t="str">
+        <f>IF(B76 &lt;&gt; "", VLOOKUP(B76, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="16"/>
       <c r="C77" s="16"/>
@@ -4771,8 +5104,12 @@
         <f>IF(K77 &lt;&gt; "", VLOOKUP(K77, IF(J77="1", Ward!$A$2:$B$11, IF(J77="2", Ward!$C$2:$D$12, IF(J77="3", Ward!$E$2:$F$15, IF(J77="4", Ward!$G$2:$H$16, IF(J77="5", Ward!$I$2:$J$16, IF(J77="6", Ward!$K$2:$L$15, IF(J77="7", Ward!$M$2:$N$11, IF(J77="8", Ward!$O$2:$P$17, IF(J77="9", Ward!$Q$2:$R$14, IF(J77="10", Ward!$S$2:$T$16, IF(J77="11", Ward!$U$2:$V$17, IF(J77="12", Ward!$W$2:$X$12, IF(J77="Bình Chánh", Ward!$Y$2:$Z$17, IF(J77="Bình Tân", Ward!$AA$2:$AB$11, IF(J77="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J77="Cần Giờ", Ward!$AE$2:$AF$8, IF(J77="Củ Chi", Ward!$AG$2:$AH$22, IF(J77="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J77="Hóc Môn", Ward!$AK$2:$AL$13, IF(J77="Nhà Bè", Ward!$AM$2:$AN$8, IF(J77="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J77="Tân Bình", Ward!$AQ$2:$AR$16, IF(J77="Tân Phú", Ward!$AS$2:$AT$12, IF(J77="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X77" t="str">
+        <f>IF(B77 &lt;&gt; "", VLOOKUP(B77, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="16"/>
       <c r="C78" s="16"/>
@@ -4805,8 +5142,12 @@
         <f>IF(K78 &lt;&gt; "", VLOOKUP(K78, IF(J78="1", Ward!$A$2:$B$11, IF(J78="2", Ward!$C$2:$D$12, IF(J78="3", Ward!$E$2:$F$15, IF(J78="4", Ward!$G$2:$H$16, IF(J78="5", Ward!$I$2:$J$16, IF(J78="6", Ward!$K$2:$L$15, IF(J78="7", Ward!$M$2:$N$11, IF(J78="8", Ward!$O$2:$P$17, IF(J78="9", Ward!$Q$2:$R$14, IF(J78="10", Ward!$S$2:$T$16, IF(J78="11", Ward!$U$2:$V$17, IF(J78="12", Ward!$W$2:$X$12, IF(J78="Bình Chánh", Ward!$Y$2:$Z$17, IF(J78="Bình Tân", Ward!$AA$2:$AB$11, IF(J78="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J78="Cần Giờ", Ward!$AE$2:$AF$8, IF(J78="Củ Chi", Ward!$AG$2:$AH$22, IF(J78="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J78="Hóc Môn", Ward!$AK$2:$AL$13, IF(J78="Nhà Bè", Ward!$AM$2:$AN$8, IF(J78="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J78="Tân Bình", Ward!$AQ$2:$AR$16, IF(J78="Tân Phú", Ward!$AS$2:$AT$12, IF(J78="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X78" t="str">
+        <f>IF(B78 &lt;&gt; "", VLOOKUP(B78, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="16"/>
       <c r="C79" s="16"/>
@@ -4839,8 +5180,12 @@
         <f>IF(K79 &lt;&gt; "", VLOOKUP(K79, IF(J79="1", Ward!$A$2:$B$11, IF(J79="2", Ward!$C$2:$D$12, IF(J79="3", Ward!$E$2:$F$15, IF(J79="4", Ward!$G$2:$H$16, IF(J79="5", Ward!$I$2:$J$16, IF(J79="6", Ward!$K$2:$L$15, IF(J79="7", Ward!$M$2:$N$11, IF(J79="8", Ward!$O$2:$P$17, IF(J79="9", Ward!$Q$2:$R$14, IF(J79="10", Ward!$S$2:$T$16, IF(J79="11", Ward!$U$2:$V$17, IF(J79="12", Ward!$W$2:$X$12, IF(J79="Bình Chánh", Ward!$Y$2:$Z$17, IF(J79="Bình Tân", Ward!$AA$2:$AB$11, IF(J79="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J79="Cần Giờ", Ward!$AE$2:$AF$8, IF(J79="Củ Chi", Ward!$AG$2:$AH$22, IF(J79="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J79="Hóc Môn", Ward!$AK$2:$AL$13, IF(J79="Nhà Bè", Ward!$AM$2:$AN$8, IF(J79="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J79="Tân Bình", Ward!$AQ$2:$AR$16, IF(J79="Tân Phú", Ward!$AS$2:$AT$12, IF(J79="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X79" t="str">
+        <f>IF(B79 &lt;&gt; "", VLOOKUP(B79, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="16"/>
       <c r="C80" s="16"/>
@@ -4873,8 +5218,12 @@
         <f>IF(K80 &lt;&gt; "", VLOOKUP(K80, IF(J80="1", Ward!$A$2:$B$11, IF(J80="2", Ward!$C$2:$D$12, IF(J80="3", Ward!$E$2:$F$15, IF(J80="4", Ward!$G$2:$H$16, IF(J80="5", Ward!$I$2:$J$16, IF(J80="6", Ward!$K$2:$L$15, IF(J80="7", Ward!$M$2:$N$11, IF(J80="8", Ward!$O$2:$P$17, IF(J80="9", Ward!$Q$2:$R$14, IF(J80="10", Ward!$S$2:$T$16, IF(J80="11", Ward!$U$2:$V$17, IF(J80="12", Ward!$W$2:$X$12, IF(J80="Bình Chánh", Ward!$Y$2:$Z$17, IF(J80="Bình Tân", Ward!$AA$2:$AB$11, IF(J80="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J80="Cần Giờ", Ward!$AE$2:$AF$8, IF(J80="Củ Chi", Ward!$AG$2:$AH$22, IF(J80="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J80="Hóc Môn", Ward!$AK$2:$AL$13, IF(J80="Nhà Bè", Ward!$AM$2:$AN$8, IF(J80="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J80="Tân Bình", Ward!$AQ$2:$AR$16, IF(J80="Tân Phú", Ward!$AS$2:$AT$12, IF(J80="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X80" t="str">
+        <f>IF(B80 &lt;&gt; "", VLOOKUP(B80, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="16"/>
       <c r="C81" s="16"/>
@@ -4907,8 +5256,12 @@
         <f>IF(K81 &lt;&gt; "", VLOOKUP(K81, IF(J81="1", Ward!$A$2:$B$11, IF(J81="2", Ward!$C$2:$D$12, IF(J81="3", Ward!$E$2:$F$15, IF(J81="4", Ward!$G$2:$H$16, IF(J81="5", Ward!$I$2:$J$16, IF(J81="6", Ward!$K$2:$L$15, IF(J81="7", Ward!$M$2:$N$11, IF(J81="8", Ward!$O$2:$P$17, IF(J81="9", Ward!$Q$2:$R$14, IF(J81="10", Ward!$S$2:$T$16, IF(J81="11", Ward!$U$2:$V$17, IF(J81="12", Ward!$W$2:$X$12, IF(J81="Bình Chánh", Ward!$Y$2:$Z$17, IF(J81="Bình Tân", Ward!$AA$2:$AB$11, IF(J81="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J81="Cần Giờ", Ward!$AE$2:$AF$8, IF(J81="Củ Chi", Ward!$AG$2:$AH$22, IF(J81="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J81="Hóc Môn", Ward!$AK$2:$AL$13, IF(J81="Nhà Bè", Ward!$AM$2:$AN$8, IF(J81="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J81="Tân Bình", Ward!$AQ$2:$AR$16, IF(J81="Tân Phú", Ward!$AS$2:$AT$12, IF(J81="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X81" t="str">
+        <f>IF(B81 &lt;&gt; "", VLOOKUP(B81, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="16"/>
       <c r="C82" s="16"/>
@@ -4941,8 +5294,12 @@
         <f>IF(K82 &lt;&gt; "", VLOOKUP(K82, IF(J82="1", Ward!$A$2:$B$11, IF(J82="2", Ward!$C$2:$D$12, IF(J82="3", Ward!$E$2:$F$15, IF(J82="4", Ward!$G$2:$H$16, IF(J82="5", Ward!$I$2:$J$16, IF(J82="6", Ward!$K$2:$L$15, IF(J82="7", Ward!$M$2:$N$11, IF(J82="8", Ward!$O$2:$P$17, IF(J82="9", Ward!$Q$2:$R$14, IF(J82="10", Ward!$S$2:$T$16, IF(J82="11", Ward!$U$2:$V$17, IF(J82="12", Ward!$W$2:$X$12, IF(J82="Bình Chánh", Ward!$Y$2:$Z$17, IF(J82="Bình Tân", Ward!$AA$2:$AB$11, IF(J82="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J82="Cần Giờ", Ward!$AE$2:$AF$8, IF(J82="Củ Chi", Ward!$AG$2:$AH$22, IF(J82="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J82="Hóc Môn", Ward!$AK$2:$AL$13, IF(J82="Nhà Bè", Ward!$AM$2:$AN$8, IF(J82="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J82="Tân Bình", Ward!$AQ$2:$AR$16, IF(J82="Tân Phú", Ward!$AS$2:$AT$12, IF(J82="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X82" t="str">
+        <f>IF(B82 &lt;&gt; "", VLOOKUP(B82, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="16"/>
       <c r="C83" s="16"/>
@@ -4975,8 +5332,12 @@
         <f>IF(K83 &lt;&gt; "", VLOOKUP(K83, IF(J83="1", Ward!$A$2:$B$11, IF(J83="2", Ward!$C$2:$D$12, IF(J83="3", Ward!$E$2:$F$15, IF(J83="4", Ward!$G$2:$H$16, IF(J83="5", Ward!$I$2:$J$16, IF(J83="6", Ward!$K$2:$L$15, IF(J83="7", Ward!$M$2:$N$11, IF(J83="8", Ward!$O$2:$P$17, IF(J83="9", Ward!$Q$2:$R$14, IF(J83="10", Ward!$S$2:$T$16, IF(J83="11", Ward!$U$2:$V$17, IF(J83="12", Ward!$W$2:$X$12, IF(J83="Bình Chánh", Ward!$Y$2:$Z$17, IF(J83="Bình Tân", Ward!$AA$2:$AB$11, IF(J83="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J83="Cần Giờ", Ward!$AE$2:$AF$8, IF(J83="Củ Chi", Ward!$AG$2:$AH$22, IF(J83="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J83="Hóc Môn", Ward!$AK$2:$AL$13, IF(J83="Nhà Bè", Ward!$AM$2:$AN$8, IF(J83="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J83="Tân Bình", Ward!$AQ$2:$AR$16, IF(J83="Tân Phú", Ward!$AS$2:$AT$12, IF(J83="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X83" t="str">
+        <f>IF(B83 &lt;&gt; "", VLOOKUP(B83, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="16"/>
       <c r="C84" s="16"/>
@@ -5009,8 +5370,12 @@
         <f>IF(K84 &lt;&gt; "", VLOOKUP(K84, IF(J84="1", Ward!$A$2:$B$11, IF(J84="2", Ward!$C$2:$D$12, IF(J84="3", Ward!$E$2:$F$15, IF(J84="4", Ward!$G$2:$H$16, IF(J84="5", Ward!$I$2:$J$16, IF(J84="6", Ward!$K$2:$L$15, IF(J84="7", Ward!$M$2:$N$11, IF(J84="8", Ward!$O$2:$P$17, IF(J84="9", Ward!$Q$2:$R$14, IF(J84="10", Ward!$S$2:$T$16, IF(J84="11", Ward!$U$2:$V$17, IF(J84="12", Ward!$W$2:$X$12, IF(J84="Bình Chánh", Ward!$Y$2:$Z$17, IF(J84="Bình Tân", Ward!$AA$2:$AB$11, IF(J84="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J84="Cần Giờ", Ward!$AE$2:$AF$8, IF(J84="Củ Chi", Ward!$AG$2:$AH$22, IF(J84="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J84="Hóc Môn", Ward!$AK$2:$AL$13, IF(J84="Nhà Bè", Ward!$AM$2:$AN$8, IF(J84="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J84="Tân Bình", Ward!$AQ$2:$AR$16, IF(J84="Tân Phú", Ward!$AS$2:$AT$12, IF(J84="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X84" t="str">
+        <f>IF(B84 &lt;&gt; "", VLOOKUP(B84, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="16"/>
       <c r="C85" s="16"/>
@@ -5043,8 +5408,12 @@
         <f>IF(K85 &lt;&gt; "", VLOOKUP(K85, IF(J85="1", Ward!$A$2:$B$11, IF(J85="2", Ward!$C$2:$D$12, IF(J85="3", Ward!$E$2:$F$15, IF(J85="4", Ward!$G$2:$H$16, IF(J85="5", Ward!$I$2:$J$16, IF(J85="6", Ward!$K$2:$L$15, IF(J85="7", Ward!$M$2:$N$11, IF(J85="8", Ward!$O$2:$P$17, IF(J85="9", Ward!$Q$2:$R$14, IF(J85="10", Ward!$S$2:$T$16, IF(J85="11", Ward!$U$2:$V$17, IF(J85="12", Ward!$W$2:$X$12, IF(J85="Bình Chánh", Ward!$Y$2:$Z$17, IF(J85="Bình Tân", Ward!$AA$2:$AB$11, IF(J85="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J85="Cần Giờ", Ward!$AE$2:$AF$8, IF(J85="Củ Chi", Ward!$AG$2:$AH$22, IF(J85="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J85="Hóc Môn", Ward!$AK$2:$AL$13, IF(J85="Nhà Bè", Ward!$AM$2:$AN$8, IF(J85="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J85="Tân Bình", Ward!$AQ$2:$AR$16, IF(J85="Tân Phú", Ward!$AS$2:$AT$12, IF(J85="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X85" t="str">
+        <f>IF(B85 &lt;&gt; "", VLOOKUP(B85, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="16"/>
       <c r="C86" s="16"/>
@@ -5077,8 +5446,12 @@
         <f>IF(K86 &lt;&gt; "", VLOOKUP(K86, IF(J86="1", Ward!$A$2:$B$11, IF(J86="2", Ward!$C$2:$D$12, IF(J86="3", Ward!$E$2:$F$15, IF(J86="4", Ward!$G$2:$H$16, IF(J86="5", Ward!$I$2:$J$16, IF(J86="6", Ward!$K$2:$L$15, IF(J86="7", Ward!$M$2:$N$11, IF(J86="8", Ward!$O$2:$P$17, IF(J86="9", Ward!$Q$2:$R$14, IF(J86="10", Ward!$S$2:$T$16, IF(J86="11", Ward!$U$2:$V$17, IF(J86="12", Ward!$W$2:$X$12, IF(J86="Bình Chánh", Ward!$Y$2:$Z$17, IF(J86="Bình Tân", Ward!$AA$2:$AB$11, IF(J86="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J86="Cần Giờ", Ward!$AE$2:$AF$8, IF(J86="Củ Chi", Ward!$AG$2:$AH$22, IF(J86="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J86="Hóc Môn", Ward!$AK$2:$AL$13, IF(J86="Nhà Bè", Ward!$AM$2:$AN$8, IF(J86="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J86="Tân Bình", Ward!$AQ$2:$AR$16, IF(J86="Tân Phú", Ward!$AS$2:$AT$12, IF(J86="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X86" t="str">
+        <f>IF(B86 &lt;&gt; "", VLOOKUP(B86, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="16"/>
       <c r="C87" s="16"/>
@@ -5111,8 +5484,12 @@
         <f>IF(K87 &lt;&gt; "", VLOOKUP(K87, IF(J87="1", Ward!$A$2:$B$11, IF(J87="2", Ward!$C$2:$D$12, IF(J87="3", Ward!$E$2:$F$15, IF(J87="4", Ward!$G$2:$H$16, IF(J87="5", Ward!$I$2:$J$16, IF(J87="6", Ward!$K$2:$L$15, IF(J87="7", Ward!$M$2:$N$11, IF(J87="8", Ward!$O$2:$P$17, IF(J87="9", Ward!$Q$2:$R$14, IF(J87="10", Ward!$S$2:$T$16, IF(J87="11", Ward!$U$2:$V$17, IF(J87="12", Ward!$W$2:$X$12, IF(J87="Bình Chánh", Ward!$Y$2:$Z$17, IF(J87="Bình Tân", Ward!$AA$2:$AB$11, IF(J87="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J87="Cần Giờ", Ward!$AE$2:$AF$8, IF(J87="Củ Chi", Ward!$AG$2:$AH$22, IF(J87="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J87="Hóc Môn", Ward!$AK$2:$AL$13, IF(J87="Nhà Bè", Ward!$AM$2:$AN$8, IF(J87="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J87="Tân Bình", Ward!$AQ$2:$AR$16, IF(J87="Tân Phú", Ward!$AS$2:$AT$12, IF(J87="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X87" t="str">
+        <f>IF(B87 &lt;&gt; "", VLOOKUP(B87, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="16"/>
       <c r="C88" s="16"/>
@@ -5145,8 +5522,12 @@
         <f>IF(K88 &lt;&gt; "", VLOOKUP(K88, IF(J88="1", Ward!$A$2:$B$11, IF(J88="2", Ward!$C$2:$D$12, IF(J88="3", Ward!$E$2:$F$15, IF(J88="4", Ward!$G$2:$H$16, IF(J88="5", Ward!$I$2:$J$16, IF(J88="6", Ward!$K$2:$L$15, IF(J88="7", Ward!$M$2:$N$11, IF(J88="8", Ward!$O$2:$P$17, IF(J88="9", Ward!$Q$2:$R$14, IF(J88="10", Ward!$S$2:$T$16, IF(J88="11", Ward!$U$2:$V$17, IF(J88="12", Ward!$W$2:$X$12, IF(J88="Bình Chánh", Ward!$Y$2:$Z$17, IF(J88="Bình Tân", Ward!$AA$2:$AB$11, IF(J88="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J88="Cần Giờ", Ward!$AE$2:$AF$8, IF(J88="Củ Chi", Ward!$AG$2:$AH$22, IF(J88="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J88="Hóc Môn", Ward!$AK$2:$AL$13, IF(J88="Nhà Bè", Ward!$AM$2:$AN$8, IF(J88="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J88="Tân Bình", Ward!$AQ$2:$AR$16, IF(J88="Tân Phú", Ward!$AS$2:$AT$12, IF(J88="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X88" t="str">
+        <f>IF(B88 &lt;&gt; "", VLOOKUP(B88, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="16"/>
       <c r="C89" s="16"/>
@@ -5179,8 +5560,12 @@
         <f>IF(K89 &lt;&gt; "", VLOOKUP(K89, IF(J89="1", Ward!$A$2:$B$11, IF(J89="2", Ward!$C$2:$D$12, IF(J89="3", Ward!$E$2:$F$15, IF(J89="4", Ward!$G$2:$H$16, IF(J89="5", Ward!$I$2:$J$16, IF(J89="6", Ward!$K$2:$L$15, IF(J89="7", Ward!$M$2:$N$11, IF(J89="8", Ward!$O$2:$P$17, IF(J89="9", Ward!$Q$2:$R$14, IF(J89="10", Ward!$S$2:$T$16, IF(J89="11", Ward!$U$2:$V$17, IF(J89="12", Ward!$W$2:$X$12, IF(J89="Bình Chánh", Ward!$Y$2:$Z$17, IF(J89="Bình Tân", Ward!$AA$2:$AB$11, IF(J89="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J89="Cần Giờ", Ward!$AE$2:$AF$8, IF(J89="Củ Chi", Ward!$AG$2:$AH$22, IF(J89="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J89="Hóc Môn", Ward!$AK$2:$AL$13, IF(J89="Nhà Bè", Ward!$AM$2:$AN$8, IF(J89="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J89="Tân Bình", Ward!$AQ$2:$AR$16, IF(J89="Tân Phú", Ward!$AS$2:$AT$12, IF(J89="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X89" t="str">
+        <f>IF(B89 &lt;&gt; "", VLOOKUP(B89, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="16"/>
       <c r="C90" s="16"/>
@@ -5213,8 +5598,12 @@
         <f>IF(K90 &lt;&gt; "", VLOOKUP(K90, IF(J90="1", Ward!$A$2:$B$11, IF(J90="2", Ward!$C$2:$D$12, IF(J90="3", Ward!$E$2:$F$15, IF(J90="4", Ward!$G$2:$H$16, IF(J90="5", Ward!$I$2:$J$16, IF(J90="6", Ward!$K$2:$L$15, IF(J90="7", Ward!$M$2:$N$11, IF(J90="8", Ward!$O$2:$P$17, IF(J90="9", Ward!$Q$2:$R$14, IF(J90="10", Ward!$S$2:$T$16, IF(J90="11", Ward!$U$2:$V$17, IF(J90="12", Ward!$W$2:$X$12, IF(J90="Bình Chánh", Ward!$Y$2:$Z$17, IF(J90="Bình Tân", Ward!$AA$2:$AB$11, IF(J90="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J90="Cần Giờ", Ward!$AE$2:$AF$8, IF(J90="Củ Chi", Ward!$AG$2:$AH$22, IF(J90="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J90="Hóc Môn", Ward!$AK$2:$AL$13, IF(J90="Nhà Bè", Ward!$AM$2:$AN$8, IF(J90="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J90="Tân Bình", Ward!$AQ$2:$AR$16, IF(J90="Tân Phú", Ward!$AS$2:$AT$12, IF(J90="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X90" t="str">
+        <f>IF(B90 &lt;&gt; "", VLOOKUP(B90, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="16"/>
       <c r="C91" s="16"/>
@@ -5247,8 +5636,12 @@
         <f>IF(K91 &lt;&gt; "", VLOOKUP(K91, IF(J91="1", Ward!$A$2:$B$11, IF(J91="2", Ward!$C$2:$D$12, IF(J91="3", Ward!$E$2:$F$15, IF(J91="4", Ward!$G$2:$H$16, IF(J91="5", Ward!$I$2:$J$16, IF(J91="6", Ward!$K$2:$L$15, IF(J91="7", Ward!$M$2:$N$11, IF(J91="8", Ward!$O$2:$P$17, IF(J91="9", Ward!$Q$2:$R$14, IF(J91="10", Ward!$S$2:$T$16, IF(J91="11", Ward!$U$2:$V$17, IF(J91="12", Ward!$W$2:$X$12, IF(J91="Bình Chánh", Ward!$Y$2:$Z$17, IF(J91="Bình Tân", Ward!$AA$2:$AB$11, IF(J91="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J91="Cần Giờ", Ward!$AE$2:$AF$8, IF(J91="Củ Chi", Ward!$AG$2:$AH$22, IF(J91="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J91="Hóc Môn", Ward!$AK$2:$AL$13, IF(J91="Nhà Bè", Ward!$AM$2:$AN$8, IF(J91="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J91="Tân Bình", Ward!$AQ$2:$AR$16, IF(J91="Tân Phú", Ward!$AS$2:$AT$12, IF(J91="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X91" t="str">
+        <f>IF(B91 &lt;&gt; "", VLOOKUP(B91, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="16"/>
       <c r="C92" s="16"/>
@@ -5281,8 +5674,12 @@
         <f>IF(K92 &lt;&gt; "", VLOOKUP(K92, IF(J92="1", Ward!$A$2:$B$11, IF(J92="2", Ward!$C$2:$D$12, IF(J92="3", Ward!$E$2:$F$15, IF(J92="4", Ward!$G$2:$H$16, IF(J92="5", Ward!$I$2:$J$16, IF(J92="6", Ward!$K$2:$L$15, IF(J92="7", Ward!$M$2:$N$11, IF(J92="8", Ward!$O$2:$P$17, IF(J92="9", Ward!$Q$2:$R$14, IF(J92="10", Ward!$S$2:$T$16, IF(J92="11", Ward!$U$2:$V$17, IF(J92="12", Ward!$W$2:$X$12, IF(J92="Bình Chánh", Ward!$Y$2:$Z$17, IF(J92="Bình Tân", Ward!$AA$2:$AB$11, IF(J92="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J92="Cần Giờ", Ward!$AE$2:$AF$8, IF(J92="Củ Chi", Ward!$AG$2:$AH$22, IF(J92="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J92="Hóc Môn", Ward!$AK$2:$AL$13, IF(J92="Nhà Bè", Ward!$AM$2:$AN$8, IF(J92="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J92="Tân Bình", Ward!$AQ$2:$AR$16, IF(J92="Tân Phú", Ward!$AS$2:$AT$12, IF(J92="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X92" t="str">
+        <f>IF(B92 &lt;&gt; "", VLOOKUP(B92, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="16"/>
       <c r="C93" s="16"/>
@@ -5315,8 +5712,12 @@
         <f>IF(K93 &lt;&gt; "", VLOOKUP(K93, IF(J93="1", Ward!$A$2:$B$11, IF(J93="2", Ward!$C$2:$D$12, IF(J93="3", Ward!$E$2:$F$15, IF(J93="4", Ward!$G$2:$H$16, IF(J93="5", Ward!$I$2:$J$16, IF(J93="6", Ward!$K$2:$L$15, IF(J93="7", Ward!$M$2:$N$11, IF(J93="8", Ward!$O$2:$P$17, IF(J93="9", Ward!$Q$2:$R$14, IF(J93="10", Ward!$S$2:$T$16, IF(J93="11", Ward!$U$2:$V$17, IF(J93="12", Ward!$W$2:$X$12, IF(J93="Bình Chánh", Ward!$Y$2:$Z$17, IF(J93="Bình Tân", Ward!$AA$2:$AB$11, IF(J93="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J93="Cần Giờ", Ward!$AE$2:$AF$8, IF(J93="Củ Chi", Ward!$AG$2:$AH$22, IF(J93="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J93="Hóc Môn", Ward!$AK$2:$AL$13, IF(J93="Nhà Bè", Ward!$AM$2:$AN$8, IF(J93="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J93="Tân Bình", Ward!$AQ$2:$AR$16, IF(J93="Tân Phú", Ward!$AS$2:$AT$12, IF(J93="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X93" t="str">
+        <f>IF(B93 &lt;&gt; "", VLOOKUP(B93, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="16"/>
       <c r="C94" s="16"/>
@@ -5349,8 +5750,12 @@
         <f>IF(K94 &lt;&gt; "", VLOOKUP(K94, IF(J94="1", Ward!$A$2:$B$11, IF(J94="2", Ward!$C$2:$D$12, IF(J94="3", Ward!$E$2:$F$15, IF(J94="4", Ward!$G$2:$H$16, IF(J94="5", Ward!$I$2:$J$16, IF(J94="6", Ward!$K$2:$L$15, IF(J94="7", Ward!$M$2:$N$11, IF(J94="8", Ward!$O$2:$P$17, IF(J94="9", Ward!$Q$2:$R$14, IF(J94="10", Ward!$S$2:$T$16, IF(J94="11", Ward!$U$2:$V$17, IF(J94="12", Ward!$W$2:$X$12, IF(J94="Bình Chánh", Ward!$Y$2:$Z$17, IF(J94="Bình Tân", Ward!$AA$2:$AB$11, IF(J94="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J94="Cần Giờ", Ward!$AE$2:$AF$8, IF(J94="Củ Chi", Ward!$AG$2:$AH$22, IF(J94="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J94="Hóc Môn", Ward!$AK$2:$AL$13, IF(J94="Nhà Bè", Ward!$AM$2:$AN$8, IF(J94="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J94="Tân Bình", Ward!$AQ$2:$AR$16, IF(J94="Tân Phú", Ward!$AS$2:$AT$12, IF(J94="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X94" t="str">
+        <f>IF(B94 &lt;&gt; "", VLOOKUP(B94, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="16"/>
       <c r="C95" s="16"/>
@@ -5383,8 +5788,12 @@
         <f>IF(K95 &lt;&gt; "", VLOOKUP(K95, IF(J95="1", Ward!$A$2:$B$11, IF(J95="2", Ward!$C$2:$D$12, IF(J95="3", Ward!$E$2:$F$15, IF(J95="4", Ward!$G$2:$H$16, IF(J95="5", Ward!$I$2:$J$16, IF(J95="6", Ward!$K$2:$L$15, IF(J95="7", Ward!$M$2:$N$11, IF(J95="8", Ward!$O$2:$P$17, IF(J95="9", Ward!$Q$2:$R$14, IF(J95="10", Ward!$S$2:$T$16, IF(J95="11", Ward!$U$2:$V$17, IF(J95="12", Ward!$W$2:$X$12, IF(J95="Bình Chánh", Ward!$Y$2:$Z$17, IF(J95="Bình Tân", Ward!$AA$2:$AB$11, IF(J95="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J95="Cần Giờ", Ward!$AE$2:$AF$8, IF(J95="Củ Chi", Ward!$AG$2:$AH$22, IF(J95="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J95="Hóc Môn", Ward!$AK$2:$AL$13, IF(J95="Nhà Bè", Ward!$AM$2:$AN$8, IF(J95="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J95="Tân Bình", Ward!$AQ$2:$AR$16, IF(J95="Tân Phú", Ward!$AS$2:$AT$12, IF(J95="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X95" t="str">
+        <f>IF(B95 &lt;&gt; "", VLOOKUP(B95, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="16"/>
       <c r="C96" s="16"/>
@@ -5417,8 +5826,12 @@
         <f>IF(K96 &lt;&gt; "", VLOOKUP(K96, IF(J96="1", Ward!$A$2:$B$11, IF(J96="2", Ward!$C$2:$D$12, IF(J96="3", Ward!$E$2:$F$15, IF(J96="4", Ward!$G$2:$H$16, IF(J96="5", Ward!$I$2:$J$16, IF(J96="6", Ward!$K$2:$L$15, IF(J96="7", Ward!$M$2:$N$11, IF(J96="8", Ward!$O$2:$P$17, IF(J96="9", Ward!$Q$2:$R$14, IF(J96="10", Ward!$S$2:$T$16, IF(J96="11", Ward!$U$2:$V$17, IF(J96="12", Ward!$W$2:$X$12, IF(J96="Bình Chánh", Ward!$Y$2:$Z$17, IF(J96="Bình Tân", Ward!$AA$2:$AB$11, IF(J96="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J96="Cần Giờ", Ward!$AE$2:$AF$8, IF(J96="Củ Chi", Ward!$AG$2:$AH$22, IF(J96="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J96="Hóc Môn", Ward!$AK$2:$AL$13, IF(J96="Nhà Bè", Ward!$AM$2:$AN$8, IF(J96="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J96="Tân Bình", Ward!$AQ$2:$AR$16, IF(J96="Tân Phú", Ward!$AS$2:$AT$12, IF(J96="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X96" t="str">
+        <f>IF(B96 &lt;&gt; "", VLOOKUP(B96, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="16"/>
       <c r="C97" s="16"/>
@@ -5451,8 +5864,12 @@
         <f>IF(K97 &lt;&gt; "", VLOOKUP(K97, IF(J97="1", Ward!$A$2:$B$11, IF(J97="2", Ward!$C$2:$D$12, IF(J97="3", Ward!$E$2:$F$15, IF(J97="4", Ward!$G$2:$H$16, IF(J97="5", Ward!$I$2:$J$16, IF(J97="6", Ward!$K$2:$L$15, IF(J97="7", Ward!$M$2:$N$11, IF(J97="8", Ward!$O$2:$P$17, IF(J97="9", Ward!$Q$2:$R$14, IF(J97="10", Ward!$S$2:$T$16, IF(J97="11", Ward!$U$2:$V$17, IF(J97="12", Ward!$W$2:$X$12, IF(J97="Bình Chánh", Ward!$Y$2:$Z$17, IF(J97="Bình Tân", Ward!$AA$2:$AB$11, IF(J97="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J97="Cần Giờ", Ward!$AE$2:$AF$8, IF(J97="Củ Chi", Ward!$AG$2:$AH$22, IF(J97="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J97="Hóc Môn", Ward!$AK$2:$AL$13, IF(J97="Nhà Bè", Ward!$AM$2:$AN$8, IF(J97="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J97="Tân Bình", Ward!$AQ$2:$AR$16, IF(J97="Tân Phú", Ward!$AS$2:$AT$12, IF(J97="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X97" t="str">
+        <f>IF(B97 &lt;&gt; "", VLOOKUP(B97, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="16"/>
       <c r="C98" s="16"/>
@@ -5485,8 +5902,12 @@
         <f>IF(K98 &lt;&gt; "", VLOOKUP(K98, IF(J98="1", Ward!$A$2:$B$11, IF(J98="2", Ward!$C$2:$D$12, IF(J98="3", Ward!$E$2:$F$15, IF(J98="4", Ward!$G$2:$H$16, IF(J98="5", Ward!$I$2:$J$16, IF(J98="6", Ward!$K$2:$L$15, IF(J98="7", Ward!$M$2:$N$11, IF(J98="8", Ward!$O$2:$P$17, IF(J98="9", Ward!$Q$2:$R$14, IF(J98="10", Ward!$S$2:$T$16, IF(J98="11", Ward!$U$2:$V$17, IF(J98="12", Ward!$W$2:$X$12, IF(J98="Bình Chánh", Ward!$Y$2:$Z$17, IF(J98="Bình Tân", Ward!$AA$2:$AB$11, IF(J98="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J98="Cần Giờ", Ward!$AE$2:$AF$8, IF(J98="Củ Chi", Ward!$AG$2:$AH$22, IF(J98="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J98="Hóc Môn", Ward!$AK$2:$AL$13, IF(J98="Nhà Bè", Ward!$AM$2:$AN$8, IF(J98="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J98="Tân Bình", Ward!$AQ$2:$AR$16, IF(J98="Tân Phú", Ward!$AS$2:$AT$12, IF(J98="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X98" t="str">
+        <f>IF(B98 &lt;&gt; "", VLOOKUP(B98, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="16"/>
       <c r="C99" s="16"/>
@@ -5519,8 +5940,12 @@
         <f>IF(K99 &lt;&gt; "", VLOOKUP(K99, IF(J99="1", Ward!$A$2:$B$11, IF(J99="2", Ward!$C$2:$D$12, IF(J99="3", Ward!$E$2:$F$15, IF(J99="4", Ward!$G$2:$H$16, IF(J99="5", Ward!$I$2:$J$16, IF(J99="6", Ward!$K$2:$L$15, IF(J99="7", Ward!$M$2:$N$11, IF(J99="8", Ward!$O$2:$P$17, IF(J99="9", Ward!$Q$2:$R$14, IF(J99="10", Ward!$S$2:$T$16, IF(J99="11", Ward!$U$2:$V$17, IF(J99="12", Ward!$W$2:$X$12, IF(J99="Bình Chánh", Ward!$Y$2:$Z$17, IF(J99="Bình Tân", Ward!$AA$2:$AB$11, IF(J99="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J99="Cần Giờ", Ward!$AE$2:$AF$8, IF(J99="Củ Chi", Ward!$AG$2:$AH$22, IF(J99="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J99="Hóc Môn", Ward!$AK$2:$AL$13, IF(J99="Nhà Bè", Ward!$AM$2:$AN$8, IF(J99="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J99="Tân Bình", Ward!$AQ$2:$AR$16, IF(J99="Tân Phú", Ward!$AS$2:$AT$12, IF(J99="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X99" t="str">
+        <f>IF(B99 &lt;&gt; "", VLOOKUP(B99, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="16"/>
       <c r="C100" s="16"/>
@@ -5553,8 +5978,12 @@
         <f>IF(K100 &lt;&gt; "", VLOOKUP(K100, IF(J100="1", Ward!$A$2:$B$11, IF(J100="2", Ward!$C$2:$D$12, IF(J100="3", Ward!$E$2:$F$15, IF(J100="4", Ward!$G$2:$H$16, IF(J100="5", Ward!$I$2:$J$16, IF(J100="6", Ward!$K$2:$L$15, IF(J100="7", Ward!$M$2:$N$11, IF(J100="8", Ward!$O$2:$P$17, IF(J100="9", Ward!$Q$2:$R$14, IF(J100="10", Ward!$S$2:$T$16, IF(J100="11", Ward!$U$2:$V$17, IF(J100="12", Ward!$W$2:$X$12, IF(J100="Bình Chánh", Ward!$Y$2:$Z$17, IF(J100="Bình Tân", Ward!$AA$2:$AB$11, IF(J100="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J100="Cần Giờ", Ward!$AE$2:$AF$8, IF(J100="Củ Chi", Ward!$AG$2:$AH$22, IF(J100="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J100="Hóc Môn", Ward!$AK$2:$AL$13, IF(J100="Nhà Bè", Ward!$AM$2:$AN$8, IF(J100="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J100="Tân Bình", Ward!$AQ$2:$AR$16, IF(J100="Tân Phú", Ward!$AS$2:$AT$12, IF(J100="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X100" t="str">
+        <f>IF(B100 &lt;&gt; "", VLOOKUP(B100, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="16"/>
       <c r="C101" s="16"/>
@@ -5587,8 +6016,12 @@
         <f>IF(K101 &lt;&gt; "", VLOOKUP(K101, IF(J101="1", Ward!$A$2:$B$11, IF(J101="2", Ward!$C$2:$D$12, IF(J101="3", Ward!$E$2:$F$15, IF(J101="4", Ward!$G$2:$H$16, IF(J101="5", Ward!$I$2:$J$16, IF(J101="6", Ward!$K$2:$L$15, IF(J101="7", Ward!$M$2:$N$11, IF(J101="8", Ward!$O$2:$P$17, IF(J101="9", Ward!$Q$2:$R$14, IF(J101="10", Ward!$S$2:$T$16, IF(J101="11", Ward!$U$2:$V$17, IF(J101="12", Ward!$W$2:$X$12, IF(J101="Bình Chánh", Ward!$Y$2:$Z$17, IF(J101="Bình Tân", Ward!$AA$2:$AB$11, IF(J101="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J101="Cần Giờ", Ward!$AE$2:$AF$8, IF(J101="Củ Chi", Ward!$AG$2:$AH$22, IF(J101="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J101="Hóc Môn", Ward!$AK$2:$AL$13, IF(J101="Nhà Bè", Ward!$AM$2:$AN$8, IF(J101="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J101="Tân Bình", Ward!$AQ$2:$AR$16, IF(J101="Tân Phú", Ward!$AS$2:$AT$12, IF(J101="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X101" t="str">
+        <f>IF(B101 &lt;&gt; "", VLOOKUP(B101, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="16"/>
       <c r="C102" s="16"/>
@@ -5621,8 +6054,12 @@
         <f>IF(K102 &lt;&gt; "", VLOOKUP(K102, IF(J102="1", Ward!$A$2:$B$11, IF(J102="2", Ward!$C$2:$D$12, IF(J102="3", Ward!$E$2:$F$15, IF(J102="4", Ward!$G$2:$H$16, IF(J102="5", Ward!$I$2:$J$16, IF(J102="6", Ward!$K$2:$L$15, IF(J102="7", Ward!$M$2:$N$11, IF(J102="8", Ward!$O$2:$P$17, IF(J102="9", Ward!$Q$2:$R$14, IF(J102="10", Ward!$S$2:$T$16, IF(J102="11", Ward!$U$2:$V$17, IF(J102="12", Ward!$W$2:$X$12, IF(J102="Bình Chánh", Ward!$Y$2:$Z$17, IF(J102="Bình Tân", Ward!$AA$2:$AB$11, IF(J102="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J102="Cần Giờ", Ward!$AE$2:$AF$8, IF(J102="Củ Chi", Ward!$AG$2:$AH$22, IF(J102="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J102="Hóc Môn", Ward!$AK$2:$AL$13, IF(J102="Nhà Bè", Ward!$AM$2:$AN$8, IF(J102="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J102="Tân Bình", Ward!$AQ$2:$AR$16, IF(J102="Tân Phú", Ward!$AS$2:$AT$12, IF(J102="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X102" t="str">
+        <f>IF(B102 &lt;&gt; "", VLOOKUP(B102, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="16"/>
       <c r="C103" s="16"/>
@@ -5655,8 +6092,12 @@
         <f>IF(K103 &lt;&gt; "", VLOOKUP(K103, IF(J103="1", Ward!$A$2:$B$11, IF(J103="2", Ward!$C$2:$D$12, IF(J103="3", Ward!$E$2:$F$15, IF(J103="4", Ward!$G$2:$H$16, IF(J103="5", Ward!$I$2:$J$16, IF(J103="6", Ward!$K$2:$L$15, IF(J103="7", Ward!$M$2:$N$11, IF(J103="8", Ward!$O$2:$P$17, IF(J103="9", Ward!$Q$2:$R$14, IF(J103="10", Ward!$S$2:$T$16, IF(J103="11", Ward!$U$2:$V$17, IF(J103="12", Ward!$W$2:$X$12, IF(J103="Bình Chánh", Ward!$Y$2:$Z$17, IF(J103="Bình Tân", Ward!$AA$2:$AB$11, IF(J103="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J103="Cần Giờ", Ward!$AE$2:$AF$8, IF(J103="Củ Chi", Ward!$AG$2:$AH$22, IF(J103="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J103="Hóc Môn", Ward!$AK$2:$AL$13, IF(J103="Nhà Bè", Ward!$AM$2:$AN$8, IF(J103="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J103="Tân Bình", Ward!$AQ$2:$AR$16, IF(J103="Tân Phú", Ward!$AS$2:$AT$12, IF(J103="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X103" t="str">
+        <f>IF(B103 &lt;&gt; "", VLOOKUP(B103, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="16"/>
       <c r="C104" s="16"/>
@@ -5689,8 +6130,12 @@
         <f>IF(K104 &lt;&gt; "", VLOOKUP(K104, IF(J104="1", Ward!$A$2:$B$11, IF(J104="2", Ward!$C$2:$D$12, IF(J104="3", Ward!$E$2:$F$15, IF(J104="4", Ward!$G$2:$H$16, IF(J104="5", Ward!$I$2:$J$16, IF(J104="6", Ward!$K$2:$L$15, IF(J104="7", Ward!$M$2:$N$11, IF(J104="8", Ward!$O$2:$P$17, IF(J104="9", Ward!$Q$2:$R$14, IF(J104="10", Ward!$S$2:$T$16, IF(J104="11", Ward!$U$2:$V$17, IF(J104="12", Ward!$W$2:$X$12, IF(J104="Bình Chánh", Ward!$Y$2:$Z$17, IF(J104="Bình Tân", Ward!$AA$2:$AB$11, IF(J104="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J104="Cần Giờ", Ward!$AE$2:$AF$8, IF(J104="Củ Chi", Ward!$AG$2:$AH$22, IF(J104="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J104="Hóc Môn", Ward!$AK$2:$AL$13, IF(J104="Nhà Bè", Ward!$AM$2:$AN$8, IF(J104="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J104="Tân Bình", Ward!$AQ$2:$AR$16, IF(J104="Tân Phú", Ward!$AS$2:$AT$12, IF(J104="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X104" t="str">
+        <f>IF(B104 &lt;&gt; "", VLOOKUP(B104, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="16"/>
       <c r="C105" s="16"/>
@@ -5723,8 +6168,12 @@
         <f>IF(K105 &lt;&gt; "", VLOOKUP(K105, IF(J105="1", Ward!$A$2:$B$11, IF(J105="2", Ward!$C$2:$D$12, IF(J105="3", Ward!$E$2:$F$15, IF(J105="4", Ward!$G$2:$H$16, IF(J105="5", Ward!$I$2:$J$16, IF(J105="6", Ward!$K$2:$L$15, IF(J105="7", Ward!$M$2:$N$11, IF(J105="8", Ward!$O$2:$P$17, IF(J105="9", Ward!$Q$2:$R$14, IF(J105="10", Ward!$S$2:$T$16, IF(J105="11", Ward!$U$2:$V$17, IF(J105="12", Ward!$W$2:$X$12, IF(J105="Bình Chánh", Ward!$Y$2:$Z$17, IF(J105="Bình Tân", Ward!$AA$2:$AB$11, IF(J105="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J105="Cần Giờ", Ward!$AE$2:$AF$8, IF(J105="Củ Chi", Ward!$AG$2:$AH$22, IF(J105="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J105="Hóc Môn", Ward!$AK$2:$AL$13, IF(J105="Nhà Bè", Ward!$AM$2:$AN$8, IF(J105="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J105="Tân Bình", Ward!$AQ$2:$AR$16, IF(J105="Tân Phú", Ward!$AS$2:$AT$12, IF(J105="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X105" t="str">
+        <f>IF(B105 &lt;&gt; "", VLOOKUP(B105, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="16"/>
       <c r="C106" s="16"/>
@@ -5757,8 +6206,12 @@
         <f>IF(K106 &lt;&gt; "", VLOOKUP(K106, IF(J106="1", Ward!$A$2:$B$11, IF(J106="2", Ward!$C$2:$D$12, IF(J106="3", Ward!$E$2:$F$15, IF(J106="4", Ward!$G$2:$H$16, IF(J106="5", Ward!$I$2:$J$16, IF(J106="6", Ward!$K$2:$L$15, IF(J106="7", Ward!$M$2:$N$11, IF(J106="8", Ward!$O$2:$P$17, IF(J106="9", Ward!$Q$2:$R$14, IF(J106="10", Ward!$S$2:$T$16, IF(J106="11", Ward!$U$2:$V$17, IF(J106="12", Ward!$W$2:$X$12, IF(J106="Bình Chánh", Ward!$Y$2:$Z$17, IF(J106="Bình Tân", Ward!$AA$2:$AB$11, IF(J106="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J106="Cần Giờ", Ward!$AE$2:$AF$8, IF(J106="Củ Chi", Ward!$AG$2:$AH$22, IF(J106="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J106="Hóc Môn", Ward!$AK$2:$AL$13, IF(J106="Nhà Bè", Ward!$AM$2:$AN$8, IF(J106="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J106="Tân Bình", Ward!$AQ$2:$AR$16, IF(J106="Tân Phú", Ward!$AS$2:$AT$12, IF(J106="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X106" t="str">
+        <f>IF(B106 &lt;&gt; "", VLOOKUP(B106, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="16"/>
       <c r="C107" s="16"/>
@@ -5791,8 +6244,12 @@
         <f>IF(K107 &lt;&gt; "", VLOOKUP(K107, IF(J107="1", Ward!$A$2:$B$11, IF(J107="2", Ward!$C$2:$D$12, IF(J107="3", Ward!$E$2:$F$15, IF(J107="4", Ward!$G$2:$H$16, IF(J107="5", Ward!$I$2:$J$16, IF(J107="6", Ward!$K$2:$L$15, IF(J107="7", Ward!$M$2:$N$11, IF(J107="8", Ward!$O$2:$P$17, IF(J107="9", Ward!$Q$2:$R$14, IF(J107="10", Ward!$S$2:$T$16, IF(J107="11", Ward!$U$2:$V$17, IF(J107="12", Ward!$W$2:$X$12, IF(J107="Bình Chánh", Ward!$Y$2:$Z$17, IF(J107="Bình Tân", Ward!$AA$2:$AB$11, IF(J107="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J107="Cần Giờ", Ward!$AE$2:$AF$8, IF(J107="Củ Chi", Ward!$AG$2:$AH$22, IF(J107="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J107="Hóc Môn", Ward!$AK$2:$AL$13, IF(J107="Nhà Bè", Ward!$AM$2:$AN$8, IF(J107="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J107="Tân Bình", Ward!$AQ$2:$AR$16, IF(J107="Tân Phú", Ward!$AS$2:$AT$12, IF(J107="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X107" t="str">
+        <f>IF(B107 &lt;&gt; "", VLOOKUP(B107, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="16"/>
       <c r="C108" s="16"/>
@@ -5825,8 +6282,12 @@
         <f>IF(K108 &lt;&gt; "", VLOOKUP(K108, IF(J108="1", Ward!$A$2:$B$11, IF(J108="2", Ward!$C$2:$D$12, IF(J108="3", Ward!$E$2:$F$15, IF(J108="4", Ward!$G$2:$H$16, IF(J108="5", Ward!$I$2:$J$16, IF(J108="6", Ward!$K$2:$L$15, IF(J108="7", Ward!$M$2:$N$11, IF(J108="8", Ward!$O$2:$P$17, IF(J108="9", Ward!$Q$2:$R$14, IF(J108="10", Ward!$S$2:$T$16, IF(J108="11", Ward!$U$2:$V$17, IF(J108="12", Ward!$W$2:$X$12, IF(J108="Bình Chánh", Ward!$Y$2:$Z$17, IF(J108="Bình Tân", Ward!$AA$2:$AB$11, IF(J108="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J108="Cần Giờ", Ward!$AE$2:$AF$8, IF(J108="Củ Chi", Ward!$AG$2:$AH$22, IF(J108="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J108="Hóc Môn", Ward!$AK$2:$AL$13, IF(J108="Nhà Bè", Ward!$AM$2:$AN$8, IF(J108="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J108="Tân Bình", Ward!$AQ$2:$AR$16, IF(J108="Tân Phú", Ward!$AS$2:$AT$12, IF(J108="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X108" t="str">
+        <f>IF(B108 &lt;&gt; "", VLOOKUP(B108, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="16"/>
       <c r="C109" s="16"/>
@@ -5859,8 +6320,12 @@
         <f>IF(K109 &lt;&gt; "", VLOOKUP(K109, IF(J109="1", Ward!$A$2:$B$11, IF(J109="2", Ward!$C$2:$D$12, IF(J109="3", Ward!$E$2:$F$15, IF(J109="4", Ward!$G$2:$H$16, IF(J109="5", Ward!$I$2:$J$16, IF(J109="6", Ward!$K$2:$L$15, IF(J109="7", Ward!$M$2:$N$11, IF(J109="8", Ward!$O$2:$P$17, IF(J109="9", Ward!$Q$2:$R$14, IF(J109="10", Ward!$S$2:$T$16, IF(J109="11", Ward!$U$2:$V$17, IF(J109="12", Ward!$W$2:$X$12, IF(J109="Bình Chánh", Ward!$Y$2:$Z$17, IF(J109="Bình Tân", Ward!$AA$2:$AB$11, IF(J109="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J109="Cần Giờ", Ward!$AE$2:$AF$8, IF(J109="Củ Chi", Ward!$AG$2:$AH$22, IF(J109="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J109="Hóc Môn", Ward!$AK$2:$AL$13, IF(J109="Nhà Bè", Ward!$AM$2:$AN$8, IF(J109="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J109="Tân Bình", Ward!$AQ$2:$AR$16, IF(J109="Tân Phú", Ward!$AS$2:$AT$12, IF(J109="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X109" t="str">
+        <f>IF(B109 &lt;&gt; "", VLOOKUP(B109, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="16"/>
       <c r="C110" s="16"/>
@@ -5893,8 +6358,12 @@
         <f>IF(K110 &lt;&gt; "", VLOOKUP(K110, IF(J110="1", Ward!$A$2:$B$11, IF(J110="2", Ward!$C$2:$D$12, IF(J110="3", Ward!$E$2:$F$15, IF(J110="4", Ward!$G$2:$H$16, IF(J110="5", Ward!$I$2:$J$16, IF(J110="6", Ward!$K$2:$L$15, IF(J110="7", Ward!$M$2:$N$11, IF(J110="8", Ward!$O$2:$P$17, IF(J110="9", Ward!$Q$2:$R$14, IF(J110="10", Ward!$S$2:$T$16, IF(J110="11", Ward!$U$2:$V$17, IF(J110="12", Ward!$W$2:$X$12, IF(J110="Bình Chánh", Ward!$Y$2:$Z$17, IF(J110="Bình Tân", Ward!$AA$2:$AB$11, IF(J110="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J110="Cần Giờ", Ward!$AE$2:$AF$8, IF(J110="Củ Chi", Ward!$AG$2:$AH$22, IF(J110="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J110="Hóc Môn", Ward!$AK$2:$AL$13, IF(J110="Nhà Bè", Ward!$AM$2:$AN$8, IF(J110="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J110="Tân Bình", Ward!$AQ$2:$AR$16, IF(J110="Tân Phú", Ward!$AS$2:$AT$12, IF(J110="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X110" t="str">
+        <f>IF(B110 &lt;&gt; "", VLOOKUP(B110, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="16"/>
       <c r="C111" s="16"/>
@@ -5927,8 +6396,12 @@
         <f>IF(K111 &lt;&gt; "", VLOOKUP(K111, IF(J111="1", Ward!$A$2:$B$11, IF(J111="2", Ward!$C$2:$D$12, IF(J111="3", Ward!$E$2:$F$15, IF(J111="4", Ward!$G$2:$H$16, IF(J111="5", Ward!$I$2:$J$16, IF(J111="6", Ward!$K$2:$L$15, IF(J111="7", Ward!$M$2:$N$11, IF(J111="8", Ward!$O$2:$P$17, IF(J111="9", Ward!$Q$2:$R$14, IF(J111="10", Ward!$S$2:$T$16, IF(J111="11", Ward!$U$2:$V$17, IF(J111="12", Ward!$W$2:$X$12, IF(J111="Bình Chánh", Ward!$Y$2:$Z$17, IF(J111="Bình Tân", Ward!$AA$2:$AB$11, IF(J111="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J111="Cần Giờ", Ward!$AE$2:$AF$8, IF(J111="Củ Chi", Ward!$AG$2:$AH$22, IF(J111="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J111="Hóc Môn", Ward!$AK$2:$AL$13, IF(J111="Nhà Bè", Ward!$AM$2:$AN$8, IF(J111="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J111="Tân Bình", Ward!$AQ$2:$AR$16, IF(J111="Tân Phú", Ward!$AS$2:$AT$12, IF(J111="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X111" t="str">
+        <f>IF(B111 &lt;&gt; "", VLOOKUP(B111, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="112" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="16"/>
       <c r="C112" s="16"/>
@@ -5961,8 +6434,12 @@
         <f>IF(K112 &lt;&gt; "", VLOOKUP(K112, IF(J112="1", Ward!$A$2:$B$11, IF(J112="2", Ward!$C$2:$D$12, IF(J112="3", Ward!$E$2:$F$15, IF(J112="4", Ward!$G$2:$H$16, IF(J112="5", Ward!$I$2:$J$16, IF(J112="6", Ward!$K$2:$L$15, IF(J112="7", Ward!$M$2:$N$11, IF(J112="8", Ward!$O$2:$P$17, IF(J112="9", Ward!$Q$2:$R$14, IF(J112="10", Ward!$S$2:$T$16, IF(J112="11", Ward!$U$2:$V$17, IF(J112="12", Ward!$W$2:$X$12, IF(J112="Bình Chánh", Ward!$Y$2:$Z$17, IF(J112="Bình Tân", Ward!$AA$2:$AB$11, IF(J112="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J112="Cần Giờ", Ward!$AE$2:$AF$8, IF(J112="Củ Chi", Ward!$AG$2:$AH$22, IF(J112="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J112="Hóc Môn", Ward!$AK$2:$AL$13, IF(J112="Nhà Bè", Ward!$AM$2:$AN$8, IF(J112="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J112="Tân Bình", Ward!$AQ$2:$AR$16, IF(J112="Tân Phú", Ward!$AS$2:$AT$12, IF(J112="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X112" t="str">
+        <f>IF(B112 &lt;&gt; "", VLOOKUP(B112, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="16"/>
       <c r="C113" s="16"/>
@@ -5995,8 +6472,12 @@
         <f>IF(K113 &lt;&gt; "", VLOOKUP(K113, IF(J113="1", Ward!$A$2:$B$11, IF(J113="2", Ward!$C$2:$D$12, IF(J113="3", Ward!$E$2:$F$15, IF(J113="4", Ward!$G$2:$H$16, IF(J113="5", Ward!$I$2:$J$16, IF(J113="6", Ward!$K$2:$L$15, IF(J113="7", Ward!$M$2:$N$11, IF(J113="8", Ward!$O$2:$P$17, IF(J113="9", Ward!$Q$2:$R$14, IF(J113="10", Ward!$S$2:$T$16, IF(J113="11", Ward!$U$2:$V$17, IF(J113="12", Ward!$W$2:$X$12, IF(J113="Bình Chánh", Ward!$Y$2:$Z$17, IF(J113="Bình Tân", Ward!$AA$2:$AB$11, IF(J113="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J113="Cần Giờ", Ward!$AE$2:$AF$8, IF(J113="Củ Chi", Ward!$AG$2:$AH$22, IF(J113="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J113="Hóc Môn", Ward!$AK$2:$AL$13, IF(J113="Nhà Bè", Ward!$AM$2:$AN$8, IF(J113="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J113="Tân Bình", Ward!$AQ$2:$AR$16, IF(J113="Tân Phú", Ward!$AS$2:$AT$12, IF(J113="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X113" t="str">
+        <f>IF(B113 &lt;&gt; "", VLOOKUP(B113, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="16"/>
       <c r="C114" s="16"/>
@@ -6029,8 +6510,12 @@
         <f>IF(K114 &lt;&gt; "", VLOOKUP(K114, IF(J114="1", Ward!$A$2:$B$11, IF(J114="2", Ward!$C$2:$D$12, IF(J114="3", Ward!$E$2:$F$15, IF(J114="4", Ward!$G$2:$H$16, IF(J114="5", Ward!$I$2:$J$16, IF(J114="6", Ward!$K$2:$L$15, IF(J114="7", Ward!$M$2:$N$11, IF(J114="8", Ward!$O$2:$P$17, IF(J114="9", Ward!$Q$2:$R$14, IF(J114="10", Ward!$S$2:$T$16, IF(J114="11", Ward!$U$2:$V$17, IF(J114="12", Ward!$W$2:$X$12, IF(J114="Bình Chánh", Ward!$Y$2:$Z$17, IF(J114="Bình Tân", Ward!$AA$2:$AB$11, IF(J114="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J114="Cần Giờ", Ward!$AE$2:$AF$8, IF(J114="Củ Chi", Ward!$AG$2:$AH$22, IF(J114="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J114="Hóc Môn", Ward!$AK$2:$AL$13, IF(J114="Nhà Bè", Ward!$AM$2:$AN$8, IF(J114="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J114="Tân Bình", Ward!$AQ$2:$AR$16, IF(J114="Tân Phú", Ward!$AS$2:$AT$12, IF(J114="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X114" t="str">
+        <f>IF(B114 &lt;&gt; "", VLOOKUP(B114, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="16"/>
       <c r="C115" s="16"/>
@@ -6063,8 +6548,12 @@
         <f>IF(K115 &lt;&gt; "", VLOOKUP(K115, IF(J115="1", Ward!$A$2:$B$11, IF(J115="2", Ward!$C$2:$D$12, IF(J115="3", Ward!$E$2:$F$15, IF(J115="4", Ward!$G$2:$H$16, IF(J115="5", Ward!$I$2:$J$16, IF(J115="6", Ward!$K$2:$L$15, IF(J115="7", Ward!$M$2:$N$11, IF(J115="8", Ward!$O$2:$P$17, IF(J115="9", Ward!$Q$2:$R$14, IF(J115="10", Ward!$S$2:$T$16, IF(J115="11", Ward!$U$2:$V$17, IF(J115="12", Ward!$W$2:$X$12, IF(J115="Bình Chánh", Ward!$Y$2:$Z$17, IF(J115="Bình Tân", Ward!$AA$2:$AB$11, IF(J115="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J115="Cần Giờ", Ward!$AE$2:$AF$8, IF(J115="Củ Chi", Ward!$AG$2:$AH$22, IF(J115="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J115="Hóc Môn", Ward!$AK$2:$AL$13, IF(J115="Nhà Bè", Ward!$AM$2:$AN$8, IF(J115="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J115="Tân Bình", Ward!$AQ$2:$AR$16, IF(J115="Tân Phú", Ward!$AS$2:$AT$12, IF(J115="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X115" t="str">
+        <f>IF(B115 &lt;&gt; "", VLOOKUP(B115, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="16"/>
       <c r="C116" s="16"/>
@@ -6097,8 +6586,12 @@
         <f>IF(K116 &lt;&gt; "", VLOOKUP(K116, IF(J116="1", Ward!$A$2:$B$11, IF(J116="2", Ward!$C$2:$D$12, IF(J116="3", Ward!$E$2:$F$15, IF(J116="4", Ward!$G$2:$H$16, IF(J116="5", Ward!$I$2:$J$16, IF(J116="6", Ward!$K$2:$L$15, IF(J116="7", Ward!$M$2:$N$11, IF(J116="8", Ward!$O$2:$P$17, IF(J116="9", Ward!$Q$2:$R$14, IF(J116="10", Ward!$S$2:$T$16, IF(J116="11", Ward!$U$2:$V$17, IF(J116="12", Ward!$W$2:$X$12, IF(J116="Bình Chánh", Ward!$Y$2:$Z$17, IF(J116="Bình Tân", Ward!$AA$2:$AB$11, IF(J116="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J116="Cần Giờ", Ward!$AE$2:$AF$8, IF(J116="Củ Chi", Ward!$AG$2:$AH$22, IF(J116="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J116="Hóc Môn", Ward!$AK$2:$AL$13, IF(J116="Nhà Bè", Ward!$AM$2:$AN$8, IF(J116="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J116="Tân Bình", Ward!$AQ$2:$AR$16, IF(J116="Tân Phú", Ward!$AS$2:$AT$12, IF(J116="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X116" t="str">
+        <f>IF(B116 &lt;&gt; "", VLOOKUP(B116, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
       <c r="B117" s="16"/>
       <c r="C117" s="16"/>
@@ -6131,8 +6624,12 @@
         <f>IF(K117 &lt;&gt; "", VLOOKUP(K117, IF(J117="1", Ward!$A$2:$B$11, IF(J117="2", Ward!$C$2:$D$12, IF(J117="3", Ward!$E$2:$F$15, IF(J117="4", Ward!$G$2:$H$16, IF(J117="5", Ward!$I$2:$J$16, IF(J117="6", Ward!$K$2:$L$15, IF(J117="7", Ward!$M$2:$N$11, IF(J117="8", Ward!$O$2:$P$17, IF(J117="9", Ward!$Q$2:$R$14, IF(J117="10", Ward!$S$2:$T$16, IF(J117="11", Ward!$U$2:$V$17, IF(J117="12", Ward!$W$2:$X$12, IF(J117="Bình Chánh", Ward!$Y$2:$Z$17, IF(J117="Bình Tân", Ward!$AA$2:$AB$11, IF(J117="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J117="Cần Giờ", Ward!$AE$2:$AF$8, IF(J117="Củ Chi", Ward!$AG$2:$AH$22, IF(J117="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J117="Hóc Môn", Ward!$AK$2:$AL$13, IF(J117="Nhà Bè", Ward!$AM$2:$AN$8, IF(J117="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J117="Tân Bình", Ward!$AQ$2:$AR$16, IF(J117="Tân Phú", Ward!$AS$2:$AT$12, IF(J117="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X117" t="str">
+        <f>IF(B117 &lt;&gt; "", VLOOKUP(B117, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="16"/>
       <c r="C118" s="16"/>
@@ -6165,8 +6662,12 @@
         <f>IF(K118 &lt;&gt; "", VLOOKUP(K118, IF(J118="1", Ward!$A$2:$B$11, IF(J118="2", Ward!$C$2:$D$12, IF(J118="3", Ward!$E$2:$F$15, IF(J118="4", Ward!$G$2:$H$16, IF(J118="5", Ward!$I$2:$J$16, IF(J118="6", Ward!$K$2:$L$15, IF(J118="7", Ward!$M$2:$N$11, IF(J118="8", Ward!$O$2:$P$17, IF(J118="9", Ward!$Q$2:$R$14, IF(J118="10", Ward!$S$2:$T$16, IF(J118="11", Ward!$U$2:$V$17, IF(J118="12", Ward!$W$2:$X$12, IF(J118="Bình Chánh", Ward!$Y$2:$Z$17, IF(J118="Bình Tân", Ward!$AA$2:$AB$11, IF(J118="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J118="Cần Giờ", Ward!$AE$2:$AF$8, IF(J118="Củ Chi", Ward!$AG$2:$AH$22, IF(J118="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J118="Hóc Môn", Ward!$AK$2:$AL$13, IF(J118="Nhà Bè", Ward!$AM$2:$AN$8, IF(J118="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J118="Tân Bình", Ward!$AQ$2:$AR$16, IF(J118="Tân Phú", Ward!$AS$2:$AT$12, IF(J118="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X118" t="str">
+        <f>IF(B118 &lt;&gt; "", VLOOKUP(B118, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="16"/>
       <c r="C119" s="16"/>
@@ -6199,8 +6700,12 @@
         <f>IF(K119 &lt;&gt; "", VLOOKUP(K119, IF(J119="1", Ward!$A$2:$B$11, IF(J119="2", Ward!$C$2:$D$12, IF(J119="3", Ward!$E$2:$F$15, IF(J119="4", Ward!$G$2:$H$16, IF(J119="5", Ward!$I$2:$J$16, IF(J119="6", Ward!$K$2:$L$15, IF(J119="7", Ward!$M$2:$N$11, IF(J119="8", Ward!$O$2:$P$17, IF(J119="9", Ward!$Q$2:$R$14, IF(J119="10", Ward!$S$2:$T$16, IF(J119="11", Ward!$U$2:$V$17, IF(J119="12", Ward!$W$2:$X$12, IF(J119="Bình Chánh", Ward!$Y$2:$Z$17, IF(J119="Bình Tân", Ward!$AA$2:$AB$11, IF(J119="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J119="Cần Giờ", Ward!$AE$2:$AF$8, IF(J119="Củ Chi", Ward!$AG$2:$AH$22, IF(J119="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J119="Hóc Môn", Ward!$AK$2:$AL$13, IF(J119="Nhà Bè", Ward!$AM$2:$AN$8, IF(J119="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J119="Tân Bình", Ward!$AQ$2:$AR$16, IF(J119="Tân Phú", Ward!$AS$2:$AT$12, IF(J119="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X119" t="str">
+        <f>IF(B119 &lt;&gt; "", VLOOKUP(B119, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="16"/>
       <c r="C120" s="16"/>
@@ -6233,8 +6738,12 @@
         <f>IF(K120 &lt;&gt; "", VLOOKUP(K120, IF(J120="1", Ward!$A$2:$B$11, IF(J120="2", Ward!$C$2:$D$12, IF(J120="3", Ward!$E$2:$F$15, IF(J120="4", Ward!$G$2:$H$16, IF(J120="5", Ward!$I$2:$J$16, IF(J120="6", Ward!$K$2:$L$15, IF(J120="7", Ward!$M$2:$N$11, IF(J120="8", Ward!$O$2:$P$17, IF(J120="9", Ward!$Q$2:$R$14, IF(J120="10", Ward!$S$2:$T$16, IF(J120="11", Ward!$U$2:$V$17, IF(J120="12", Ward!$W$2:$X$12, IF(J120="Bình Chánh", Ward!$Y$2:$Z$17, IF(J120="Bình Tân", Ward!$AA$2:$AB$11, IF(J120="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J120="Cần Giờ", Ward!$AE$2:$AF$8, IF(J120="Củ Chi", Ward!$AG$2:$AH$22, IF(J120="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J120="Hóc Môn", Ward!$AK$2:$AL$13, IF(J120="Nhà Bè", Ward!$AM$2:$AN$8, IF(J120="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J120="Tân Bình", Ward!$AQ$2:$AR$16, IF(J120="Tân Phú", Ward!$AS$2:$AT$12, IF(J120="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X120" t="str">
+        <f>IF(B120 &lt;&gt; "", VLOOKUP(B120, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="16"/>
       <c r="C121" s="16"/>
@@ -6267,8 +6776,12 @@
         <f>IF(K121 &lt;&gt; "", VLOOKUP(K121, IF(J121="1", Ward!$A$2:$B$11, IF(J121="2", Ward!$C$2:$D$12, IF(J121="3", Ward!$E$2:$F$15, IF(J121="4", Ward!$G$2:$H$16, IF(J121="5", Ward!$I$2:$J$16, IF(J121="6", Ward!$K$2:$L$15, IF(J121="7", Ward!$M$2:$N$11, IF(J121="8", Ward!$O$2:$P$17, IF(J121="9", Ward!$Q$2:$R$14, IF(J121="10", Ward!$S$2:$T$16, IF(J121="11", Ward!$U$2:$V$17, IF(J121="12", Ward!$W$2:$X$12, IF(J121="Bình Chánh", Ward!$Y$2:$Z$17, IF(J121="Bình Tân", Ward!$AA$2:$AB$11, IF(J121="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J121="Cần Giờ", Ward!$AE$2:$AF$8, IF(J121="Củ Chi", Ward!$AG$2:$AH$22, IF(J121="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J121="Hóc Môn", Ward!$AK$2:$AL$13, IF(J121="Nhà Bè", Ward!$AM$2:$AN$8, IF(J121="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J121="Tân Bình", Ward!$AQ$2:$AR$16, IF(J121="Tân Phú", Ward!$AS$2:$AT$12, IF(J121="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X121" t="str">
+        <f>IF(B121 &lt;&gt; "", VLOOKUP(B121, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="16"/>
       <c r="C122" s="16"/>
@@ -6301,8 +6814,12 @@
         <f>IF(K122 &lt;&gt; "", VLOOKUP(K122, IF(J122="1", Ward!$A$2:$B$11, IF(J122="2", Ward!$C$2:$D$12, IF(J122="3", Ward!$E$2:$F$15, IF(J122="4", Ward!$G$2:$H$16, IF(J122="5", Ward!$I$2:$J$16, IF(J122="6", Ward!$K$2:$L$15, IF(J122="7", Ward!$M$2:$N$11, IF(J122="8", Ward!$O$2:$P$17, IF(J122="9", Ward!$Q$2:$R$14, IF(J122="10", Ward!$S$2:$T$16, IF(J122="11", Ward!$U$2:$V$17, IF(J122="12", Ward!$W$2:$X$12, IF(J122="Bình Chánh", Ward!$Y$2:$Z$17, IF(J122="Bình Tân", Ward!$AA$2:$AB$11, IF(J122="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J122="Cần Giờ", Ward!$AE$2:$AF$8, IF(J122="Củ Chi", Ward!$AG$2:$AH$22, IF(J122="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J122="Hóc Môn", Ward!$AK$2:$AL$13, IF(J122="Nhà Bè", Ward!$AM$2:$AN$8, IF(J122="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J122="Tân Bình", Ward!$AQ$2:$AR$16, IF(J122="Tân Phú", Ward!$AS$2:$AT$12, IF(J122="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X122" t="str">
+        <f>IF(B122 &lt;&gt; "", VLOOKUP(B122, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="16"/>
       <c r="C123" s="16"/>
@@ -6335,8 +6852,12 @@
         <f>IF(K123 &lt;&gt; "", VLOOKUP(K123, IF(J123="1", Ward!$A$2:$B$11, IF(J123="2", Ward!$C$2:$D$12, IF(J123="3", Ward!$E$2:$F$15, IF(J123="4", Ward!$G$2:$H$16, IF(J123="5", Ward!$I$2:$J$16, IF(J123="6", Ward!$K$2:$L$15, IF(J123="7", Ward!$M$2:$N$11, IF(J123="8", Ward!$O$2:$P$17, IF(J123="9", Ward!$Q$2:$R$14, IF(J123="10", Ward!$S$2:$T$16, IF(J123="11", Ward!$U$2:$V$17, IF(J123="12", Ward!$W$2:$X$12, IF(J123="Bình Chánh", Ward!$Y$2:$Z$17, IF(J123="Bình Tân", Ward!$AA$2:$AB$11, IF(J123="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J123="Cần Giờ", Ward!$AE$2:$AF$8, IF(J123="Củ Chi", Ward!$AG$2:$AH$22, IF(J123="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J123="Hóc Môn", Ward!$AK$2:$AL$13, IF(J123="Nhà Bè", Ward!$AM$2:$AN$8, IF(J123="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J123="Tân Bình", Ward!$AQ$2:$AR$16, IF(J123="Tân Phú", Ward!$AS$2:$AT$12, IF(J123="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X123" t="str">
+        <f>IF(B123 &lt;&gt; "", VLOOKUP(B123, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="16"/>
       <c r="C124" s="16"/>
@@ -6369,8 +6890,12 @@
         <f>IF(K124 &lt;&gt; "", VLOOKUP(K124, IF(J124="1", Ward!$A$2:$B$11, IF(J124="2", Ward!$C$2:$D$12, IF(J124="3", Ward!$E$2:$F$15, IF(J124="4", Ward!$G$2:$H$16, IF(J124="5", Ward!$I$2:$J$16, IF(J124="6", Ward!$K$2:$L$15, IF(J124="7", Ward!$M$2:$N$11, IF(J124="8", Ward!$O$2:$P$17, IF(J124="9", Ward!$Q$2:$R$14, IF(J124="10", Ward!$S$2:$T$16, IF(J124="11", Ward!$U$2:$V$17, IF(J124="12", Ward!$W$2:$X$12, IF(J124="Bình Chánh", Ward!$Y$2:$Z$17, IF(J124="Bình Tân", Ward!$AA$2:$AB$11, IF(J124="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J124="Cần Giờ", Ward!$AE$2:$AF$8, IF(J124="Củ Chi", Ward!$AG$2:$AH$22, IF(J124="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J124="Hóc Môn", Ward!$AK$2:$AL$13, IF(J124="Nhà Bè", Ward!$AM$2:$AN$8, IF(J124="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J124="Tân Bình", Ward!$AQ$2:$AR$16, IF(J124="Tân Phú", Ward!$AS$2:$AT$12, IF(J124="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X124" t="str">
+        <f>IF(B124 &lt;&gt; "", VLOOKUP(B124, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="16"/>
       <c r="C125" s="16"/>
@@ -6403,8 +6928,12 @@
         <f>IF(K125 &lt;&gt; "", VLOOKUP(K125, IF(J125="1", Ward!$A$2:$B$11, IF(J125="2", Ward!$C$2:$D$12, IF(J125="3", Ward!$E$2:$F$15, IF(J125="4", Ward!$G$2:$H$16, IF(J125="5", Ward!$I$2:$J$16, IF(J125="6", Ward!$K$2:$L$15, IF(J125="7", Ward!$M$2:$N$11, IF(J125="8", Ward!$O$2:$P$17, IF(J125="9", Ward!$Q$2:$R$14, IF(J125="10", Ward!$S$2:$T$16, IF(J125="11", Ward!$U$2:$V$17, IF(J125="12", Ward!$W$2:$X$12, IF(J125="Bình Chánh", Ward!$Y$2:$Z$17, IF(J125="Bình Tân", Ward!$AA$2:$AB$11, IF(J125="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J125="Cần Giờ", Ward!$AE$2:$AF$8, IF(J125="Củ Chi", Ward!$AG$2:$AH$22, IF(J125="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J125="Hóc Môn", Ward!$AK$2:$AL$13, IF(J125="Nhà Bè", Ward!$AM$2:$AN$8, IF(J125="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J125="Tân Bình", Ward!$AQ$2:$AR$16, IF(J125="Tân Phú", Ward!$AS$2:$AT$12, IF(J125="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X125" t="str">
+        <f>IF(B125 &lt;&gt; "", VLOOKUP(B125, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="126" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="16"/>
       <c r="C126" s="16"/>
@@ -6437,8 +6966,12 @@
         <f>IF(K126 &lt;&gt; "", VLOOKUP(K126, IF(J126="1", Ward!$A$2:$B$11, IF(J126="2", Ward!$C$2:$D$12, IF(J126="3", Ward!$E$2:$F$15, IF(J126="4", Ward!$G$2:$H$16, IF(J126="5", Ward!$I$2:$J$16, IF(J126="6", Ward!$K$2:$L$15, IF(J126="7", Ward!$M$2:$N$11, IF(J126="8", Ward!$O$2:$P$17, IF(J126="9", Ward!$Q$2:$R$14, IF(J126="10", Ward!$S$2:$T$16, IF(J126="11", Ward!$U$2:$V$17, IF(J126="12", Ward!$W$2:$X$12, IF(J126="Bình Chánh", Ward!$Y$2:$Z$17, IF(J126="Bình Tân", Ward!$AA$2:$AB$11, IF(J126="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J126="Cần Giờ", Ward!$AE$2:$AF$8, IF(J126="Củ Chi", Ward!$AG$2:$AH$22, IF(J126="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J126="Hóc Môn", Ward!$AK$2:$AL$13, IF(J126="Nhà Bè", Ward!$AM$2:$AN$8, IF(J126="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J126="Tân Bình", Ward!$AQ$2:$AR$16, IF(J126="Tân Phú", Ward!$AS$2:$AT$12, IF(J126="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X126" t="str">
+        <f>IF(B126 &lt;&gt; "", VLOOKUP(B126, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="127" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="16"/>
       <c r="C127" s="16"/>
@@ -6471,8 +7004,12 @@
         <f>IF(K127 &lt;&gt; "", VLOOKUP(K127, IF(J127="1", Ward!$A$2:$B$11, IF(J127="2", Ward!$C$2:$D$12, IF(J127="3", Ward!$E$2:$F$15, IF(J127="4", Ward!$G$2:$H$16, IF(J127="5", Ward!$I$2:$J$16, IF(J127="6", Ward!$K$2:$L$15, IF(J127="7", Ward!$M$2:$N$11, IF(J127="8", Ward!$O$2:$P$17, IF(J127="9", Ward!$Q$2:$R$14, IF(J127="10", Ward!$S$2:$T$16, IF(J127="11", Ward!$U$2:$V$17, IF(J127="12", Ward!$W$2:$X$12, IF(J127="Bình Chánh", Ward!$Y$2:$Z$17, IF(J127="Bình Tân", Ward!$AA$2:$AB$11, IF(J127="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J127="Cần Giờ", Ward!$AE$2:$AF$8, IF(J127="Củ Chi", Ward!$AG$2:$AH$22, IF(J127="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J127="Hóc Môn", Ward!$AK$2:$AL$13, IF(J127="Nhà Bè", Ward!$AM$2:$AN$8, IF(J127="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J127="Tân Bình", Ward!$AQ$2:$AR$16, IF(J127="Tân Phú", Ward!$AS$2:$AT$12, IF(J127="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X127" t="str">
+        <f>IF(B127 &lt;&gt; "", VLOOKUP(B127, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="16"/>
       <c r="C128" s="16"/>
@@ -6505,8 +7042,12 @@
         <f>IF(K128 &lt;&gt; "", VLOOKUP(K128, IF(J128="1", Ward!$A$2:$B$11, IF(J128="2", Ward!$C$2:$D$12, IF(J128="3", Ward!$E$2:$F$15, IF(J128="4", Ward!$G$2:$H$16, IF(J128="5", Ward!$I$2:$J$16, IF(J128="6", Ward!$K$2:$L$15, IF(J128="7", Ward!$M$2:$N$11, IF(J128="8", Ward!$O$2:$P$17, IF(J128="9", Ward!$Q$2:$R$14, IF(J128="10", Ward!$S$2:$T$16, IF(J128="11", Ward!$U$2:$V$17, IF(J128="12", Ward!$W$2:$X$12, IF(J128="Bình Chánh", Ward!$Y$2:$Z$17, IF(J128="Bình Tân", Ward!$AA$2:$AB$11, IF(J128="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J128="Cần Giờ", Ward!$AE$2:$AF$8, IF(J128="Củ Chi", Ward!$AG$2:$AH$22, IF(J128="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J128="Hóc Môn", Ward!$AK$2:$AL$13, IF(J128="Nhà Bè", Ward!$AM$2:$AN$8, IF(J128="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J128="Tân Bình", Ward!$AQ$2:$AR$16, IF(J128="Tân Phú", Ward!$AS$2:$AT$12, IF(J128="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X128" t="str">
+        <f>IF(B128 &lt;&gt; "", VLOOKUP(B128, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="129" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="16"/>
       <c r="C129" s="16"/>
@@ -6539,8 +7080,12 @@
         <f>IF(K129 &lt;&gt; "", VLOOKUP(K129, IF(J129="1", Ward!$A$2:$B$11, IF(J129="2", Ward!$C$2:$D$12, IF(J129="3", Ward!$E$2:$F$15, IF(J129="4", Ward!$G$2:$H$16, IF(J129="5", Ward!$I$2:$J$16, IF(J129="6", Ward!$K$2:$L$15, IF(J129="7", Ward!$M$2:$N$11, IF(J129="8", Ward!$O$2:$P$17, IF(J129="9", Ward!$Q$2:$R$14, IF(J129="10", Ward!$S$2:$T$16, IF(J129="11", Ward!$U$2:$V$17, IF(J129="12", Ward!$W$2:$X$12, IF(J129="Bình Chánh", Ward!$Y$2:$Z$17, IF(J129="Bình Tân", Ward!$AA$2:$AB$11, IF(J129="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J129="Cần Giờ", Ward!$AE$2:$AF$8, IF(J129="Củ Chi", Ward!$AG$2:$AH$22, IF(J129="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J129="Hóc Môn", Ward!$AK$2:$AL$13, IF(J129="Nhà Bè", Ward!$AM$2:$AN$8, IF(J129="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J129="Tân Bình", Ward!$AQ$2:$AR$16, IF(J129="Tân Phú", Ward!$AS$2:$AT$12, IF(J129="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X129" t="str">
+        <f>IF(B129 &lt;&gt; "", VLOOKUP(B129, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="16"/>
       <c r="C130" s="16"/>
@@ -6573,8 +7118,12 @@
         <f>IF(K130 &lt;&gt; "", VLOOKUP(K130, IF(J130="1", Ward!$A$2:$B$11, IF(J130="2", Ward!$C$2:$D$12, IF(J130="3", Ward!$E$2:$F$15, IF(J130="4", Ward!$G$2:$H$16, IF(J130="5", Ward!$I$2:$J$16, IF(J130="6", Ward!$K$2:$L$15, IF(J130="7", Ward!$M$2:$N$11, IF(J130="8", Ward!$O$2:$P$17, IF(J130="9", Ward!$Q$2:$R$14, IF(J130="10", Ward!$S$2:$T$16, IF(J130="11", Ward!$U$2:$V$17, IF(J130="12", Ward!$W$2:$X$12, IF(J130="Bình Chánh", Ward!$Y$2:$Z$17, IF(J130="Bình Tân", Ward!$AA$2:$AB$11, IF(J130="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J130="Cần Giờ", Ward!$AE$2:$AF$8, IF(J130="Củ Chi", Ward!$AG$2:$AH$22, IF(J130="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J130="Hóc Môn", Ward!$AK$2:$AL$13, IF(J130="Nhà Bè", Ward!$AM$2:$AN$8, IF(J130="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J130="Tân Bình", Ward!$AQ$2:$AR$16, IF(J130="Tân Phú", Ward!$AS$2:$AT$12, IF(J130="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X130" t="str">
+        <f>IF(B130 &lt;&gt; "", VLOOKUP(B130, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="131" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="16"/>
       <c r="C131" s="16"/>
@@ -6607,8 +7156,12 @@
         <f>IF(K131 &lt;&gt; "", VLOOKUP(K131, IF(J131="1", Ward!$A$2:$B$11, IF(J131="2", Ward!$C$2:$D$12, IF(J131="3", Ward!$E$2:$F$15, IF(J131="4", Ward!$G$2:$H$16, IF(J131="5", Ward!$I$2:$J$16, IF(J131="6", Ward!$K$2:$L$15, IF(J131="7", Ward!$M$2:$N$11, IF(J131="8", Ward!$O$2:$P$17, IF(J131="9", Ward!$Q$2:$R$14, IF(J131="10", Ward!$S$2:$T$16, IF(J131="11", Ward!$U$2:$V$17, IF(J131="12", Ward!$W$2:$X$12, IF(J131="Bình Chánh", Ward!$Y$2:$Z$17, IF(J131="Bình Tân", Ward!$AA$2:$AB$11, IF(J131="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J131="Cần Giờ", Ward!$AE$2:$AF$8, IF(J131="Củ Chi", Ward!$AG$2:$AH$22, IF(J131="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J131="Hóc Môn", Ward!$AK$2:$AL$13, IF(J131="Nhà Bè", Ward!$AM$2:$AN$8, IF(J131="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J131="Tân Bình", Ward!$AQ$2:$AR$16, IF(J131="Tân Phú", Ward!$AS$2:$AT$12, IF(J131="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X131" t="str">
+        <f>IF(B131 &lt;&gt; "", VLOOKUP(B131, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="132" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="16"/>
       <c r="C132" s="16"/>
@@ -6641,8 +7194,12 @@
         <f>IF(K132 &lt;&gt; "", VLOOKUP(K132, IF(J132="1", Ward!$A$2:$B$11, IF(J132="2", Ward!$C$2:$D$12, IF(J132="3", Ward!$E$2:$F$15, IF(J132="4", Ward!$G$2:$H$16, IF(J132="5", Ward!$I$2:$J$16, IF(J132="6", Ward!$K$2:$L$15, IF(J132="7", Ward!$M$2:$N$11, IF(J132="8", Ward!$O$2:$P$17, IF(J132="9", Ward!$Q$2:$R$14, IF(J132="10", Ward!$S$2:$T$16, IF(J132="11", Ward!$U$2:$V$17, IF(J132="12", Ward!$W$2:$X$12, IF(J132="Bình Chánh", Ward!$Y$2:$Z$17, IF(J132="Bình Tân", Ward!$AA$2:$AB$11, IF(J132="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J132="Cần Giờ", Ward!$AE$2:$AF$8, IF(J132="Củ Chi", Ward!$AG$2:$AH$22, IF(J132="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J132="Hóc Môn", Ward!$AK$2:$AL$13, IF(J132="Nhà Bè", Ward!$AM$2:$AN$8, IF(J132="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J132="Tân Bình", Ward!$AQ$2:$AR$16, IF(J132="Tân Phú", Ward!$AS$2:$AT$12, IF(J132="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X132" t="str">
+        <f>IF(B132 &lt;&gt; "", VLOOKUP(B132, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="133" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="16"/>
       <c r="C133" s="16"/>
@@ -6675,8 +7232,12 @@
         <f>IF(K133 &lt;&gt; "", VLOOKUP(K133, IF(J133="1", Ward!$A$2:$B$11, IF(J133="2", Ward!$C$2:$D$12, IF(J133="3", Ward!$E$2:$F$15, IF(J133="4", Ward!$G$2:$H$16, IF(J133="5", Ward!$I$2:$J$16, IF(J133="6", Ward!$K$2:$L$15, IF(J133="7", Ward!$M$2:$N$11, IF(J133="8", Ward!$O$2:$P$17, IF(J133="9", Ward!$Q$2:$R$14, IF(J133="10", Ward!$S$2:$T$16, IF(J133="11", Ward!$U$2:$V$17, IF(J133="12", Ward!$W$2:$X$12, IF(J133="Bình Chánh", Ward!$Y$2:$Z$17, IF(J133="Bình Tân", Ward!$AA$2:$AB$11, IF(J133="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J133="Cần Giờ", Ward!$AE$2:$AF$8, IF(J133="Củ Chi", Ward!$AG$2:$AH$22, IF(J133="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J133="Hóc Môn", Ward!$AK$2:$AL$13, IF(J133="Nhà Bè", Ward!$AM$2:$AN$8, IF(J133="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J133="Tân Bình", Ward!$AQ$2:$AR$16, IF(J133="Tân Phú", Ward!$AS$2:$AT$12, IF(J133="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X133" t="str">
+        <f>IF(B133 &lt;&gt; "", VLOOKUP(B133, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="134" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="16"/>
       <c r="C134" s="16"/>
@@ -6709,8 +7270,12 @@
         <f>IF(K134 &lt;&gt; "", VLOOKUP(K134, IF(J134="1", Ward!$A$2:$B$11, IF(J134="2", Ward!$C$2:$D$12, IF(J134="3", Ward!$E$2:$F$15, IF(J134="4", Ward!$G$2:$H$16, IF(J134="5", Ward!$I$2:$J$16, IF(J134="6", Ward!$K$2:$L$15, IF(J134="7", Ward!$M$2:$N$11, IF(J134="8", Ward!$O$2:$P$17, IF(J134="9", Ward!$Q$2:$R$14, IF(J134="10", Ward!$S$2:$T$16, IF(J134="11", Ward!$U$2:$V$17, IF(J134="12", Ward!$W$2:$X$12, IF(J134="Bình Chánh", Ward!$Y$2:$Z$17, IF(J134="Bình Tân", Ward!$AA$2:$AB$11, IF(J134="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J134="Cần Giờ", Ward!$AE$2:$AF$8, IF(J134="Củ Chi", Ward!$AG$2:$AH$22, IF(J134="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J134="Hóc Môn", Ward!$AK$2:$AL$13, IF(J134="Nhà Bè", Ward!$AM$2:$AN$8, IF(J134="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J134="Tân Bình", Ward!$AQ$2:$AR$16, IF(J134="Tân Phú", Ward!$AS$2:$AT$12, IF(J134="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X134" t="str">
+        <f>IF(B134 &lt;&gt; "", VLOOKUP(B134, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="135" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="16"/>
       <c r="C135" s="16"/>
@@ -6743,8 +7308,12 @@
         <f>IF(K135 &lt;&gt; "", VLOOKUP(K135, IF(J135="1", Ward!$A$2:$B$11, IF(J135="2", Ward!$C$2:$D$12, IF(J135="3", Ward!$E$2:$F$15, IF(J135="4", Ward!$G$2:$H$16, IF(J135="5", Ward!$I$2:$J$16, IF(J135="6", Ward!$K$2:$L$15, IF(J135="7", Ward!$M$2:$N$11, IF(J135="8", Ward!$O$2:$P$17, IF(J135="9", Ward!$Q$2:$R$14, IF(J135="10", Ward!$S$2:$T$16, IF(J135="11", Ward!$U$2:$V$17, IF(J135="12", Ward!$W$2:$X$12, IF(J135="Bình Chánh", Ward!$Y$2:$Z$17, IF(J135="Bình Tân", Ward!$AA$2:$AB$11, IF(J135="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J135="Cần Giờ", Ward!$AE$2:$AF$8, IF(J135="Củ Chi", Ward!$AG$2:$AH$22, IF(J135="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J135="Hóc Môn", Ward!$AK$2:$AL$13, IF(J135="Nhà Bè", Ward!$AM$2:$AN$8, IF(J135="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J135="Tân Bình", Ward!$AQ$2:$AR$16, IF(J135="Tân Phú", Ward!$AS$2:$AT$12, IF(J135="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X135" t="str">
+        <f>IF(B135 &lt;&gt; "", VLOOKUP(B135, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="136" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="16"/>
       <c r="C136" s="16"/>
@@ -6777,8 +7346,12 @@
         <f>IF(K136 &lt;&gt; "", VLOOKUP(K136, IF(J136="1", Ward!$A$2:$B$11, IF(J136="2", Ward!$C$2:$D$12, IF(J136="3", Ward!$E$2:$F$15, IF(J136="4", Ward!$G$2:$H$16, IF(J136="5", Ward!$I$2:$J$16, IF(J136="6", Ward!$K$2:$L$15, IF(J136="7", Ward!$M$2:$N$11, IF(J136="8", Ward!$O$2:$P$17, IF(J136="9", Ward!$Q$2:$R$14, IF(J136="10", Ward!$S$2:$T$16, IF(J136="11", Ward!$U$2:$V$17, IF(J136="12", Ward!$W$2:$X$12, IF(J136="Bình Chánh", Ward!$Y$2:$Z$17, IF(J136="Bình Tân", Ward!$AA$2:$AB$11, IF(J136="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J136="Cần Giờ", Ward!$AE$2:$AF$8, IF(J136="Củ Chi", Ward!$AG$2:$AH$22, IF(J136="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J136="Hóc Môn", Ward!$AK$2:$AL$13, IF(J136="Nhà Bè", Ward!$AM$2:$AN$8, IF(J136="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J136="Tân Bình", Ward!$AQ$2:$AR$16, IF(J136="Tân Phú", Ward!$AS$2:$AT$12, IF(J136="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X136" t="str">
+        <f>IF(B136 &lt;&gt; "", VLOOKUP(B136, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="137" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="16"/>
       <c r="C137" s="16"/>
@@ -6811,8 +7384,12 @@
         <f>IF(K137 &lt;&gt; "", VLOOKUP(K137, IF(J137="1", Ward!$A$2:$B$11, IF(J137="2", Ward!$C$2:$D$12, IF(J137="3", Ward!$E$2:$F$15, IF(J137="4", Ward!$G$2:$H$16, IF(J137="5", Ward!$I$2:$J$16, IF(J137="6", Ward!$K$2:$L$15, IF(J137="7", Ward!$M$2:$N$11, IF(J137="8", Ward!$O$2:$P$17, IF(J137="9", Ward!$Q$2:$R$14, IF(J137="10", Ward!$S$2:$T$16, IF(J137="11", Ward!$U$2:$V$17, IF(J137="12", Ward!$W$2:$X$12, IF(J137="Bình Chánh", Ward!$Y$2:$Z$17, IF(J137="Bình Tân", Ward!$AA$2:$AB$11, IF(J137="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J137="Cần Giờ", Ward!$AE$2:$AF$8, IF(J137="Củ Chi", Ward!$AG$2:$AH$22, IF(J137="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J137="Hóc Môn", Ward!$AK$2:$AL$13, IF(J137="Nhà Bè", Ward!$AM$2:$AN$8, IF(J137="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J137="Tân Bình", Ward!$AQ$2:$AR$16, IF(J137="Tân Phú", Ward!$AS$2:$AT$12, IF(J137="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X137" t="str">
+        <f>IF(B137 &lt;&gt; "", VLOOKUP(B137, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="138" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="B138" s="16"/>
       <c r="C138" s="16"/>
@@ -6845,8 +7422,12 @@
         <f>IF(K138 &lt;&gt; "", VLOOKUP(K138, IF(J138="1", Ward!$A$2:$B$11, IF(J138="2", Ward!$C$2:$D$12, IF(J138="3", Ward!$E$2:$F$15, IF(J138="4", Ward!$G$2:$H$16, IF(J138="5", Ward!$I$2:$J$16, IF(J138="6", Ward!$K$2:$L$15, IF(J138="7", Ward!$M$2:$N$11, IF(J138="8", Ward!$O$2:$P$17, IF(J138="9", Ward!$Q$2:$R$14, IF(J138="10", Ward!$S$2:$T$16, IF(J138="11", Ward!$U$2:$V$17, IF(J138="12", Ward!$W$2:$X$12, IF(J138="Bình Chánh", Ward!$Y$2:$Z$17, IF(J138="Bình Tân", Ward!$AA$2:$AB$11, IF(J138="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J138="Cần Giờ", Ward!$AE$2:$AF$8, IF(J138="Củ Chi", Ward!$AG$2:$AH$22, IF(J138="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J138="Hóc Môn", Ward!$AK$2:$AL$13, IF(J138="Nhà Bè", Ward!$AM$2:$AN$8, IF(J138="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J138="Tân Bình", Ward!$AQ$2:$AR$16, IF(J138="Tân Phú", Ward!$AS$2:$AT$12, IF(J138="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X138" t="str">
+        <f>IF(B138 &lt;&gt; "", VLOOKUP(B138, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="139" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="16"/>
       <c r="C139" s="16"/>
@@ -6879,8 +7460,12 @@
         <f>IF(K139 &lt;&gt; "", VLOOKUP(K139, IF(J139="1", Ward!$A$2:$B$11, IF(J139="2", Ward!$C$2:$D$12, IF(J139="3", Ward!$E$2:$F$15, IF(J139="4", Ward!$G$2:$H$16, IF(J139="5", Ward!$I$2:$J$16, IF(J139="6", Ward!$K$2:$L$15, IF(J139="7", Ward!$M$2:$N$11, IF(J139="8", Ward!$O$2:$P$17, IF(J139="9", Ward!$Q$2:$R$14, IF(J139="10", Ward!$S$2:$T$16, IF(J139="11", Ward!$U$2:$V$17, IF(J139="12", Ward!$W$2:$X$12, IF(J139="Bình Chánh", Ward!$Y$2:$Z$17, IF(J139="Bình Tân", Ward!$AA$2:$AB$11, IF(J139="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J139="Cần Giờ", Ward!$AE$2:$AF$8, IF(J139="Củ Chi", Ward!$AG$2:$AH$22, IF(J139="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J139="Hóc Môn", Ward!$AK$2:$AL$13, IF(J139="Nhà Bè", Ward!$AM$2:$AN$8, IF(J139="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J139="Tân Bình", Ward!$AQ$2:$AR$16, IF(J139="Tân Phú", Ward!$AS$2:$AT$12, IF(J139="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X139" t="str">
+        <f>IF(B139 &lt;&gt; "", VLOOKUP(B139, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="140" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="16"/>
       <c r="C140" s="16"/>
@@ -6913,8 +7498,12 @@
         <f>IF(K140 &lt;&gt; "", VLOOKUP(K140, IF(J140="1", Ward!$A$2:$B$11, IF(J140="2", Ward!$C$2:$D$12, IF(J140="3", Ward!$E$2:$F$15, IF(J140="4", Ward!$G$2:$H$16, IF(J140="5", Ward!$I$2:$J$16, IF(J140="6", Ward!$K$2:$L$15, IF(J140="7", Ward!$M$2:$N$11, IF(J140="8", Ward!$O$2:$P$17, IF(J140="9", Ward!$Q$2:$R$14, IF(J140="10", Ward!$S$2:$T$16, IF(J140="11", Ward!$U$2:$V$17, IF(J140="12", Ward!$W$2:$X$12, IF(J140="Bình Chánh", Ward!$Y$2:$Z$17, IF(J140="Bình Tân", Ward!$AA$2:$AB$11, IF(J140="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J140="Cần Giờ", Ward!$AE$2:$AF$8, IF(J140="Củ Chi", Ward!$AG$2:$AH$22, IF(J140="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J140="Hóc Môn", Ward!$AK$2:$AL$13, IF(J140="Nhà Bè", Ward!$AM$2:$AN$8, IF(J140="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J140="Tân Bình", Ward!$AQ$2:$AR$16, IF(J140="Tân Phú", Ward!$AS$2:$AT$12, IF(J140="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X140" t="str">
+        <f>IF(B140 &lt;&gt; "", VLOOKUP(B140, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="141" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
       <c r="B141" s="16"/>
       <c r="C141" s="16"/>
@@ -6947,8 +7536,12 @@
         <f>IF(K141 &lt;&gt; "", VLOOKUP(K141, IF(J141="1", Ward!$A$2:$B$11, IF(J141="2", Ward!$C$2:$D$12, IF(J141="3", Ward!$E$2:$F$15, IF(J141="4", Ward!$G$2:$H$16, IF(J141="5", Ward!$I$2:$J$16, IF(J141="6", Ward!$K$2:$L$15, IF(J141="7", Ward!$M$2:$N$11, IF(J141="8", Ward!$O$2:$P$17, IF(J141="9", Ward!$Q$2:$R$14, IF(J141="10", Ward!$S$2:$T$16, IF(J141="11", Ward!$U$2:$V$17, IF(J141="12", Ward!$W$2:$X$12, IF(J141="Bình Chánh", Ward!$Y$2:$Z$17, IF(J141="Bình Tân", Ward!$AA$2:$AB$11, IF(J141="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J141="Cần Giờ", Ward!$AE$2:$AF$8, IF(J141="Củ Chi", Ward!$AG$2:$AH$22, IF(J141="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J141="Hóc Môn", Ward!$AK$2:$AL$13, IF(J141="Nhà Bè", Ward!$AM$2:$AN$8, IF(J141="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J141="Tân Bình", Ward!$AQ$2:$AR$16, IF(J141="Tân Phú", Ward!$AS$2:$AT$12, IF(J141="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X141" t="str">
+        <f>IF(B141 &lt;&gt; "", VLOOKUP(B141, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="142" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
       <c r="B142" s="16"/>
       <c r="C142" s="16"/>
@@ -6981,8 +7574,12 @@
         <f>IF(K142 &lt;&gt; "", VLOOKUP(K142, IF(J142="1", Ward!$A$2:$B$11, IF(J142="2", Ward!$C$2:$D$12, IF(J142="3", Ward!$E$2:$F$15, IF(J142="4", Ward!$G$2:$H$16, IF(J142="5", Ward!$I$2:$J$16, IF(J142="6", Ward!$K$2:$L$15, IF(J142="7", Ward!$M$2:$N$11, IF(J142="8", Ward!$O$2:$P$17, IF(J142="9", Ward!$Q$2:$R$14, IF(J142="10", Ward!$S$2:$T$16, IF(J142="11", Ward!$U$2:$V$17, IF(J142="12", Ward!$W$2:$X$12, IF(J142="Bình Chánh", Ward!$Y$2:$Z$17, IF(J142="Bình Tân", Ward!$AA$2:$AB$11, IF(J142="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J142="Cần Giờ", Ward!$AE$2:$AF$8, IF(J142="Củ Chi", Ward!$AG$2:$AH$22, IF(J142="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J142="Hóc Môn", Ward!$AK$2:$AL$13, IF(J142="Nhà Bè", Ward!$AM$2:$AN$8, IF(J142="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J142="Tân Bình", Ward!$AQ$2:$AR$16, IF(J142="Tân Phú", Ward!$AS$2:$AT$12, IF(J142="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X142" t="str">
+        <f>IF(B142 &lt;&gt; "", VLOOKUP(B142, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="143" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
       <c r="B143" s="16"/>
       <c r="C143" s="16"/>
@@ -7015,8 +7612,12 @@
         <f>IF(K143 &lt;&gt; "", VLOOKUP(K143, IF(J143="1", Ward!$A$2:$B$11, IF(J143="2", Ward!$C$2:$D$12, IF(J143="3", Ward!$E$2:$F$15, IF(J143="4", Ward!$G$2:$H$16, IF(J143="5", Ward!$I$2:$J$16, IF(J143="6", Ward!$K$2:$L$15, IF(J143="7", Ward!$M$2:$N$11, IF(J143="8", Ward!$O$2:$P$17, IF(J143="9", Ward!$Q$2:$R$14, IF(J143="10", Ward!$S$2:$T$16, IF(J143="11", Ward!$U$2:$V$17, IF(J143="12", Ward!$W$2:$X$12, IF(J143="Bình Chánh", Ward!$Y$2:$Z$17, IF(J143="Bình Tân", Ward!$AA$2:$AB$11, IF(J143="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J143="Cần Giờ", Ward!$AE$2:$AF$8, IF(J143="Củ Chi", Ward!$AG$2:$AH$22, IF(J143="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J143="Hóc Môn", Ward!$AK$2:$AL$13, IF(J143="Nhà Bè", Ward!$AM$2:$AN$8, IF(J143="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J143="Tân Bình", Ward!$AQ$2:$AR$16, IF(J143="Tân Phú", Ward!$AS$2:$AT$12, IF(J143="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X143" t="str">
+        <f>IF(B143 &lt;&gt; "", VLOOKUP(B143, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="144" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
       <c r="B144" s="16"/>
       <c r="C144" s="16"/>
@@ -7049,8 +7650,12 @@
         <f>IF(K144 &lt;&gt; "", VLOOKUP(K144, IF(J144="1", Ward!$A$2:$B$11, IF(J144="2", Ward!$C$2:$D$12, IF(J144="3", Ward!$E$2:$F$15, IF(J144="4", Ward!$G$2:$H$16, IF(J144="5", Ward!$I$2:$J$16, IF(J144="6", Ward!$K$2:$L$15, IF(J144="7", Ward!$M$2:$N$11, IF(J144="8", Ward!$O$2:$P$17, IF(J144="9", Ward!$Q$2:$R$14, IF(J144="10", Ward!$S$2:$T$16, IF(J144="11", Ward!$U$2:$V$17, IF(J144="12", Ward!$W$2:$X$12, IF(J144="Bình Chánh", Ward!$Y$2:$Z$17, IF(J144="Bình Tân", Ward!$AA$2:$AB$11, IF(J144="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J144="Cần Giờ", Ward!$AE$2:$AF$8, IF(J144="Củ Chi", Ward!$AG$2:$AH$22, IF(J144="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J144="Hóc Môn", Ward!$AK$2:$AL$13, IF(J144="Nhà Bè", Ward!$AM$2:$AN$8, IF(J144="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J144="Tân Bình", Ward!$AQ$2:$AR$16, IF(J144="Tân Phú", Ward!$AS$2:$AT$12, IF(J144="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X144" t="str">
+        <f>IF(B144 &lt;&gt; "", VLOOKUP(B144, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="145" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A145" s="3"/>
       <c r="B145" s="16"/>
       <c r="C145" s="16"/>
@@ -7083,8 +7688,12 @@
         <f>IF(K145 &lt;&gt; "", VLOOKUP(K145, IF(J145="1", Ward!$A$2:$B$11, IF(J145="2", Ward!$C$2:$D$12, IF(J145="3", Ward!$E$2:$F$15, IF(J145="4", Ward!$G$2:$H$16, IF(J145="5", Ward!$I$2:$J$16, IF(J145="6", Ward!$K$2:$L$15, IF(J145="7", Ward!$M$2:$N$11, IF(J145="8", Ward!$O$2:$P$17, IF(J145="9", Ward!$Q$2:$R$14, IF(J145="10", Ward!$S$2:$T$16, IF(J145="11", Ward!$U$2:$V$17, IF(J145="12", Ward!$W$2:$X$12, IF(J145="Bình Chánh", Ward!$Y$2:$Z$17, IF(J145="Bình Tân", Ward!$AA$2:$AB$11, IF(J145="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J145="Cần Giờ", Ward!$AE$2:$AF$8, IF(J145="Củ Chi", Ward!$AG$2:$AH$22, IF(J145="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J145="Hóc Môn", Ward!$AK$2:$AL$13, IF(J145="Nhà Bè", Ward!$AM$2:$AN$8, IF(J145="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J145="Tân Bình", Ward!$AQ$2:$AR$16, IF(J145="Tân Phú", Ward!$AS$2:$AT$12, IF(J145="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X145" t="str">
+        <f>IF(B145 &lt;&gt; "", VLOOKUP(B145, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="146" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
       <c r="B146" s="16"/>
       <c r="C146" s="16"/>
@@ -7117,8 +7726,12 @@
         <f>IF(K146 &lt;&gt; "", VLOOKUP(K146, IF(J146="1", Ward!$A$2:$B$11, IF(J146="2", Ward!$C$2:$D$12, IF(J146="3", Ward!$E$2:$F$15, IF(J146="4", Ward!$G$2:$H$16, IF(J146="5", Ward!$I$2:$J$16, IF(J146="6", Ward!$K$2:$L$15, IF(J146="7", Ward!$M$2:$N$11, IF(J146="8", Ward!$O$2:$P$17, IF(J146="9", Ward!$Q$2:$R$14, IF(J146="10", Ward!$S$2:$T$16, IF(J146="11", Ward!$U$2:$V$17, IF(J146="12", Ward!$W$2:$X$12, IF(J146="Bình Chánh", Ward!$Y$2:$Z$17, IF(J146="Bình Tân", Ward!$AA$2:$AB$11, IF(J146="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J146="Cần Giờ", Ward!$AE$2:$AF$8, IF(J146="Củ Chi", Ward!$AG$2:$AH$22, IF(J146="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J146="Hóc Môn", Ward!$AK$2:$AL$13, IF(J146="Nhà Bè", Ward!$AM$2:$AN$8, IF(J146="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J146="Tân Bình", Ward!$AQ$2:$AR$16, IF(J146="Tân Phú", Ward!$AS$2:$AT$12, IF(J146="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X146" t="str">
+        <f>IF(B146 &lt;&gt; "", VLOOKUP(B146, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="147" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A147" s="3"/>
       <c r="B147" s="16"/>
       <c r="C147" s="16"/>
@@ -7151,8 +7764,12 @@
         <f>IF(K147 &lt;&gt; "", VLOOKUP(K147, IF(J147="1", Ward!$A$2:$B$11, IF(J147="2", Ward!$C$2:$D$12, IF(J147="3", Ward!$E$2:$F$15, IF(J147="4", Ward!$G$2:$H$16, IF(J147="5", Ward!$I$2:$J$16, IF(J147="6", Ward!$K$2:$L$15, IF(J147="7", Ward!$M$2:$N$11, IF(J147="8", Ward!$O$2:$P$17, IF(J147="9", Ward!$Q$2:$R$14, IF(J147="10", Ward!$S$2:$T$16, IF(J147="11", Ward!$U$2:$V$17, IF(J147="12", Ward!$W$2:$X$12, IF(J147="Bình Chánh", Ward!$Y$2:$Z$17, IF(J147="Bình Tân", Ward!$AA$2:$AB$11, IF(J147="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J147="Cần Giờ", Ward!$AE$2:$AF$8, IF(J147="Củ Chi", Ward!$AG$2:$AH$22, IF(J147="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J147="Hóc Môn", Ward!$AK$2:$AL$13, IF(J147="Nhà Bè", Ward!$AM$2:$AN$8, IF(J147="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J147="Tân Bình", Ward!$AQ$2:$AR$16, IF(J147="Tân Phú", Ward!$AS$2:$AT$12, IF(J147="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X147" t="str">
+        <f>IF(B147 &lt;&gt; "", VLOOKUP(B147, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="148" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
       <c r="B148" s="16"/>
       <c r="C148" s="16"/>
@@ -7185,8 +7802,12 @@
         <f>IF(K148 &lt;&gt; "", VLOOKUP(K148, IF(J148="1", Ward!$A$2:$B$11, IF(J148="2", Ward!$C$2:$D$12, IF(J148="3", Ward!$E$2:$F$15, IF(J148="4", Ward!$G$2:$H$16, IF(J148="5", Ward!$I$2:$J$16, IF(J148="6", Ward!$K$2:$L$15, IF(J148="7", Ward!$M$2:$N$11, IF(J148="8", Ward!$O$2:$P$17, IF(J148="9", Ward!$Q$2:$R$14, IF(J148="10", Ward!$S$2:$T$16, IF(J148="11", Ward!$U$2:$V$17, IF(J148="12", Ward!$W$2:$X$12, IF(J148="Bình Chánh", Ward!$Y$2:$Z$17, IF(J148="Bình Tân", Ward!$AA$2:$AB$11, IF(J148="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J148="Cần Giờ", Ward!$AE$2:$AF$8, IF(J148="Củ Chi", Ward!$AG$2:$AH$22, IF(J148="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J148="Hóc Môn", Ward!$AK$2:$AL$13, IF(J148="Nhà Bè", Ward!$AM$2:$AN$8, IF(J148="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J148="Tân Bình", Ward!$AQ$2:$AR$16, IF(J148="Tân Phú", Ward!$AS$2:$AT$12, IF(J148="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X148" t="str">
+        <f>IF(B148 &lt;&gt; "", VLOOKUP(B148, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="149" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
       <c r="B149" s="16"/>
       <c r="C149" s="16"/>
@@ -7219,8 +7840,12 @@
         <f>IF(K149 &lt;&gt; "", VLOOKUP(K149, IF(J149="1", Ward!$A$2:$B$11, IF(J149="2", Ward!$C$2:$D$12, IF(J149="3", Ward!$E$2:$F$15, IF(J149="4", Ward!$G$2:$H$16, IF(J149="5", Ward!$I$2:$J$16, IF(J149="6", Ward!$K$2:$L$15, IF(J149="7", Ward!$M$2:$N$11, IF(J149="8", Ward!$O$2:$P$17, IF(J149="9", Ward!$Q$2:$R$14, IF(J149="10", Ward!$S$2:$T$16, IF(J149="11", Ward!$U$2:$V$17, IF(J149="12", Ward!$W$2:$X$12, IF(J149="Bình Chánh", Ward!$Y$2:$Z$17, IF(J149="Bình Tân", Ward!$AA$2:$AB$11, IF(J149="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J149="Cần Giờ", Ward!$AE$2:$AF$8, IF(J149="Củ Chi", Ward!$AG$2:$AH$22, IF(J149="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J149="Hóc Môn", Ward!$AK$2:$AL$13, IF(J149="Nhà Bè", Ward!$AM$2:$AN$8, IF(J149="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J149="Tân Bình", Ward!$AQ$2:$AR$16, IF(J149="Tân Phú", Ward!$AS$2:$AT$12, IF(J149="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X149" t="str">
+        <f>IF(B149 &lt;&gt; "", VLOOKUP(B149, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="150" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
       <c r="B150" s="16"/>
       <c r="C150" s="16"/>
@@ -7253,8 +7878,12 @@
         <f>IF(K150 &lt;&gt; "", VLOOKUP(K150, IF(J150="1", Ward!$A$2:$B$11, IF(J150="2", Ward!$C$2:$D$12, IF(J150="3", Ward!$E$2:$F$15, IF(J150="4", Ward!$G$2:$H$16, IF(J150="5", Ward!$I$2:$J$16, IF(J150="6", Ward!$K$2:$L$15, IF(J150="7", Ward!$M$2:$N$11, IF(J150="8", Ward!$O$2:$P$17, IF(J150="9", Ward!$Q$2:$R$14, IF(J150="10", Ward!$S$2:$T$16, IF(J150="11", Ward!$U$2:$V$17, IF(J150="12", Ward!$W$2:$X$12, IF(J150="Bình Chánh", Ward!$Y$2:$Z$17, IF(J150="Bình Tân", Ward!$AA$2:$AB$11, IF(J150="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J150="Cần Giờ", Ward!$AE$2:$AF$8, IF(J150="Củ Chi", Ward!$AG$2:$AH$22, IF(J150="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J150="Hóc Môn", Ward!$AK$2:$AL$13, IF(J150="Nhà Bè", Ward!$AM$2:$AN$8, IF(J150="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J150="Tân Bình", Ward!$AQ$2:$AR$16, IF(J150="Tân Phú", Ward!$AS$2:$AT$12, IF(J150="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X150" t="str">
+        <f>IF(B150 &lt;&gt; "", VLOOKUP(B150, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="151" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="16"/>
       <c r="C151" s="16"/>
@@ -7287,8 +7916,12 @@
         <f>IF(K151 &lt;&gt; "", VLOOKUP(K151, IF(J151="1", Ward!$A$2:$B$11, IF(J151="2", Ward!$C$2:$D$12, IF(J151="3", Ward!$E$2:$F$15, IF(J151="4", Ward!$G$2:$H$16, IF(J151="5", Ward!$I$2:$J$16, IF(J151="6", Ward!$K$2:$L$15, IF(J151="7", Ward!$M$2:$N$11, IF(J151="8", Ward!$O$2:$P$17, IF(J151="9", Ward!$Q$2:$R$14, IF(J151="10", Ward!$S$2:$T$16, IF(J151="11", Ward!$U$2:$V$17, IF(J151="12", Ward!$W$2:$X$12, IF(J151="Bình Chánh", Ward!$Y$2:$Z$17, IF(J151="Bình Tân", Ward!$AA$2:$AB$11, IF(J151="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J151="Cần Giờ", Ward!$AE$2:$AF$8, IF(J151="Củ Chi", Ward!$AG$2:$AH$22, IF(J151="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J151="Hóc Môn", Ward!$AK$2:$AL$13, IF(J151="Nhà Bè", Ward!$AM$2:$AN$8, IF(J151="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J151="Tân Bình", Ward!$AQ$2:$AR$16, IF(J151="Tân Phú", Ward!$AS$2:$AT$12, IF(J151="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X151" t="str">
+        <f>IF(B151 &lt;&gt; "", VLOOKUP(B151, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="152" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="16"/>
       <c r="C152" s="16"/>
@@ -7321,8 +7954,12 @@
         <f>IF(K152 &lt;&gt; "", VLOOKUP(K152, IF(J152="1", Ward!$A$2:$B$11, IF(J152="2", Ward!$C$2:$D$12, IF(J152="3", Ward!$E$2:$F$15, IF(J152="4", Ward!$G$2:$H$16, IF(J152="5", Ward!$I$2:$J$16, IF(J152="6", Ward!$K$2:$L$15, IF(J152="7", Ward!$M$2:$N$11, IF(J152="8", Ward!$O$2:$P$17, IF(J152="9", Ward!$Q$2:$R$14, IF(J152="10", Ward!$S$2:$T$16, IF(J152="11", Ward!$U$2:$V$17, IF(J152="12", Ward!$W$2:$X$12, IF(J152="Bình Chánh", Ward!$Y$2:$Z$17, IF(J152="Bình Tân", Ward!$AA$2:$AB$11, IF(J152="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J152="Cần Giờ", Ward!$AE$2:$AF$8, IF(J152="Củ Chi", Ward!$AG$2:$AH$22, IF(J152="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J152="Hóc Môn", Ward!$AK$2:$AL$13, IF(J152="Nhà Bè", Ward!$AM$2:$AN$8, IF(J152="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J152="Tân Bình", Ward!$AQ$2:$AR$16, IF(J152="Tân Phú", Ward!$AS$2:$AT$12, IF(J152="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X152" t="str">
+        <f>IF(B152 &lt;&gt; "", VLOOKUP(B152, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="153" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="16"/>
       <c r="C153" s="16"/>
@@ -7355,8 +7992,12 @@
         <f>IF(K153 &lt;&gt; "", VLOOKUP(K153, IF(J153="1", Ward!$A$2:$B$11, IF(J153="2", Ward!$C$2:$D$12, IF(J153="3", Ward!$E$2:$F$15, IF(J153="4", Ward!$G$2:$H$16, IF(J153="5", Ward!$I$2:$J$16, IF(J153="6", Ward!$K$2:$L$15, IF(J153="7", Ward!$M$2:$N$11, IF(J153="8", Ward!$O$2:$P$17, IF(J153="9", Ward!$Q$2:$R$14, IF(J153="10", Ward!$S$2:$T$16, IF(J153="11", Ward!$U$2:$V$17, IF(J153="12", Ward!$W$2:$X$12, IF(J153="Bình Chánh", Ward!$Y$2:$Z$17, IF(J153="Bình Tân", Ward!$AA$2:$AB$11, IF(J153="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J153="Cần Giờ", Ward!$AE$2:$AF$8, IF(J153="Củ Chi", Ward!$AG$2:$AH$22, IF(J153="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J153="Hóc Môn", Ward!$AK$2:$AL$13, IF(J153="Nhà Bè", Ward!$AM$2:$AN$8, IF(J153="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J153="Tân Bình", Ward!$AQ$2:$AR$16, IF(J153="Tân Phú", Ward!$AS$2:$AT$12, IF(J153="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X153" t="str">
+        <f>IF(B153 &lt;&gt; "", VLOOKUP(B153, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="154" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="16"/>
       <c r="C154" s="16"/>
@@ -7389,8 +8030,12 @@
         <f>IF(K154 &lt;&gt; "", VLOOKUP(K154, IF(J154="1", Ward!$A$2:$B$11, IF(J154="2", Ward!$C$2:$D$12, IF(J154="3", Ward!$E$2:$F$15, IF(J154="4", Ward!$G$2:$H$16, IF(J154="5", Ward!$I$2:$J$16, IF(J154="6", Ward!$K$2:$L$15, IF(J154="7", Ward!$M$2:$N$11, IF(J154="8", Ward!$O$2:$P$17, IF(J154="9", Ward!$Q$2:$R$14, IF(J154="10", Ward!$S$2:$T$16, IF(J154="11", Ward!$U$2:$V$17, IF(J154="12", Ward!$W$2:$X$12, IF(J154="Bình Chánh", Ward!$Y$2:$Z$17, IF(J154="Bình Tân", Ward!$AA$2:$AB$11, IF(J154="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J154="Cần Giờ", Ward!$AE$2:$AF$8, IF(J154="Củ Chi", Ward!$AG$2:$AH$22, IF(J154="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J154="Hóc Môn", Ward!$AK$2:$AL$13, IF(J154="Nhà Bè", Ward!$AM$2:$AN$8, IF(J154="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J154="Tân Bình", Ward!$AQ$2:$AR$16, IF(J154="Tân Phú", Ward!$AS$2:$AT$12, IF(J154="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X154" t="str">
+        <f>IF(B154 &lt;&gt; "", VLOOKUP(B154, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="155" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="16"/>
       <c r="C155" s="16"/>
@@ -7423,8 +8068,12 @@
         <f>IF(K155 &lt;&gt; "", VLOOKUP(K155, IF(J155="1", Ward!$A$2:$B$11, IF(J155="2", Ward!$C$2:$D$12, IF(J155="3", Ward!$E$2:$F$15, IF(J155="4", Ward!$G$2:$H$16, IF(J155="5", Ward!$I$2:$J$16, IF(J155="6", Ward!$K$2:$L$15, IF(J155="7", Ward!$M$2:$N$11, IF(J155="8", Ward!$O$2:$P$17, IF(J155="9", Ward!$Q$2:$R$14, IF(J155="10", Ward!$S$2:$T$16, IF(J155="11", Ward!$U$2:$V$17, IF(J155="12", Ward!$W$2:$X$12, IF(J155="Bình Chánh", Ward!$Y$2:$Z$17, IF(J155="Bình Tân", Ward!$AA$2:$AB$11, IF(J155="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J155="Cần Giờ", Ward!$AE$2:$AF$8, IF(J155="Củ Chi", Ward!$AG$2:$AH$22, IF(J155="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J155="Hóc Môn", Ward!$AK$2:$AL$13, IF(J155="Nhà Bè", Ward!$AM$2:$AN$8, IF(J155="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J155="Tân Bình", Ward!$AQ$2:$AR$16, IF(J155="Tân Phú", Ward!$AS$2:$AT$12, IF(J155="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X155" t="str">
+        <f>IF(B155 &lt;&gt; "", VLOOKUP(B155, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="156" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
       <c r="B156" s="16"/>
       <c r="C156" s="16"/>
@@ -7457,8 +8106,12 @@
         <f>IF(K156 &lt;&gt; "", VLOOKUP(K156, IF(J156="1", Ward!$A$2:$B$11, IF(J156="2", Ward!$C$2:$D$12, IF(J156="3", Ward!$E$2:$F$15, IF(J156="4", Ward!$G$2:$H$16, IF(J156="5", Ward!$I$2:$J$16, IF(J156="6", Ward!$K$2:$L$15, IF(J156="7", Ward!$M$2:$N$11, IF(J156="8", Ward!$O$2:$P$17, IF(J156="9", Ward!$Q$2:$R$14, IF(J156="10", Ward!$S$2:$T$16, IF(J156="11", Ward!$U$2:$V$17, IF(J156="12", Ward!$W$2:$X$12, IF(J156="Bình Chánh", Ward!$Y$2:$Z$17, IF(J156="Bình Tân", Ward!$AA$2:$AB$11, IF(J156="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J156="Cần Giờ", Ward!$AE$2:$AF$8, IF(J156="Củ Chi", Ward!$AG$2:$AH$22, IF(J156="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J156="Hóc Môn", Ward!$AK$2:$AL$13, IF(J156="Nhà Bè", Ward!$AM$2:$AN$8, IF(J156="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J156="Tân Bình", Ward!$AQ$2:$AR$16, IF(J156="Tân Phú", Ward!$AS$2:$AT$12, IF(J156="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X156" t="str">
+        <f>IF(B156 &lt;&gt; "", VLOOKUP(B156, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="157" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A157" s="3"/>
       <c r="B157" s="16"/>
       <c r="C157" s="16"/>
@@ -7491,8 +8144,12 @@
         <f>IF(K157 &lt;&gt; "", VLOOKUP(K157, IF(J157="1", Ward!$A$2:$B$11, IF(J157="2", Ward!$C$2:$D$12, IF(J157="3", Ward!$E$2:$F$15, IF(J157="4", Ward!$G$2:$H$16, IF(J157="5", Ward!$I$2:$J$16, IF(J157="6", Ward!$K$2:$L$15, IF(J157="7", Ward!$M$2:$N$11, IF(J157="8", Ward!$O$2:$P$17, IF(J157="9", Ward!$Q$2:$R$14, IF(J157="10", Ward!$S$2:$T$16, IF(J157="11", Ward!$U$2:$V$17, IF(J157="12", Ward!$W$2:$X$12, IF(J157="Bình Chánh", Ward!$Y$2:$Z$17, IF(J157="Bình Tân", Ward!$AA$2:$AB$11, IF(J157="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J157="Cần Giờ", Ward!$AE$2:$AF$8, IF(J157="Củ Chi", Ward!$AG$2:$AH$22, IF(J157="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J157="Hóc Môn", Ward!$AK$2:$AL$13, IF(J157="Nhà Bè", Ward!$AM$2:$AN$8, IF(J157="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J157="Tân Bình", Ward!$AQ$2:$AR$16, IF(J157="Tân Phú", Ward!$AS$2:$AT$12, IF(J157="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X157" t="str">
+        <f>IF(B157 &lt;&gt; "", VLOOKUP(B157, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="158" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A158" s="3"/>
       <c r="B158" s="16"/>
       <c r="C158" s="16"/>
@@ -7525,8 +8182,12 @@
         <f>IF(K158 &lt;&gt; "", VLOOKUP(K158, IF(J158="1", Ward!$A$2:$B$11, IF(J158="2", Ward!$C$2:$D$12, IF(J158="3", Ward!$E$2:$F$15, IF(J158="4", Ward!$G$2:$H$16, IF(J158="5", Ward!$I$2:$J$16, IF(J158="6", Ward!$K$2:$L$15, IF(J158="7", Ward!$M$2:$N$11, IF(J158="8", Ward!$O$2:$P$17, IF(J158="9", Ward!$Q$2:$R$14, IF(J158="10", Ward!$S$2:$T$16, IF(J158="11", Ward!$U$2:$V$17, IF(J158="12", Ward!$W$2:$X$12, IF(J158="Bình Chánh", Ward!$Y$2:$Z$17, IF(J158="Bình Tân", Ward!$AA$2:$AB$11, IF(J158="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J158="Cần Giờ", Ward!$AE$2:$AF$8, IF(J158="Củ Chi", Ward!$AG$2:$AH$22, IF(J158="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J158="Hóc Môn", Ward!$AK$2:$AL$13, IF(J158="Nhà Bè", Ward!$AM$2:$AN$8, IF(J158="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J158="Tân Bình", Ward!$AQ$2:$AR$16, IF(J158="Tân Phú", Ward!$AS$2:$AT$12, IF(J158="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X158" t="str">
+        <f>IF(B158 &lt;&gt; "", VLOOKUP(B158, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="159" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A159" s="3"/>
       <c r="B159" s="16"/>
       <c r="C159" s="16"/>
@@ -7559,8 +8220,12 @@
         <f>IF(K159 &lt;&gt; "", VLOOKUP(K159, IF(J159="1", Ward!$A$2:$B$11, IF(J159="2", Ward!$C$2:$D$12, IF(J159="3", Ward!$E$2:$F$15, IF(J159="4", Ward!$G$2:$H$16, IF(J159="5", Ward!$I$2:$J$16, IF(J159="6", Ward!$K$2:$L$15, IF(J159="7", Ward!$M$2:$N$11, IF(J159="8", Ward!$O$2:$P$17, IF(J159="9", Ward!$Q$2:$R$14, IF(J159="10", Ward!$S$2:$T$16, IF(J159="11", Ward!$U$2:$V$17, IF(J159="12", Ward!$W$2:$X$12, IF(J159="Bình Chánh", Ward!$Y$2:$Z$17, IF(J159="Bình Tân", Ward!$AA$2:$AB$11, IF(J159="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J159="Cần Giờ", Ward!$AE$2:$AF$8, IF(J159="Củ Chi", Ward!$AG$2:$AH$22, IF(J159="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J159="Hóc Môn", Ward!$AK$2:$AL$13, IF(J159="Nhà Bè", Ward!$AM$2:$AN$8, IF(J159="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J159="Tân Bình", Ward!$AQ$2:$AR$16, IF(J159="Tân Phú", Ward!$AS$2:$AT$12, IF(J159="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X159" t="str">
+        <f>IF(B159 &lt;&gt; "", VLOOKUP(B159, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="160" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A160" s="3"/>
       <c r="B160" s="16"/>
       <c r="C160" s="16"/>
@@ -7593,8 +8258,12 @@
         <f>IF(K160 &lt;&gt; "", VLOOKUP(K160, IF(J160="1", Ward!$A$2:$B$11, IF(J160="2", Ward!$C$2:$D$12, IF(J160="3", Ward!$E$2:$F$15, IF(J160="4", Ward!$G$2:$H$16, IF(J160="5", Ward!$I$2:$J$16, IF(J160="6", Ward!$K$2:$L$15, IF(J160="7", Ward!$M$2:$N$11, IF(J160="8", Ward!$O$2:$P$17, IF(J160="9", Ward!$Q$2:$R$14, IF(J160="10", Ward!$S$2:$T$16, IF(J160="11", Ward!$U$2:$V$17, IF(J160="12", Ward!$W$2:$X$12, IF(J160="Bình Chánh", Ward!$Y$2:$Z$17, IF(J160="Bình Tân", Ward!$AA$2:$AB$11, IF(J160="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J160="Cần Giờ", Ward!$AE$2:$AF$8, IF(J160="Củ Chi", Ward!$AG$2:$AH$22, IF(J160="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J160="Hóc Môn", Ward!$AK$2:$AL$13, IF(J160="Nhà Bè", Ward!$AM$2:$AN$8, IF(J160="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J160="Tân Bình", Ward!$AQ$2:$AR$16, IF(J160="Tân Phú", Ward!$AS$2:$AT$12, IF(J160="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X160" t="str">
+        <f>IF(B160 &lt;&gt; "", VLOOKUP(B160, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="161" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A161" s="3"/>
       <c r="B161" s="16"/>
       <c r="C161" s="16"/>
@@ -7627,8 +8296,12 @@
         <f>IF(K161 &lt;&gt; "", VLOOKUP(K161, IF(J161="1", Ward!$A$2:$B$11, IF(J161="2", Ward!$C$2:$D$12, IF(J161="3", Ward!$E$2:$F$15, IF(J161="4", Ward!$G$2:$H$16, IF(J161="5", Ward!$I$2:$J$16, IF(J161="6", Ward!$K$2:$L$15, IF(J161="7", Ward!$M$2:$N$11, IF(J161="8", Ward!$O$2:$P$17, IF(J161="9", Ward!$Q$2:$R$14, IF(J161="10", Ward!$S$2:$T$16, IF(J161="11", Ward!$U$2:$V$17, IF(J161="12", Ward!$W$2:$X$12, IF(J161="Bình Chánh", Ward!$Y$2:$Z$17, IF(J161="Bình Tân", Ward!$AA$2:$AB$11, IF(J161="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J161="Cần Giờ", Ward!$AE$2:$AF$8, IF(J161="Củ Chi", Ward!$AG$2:$AH$22, IF(J161="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J161="Hóc Môn", Ward!$AK$2:$AL$13, IF(J161="Nhà Bè", Ward!$AM$2:$AN$8, IF(J161="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J161="Tân Bình", Ward!$AQ$2:$AR$16, IF(J161="Tân Phú", Ward!$AS$2:$AT$12, IF(J161="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X161" t="str">
+        <f>IF(B161 &lt;&gt; "", VLOOKUP(B161, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="162" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A162" s="3"/>
       <c r="B162" s="16"/>
       <c r="C162" s="16"/>
@@ -7661,8 +8334,12 @@
         <f>IF(K162 &lt;&gt; "", VLOOKUP(K162, IF(J162="1", Ward!$A$2:$B$11, IF(J162="2", Ward!$C$2:$D$12, IF(J162="3", Ward!$E$2:$F$15, IF(J162="4", Ward!$G$2:$H$16, IF(J162="5", Ward!$I$2:$J$16, IF(J162="6", Ward!$K$2:$L$15, IF(J162="7", Ward!$M$2:$N$11, IF(J162="8", Ward!$O$2:$P$17, IF(J162="9", Ward!$Q$2:$R$14, IF(J162="10", Ward!$S$2:$T$16, IF(J162="11", Ward!$U$2:$V$17, IF(J162="12", Ward!$W$2:$X$12, IF(J162="Bình Chánh", Ward!$Y$2:$Z$17, IF(J162="Bình Tân", Ward!$AA$2:$AB$11, IF(J162="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J162="Cần Giờ", Ward!$AE$2:$AF$8, IF(J162="Củ Chi", Ward!$AG$2:$AH$22, IF(J162="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J162="Hóc Môn", Ward!$AK$2:$AL$13, IF(J162="Nhà Bè", Ward!$AM$2:$AN$8, IF(J162="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J162="Tân Bình", Ward!$AQ$2:$AR$16, IF(J162="Tân Phú", Ward!$AS$2:$AT$12, IF(J162="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="163" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X162" t="str">
+        <f>IF(B162 &lt;&gt; "", VLOOKUP(B162, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="163" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A163" s="3"/>
       <c r="B163" s="16"/>
       <c r="C163" s="16"/>
@@ -7695,8 +8372,12 @@
         <f>IF(K163 &lt;&gt; "", VLOOKUP(K163, IF(J163="1", Ward!$A$2:$B$11, IF(J163="2", Ward!$C$2:$D$12, IF(J163="3", Ward!$E$2:$F$15, IF(J163="4", Ward!$G$2:$H$16, IF(J163="5", Ward!$I$2:$J$16, IF(J163="6", Ward!$K$2:$L$15, IF(J163="7", Ward!$M$2:$N$11, IF(J163="8", Ward!$O$2:$P$17, IF(J163="9", Ward!$Q$2:$R$14, IF(J163="10", Ward!$S$2:$T$16, IF(J163="11", Ward!$U$2:$V$17, IF(J163="12", Ward!$W$2:$X$12, IF(J163="Bình Chánh", Ward!$Y$2:$Z$17, IF(J163="Bình Tân", Ward!$AA$2:$AB$11, IF(J163="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J163="Cần Giờ", Ward!$AE$2:$AF$8, IF(J163="Củ Chi", Ward!$AG$2:$AH$22, IF(J163="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J163="Hóc Môn", Ward!$AK$2:$AL$13, IF(J163="Nhà Bè", Ward!$AM$2:$AN$8, IF(J163="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J163="Tân Bình", Ward!$AQ$2:$AR$16, IF(J163="Tân Phú", Ward!$AS$2:$AT$12, IF(J163="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="164" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X163" t="str">
+        <f>IF(B163 &lt;&gt; "", VLOOKUP(B163, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="164" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A164" s="3"/>
       <c r="B164" s="16"/>
       <c r="C164" s="16"/>
@@ -7729,8 +8410,12 @@
         <f>IF(K164 &lt;&gt; "", VLOOKUP(K164, IF(J164="1", Ward!$A$2:$B$11, IF(J164="2", Ward!$C$2:$D$12, IF(J164="3", Ward!$E$2:$F$15, IF(J164="4", Ward!$G$2:$H$16, IF(J164="5", Ward!$I$2:$J$16, IF(J164="6", Ward!$K$2:$L$15, IF(J164="7", Ward!$M$2:$N$11, IF(J164="8", Ward!$O$2:$P$17, IF(J164="9", Ward!$Q$2:$R$14, IF(J164="10", Ward!$S$2:$T$16, IF(J164="11", Ward!$U$2:$V$17, IF(J164="12", Ward!$W$2:$X$12, IF(J164="Bình Chánh", Ward!$Y$2:$Z$17, IF(J164="Bình Tân", Ward!$AA$2:$AB$11, IF(J164="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J164="Cần Giờ", Ward!$AE$2:$AF$8, IF(J164="Củ Chi", Ward!$AG$2:$AH$22, IF(J164="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J164="Hóc Môn", Ward!$AK$2:$AL$13, IF(J164="Nhà Bè", Ward!$AM$2:$AN$8, IF(J164="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J164="Tân Bình", Ward!$AQ$2:$AR$16, IF(J164="Tân Phú", Ward!$AS$2:$AT$12, IF(J164="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="165" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X164" t="str">
+        <f>IF(B164 &lt;&gt; "", VLOOKUP(B164, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="165" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A165" s="3"/>
       <c r="B165" s="16"/>
       <c r="C165" s="16"/>
@@ -7763,8 +8448,12 @@
         <f>IF(K165 &lt;&gt; "", VLOOKUP(K165, IF(J165="1", Ward!$A$2:$B$11, IF(J165="2", Ward!$C$2:$D$12, IF(J165="3", Ward!$E$2:$F$15, IF(J165="4", Ward!$G$2:$H$16, IF(J165="5", Ward!$I$2:$J$16, IF(J165="6", Ward!$K$2:$L$15, IF(J165="7", Ward!$M$2:$N$11, IF(J165="8", Ward!$O$2:$P$17, IF(J165="9", Ward!$Q$2:$R$14, IF(J165="10", Ward!$S$2:$T$16, IF(J165="11", Ward!$U$2:$V$17, IF(J165="12", Ward!$W$2:$X$12, IF(J165="Bình Chánh", Ward!$Y$2:$Z$17, IF(J165="Bình Tân", Ward!$AA$2:$AB$11, IF(J165="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J165="Cần Giờ", Ward!$AE$2:$AF$8, IF(J165="Củ Chi", Ward!$AG$2:$AH$22, IF(J165="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J165="Hóc Môn", Ward!$AK$2:$AL$13, IF(J165="Nhà Bè", Ward!$AM$2:$AN$8, IF(J165="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J165="Tân Bình", Ward!$AQ$2:$AR$16, IF(J165="Tân Phú", Ward!$AS$2:$AT$12, IF(J165="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="166" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X165" t="str">
+        <f>IF(B165 &lt;&gt; "", VLOOKUP(B165, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="166" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A166" s="3"/>
       <c r="B166" s="16"/>
       <c r="C166" s="16"/>
@@ -7797,8 +8486,12 @@
         <f>IF(K166 &lt;&gt; "", VLOOKUP(K166, IF(J166="1", Ward!$A$2:$B$11, IF(J166="2", Ward!$C$2:$D$12, IF(J166="3", Ward!$E$2:$F$15, IF(J166="4", Ward!$G$2:$H$16, IF(J166="5", Ward!$I$2:$J$16, IF(J166="6", Ward!$K$2:$L$15, IF(J166="7", Ward!$M$2:$N$11, IF(J166="8", Ward!$O$2:$P$17, IF(J166="9", Ward!$Q$2:$R$14, IF(J166="10", Ward!$S$2:$T$16, IF(J166="11", Ward!$U$2:$V$17, IF(J166="12", Ward!$W$2:$X$12, IF(J166="Bình Chánh", Ward!$Y$2:$Z$17, IF(J166="Bình Tân", Ward!$AA$2:$AB$11, IF(J166="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J166="Cần Giờ", Ward!$AE$2:$AF$8, IF(J166="Củ Chi", Ward!$AG$2:$AH$22, IF(J166="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J166="Hóc Môn", Ward!$AK$2:$AL$13, IF(J166="Nhà Bè", Ward!$AM$2:$AN$8, IF(J166="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J166="Tân Bình", Ward!$AQ$2:$AR$16, IF(J166="Tân Phú", Ward!$AS$2:$AT$12, IF(J166="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="167" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X166" t="str">
+        <f>IF(B166 &lt;&gt; "", VLOOKUP(B166, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="167" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A167" s="3"/>
       <c r="B167" s="16"/>
       <c r="C167" s="16"/>
@@ -7831,8 +8524,12 @@
         <f>IF(K167 &lt;&gt; "", VLOOKUP(K167, IF(J167="1", Ward!$A$2:$B$11, IF(J167="2", Ward!$C$2:$D$12, IF(J167="3", Ward!$E$2:$F$15, IF(J167="4", Ward!$G$2:$H$16, IF(J167="5", Ward!$I$2:$J$16, IF(J167="6", Ward!$K$2:$L$15, IF(J167="7", Ward!$M$2:$N$11, IF(J167="8", Ward!$O$2:$P$17, IF(J167="9", Ward!$Q$2:$R$14, IF(J167="10", Ward!$S$2:$T$16, IF(J167="11", Ward!$U$2:$V$17, IF(J167="12", Ward!$W$2:$X$12, IF(J167="Bình Chánh", Ward!$Y$2:$Z$17, IF(J167="Bình Tân", Ward!$AA$2:$AB$11, IF(J167="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J167="Cần Giờ", Ward!$AE$2:$AF$8, IF(J167="Củ Chi", Ward!$AG$2:$AH$22, IF(J167="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J167="Hóc Môn", Ward!$AK$2:$AL$13, IF(J167="Nhà Bè", Ward!$AM$2:$AN$8, IF(J167="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J167="Tân Bình", Ward!$AQ$2:$AR$16, IF(J167="Tân Phú", Ward!$AS$2:$AT$12, IF(J167="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="168" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X167" t="str">
+        <f>IF(B167 &lt;&gt; "", VLOOKUP(B167, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="168" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A168" s="3"/>
       <c r="B168" s="16"/>
       <c r="C168" s="16"/>
@@ -7865,8 +8562,12 @@
         <f>IF(K168 &lt;&gt; "", VLOOKUP(K168, IF(J168="1", Ward!$A$2:$B$11, IF(J168="2", Ward!$C$2:$D$12, IF(J168="3", Ward!$E$2:$F$15, IF(J168="4", Ward!$G$2:$H$16, IF(J168="5", Ward!$I$2:$J$16, IF(J168="6", Ward!$K$2:$L$15, IF(J168="7", Ward!$M$2:$N$11, IF(J168="8", Ward!$O$2:$P$17, IF(J168="9", Ward!$Q$2:$R$14, IF(J168="10", Ward!$S$2:$T$16, IF(J168="11", Ward!$U$2:$V$17, IF(J168="12", Ward!$W$2:$X$12, IF(J168="Bình Chánh", Ward!$Y$2:$Z$17, IF(J168="Bình Tân", Ward!$AA$2:$AB$11, IF(J168="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J168="Cần Giờ", Ward!$AE$2:$AF$8, IF(J168="Củ Chi", Ward!$AG$2:$AH$22, IF(J168="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J168="Hóc Môn", Ward!$AK$2:$AL$13, IF(J168="Nhà Bè", Ward!$AM$2:$AN$8, IF(J168="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J168="Tân Bình", Ward!$AQ$2:$AR$16, IF(J168="Tân Phú", Ward!$AS$2:$AT$12, IF(J168="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="169" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X168" t="str">
+        <f>IF(B168 &lt;&gt; "", VLOOKUP(B168, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="169" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A169" s="3"/>
       <c r="B169" s="16"/>
       <c r="C169" s="16"/>
@@ -7899,8 +8600,12 @@
         <f>IF(K169 &lt;&gt; "", VLOOKUP(K169, IF(J169="1", Ward!$A$2:$B$11, IF(J169="2", Ward!$C$2:$D$12, IF(J169="3", Ward!$E$2:$F$15, IF(J169="4", Ward!$G$2:$H$16, IF(J169="5", Ward!$I$2:$J$16, IF(J169="6", Ward!$K$2:$L$15, IF(J169="7", Ward!$M$2:$N$11, IF(J169="8", Ward!$O$2:$P$17, IF(J169="9", Ward!$Q$2:$R$14, IF(J169="10", Ward!$S$2:$T$16, IF(J169="11", Ward!$U$2:$V$17, IF(J169="12", Ward!$W$2:$X$12, IF(J169="Bình Chánh", Ward!$Y$2:$Z$17, IF(J169="Bình Tân", Ward!$AA$2:$AB$11, IF(J169="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J169="Cần Giờ", Ward!$AE$2:$AF$8, IF(J169="Củ Chi", Ward!$AG$2:$AH$22, IF(J169="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J169="Hóc Môn", Ward!$AK$2:$AL$13, IF(J169="Nhà Bè", Ward!$AM$2:$AN$8, IF(J169="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J169="Tân Bình", Ward!$AQ$2:$AR$16, IF(J169="Tân Phú", Ward!$AS$2:$AT$12, IF(J169="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="170" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X169" t="str">
+        <f>IF(B169 &lt;&gt; "", VLOOKUP(B169, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="170" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A170" s="3"/>
       <c r="B170" s="16"/>
       <c r="C170" s="16"/>
@@ -7933,8 +8638,12 @@
         <f>IF(K170 &lt;&gt; "", VLOOKUP(K170, IF(J170="1", Ward!$A$2:$B$11, IF(J170="2", Ward!$C$2:$D$12, IF(J170="3", Ward!$E$2:$F$15, IF(J170="4", Ward!$G$2:$H$16, IF(J170="5", Ward!$I$2:$J$16, IF(J170="6", Ward!$K$2:$L$15, IF(J170="7", Ward!$M$2:$N$11, IF(J170="8", Ward!$O$2:$P$17, IF(J170="9", Ward!$Q$2:$R$14, IF(J170="10", Ward!$S$2:$T$16, IF(J170="11", Ward!$U$2:$V$17, IF(J170="12", Ward!$W$2:$X$12, IF(J170="Bình Chánh", Ward!$Y$2:$Z$17, IF(J170="Bình Tân", Ward!$AA$2:$AB$11, IF(J170="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J170="Cần Giờ", Ward!$AE$2:$AF$8, IF(J170="Củ Chi", Ward!$AG$2:$AH$22, IF(J170="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J170="Hóc Môn", Ward!$AK$2:$AL$13, IF(J170="Nhà Bè", Ward!$AM$2:$AN$8, IF(J170="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J170="Tân Bình", Ward!$AQ$2:$AR$16, IF(J170="Tân Phú", Ward!$AS$2:$AT$12, IF(J170="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="171" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X170" t="str">
+        <f>IF(B170 &lt;&gt; "", VLOOKUP(B170, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="171" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A171" s="3"/>
       <c r="B171" s="16"/>
       <c r="C171" s="16"/>
@@ -7967,8 +8676,12 @@
         <f>IF(K171 &lt;&gt; "", VLOOKUP(K171, IF(J171="1", Ward!$A$2:$B$11, IF(J171="2", Ward!$C$2:$D$12, IF(J171="3", Ward!$E$2:$F$15, IF(J171="4", Ward!$G$2:$H$16, IF(J171="5", Ward!$I$2:$J$16, IF(J171="6", Ward!$K$2:$L$15, IF(J171="7", Ward!$M$2:$N$11, IF(J171="8", Ward!$O$2:$P$17, IF(J171="9", Ward!$Q$2:$R$14, IF(J171="10", Ward!$S$2:$T$16, IF(J171="11", Ward!$U$2:$V$17, IF(J171="12", Ward!$W$2:$X$12, IF(J171="Bình Chánh", Ward!$Y$2:$Z$17, IF(J171="Bình Tân", Ward!$AA$2:$AB$11, IF(J171="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J171="Cần Giờ", Ward!$AE$2:$AF$8, IF(J171="Củ Chi", Ward!$AG$2:$AH$22, IF(J171="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J171="Hóc Môn", Ward!$AK$2:$AL$13, IF(J171="Nhà Bè", Ward!$AM$2:$AN$8, IF(J171="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J171="Tân Bình", Ward!$AQ$2:$AR$16, IF(J171="Tân Phú", Ward!$AS$2:$AT$12, IF(J171="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="172" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X171" t="str">
+        <f>IF(B171 &lt;&gt; "", VLOOKUP(B171, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="172" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A172" s="3"/>
       <c r="B172" s="16"/>
       <c r="C172" s="16"/>
@@ -8001,8 +8714,12 @@
         <f>IF(K172 &lt;&gt; "", VLOOKUP(K172, IF(J172="1", Ward!$A$2:$B$11, IF(J172="2", Ward!$C$2:$D$12, IF(J172="3", Ward!$E$2:$F$15, IF(J172="4", Ward!$G$2:$H$16, IF(J172="5", Ward!$I$2:$J$16, IF(J172="6", Ward!$K$2:$L$15, IF(J172="7", Ward!$M$2:$N$11, IF(J172="8", Ward!$O$2:$P$17, IF(J172="9", Ward!$Q$2:$R$14, IF(J172="10", Ward!$S$2:$T$16, IF(J172="11", Ward!$U$2:$V$17, IF(J172="12", Ward!$W$2:$X$12, IF(J172="Bình Chánh", Ward!$Y$2:$Z$17, IF(J172="Bình Tân", Ward!$AA$2:$AB$11, IF(J172="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J172="Cần Giờ", Ward!$AE$2:$AF$8, IF(J172="Củ Chi", Ward!$AG$2:$AH$22, IF(J172="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J172="Hóc Môn", Ward!$AK$2:$AL$13, IF(J172="Nhà Bè", Ward!$AM$2:$AN$8, IF(J172="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J172="Tân Bình", Ward!$AQ$2:$AR$16, IF(J172="Tân Phú", Ward!$AS$2:$AT$12, IF(J172="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="173" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X172" t="str">
+        <f>IF(B172 &lt;&gt; "", VLOOKUP(B172, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="173" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A173" s="3"/>
       <c r="B173" s="16"/>
       <c r="C173" s="16"/>
@@ -8035,8 +8752,12 @@
         <f>IF(K173 &lt;&gt; "", VLOOKUP(K173, IF(J173="1", Ward!$A$2:$B$11, IF(J173="2", Ward!$C$2:$D$12, IF(J173="3", Ward!$E$2:$F$15, IF(J173="4", Ward!$G$2:$H$16, IF(J173="5", Ward!$I$2:$J$16, IF(J173="6", Ward!$K$2:$L$15, IF(J173="7", Ward!$M$2:$N$11, IF(J173="8", Ward!$O$2:$P$17, IF(J173="9", Ward!$Q$2:$R$14, IF(J173="10", Ward!$S$2:$T$16, IF(J173="11", Ward!$U$2:$V$17, IF(J173="12", Ward!$W$2:$X$12, IF(J173="Bình Chánh", Ward!$Y$2:$Z$17, IF(J173="Bình Tân", Ward!$AA$2:$AB$11, IF(J173="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J173="Cần Giờ", Ward!$AE$2:$AF$8, IF(J173="Củ Chi", Ward!$AG$2:$AH$22, IF(J173="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J173="Hóc Môn", Ward!$AK$2:$AL$13, IF(J173="Nhà Bè", Ward!$AM$2:$AN$8, IF(J173="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J173="Tân Bình", Ward!$AQ$2:$AR$16, IF(J173="Tân Phú", Ward!$AS$2:$AT$12, IF(J173="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="174" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X173" t="str">
+        <f>IF(B173 &lt;&gt; "", VLOOKUP(B173, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="174" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A174" s="3"/>
       <c r="B174" s="16"/>
       <c r="C174" s="16"/>
@@ -8069,8 +8790,12 @@
         <f>IF(K174 &lt;&gt; "", VLOOKUP(K174, IF(J174="1", Ward!$A$2:$B$11, IF(J174="2", Ward!$C$2:$D$12, IF(J174="3", Ward!$E$2:$F$15, IF(J174="4", Ward!$G$2:$H$16, IF(J174="5", Ward!$I$2:$J$16, IF(J174="6", Ward!$K$2:$L$15, IF(J174="7", Ward!$M$2:$N$11, IF(J174="8", Ward!$O$2:$P$17, IF(J174="9", Ward!$Q$2:$R$14, IF(J174="10", Ward!$S$2:$T$16, IF(J174="11", Ward!$U$2:$V$17, IF(J174="12", Ward!$W$2:$X$12, IF(J174="Bình Chánh", Ward!$Y$2:$Z$17, IF(J174="Bình Tân", Ward!$AA$2:$AB$11, IF(J174="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J174="Cần Giờ", Ward!$AE$2:$AF$8, IF(J174="Củ Chi", Ward!$AG$2:$AH$22, IF(J174="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J174="Hóc Môn", Ward!$AK$2:$AL$13, IF(J174="Nhà Bè", Ward!$AM$2:$AN$8, IF(J174="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J174="Tân Bình", Ward!$AQ$2:$AR$16, IF(J174="Tân Phú", Ward!$AS$2:$AT$12, IF(J174="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="175" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X174" t="str">
+        <f>IF(B174 &lt;&gt; "", VLOOKUP(B174, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="175" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A175" s="3"/>
       <c r="B175" s="16"/>
       <c r="C175" s="16"/>
@@ -8103,8 +8828,12 @@
         <f>IF(K175 &lt;&gt; "", VLOOKUP(K175, IF(J175="1", Ward!$A$2:$B$11, IF(J175="2", Ward!$C$2:$D$12, IF(J175="3", Ward!$E$2:$F$15, IF(J175="4", Ward!$G$2:$H$16, IF(J175="5", Ward!$I$2:$J$16, IF(J175="6", Ward!$K$2:$L$15, IF(J175="7", Ward!$M$2:$N$11, IF(J175="8", Ward!$O$2:$P$17, IF(J175="9", Ward!$Q$2:$R$14, IF(J175="10", Ward!$S$2:$T$16, IF(J175="11", Ward!$U$2:$V$17, IF(J175="12", Ward!$W$2:$X$12, IF(J175="Bình Chánh", Ward!$Y$2:$Z$17, IF(J175="Bình Tân", Ward!$AA$2:$AB$11, IF(J175="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J175="Cần Giờ", Ward!$AE$2:$AF$8, IF(J175="Củ Chi", Ward!$AG$2:$AH$22, IF(J175="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J175="Hóc Môn", Ward!$AK$2:$AL$13, IF(J175="Nhà Bè", Ward!$AM$2:$AN$8, IF(J175="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J175="Tân Bình", Ward!$AQ$2:$AR$16, IF(J175="Tân Phú", Ward!$AS$2:$AT$12, IF(J175="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="176" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X175" t="str">
+        <f>IF(B175 &lt;&gt; "", VLOOKUP(B175, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="176" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A176" s="3"/>
       <c r="B176" s="16"/>
       <c r="C176" s="16"/>
@@ -8137,8 +8866,12 @@
         <f>IF(K176 &lt;&gt; "", VLOOKUP(K176, IF(J176="1", Ward!$A$2:$B$11, IF(J176="2", Ward!$C$2:$D$12, IF(J176="3", Ward!$E$2:$F$15, IF(J176="4", Ward!$G$2:$H$16, IF(J176="5", Ward!$I$2:$J$16, IF(J176="6", Ward!$K$2:$L$15, IF(J176="7", Ward!$M$2:$N$11, IF(J176="8", Ward!$O$2:$P$17, IF(J176="9", Ward!$Q$2:$R$14, IF(J176="10", Ward!$S$2:$T$16, IF(J176="11", Ward!$U$2:$V$17, IF(J176="12", Ward!$W$2:$X$12, IF(J176="Bình Chánh", Ward!$Y$2:$Z$17, IF(J176="Bình Tân", Ward!$AA$2:$AB$11, IF(J176="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J176="Cần Giờ", Ward!$AE$2:$AF$8, IF(J176="Củ Chi", Ward!$AG$2:$AH$22, IF(J176="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J176="Hóc Môn", Ward!$AK$2:$AL$13, IF(J176="Nhà Bè", Ward!$AM$2:$AN$8, IF(J176="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J176="Tân Bình", Ward!$AQ$2:$AR$16, IF(J176="Tân Phú", Ward!$AS$2:$AT$12, IF(J176="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="177" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X176" t="str">
+        <f>IF(B176 &lt;&gt; "", VLOOKUP(B176, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="177" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A177" s="3"/>
       <c r="B177" s="16"/>
       <c r="C177" s="16"/>
@@ -8171,8 +8904,12 @@
         <f>IF(K177 &lt;&gt; "", VLOOKUP(K177, IF(J177="1", Ward!$A$2:$B$11, IF(J177="2", Ward!$C$2:$D$12, IF(J177="3", Ward!$E$2:$F$15, IF(J177="4", Ward!$G$2:$H$16, IF(J177="5", Ward!$I$2:$J$16, IF(J177="6", Ward!$K$2:$L$15, IF(J177="7", Ward!$M$2:$N$11, IF(J177="8", Ward!$O$2:$P$17, IF(J177="9", Ward!$Q$2:$R$14, IF(J177="10", Ward!$S$2:$T$16, IF(J177="11", Ward!$U$2:$V$17, IF(J177="12", Ward!$W$2:$X$12, IF(J177="Bình Chánh", Ward!$Y$2:$Z$17, IF(J177="Bình Tân", Ward!$AA$2:$AB$11, IF(J177="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J177="Cần Giờ", Ward!$AE$2:$AF$8, IF(J177="Củ Chi", Ward!$AG$2:$AH$22, IF(J177="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J177="Hóc Môn", Ward!$AK$2:$AL$13, IF(J177="Nhà Bè", Ward!$AM$2:$AN$8, IF(J177="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J177="Tân Bình", Ward!$AQ$2:$AR$16, IF(J177="Tân Phú", Ward!$AS$2:$AT$12, IF(J177="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="178" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X177" t="str">
+        <f>IF(B177 &lt;&gt; "", VLOOKUP(B177, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="178" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A178" s="3"/>
       <c r="B178" s="16"/>
       <c r="C178" s="16"/>
@@ -8205,8 +8942,12 @@
         <f>IF(K178 &lt;&gt; "", VLOOKUP(K178, IF(J178="1", Ward!$A$2:$B$11, IF(J178="2", Ward!$C$2:$D$12, IF(J178="3", Ward!$E$2:$F$15, IF(J178="4", Ward!$G$2:$H$16, IF(J178="5", Ward!$I$2:$J$16, IF(J178="6", Ward!$K$2:$L$15, IF(J178="7", Ward!$M$2:$N$11, IF(J178="8", Ward!$O$2:$P$17, IF(J178="9", Ward!$Q$2:$R$14, IF(J178="10", Ward!$S$2:$T$16, IF(J178="11", Ward!$U$2:$V$17, IF(J178="12", Ward!$W$2:$X$12, IF(J178="Bình Chánh", Ward!$Y$2:$Z$17, IF(J178="Bình Tân", Ward!$AA$2:$AB$11, IF(J178="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J178="Cần Giờ", Ward!$AE$2:$AF$8, IF(J178="Củ Chi", Ward!$AG$2:$AH$22, IF(J178="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J178="Hóc Môn", Ward!$AK$2:$AL$13, IF(J178="Nhà Bè", Ward!$AM$2:$AN$8, IF(J178="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J178="Tân Bình", Ward!$AQ$2:$AR$16, IF(J178="Tân Phú", Ward!$AS$2:$AT$12, IF(J178="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="179" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X178" t="str">
+        <f>IF(B178 &lt;&gt; "", VLOOKUP(B178, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="179" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A179" s="3"/>
       <c r="B179" s="16"/>
       <c r="C179" s="16"/>
@@ -8239,8 +8980,12 @@
         <f>IF(K179 &lt;&gt; "", VLOOKUP(K179, IF(J179="1", Ward!$A$2:$B$11, IF(J179="2", Ward!$C$2:$D$12, IF(J179="3", Ward!$E$2:$F$15, IF(J179="4", Ward!$G$2:$H$16, IF(J179="5", Ward!$I$2:$J$16, IF(J179="6", Ward!$K$2:$L$15, IF(J179="7", Ward!$M$2:$N$11, IF(J179="8", Ward!$O$2:$P$17, IF(J179="9", Ward!$Q$2:$R$14, IF(J179="10", Ward!$S$2:$T$16, IF(J179="11", Ward!$U$2:$V$17, IF(J179="12", Ward!$W$2:$X$12, IF(J179="Bình Chánh", Ward!$Y$2:$Z$17, IF(J179="Bình Tân", Ward!$AA$2:$AB$11, IF(J179="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J179="Cần Giờ", Ward!$AE$2:$AF$8, IF(J179="Củ Chi", Ward!$AG$2:$AH$22, IF(J179="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J179="Hóc Môn", Ward!$AK$2:$AL$13, IF(J179="Nhà Bè", Ward!$AM$2:$AN$8, IF(J179="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J179="Tân Bình", Ward!$AQ$2:$AR$16, IF(J179="Tân Phú", Ward!$AS$2:$AT$12, IF(J179="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="180" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X179" t="str">
+        <f>IF(B179 &lt;&gt; "", VLOOKUP(B179, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="180" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A180" s="3"/>
       <c r="B180" s="16"/>
       <c r="C180" s="16"/>
@@ -8273,8 +9018,12 @@
         <f>IF(K180 &lt;&gt; "", VLOOKUP(K180, IF(J180="1", Ward!$A$2:$B$11, IF(J180="2", Ward!$C$2:$D$12, IF(J180="3", Ward!$E$2:$F$15, IF(J180="4", Ward!$G$2:$H$16, IF(J180="5", Ward!$I$2:$J$16, IF(J180="6", Ward!$K$2:$L$15, IF(J180="7", Ward!$M$2:$N$11, IF(J180="8", Ward!$O$2:$P$17, IF(J180="9", Ward!$Q$2:$R$14, IF(J180="10", Ward!$S$2:$T$16, IF(J180="11", Ward!$U$2:$V$17, IF(J180="12", Ward!$W$2:$X$12, IF(J180="Bình Chánh", Ward!$Y$2:$Z$17, IF(J180="Bình Tân", Ward!$AA$2:$AB$11, IF(J180="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J180="Cần Giờ", Ward!$AE$2:$AF$8, IF(J180="Củ Chi", Ward!$AG$2:$AH$22, IF(J180="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J180="Hóc Môn", Ward!$AK$2:$AL$13, IF(J180="Nhà Bè", Ward!$AM$2:$AN$8, IF(J180="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J180="Tân Bình", Ward!$AQ$2:$AR$16, IF(J180="Tân Phú", Ward!$AS$2:$AT$12, IF(J180="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="181" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X180" t="str">
+        <f>IF(B180 &lt;&gt; "", VLOOKUP(B180, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="181" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A181" s="3"/>
       <c r="B181" s="16"/>
       <c r="C181" s="16"/>
@@ -8307,8 +9056,12 @@
         <f>IF(K181 &lt;&gt; "", VLOOKUP(K181, IF(J181="1", Ward!$A$2:$B$11, IF(J181="2", Ward!$C$2:$D$12, IF(J181="3", Ward!$E$2:$F$15, IF(J181="4", Ward!$G$2:$H$16, IF(J181="5", Ward!$I$2:$J$16, IF(J181="6", Ward!$K$2:$L$15, IF(J181="7", Ward!$M$2:$N$11, IF(J181="8", Ward!$O$2:$P$17, IF(J181="9", Ward!$Q$2:$R$14, IF(J181="10", Ward!$S$2:$T$16, IF(J181="11", Ward!$U$2:$V$17, IF(J181="12", Ward!$W$2:$X$12, IF(J181="Bình Chánh", Ward!$Y$2:$Z$17, IF(J181="Bình Tân", Ward!$AA$2:$AB$11, IF(J181="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J181="Cần Giờ", Ward!$AE$2:$AF$8, IF(J181="Củ Chi", Ward!$AG$2:$AH$22, IF(J181="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J181="Hóc Môn", Ward!$AK$2:$AL$13, IF(J181="Nhà Bè", Ward!$AM$2:$AN$8, IF(J181="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J181="Tân Bình", Ward!$AQ$2:$AR$16, IF(J181="Tân Phú", Ward!$AS$2:$AT$12, IF(J181="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="182" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X181" t="str">
+        <f>IF(B181 &lt;&gt; "", VLOOKUP(B181, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="182" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A182" s="3"/>
       <c r="B182" s="16"/>
       <c r="C182" s="16"/>
@@ -8341,8 +9094,12 @@
         <f>IF(K182 &lt;&gt; "", VLOOKUP(K182, IF(J182="1", Ward!$A$2:$B$11, IF(J182="2", Ward!$C$2:$D$12, IF(J182="3", Ward!$E$2:$F$15, IF(J182="4", Ward!$G$2:$H$16, IF(J182="5", Ward!$I$2:$J$16, IF(J182="6", Ward!$K$2:$L$15, IF(J182="7", Ward!$M$2:$N$11, IF(J182="8", Ward!$O$2:$P$17, IF(J182="9", Ward!$Q$2:$R$14, IF(J182="10", Ward!$S$2:$T$16, IF(J182="11", Ward!$U$2:$V$17, IF(J182="12", Ward!$W$2:$X$12, IF(J182="Bình Chánh", Ward!$Y$2:$Z$17, IF(J182="Bình Tân", Ward!$AA$2:$AB$11, IF(J182="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J182="Cần Giờ", Ward!$AE$2:$AF$8, IF(J182="Củ Chi", Ward!$AG$2:$AH$22, IF(J182="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J182="Hóc Môn", Ward!$AK$2:$AL$13, IF(J182="Nhà Bè", Ward!$AM$2:$AN$8, IF(J182="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J182="Tân Bình", Ward!$AQ$2:$AR$16, IF(J182="Tân Phú", Ward!$AS$2:$AT$12, IF(J182="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="183" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X182" t="str">
+        <f>IF(B182 &lt;&gt; "", VLOOKUP(B182, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="183" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A183" s="3"/>
       <c r="B183" s="16"/>
       <c r="C183" s="16"/>
@@ -8375,8 +9132,12 @@
         <f>IF(K183 &lt;&gt; "", VLOOKUP(K183, IF(J183="1", Ward!$A$2:$B$11, IF(J183="2", Ward!$C$2:$D$12, IF(J183="3", Ward!$E$2:$F$15, IF(J183="4", Ward!$G$2:$H$16, IF(J183="5", Ward!$I$2:$J$16, IF(J183="6", Ward!$K$2:$L$15, IF(J183="7", Ward!$M$2:$N$11, IF(J183="8", Ward!$O$2:$P$17, IF(J183="9", Ward!$Q$2:$R$14, IF(J183="10", Ward!$S$2:$T$16, IF(J183="11", Ward!$U$2:$V$17, IF(J183="12", Ward!$W$2:$X$12, IF(J183="Bình Chánh", Ward!$Y$2:$Z$17, IF(J183="Bình Tân", Ward!$AA$2:$AB$11, IF(J183="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J183="Cần Giờ", Ward!$AE$2:$AF$8, IF(J183="Củ Chi", Ward!$AG$2:$AH$22, IF(J183="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J183="Hóc Môn", Ward!$AK$2:$AL$13, IF(J183="Nhà Bè", Ward!$AM$2:$AN$8, IF(J183="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J183="Tân Bình", Ward!$AQ$2:$AR$16, IF(J183="Tân Phú", Ward!$AS$2:$AT$12, IF(J183="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="184" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X183" t="str">
+        <f>IF(B183 &lt;&gt; "", VLOOKUP(B183, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="184" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A184" s="3"/>
       <c r="B184" s="16"/>
       <c r="C184" s="16"/>
@@ -8409,8 +9170,12 @@
         <f>IF(K184 &lt;&gt; "", VLOOKUP(K184, IF(J184="1", Ward!$A$2:$B$11, IF(J184="2", Ward!$C$2:$D$12, IF(J184="3", Ward!$E$2:$F$15, IF(J184="4", Ward!$G$2:$H$16, IF(J184="5", Ward!$I$2:$J$16, IF(J184="6", Ward!$K$2:$L$15, IF(J184="7", Ward!$M$2:$N$11, IF(J184="8", Ward!$O$2:$P$17, IF(J184="9", Ward!$Q$2:$R$14, IF(J184="10", Ward!$S$2:$T$16, IF(J184="11", Ward!$U$2:$V$17, IF(J184="12", Ward!$W$2:$X$12, IF(J184="Bình Chánh", Ward!$Y$2:$Z$17, IF(J184="Bình Tân", Ward!$AA$2:$AB$11, IF(J184="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J184="Cần Giờ", Ward!$AE$2:$AF$8, IF(J184="Củ Chi", Ward!$AG$2:$AH$22, IF(J184="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J184="Hóc Môn", Ward!$AK$2:$AL$13, IF(J184="Nhà Bè", Ward!$AM$2:$AN$8, IF(J184="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J184="Tân Bình", Ward!$AQ$2:$AR$16, IF(J184="Tân Phú", Ward!$AS$2:$AT$12, IF(J184="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="185" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X184" t="str">
+        <f>IF(B184 &lt;&gt; "", VLOOKUP(B184, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="185" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A185" s="3"/>
       <c r="B185" s="16"/>
       <c r="C185" s="16"/>
@@ -8443,8 +9208,12 @@
         <f>IF(K185 &lt;&gt; "", VLOOKUP(K185, IF(J185="1", Ward!$A$2:$B$11, IF(J185="2", Ward!$C$2:$D$12, IF(J185="3", Ward!$E$2:$F$15, IF(J185="4", Ward!$G$2:$H$16, IF(J185="5", Ward!$I$2:$J$16, IF(J185="6", Ward!$K$2:$L$15, IF(J185="7", Ward!$M$2:$N$11, IF(J185="8", Ward!$O$2:$P$17, IF(J185="9", Ward!$Q$2:$R$14, IF(J185="10", Ward!$S$2:$T$16, IF(J185="11", Ward!$U$2:$V$17, IF(J185="12", Ward!$W$2:$X$12, IF(J185="Bình Chánh", Ward!$Y$2:$Z$17, IF(J185="Bình Tân", Ward!$AA$2:$AB$11, IF(J185="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J185="Cần Giờ", Ward!$AE$2:$AF$8, IF(J185="Củ Chi", Ward!$AG$2:$AH$22, IF(J185="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J185="Hóc Môn", Ward!$AK$2:$AL$13, IF(J185="Nhà Bè", Ward!$AM$2:$AN$8, IF(J185="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J185="Tân Bình", Ward!$AQ$2:$AR$16, IF(J185="Tân Phú", Ward!$AS$2:$AT$12, IF(J185="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="186" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X185" t="str">
+        <f>IF(B185 &lt;&gt; "", VLOOKUP(B185, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="186" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A186" s="3"/>
       <c r="B186" s="16"/>
       <c r="C186" s="16"/>
@@ -8477,8 +9246,12 @@
         <f>IF(K186 &lt;&gt; "", VLOOKUP(K186, IF(J186="1", Ward!$A$2:$B$11, IF(J186="2", Ward!$C$2:$D$12, IF(J186="3", Ward!$E$2:$F$15, IF(J186="4", Ward!$G$2:$H$16, IF(J186="5", Ward!$I$2:$J$16, IF(J186="6", Ward!$K$2:$L$15, IF(J186="7", Ward!$M$2:$N$11, IF(J186="8", Ward!$O$2:$P$17, IF(J186="9", Ward!$Q$2:$R$14, IF(J186="10", Ward!$S$2:$T$16, IF(J186="11", Ward!$U$2:$V$17, IF(J186="12", Ward!$W$2:$X$12, IF(J186="Bình Chánh", Ward!$Y$2:$Z$17, IF(J186="Bình Tân", Ward!$AA$2:$AB$11, IF(J186="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J186="Cần Giờ", Ward!$AE$2:$AF$8, IF(J186="Củ Chi", Ward!$AG$2:$AH$22, IF(J186="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J186="Hóc Môn", Ward!$AK$2:$AL$13, IF(J186="Nhà Bè", Ward!$AM$2:$AN$8, IF(J186="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J186="Tân Bình", Ward!$AQ$2:$AR$16, IF(J186="Tân Phú", Ward!$AS$2:$AT$12, IF(J186="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="187" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X186" t="str">
+        <f>IF(B186 &lt;&gt; "", VLOOKUP(B186, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="187" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A187" s="3"/>
       <c r="B187" s="16"/>
       <c r="C187" s="16"/>
@@ -8511,8 +9284,12 @@
         <f>IF(K187 &lt;&gt; "", VLOOKUP(K187, IF(J187="1", Ward!$A$2:$B$11, IF(J187="2", Ward!$C$2:$D$12, IF(J187="3", Ward!$E$2:$F$15, IF(J187="4", Ward!$G$2:$H$16, IF(J187="5", Ward!$I$2:$J$16, IF(J187="6", Ward!$K$2:$L$15, IF(J187="7", Ward!$M$2:$N$11, IF(J187="8", Ward!$O$2:$P$17, IF(J187="9", Ward!$Q$2:$R$14, IF(J187="10", Ward!$S$2:$T$16, IF(J187="11", Ward!$U$2:$V$17, IF(J187="12", Ward!$W$2:$X$12, IF(J187="Bình Chánh", Ward!$Y$2:$Z$17, IF(J187="Bình Tân", Ward!$AA$2:$AB$11, IF(J187="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J187="Cần Giờ", Ward!$AE$2:$AF$8, IF(J187="Củ Chi", Ward!$AG$2:$AH$22, IF(J187="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J187="Hóc Môn", Ward!$AK$2:$AL$13, IF(J187="Nhà Bè", Ward!$AM$2:$AN$8, IF(J187="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J187="Tân Bình", Ward!$AQ$2:$AR$16, IF(J187="Tân Phú", Ward!$AS$2:$AT$12, IF(J187="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="188" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X187" t="str">
+        <f>IF(B187 &lt;&gt; "", VLOOKUP(B187, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="188" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A188" s="3"/>
       <c r="B188" s="16"/>
       <c r="C188" s="16"/>
@@ -8545,8 +9322,12 @@
         <f>IF(K188 &lt;&gt; "", VLOOKUP(K188, IF(J188="1", Ward!$A$2:$B$11, IF(J188="2", Ward!$C$2:$D$12, IF(J188="3", Ward!$E$2:$F$15, IF(J188="4", Ward!$G$2:$H$16, IF(J188="5", Ward!$I$2:$J$16, IF(J188="6", Ward!$K$2:$L$15, IF(J188="7", Ward!$M$2:$N$11, IF(J188="8", Ward!$O$2:$P$17, IF(J188="9", Ward!$Q$2:$R$14, IF(J188="10", Ward!$S$2:$T$16, IF(J188="11", Ward!$U$2:$V$17, IF(J188="12", Ward!$W$2:$X$12, IF(J188="Bình Chánh", Ward!$Y$2:$Z$17, IF(J188="Bình Tân", Ward!$AA$2:$AB$11, IF(J188="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J188="Cần Giờ", Ward!$AE$2:$AF$8, IF(J188="Củ Chi", Ward!$AG$2:$AH$22, IF(J188="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J188="Hóc Môn", Ward!$AK$2:$AL$13, IF(J188="Nhà Bè", Ward!$AM$2:$AN$8, IF(J188="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J188="Tân Bình", Ward!$AQ$2:$AR$16, IF(J188="Tân Phú", Ward!$AS$2:$AT$12, IF(J188="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="189" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X188" t="str">
+        <f>IF(B188 &lt;&gt; "", VLOOKUP(B188, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="189" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A189" s="3"/>
       <c r="B189" s="16"/>
       <c r="C189" s="16"/>
@@ -8579,8 +9360,12 @@
         <f>IF(K189 &lt;&gt; "", VLOOKUP(K189, IF(J189="1", Ward!$A$2:$B$11, IF(J189="2", Ward!$C$2:$D$12, IF(J189="3", Ward!$E$2:$F$15, IF(J189="4", Ward!$G$2:$H$16, IF(J189="5", Ward!$I$2:$J$16, IF(J189="6", Ward!$K$2:$L$15, IF(J189="7", Ward!$M$2:$N$11, IF(J189="8", Ward!$O$2:$P$17, IF(J189="9", Ward!$Q$2:$R$14, IF(J189="10", Ward!$S$2:$T$16, IF(J189="11", Ward!$U$2:$V$17, IF(J189="12", Ward!$W$2:$X$12, IF(J189="Bình Chánh", Ward!$Y$2:$Z$17, IF(J189="Bình Tân", Ward!$AA$2:$AB$11, IF(J189="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J189="Cần Giờ", Ward!$AE$2:$AF$8, IF(J189="Củ Chi", Ward!$AG$2:$AH$22, IF(J189="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J189="Hóc Môn", Ward!$AK$2:$AL$13, IF(J189="Nhà Bè", Ward!$AM$2:$AN$8, IF(J189="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J189="Tân Bình", Ward!$AQ$2:$AR$16, IF(J189="Tân Phú", Ward!$AS$2:$AT$12, IF(J189="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="190" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X189" t="str">
+        <f>IF(B189 &lt;&gt; "", VLOOKUP(B189, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="190" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A190" s="3"/>
       <c r="B190" s="16"/>
       <c r="C190" s="16"/>
@@ -8613,8 +9398,12 @@
         <f>IF(K190 &lt;&gt; "", VLOOKUP(K190, IF(J190="1", Ward!$A$2:$B$11, IF(J190="2", Ward!$C$2:$D$12, IF(J190="3", Ward!$E$2:$F$15, IF(J190="4", Ward!$G$2:$H$16, IF(J190="5", Ward!$I$2:$J$16, IF(J190="6", Ward!$K$2:$L$15, IF(J190="7", Ward!$M$2:$N$11, IF(J190="8", Ward!$O$2:$P$17, IF(J190="9", Ward!$Q$2:$R$14, IF(J190="10", Ward!$S$2:$T$16, IF(J190="11", Ward!$U$2:$V$17, IF(J190="12", Ward!$W$2:$X$12, IF(J190="Bình Chánh", Ward!$Y$2:$Z$17, IF(J190="Bình Tân", Ward!$AA$2:$AB$11, IF(J190="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J190="Cần Giờ", Ward!$AE$2:$AF$8, IF(J190="Củ Chi", Ward!$AG$2:$AH$22, IF(J190="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J190="Hóc Môn", Ward!$AK$2:$AL$13, IF(J190="Nhà Bè", Ward!$AM$2:$AN$8, IF(J190="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J190="Tân Bình", Ward!$AQ$2:$AR$16, IF(J190="Tân Phú", Ward!$AS$2:$AT$12, IF(J190="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="191" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X190" t="str">
+        <f>IF(B190 &lt;&gt; "", VLOOKUP(B190, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="191" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A191" s="3"/>
       <c r="B191" s="16"/>
       <c r="C191" s="16"/>
@@ -8647,8 +9436,12 @@
         <f>IF(K191 &lt;&gt; "", VLOOKUP(K191, IF(J191="1", Ward!$A$2:$B$11, IF(J191="2", Ward!$C$2:$D$12, IF(J191="3", Ward!$E$2:$F$15, IF(J191="4", Ward!$G$2:$H$16, IF(J191="5", Ward!$I$2:$J$16, IF(J191="6", Ward!$K$2:$L$15, IF(J191="7", Ward!$M$2:$N$11, IF(J191="8", Ward!$O$2:$P$17, IF(J191="9", Ward!$Q$2:$R$14, IF(J191="10", Ward!$S$2:$T$16, IF(J191="11", Ward!$U$2:$V$17, IF(J191="12", Ward!$W$2:$X$12, IF(J191="Bình Chánh", Ward!$Y$2:$Z$17, IF(J191="Bình Tân", Ward!$AA$2:$AB$11, IF(J191="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J191="Cần Giờ", Ward!$AE$2:$AF$8, IF(J191="Củ Chi", Ward!$AG$2:$AH$22, IF(J191="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J191="Hóc Môn", Ward!$AK$2:$AL$13, IF(J191="Nhà Bè", Ward!$AM$2:$AN$8, IF(J191="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J191="Tân Bình", Ward!$AQ$2:$AR$16, IF(J191="Tân Phú", Ward!$AS$2:$AT$12, IF(J191="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="192" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X191" t="str">
+        <f>IF(B191 &lt;&gt; "", VLOOKUP(B191, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="192" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A192" s="3"/>
       <c r="B192" s="16"/>
       <c r="C192" s="16"/>
@@ -8681,8 +9474,12 @@
         <f>IF(K192 &lt;&gt; "", VLOOKUP(K192, IF(J192="1", Ward!$A$2:$B$11, IF(J192="2", Ward!$C$2:$D$12, IF(J192="3", Ward!$E$2:$F$15, IF(J192="4", Ward!$G$2:$H$16, IF(J192="5", Ward!$I$2:$J$16, IF(J192="6", Ward!$K$2:$L$15, IF(J192="7", Ward!$M$2:$N$11, IF(J192="8", Ward!$O$2:$P$17, IF(J192="9", Ward!$Q$2:$R$14, IF(J192="10", Ward!$S$2:$T$16, IF(J192="11", Ward!$U$2:$V$17, IF(J192="12", Ward!$W$2:$X$12, IF(J192="Bình Chánh", Ward!$Y$2:$Z$17, IF(J192="Bình Tân", Ward!$AA$2:$AB$11, IF(J192="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J192="Cần Giờ", Ward!$AE$2:$AF$8, IF(J192="Củ Chi", Ward!$AG$2:$AH$22, IF(J192="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J192="Hóc Môn", Ward!$AK$2:$AL$13, IF(J192="Nhà Bè", Ward!$AM$2:$AN$8, IF(J192="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J192="Tân Bình", Ward!$AQ$2:$AR$16, IF(J192="Tân Phú", Ward!$AS$2:$AT$12, IF(J192="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="193" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X192" t="str">
+        <f>IF(B192 &lt;&gt; "", VLOOKUP(B192, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="193" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A193" s="3"/>
       <c r="B193" s="16"/>
       <c r="C193" s="16"/>
@@ -8715,8 +9512,12 @@
         <f>IF(K193 &lt;&gt; "", VLOOKUP(K193, IF(J193="1", Ward!$A$2:$B$11, IF(J193="2", Ward!$C$2:$D$12, IF(J193="3", Ward!$E$2:$F$15, IF(J193="4", Ward!$G$2:$H$16, IF(J193="5", Ward!$I$2:$J$16, IF(J193="6", Ward!$K$2:$L$15, IF(J193="7", Ward!$M$2:$N$11, IF(J193="8", Ward!$O$2:$P$17, IF(J193="9", Ward!$Q$2:$R$14, IF(J193="10", Ward!$S$2:$T$16, IF(J193="11", Ward!$U$2:$V$17, IF(J193="12", Ward!$W$2:$X$12, IF(J193="Bình Chánh", Ward!$Y$2:$Z$17, IF(J193="Bình Tân", Ward!$AA$2:$AB$11, IF(J193="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J193="Cần Giờ", Ward!$AE$2:$AF$8, IF(J193="Củ Chi", Ward!$AG$2:$AH$22, IF(J193="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J193="Hóc Môn", Ward!$AK$2:$AL$13, IF(J193="Nhà Bè", Ward!$AM$2:$AN$8, IF(J193="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J193="Tân Bình", Ward!$AQ$2:$AR$16, IF(J193="Tân Phú", Ward!$AS$2:$AT$12, IF(J193="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="194" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X193" t="str">
+        <f>IF(B193 &lt;&gt; "", VLOOKUP(B193, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="194" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A194" s="3"/>
       <c r="B194" s="16"/>
       <c r="C194" s="16"/>
@@ -8749,8 +9550,12 @@
         <f>IF(K194 &lt;&gt; "", VLOOKUP(K194, IF(J194="1", Ward!$A$2:$B$11, IF(J194="2", Ward!$C$2:$D$12, IF(J194="3", Ward!$E$2:$F$15, IF(J194="4", Ward!$G$2:$H$16, IF(J194="5", Ward!$I$2:$J$16, IF(J194="6", Ward!$K$2:$L$15, IF(J194="7", Ward!$M$2:$N$11, IF(J194="8", Ward!$O$2:$P$17, IF(J194="9", Ward!$Q$2:$R$14, IF(J194="10", Ward!$S$2:$T$16, IF(J194="11", Ward!$U$2:$V$17, IF(J194="12", Ward!$W$2:$X$12, IF(J194="Bình Chánh", Ward!$Y$2:$Z$17, IF(J194="Bình Tân", Ward!$AA$2:$AB$11, IF(J194="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J194="Cần Giờ", Ward!$AE$2:$AF$8, IF(J194="Củ Chi", Ward!$AG$2:$AH$22, IF(J194="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J194="Hóc Môn", Ward!$AK$2:$AL$13, IF(J194="Nhà Bè", Ward!$AM$2:$AN$8, IF(J194="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J194="Tân Bình", Ward!$AQ$2:$AR$16, IF(J194="Tân Phú", Ward!$AS$2:$AT$12, IF(J194="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="195" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X194" t="str">
+        <f>IF(B194 &lt;&gt; "", VLOOKUP(B194, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="195" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A195" s="3"/>
       <c r="B195" s="16"/>
       <c r="C195" s="16"/>
@@ -8783,8 +9588,12 @@
         <f>IF(K195 &lt;&gt; "", VLOOKUP(K195, IF(J195="1", Ward!$A$2:$B$11, IF(J195="2", Ward!$C$2:$D$12, IF(J195="3", Ward!$E$2:$F$15, IF(J195="4", Ward!$G$2:$H$16, IF(J195="5", Ward!$I$2:$J$16, IF(J195="6", Ward!$K$2:$L$15, IF(J195="7", Ward!$M$2:$N$11, IF(J195="8", Ward!$O$2:$P$17, IF(J195="9", Ward!$Q$2:$R$14, IF(J195="10", Ward!$S$2:$T$16, IF(J195="11", Ward!$U$2:$V$17, IF(J195="12", Ward!$W$2:$X$12, IF(J195="Bình Chánh", Ward!$Y$2:$Z$17, IF(J195="Bình Tân", Ward!$AA$2:$AB$11, IF(J195="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J195="Cần Giờ", Ward!$AE$2:$AF$8, IF(J195="Củ Chi", Ward!$AG$2:$AH$22, IF(J195="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J195="Hóc Môn", Ward!$AK$2:$AL$13, IF(J195="Nhà Bè", Ward!$AM$2:$AN$8, IF(J195="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J195="Tân Bình", Ward!$AQ$2:$AR$16, IF(J195="Tân Phú", Ward!$AS$2:$AT$12, IF(J195="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="196" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X195" t="str">
+        <f>IF(B195 &lt;&gt; "", VLOOKUP(B195, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="196" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A196" s="3"/>
       <c r="B196" s="16"/>
       <c r="C196" s="16"/>
@@ -8817,8 +9626,12 @@
         <f>IF(K196 &lt;&gt; "", VLOOKUP(K196, IF(J196="1", Ward!$A$2:$B$11, IF(J196="2", Ward!$C$2:$D$12, IF(J196="3", Ward!$E$2:$F$15, IF(J196="4", Ward!$G$2:$H$16, IF(J196="5", Ward!$I$2:$J$16, IF(J196="6", Ward!$K$2:$L$15, IF(J196="7", Ward!$M$2:$N$11, IF(J196="8", Ward!$O$2:$P$17, IF(J196="9", Ward!$Q$2:$R$14, IF(J196="10", Ward!$S$2:$T$16, IF(J196="11", Ward!$U$2:$V$17, IF(J196="12", Ward!$W$2:$X$12, IF(J196="Bình Chánh", Ward!$Y$2:$Z$17, IF(J196="Bình Tân", Ward!$AA$2:$AB$11, IF(J196="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J196="Cần Giờ", Ward!$AE$2:$AF$8, IF(J196="Củ Chi", Ward!$AG$2:$AH$22, IF(J196="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J196="Hóc Môn", Ward!$AK$2:$AL$13, IF(J196="Nhà Bè", Ward!$AM$2:$AN$8, IF(J196="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J196="Tân Bình", Ward!$AQ$2:$AR$16, IF(J196="Tân Phú", Ward!$AS$2:$AT$12, IF(J196="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="197" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X196" t="str">
+        <f>IF(B196 &lt;&gt; "", VLOOKUP(B196, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="197" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A197" s="3"/>
       <c r="B197" s="16"/>
       <c r="C197" s="16"/>
@@ -8851,8 +9664,12 @@
         <f>IF(K197 &lt;&gt; "", VLOOKUP(K197, IF(J197="1", Ward!$A$2:$B$11, IF(J197="2", Ward!$C$2:$D$12, IF(J197="3", Ward!$E$2:$F$15, IF(J197="4", Ward!$G$2:$H$16, IF(J197="5", Ward!$I$2:$J$16, IF(J197="6", Ward!$K$2:$L$15, IF(J197="7", Ward!$M$2:$N$11, IF(J197="8", Ward!$O$2:$P$17, IF(J197="9", Ward!$Q$2:$R$14, IF(J197="10", Ward!$S$2:$T$16, IF(J197="11", Ward!$U$2:$V$17, IF(J197="12", Ward!$W$2:$X$12, IF(J197="Bình Chánh", Ward!$Y$2:$Z$17, IF(J197="Bình Tân", Ward!$AA$2:$AB$11, IF(J197="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J197="Cần Giờ", Ward!$AE$2:$AF$8, IF(J197="Củ Chi", Ward!$AG$2:$AH$22, IF(J197="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J197="Hóc Môn", Ward!$AK$2:$AL$13, IF(J197="Nhà Bè", Ward!$AM$2:$AN$8, IF(J197="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J197="Tân Bình", Ward!$AQ$2:$AR$16, IF(J197="Tân Phú", Ward!$AS$2:$AT$12, IF(J197="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="198" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X197" t="str">
+        <f>IF(B197 &lt;&gt; "", VLOOKUP(B197, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="198" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A198" s="3"/>
       <c r="B198" s="16"/>
       <c r="C198" s="16"/>
@@ -8885,8 +9702,12 @@
         <f>IF(K198 &lt;&gt; "", VLOOKUP(K198, IF(J198="1", Ward!$A$2:$B$11, IF(J198="2", Ward!$C$2:$D$12, IF(J198="3", Ward!$E$2:$F$15, IF(J198="4", Ward!$G$2:$H$16, IF(J198="5", Ward!$I$2:$J$16, IF(J198="6", Ward!$K$2:$L$15, IF(J198="7", Ward!$M$2:$N$11, IF(J198="8", Ward!$O$2:$P$17, IF(J198="9", Ward!$Q$2:$R$14, IF(J198="10", Ward!$S$2:$T$16, IF(J198="11", Ward!$U$2:$V$17, IF(J198="12", Ward!$W$2:$X$12, IF(J198="Bình Chánh", Ward!$Y$2:$Z$17, IF(J198="Bình Tân", Ward!$AA$2:$AB$11, IF(J198="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J198="Cần Giờ", Ward!$AE$2:$AF$8, IF(J198="Củ Chi", Ward!$AG$2:$AH$22, IF(J198="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J198="Hóc Môn", Ward!$AK$2:$AL$13, IF(J198="Nhà Bè", Ward!$AM$2:$AN$8, IF(J198="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J198="Tân Bình", Ward!$AQ$2:$AR$16, IF(J198="Tân Phú", Ward!$AS$2:$AT$12, IF(J198="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="199" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X198" t="str">
+        <f>IF(B198 &lt;&gt; "", VLOOKUP(B198, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="199" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A199" s="3"/>
       <c r="B199" s="16"/>
       <c r="C199" s="16"/>
@@ -8919,8 +9740,12 @@
         <f>IF(K199 &lt;&gt; "", VLOOKUP(K199, IF(J199="1", Ward!$A$2:$B$11, IF(J199="2", Ward!$C$2:$D$12, IF(J199="3", Ward!$E$2:$F$15, IF(J199="4", Ward!$G$2:$H$16, IF(J199="5", Ward!$I$2:$J$16, IF(J199="6", Ward!$K$2:$L$15, IF(J199="7", Ward!$M$2:$N$11, IF(J199="8", Ward!$O$2:$P$17, IF(J199="9", Ward!$Q$2:$R$14, IF(J199="10", Ward!$S$2:$T$16, IF(J199="11", Ward!$U$2:$V$17, IF(J199="12", Ward!$W$2:$X$12, IF(J199="Bình Chánh", Ward!$Y$2:$Z$17, IF(J199="Bình Tân", Ward!$AA$2:$AB$11, IF(J199="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J199="Cần Giờ", Ward!$AE$2:$AF$8, IF(J199="Củ Chi", Ward!$AG$2:$AH$22, IF(J199="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J199="Hóc Môn", Ward!$AK$2:$AL$13, IF(J199="Nhà Bè", Ward!$AM$2:$AN$8, IF(J199="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J199="Tân Bình", Ward!$AQ$2:$AR$16, IF(J199="Tân Phú", Ward!$AS$2:$AT$12, IF(J199="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="200" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X199" t="str">
+        <f>IF(B199 &lt;&gt; "", VLOOKUP(B199, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="200" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="4"/>
       <c r="B200" s="20"/>
       <c r="C200" s="20"/>
@@ -8953,9 +9778,13 @@
         <f>IF(K200 &lt;&gt; "", VLOOKUP(K200, IF(J200="1", Ward!$A$2:$B$11, IF(J200="2", Ward!$C$2:$D$12, IF(J200="3", Ward!$E$2:$F$15, IF(J200="4", Ward!$G$2:$H$16, IF(J200="5", Ward!$I$2:$J$16, IF(J200="6", Ward!$K$2:$L$15, IF(J200="7", Ward!$M$2:$N$11, IF(J200="8", Ward!$O$2:$P$17, IF(J200="9", Ward!$Q$2:$R$14, IF(J200="10", Ward!$S$2:$T$16, IF(J200="11", Ward!$U$2:$V$17, IF(J200="12", Ward!$W$2:$X$12, IF(J200="Bình Chánh", Ward!$Y$2:$Z$17, IF(J200="Bình Tân", Ward!$AA$2:$AB$11, IF(J200="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J200="Cần Giờ", Ward!$AE$2:$AF$8, IF(J200="Củ Chi", Ward!$AG$2:$AH$22, IF(J200="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J200="Hóc Môn", Ward!$AK$2:$AL$13, IF(J200="Nhà Bè", Ward!$AM$2:$AN$8, IF(J200="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J200="Tân Bình", Ward!$AQ$2:$AR$16, IF(J200="Tân Phú", Ward!$AS$2:$AT$12, IF(J200="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
+      <c r="X200" t="str">
+        <f>IF(B200 &lt;&gt; "", VLOOKUP(B200, HospitalType!$A$2:$B$9, 2, FALSE), "")</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
+  <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I200">
       <formula1>CityList</formula1>
     </dataValidation>
@@ -8973,6 +9802,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T200">
       <formula1>FacilityList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B200">
+      <formula1>HospitalTypeList</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9021,9 +9853,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12703,4 +13533,93 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="B3" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="B4" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="B5" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="B6" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="B7" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="B8" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="B9" s="10">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update mapping field for Excel file
</commit_message>
<xml_diff>
--- a/Source Code/HospitalF Import Template - Ho Chi Minh.xlsx
+++ b/Source Code/HospitalF Import Template - Ho Chi Minh.xlsx
@@ -687,12 +687,6 @@
     <t>Số di động</t>
   </si>
   <si>
-    <t>Email bệnh viện</t>
-  </si>
-  <si>
-    <t>Trang web bệnh viện</t>
-  </si>
-  <si>
     <t>Số fax</t>
   </si>
   <si>
@@ -855,9 +849,6 @@
     <t>Y học thể thao</t>
   </si>
   <si>
-    <t>Chuyên ngành</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -1539,15 +1530,6 @@
     <t>Thông báo tái khám qua tin nhắn</t>
   </si>
   <si>
-    <t>CityID</t>
-  </si>
-  <si>
-    <t>DistrictID</t>
-  </si>
-  <si>
-    <t>WardID</t>
-  </si>
-  <si>
     <t>Bệnh viện công</t>
   </si>
   <si>
@@ -1572,7 +1554,25 @@
     <t>Trung tâm y tế</t>
   </si>
   <si>
-    <t>HospitalTypeId</t>
+    <t>Type_ID</t>
+  </si>
+  <si>
+    <t>City_ID</t>
+  </si>
+  <si>
+    <t>District_ID</t>
+  </si>
+  <si>
+    <t>Ward_ID</t>
+  </si>
+  <si>
+    <t>Địa chỉ email</t>
+  </si>
+  <si>
+    <t>Địa chỉ trang web</t>
+  </si>
+  <si>
+    <t>Chuyên khoa</t>
   </si>
 </sst>
 </file>
@@ -1822,22 +1822,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2141,84 +2141,84 @@
     <col min="14" max="15" width="20.5703125" customWidth="1"/>
     <col min="16" max="17" width="32.85546875" customWidth="1"/>
     <col min="18" max="20" width="46.7109375" customWidth="1"/>
-    <col min="21" max="21" width="6.28515625" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="7.7109375" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="11" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="8.7109375" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="8.28515625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="25" t="s">
         <v>204</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="25" t="s">
         <v>205</v>
       </c>
-      <c r="O1" s="24" t="s">
-        <v>208</v>
-      </c>
-      <c r="P1" s="24" t="s">
+      <c r="O1" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="Q1" s="24" t="s">
-        <v>207</v>
-      </c>
-      <c r="R1" s="24" t="s">
-        <v>262</v>
-      </c>
-      <c r="S1" s="24" t="s">
-        <v>435</v>
-      </c>
-      <c r="T1" s="25" t="s">
-        <v>468</v>
-      </c>
-      <c r="U1" s="26" t="s">
-        <v>490</v>
-      </c>
-      <c r="V1" s="27" t="s">
-        <v>491</v>
-      </c>
-      <c r="W1" s="27" t="s">
-        <v>492</v>
-      </c>
-      <c r="X1" s="27" t="s">
+      <c r="P1" s="25" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>500</v>
+      </c>
+      <c r="R1" s="25" t="s">
         <v>501</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>432</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="U1" s="27" t="s">
+        <v>496</v>
+      </c>
+      <c r="V1" s="28" t="s">
+        <v>497</v>
+      </c>
+      <c r="W1" s="28" t="s">
+        <v>498</v>
+      </c>
+      <c r="X1" s="28" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -2250,7 +2250,7 @@
         <f>IF(J2 &lt;&gt; "", VLOOKUP(J2, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W2" s="28" t="str">
+      <c r="W2" s="23" t="str">
         <f>IF(K2 &lt;&gt; "", VLOOKUP(K2, IF(J2="1", Ward!$A$2:$B$11, IF(J2="2", Ward!$C$2:$D$12, IF(J2="3", Ward!$E$2:$F$15, IF(J2="4", Ward!$G$2:$H$16, IF(J2="5", Ward!$I$2:$J$16, IF(J2="6", Ward!$K$2:$L$15, IF(J2="7", Ward!$M$2:$N$11, IF(J2="8", Ward!$O$2:$P$17, IF(J2="9", Ward!$Q$2:$R$14, IF(J2="10", Ward!$S$2:$T$16, IF(J2="11", Ward!$U$2:$V$17, IF(J2="12", Ward!$W$2:$X$12, IF(J2="Bình Chánh", Ward!$Y$2:$Z$17, IF(J2="Bình Tân", Ward!$AA$2:$AB$11, IF(J2="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J2="Cần Giờ", Ward!$AE$2:$AF$8, IF(J2="Củ Chi", Ward!$AG$2:$AH$22, IF(J2="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J2="Hóc Môn", Ward!$AK$2:$AL$13, IF(J2="Nhà Bè", Ward!$AM$2:$AN$8, IF(J2="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J2="Tân Bình", Ward!$AQ$2:$AR$16, IF(J2="Tân Phú", Ward!$AS$2:$AT$12, IF(J2="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2288,7 +2288,7 @@
         <f>IF(J3 &lt;&gt; "", VLOOKUP(J3, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W3" s="28" t="str">
+      <c r="W3" s="23" t="str">
         <f>IF(K3 &lt;&gt; "", VLOOKUP(K3, IF(J3="1", Ward!$A$2:$B$11, IF(J3="2", Ward!$C$2:$D$12, IF(J3="3", Ward!$E$2:$F$15, IF(J3="4", Ward!$G$2:$H$16, IF(J3="5", Ward!$I$2:$J$16, IF(J3="6", Ward!$K$2:$L$15, IF(J3="7", Ward!$M$2:$N$11, IF(J3="8", Ward!$O$2:$P$17, IF(J3="9", Ward!$Q$2:$R$14, IF(J3="10", Ward!$S$2:$T$16, IF(J3="11", Ward!$U$2:$V$17, IF(J3="12", Ward!$W$2:$X$12, IF(J3="Bình Chánh", Ward!$Y$2:$Z$17, IF(J3="Bình Tân", Ward!$AA$2:$AB$11, IF(J3="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J3="Cần Giờ", Ward!$AE$2:$AF$8, IF(J3="Củ Chi", Ward!$AG$2:$AH$22, IF(J3="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J3="Hóc Môn", Ward!$AK$2:$AL$13, IF(J3="Nhà Bè", Ward!$AM$2:$AN$8, IF(J3="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J3="Tân Bình", Ward!$AQ$2:$AR$16, IF(J3="Tân Phú", Ward!$AS$2:$AT$12, IF(J3="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2326,7 +2326,7 @@
         <f>IF(J4 &lt;&gt; "", VLOOKUP(J4, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W4" s="28" t="str">
+      <c r="W4" s="23" t="str">
         <f>IF(K4 &lt;&gt; "", VLOOKUP(K4, IF(J4="1", Ward!$A$2:$B$11, IF(J4="2", Ward!$C$2:$D$12, IF(J4="3", Ward!$E$2:$F$15, IF(J4="4", Ward!$G$2:$H$16, IF(J4="5", Ward!$I$2:$J$16, IF(J4="6", Ward!$K$2:$L$15, IF(J4="7", Ward!$M$2:$N$11, IF(J4="8", Ward!$O$2:$P$17, IF(J4="9", Ward!$Q$2:$R$14, IF(J4="10", Ward!$S$2:$T$16, IF(J4="11", Ward!$U$2:$V$17, IF(J4="12", Ward!$W$2:$X$12, IF(J4="Bình Chánh", Ward!$Y$2:$Z$17, IF(J4="Bình Tân", Ward!$AA$2:$AB$11, IF(J4="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J4="Cần Giờ", Ward!$AE$2:$AF$8, IF(J4="Củ Chi", Ward!$AG$2:$AH$22, IF(J4="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J4="Hóc Môn", Ward!$AK$2:$AL$13, IF(J4="Nhà Bè", Ward!$AM$2:$AN$8, IF(J4="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J4="Tân Bình", Ward!$AQ$2:$AR$16, IF(J4="Tân Phú", Ward!$AS$2:$AT$12, IF(J4="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2364,7 +2364,7 @@
         <f>IF(J5 &lt;&gt; "", VLOOKUP(J5, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W5" s="28" t="str">
+      <c r="W5" s="23" t="str">
         <f>IF(K5 &lt;&gt; "", VLOOKUP(K5, IF(J5="1", Ward!$A$2:$B$11, IF(J5="2", Ward!$C$2:$D$12, IF(J5="3", Ward!$E$2:$F$15, IF(J5="4", Ward!$G$2:$H$16, IF(J5="5", Ward!$I$2:$J$16, IF(J5="6", Ward!$K$2:$L$15, IF(J5="7", Ward!$M$2:$N$11, IF(J5="8", Ward!$O$2:$P$17, IF(J5="9", Ward!$Q$2:$R$14, IF(J5="10", Ward!$S$2:$T$16, IF(J5="11", Ward!$U$2:$V$17, IF(J5="12", Ward!$W$2:$X$12, IF(J5="Bình Chánh", Ward!$Y$2:$Z$17, IF(J5="Bình Tân", Ward!$AA$2:$AB$11, IF(J5="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J5="Cần Giờ", Ward!$AE$2:$AF$8, IF(J5="Củ Chi", Ward!$AG$2:$AH$22, IF(J5="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J5="Hóc Môn", Ward!$AK$2:$AL$13, IF(J5="Nhà Bè", Ward!$AM$2:$AN$8, IF(J5="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J5="Tân Bình", Ward!$AQ$2:$AR$16, IF(J5="Tân Phú", Ward!$AS$2:$AT$12, IF(J5="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2402,7 +2402,7 @@
         <f>IF(J6 &lt;&gt; "", VLOOKUP(J6, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W6" s="28" t="str">
+      <c r="W6" s="23" t="str">
         <f>IF(K6 &lt;&gt; "", VLOOKUP(K6, IF(J6="1", Ward!$A$2:$B$11, IF(J6="2", Ward!$C$2:$D$12, IF(J6="3", Ward!$E$2:$F$15, IF(J6="4", Ward!$G$2:$H$16, IF(J6="5", Ward!$I$2:$J$16, IF(J6="6", Ward!$K$2:$L$15, IF(J6="7", Ward!$M$2:$N$11, IF(J6="8", Ward!$O$2:$P$17, IF(J6="9", Ward!$Q$2:$R$14, IF(J6="10", Ward!$S$2:$T$16, IF(J6="11", Ward!$U$2:$V$17, IF(J6="12", Ward!$W$2:$X$12, IF(J6="Bình Chánh", Ward!$Y$2:$Z$17, IF(J6="Bình Tân", Ward!$AA$2:$AB$11, IF(J6="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J6="Cần Giờ", Ward!$AE$2:$AF$8, IF(J6="Củ Chi", Ward!$AG$2:$AH$22, IF(J6="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J6="Hóc Môn", Ward!$AK$2:$AL$13, IF(J6="Nhà Bè", Ward!$AM$2:$AN$8, IF(J6="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J6="Tân Bình", Ward!$AQ$2:$AR$16, IF(J6="Tân Phú", Ward!$AS$2:$AT$12, IF(J6="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2440,7 +2440,7 @@
         <f>IF(J7 &lt;&gt; "", VLOOKUP(J7, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W7" s="28" t="str">
+      <c r="W7" s="23" t="str">
         <f>IF(K7 &lt;&gt; "", VLOOKUP(K7, IF(J7="1", Ward!$A$2:$B$11, IF(J7="2", Ward!$C$2:$D$12, IF(J7="3", Ward!$E$2:$F$15, IF(J7="4", Ward!$G$2:$H$16, IF(J7="5", Ward!$I$2:$J$16, IF(J7="6", Ward!$K$2:$L$15, IF(J7="7", Ward!$M$2:$N$11, IF(J7="8", Ward!$O$2:$P$17, IF(J7="9", Ward!$Q$2:$R$14, IF(J7="10", Ward!$S$2:$T$16, IF(J7="11", Ward!$U$2:$V$17, IF(J7="12", Ward!$W$2:$X$12, IF(J7="Bình Chánh", Ward!$Y$2:$Z$17, IF(J7="Bình Tân", Ward!$AA$2:$AB$11, IF(J7="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J7="Cần Giờ", Ward!$AE$2:$AF$8, IF(J7="Củ Chi", Ward!$AG$2:$AH$22, IF(J7="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J7="Hóc Môn", Ward!$AK$2:$AL$13, IF(J7="Nhà Bè", Ward!$AM$2:$AN$8, IF(J7="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J7="Tân Bình", Ward!$AQ$2:$AR$16, IF(J7="Tân Phú", Ward!$AS$2:$AT$12, IF(J7="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2478,7 +2478,7 @@
         <f>IF(J8 &lt;&gt; "", VLOOKUP(J8, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W8" s="28" t="str">
+      <c r="W8" s="23" t="str">
         <f>IF(K8 &lt;&gt; "", VLOOKUP(K8, IF(J8="1", Ward!$A$2:$B$11, IF(J8="2", Ward!$C$2:$D$12, IF(J8="3", Ward!$E$2:$F$15, IF(J8="4", Ward!$G$2:$H$16, IF(J8="5", Ward!$I$2:$J$16, IF(J8="6", Ward!$K$2:$L$15, IF(J8="7", Ward!$M$2:$N$11, IF(J8="8", Ward!$O$2:$P$17, IF(J8="9", Ward!$Q$2:$R$14, IF(J8="10", Ward!$S$2:$T$16, IF(J8="11", Ward!$U$2:$V$17, IF(J8="12", Ward!$W$2:$X$12, IF(J8="Bình Chánh", Ward!$Y$2:$Z$17, IF(J8="Bình Tân", Ward!$AA$2:$AB$11, IF(J8="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J8="Cần Giờ", Ward!$AE$2:$AF$8, IF(J8="Củ Chi", Ward!$AG$2:$AH$22, IF(J8="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J8="Hóc Môn", Ward!$AK$2:$AL$13, IF(J8="Nhà Bè", Ward!$AM$2:$AN$8, IF(J8="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J8="Tân Bình", Ward!$AQ$2:$AR$16, IF(J8="Tân Phú", Ward!$AS$2:$AT$12, IF(J8="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2516,7 +2516,7 @@
         <f>IF(J9 &lt;&gt; "", VLOOKUP(J9, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W9" s="28" t="str">
+      <c r="W9" s="23" t="str">
         <f>IF(K9 &lt;&gt; "", VLOOKUP(K9, IF(J9="1", Ward!$A$2:$B$11, IF(J9="2", Ward!$C$2:$D$12, IF(J9="3", Ward!$E$2:$F$15, IF(J9="4", Ward!$G$2:$H$16, IF(J9="5", Ward!$I$2:$J$16, IF(J9="6", Ward!$K$2:$L$15, IF(J9="7", Ward!$M$2:$N$11, IF(J9="8", Ward!$O$2:$P$17, IF(J9="9", Ward!$Q$2:$R$14, IF(J9="10", Ward!$S$2:$T$16, IF(J9="11", Ward!$U$2:$V$17, IF(J9="12", Ward!$W$2:$X$12, IF(J9="Bình Chánh", Ward!$Y$2:$Z$17, IF(J9="Bình Tân", Ward!$AA$2:$AB$11, IF(J9="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J9="Cần Giờ", Ward!$AE$2:$AF$8, IF(J9="Củ Chi", Ward!$AG$2:$AH$22, IF(J9="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J9="Hóc Môn", Ward!$AK$2:$AL$13, IF(J9="Nhà Bè", Ward!$AM$2:$AN$8, IF(J9="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J9="Tân Bình", Ward!$AQ$2:$AR$16, IF(J9="Tân Phú", Ward!$AS$2:$AT$12, IF(J9="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2554,7 +2554,7 @@
         <f>IF(J10 &lt;&gt; "", VLOOKUP(J10, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W10" s="28" t="str">
+      <c r="W10" s="23" t="str">
         <f>IF(K10 &lt;&gt; "", VLOOKUP(K10, IF(J10="1", Ward!$A$2:$B$11, IF(J10="2", Ward!$C$2:$D$12, IF(J10="3", Ward!$E$2:$F$15, IF(J10="4", Ward!$G$2:$H$16, IF(J10="5", Ward!$I$2:$J$16, IF(J10="6", Ward!$K$2:$L$15, IF(J10="7", Ward!$M$2:$N$11, IF(J10="8", Ward!$O$2:$P$17, IF(J10="9", Ward!$Q$2:$R$14, IF(J10="10", Ward!$S$2:$T$16, IF(J10="11", Ward!$U$2:$V$17, IF(J10="12", Ward!$W$2:$X$12, IF(J10="Bình Chánh", Ward!$Y$2:$Z$17, IF(J10="Bình Tân", Ward!$AA$2:$AB$11, IF(J10="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J10="Cần Giờ", Ward!$AE$2:$AF$8, IF(J10="Củ Chi", Ward!$AG$2:$AH$22, IF(J10="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J10="Hóc Môn", Ward!$AK$2:$AL$13, IF(J10="Nhà Bè", Ward!$AM$2:$AN$8, IF(J10="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J10="Tân Bình", Ward!$AQ$2:$AR$16, IF(J10="Tân Phú", Ward!$AS$2:$AT$12, IF(J10="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2592,7 +2592,7 @@
         <f>IF(J11 &lt;&gt; "", VLOOKUP(J11, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W11" s="28" t="str">
+      <c r="W11" s="23" t="str">
         <f>IF(K11 &lt;&gt; "", VLOOKUP(K11, IF(J11="1", Ward!$A$2:$B$11, IF(J11="2", Ward!$C$2:$D$12, IF(J11="3", Ward!$E$2:$F$15, IF(J11="4", Ward!$G$2:$H$16, IF(J11="5", Ward!$I$2:$J$16, IF(J11="6", Ward!$K$2:$L$15, IF(J11="7", Ward!$M$2:$N$11, IF(J11="8", Ward!$O$2:$P$17, IF(J11="9", Ward!$Q$2:$R$14, IF(J11="10", Ward!$S$2:$T$16, IF(J11="11", Ward!$U$2:$V$17, IF(J11="12", Ward!$W$2:$X$12, IF(J11="Bình Chánh", Ward!$Y$2:$Z$17, IF(J11="Bình Tân", Ward!$AA$2:$AB$11, IF(J11="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J11="Cần Giờ", Ward!$AE$2:$AF$8, IF(J11="Củ Chi", Ward!$AG$2:$AH$22, IF(J11="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J11="Hóc Môn", Ward!$AK$2:$AL$13, IF(J11="Nhà Bè", Ward!$AM$2:$AN$8, IF(J11="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J11="Tân Bình", Ward!$AQ$2:$AR$16, IF(J11="Tân Phú", Ward!$AS$2:$AT$12, IF(J11="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2630,7 +2630,7 @@
         <f>IF(J12 &lt;&gt; "", VLOOKUP(J12, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W12" s="28" t="str">
+      <c r="W12" s="23" t="str">
         <f>IF(K12 &lt;&gt; "", VLOOKUP(K12, IF(J12="1", Ward!$A$2:$B$11, IF(J12="2", Ward!$C$2:$D$12, IF(J12="3", Ward!$E$2:$F$15, IF(J12="4", Ward!$G$2:$H$16, IF(J12="5", Ward!$I$2:$J$16, IF(J12="6", Ward!$K$2:$L$15, IF(J12="7", Ward!$M$2:$N$11, IF(J12="8", Ward!$O$2:$P$17, IF(J12="9", Ward!$Q$2:$R$14, IF(J12="10", Ward!$S$2:$T$16, IF(J12="11", Ward!$U$2:$V$17, IF(J12="12", Ward!$W$2:$X$12, IF(J12="Bình Chánh", Ward!$Y$2:$Z$17, IF(J12="Bình Tân", Ward!$AA$2:$AB$11, IF(J12="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J12="Cần Giờ", Ward!$AE$2:$AF$8, IF(J12="Củ Chi", Ward!$AG$2:$AH$22, IF(J12="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J12="Hóc Môn", Ward!$AK$2:$AL$13, IF(J12="Nhà Bè", Ward!$AM$2:$AN$8, IF(J12="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J12="Tân Bình", Ward!$AQ$2:$AR$16, IF(J12="Tân Phú", Ward!$AS$2:$AT$12, IF(J12="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2668,7 +2668,7 @@
         <f>IF(J13 &lt;&gt; "", VLOOKUP(J13, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W13" s="28" t="str">
+      <c r="W13" s="23" t="str">
         <f>IF(K13 &lt;&gt; "", VLOOKUP(K13, IF(J13="1", Ward!$A$2:$B$11, IF(J13="2", Ward!$C$2:$D$12, IF(J13="3", Ward!$E$2:$F$15, IF(J13="4", Ward!$G$2:$H$16, IF(J13="5", Ward!$I$2:$J$16, IF(J13="6", Ward!$K$2:$L$15, IF(J13="7", Ward!$M$2:$N$11, IF(J13="8", Ward!$O$2:$P$17, IF(J13="9", Ward!$Q$2:$R$14, IF(J13="10", Ward!$S$2:$T$16, IF(J13="11", Ward!$U$2:$V$17, IF(J13="12", Ward!$W$2:$X$12, IF(J13="Bình Chánh", Ward!$Y$2:$Z$17, IF(J13="Bình Tân", Ward!$AA$2:$AB$11, IF(J13="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J13="Cần Giờ", Ward!$AE$2:$AF$8, IF(J13="Củ Chi", Ward!$AG$2:$AH$22, IF(J13="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J13="Hóc Môn", Ward!$AK$2:$AL$13, IF(J13="Nhà Bè", Ward!$AM$2:$AN$8, IF(J13="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J13="Tân Bình", Ward!$AQ$2:$AR$16, IF(J13="Tân Phú", Ward!$AS$2:$AT$12, IF(J13="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2706,7 +2706,7 @@
         <f>IF(J14 &lt;&gt; "", VLOOKUP(J14, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W14" s="28" t="str">
+      <c r="W14" s="23" t="str">
         <f>IF(K14 &lt;&gt; "", VLOOKUP(K14, IF(J14="1", Ward!$A$2:$B$11, IF(J14="2", Ward!$C$2:$D$12, IF(J14="3", Ward!$E$2:$F$15, IF(J14="4", Ward!$G$2:$H$16, IF(J14="5", Ward!$I$2:$J$16, IF(J14="6", Ward!$K$2:$L$15, IF(J14="7", Ward!$M$2:$N$11, IF(J14="8", Ward!$O$2:$P$17, IF(J14="9", Ward!$Q$2:$R$14, IF(J14="10", Ward!$S$2:$T$16, IF(J14="11", Ward!$U$2:$V$17, IF(J14="12", Ward!$W$2:$X$12, IF(J14="Bình Chánh", Ward!$Y$2:$Z$17, IF(J14="Bình Tân", Ward!$AA$2:$AB$11, IF(J14="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J14="Cần Giờ", Ward!$AE$2:$AF$8, IF(J14="Củ Chi", Ward!$AG$2:$AH$22, IF(J14="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J14="Hóc Môn", Ward!$AK$2:$AL$13, IF(J14="Nhà Bè", Ward!$AM$2:$AN$8, IF(J14="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J14="Tân Bình", Ward!$AQ$2:$AR$16, IF(J14="Tân Phú", Ward!$AS$2:$AT$12, IF(J14="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2744,7 +2744,7 @@
         <f>IF(J15 &lt;&gt; "", VLOOKUP(J15, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W15" s="28" t="str">
+      <c r="W15" s="23" t="str">
         <f>IF(K15 &lt;&gt; "", VLOOKUP(K15, IF(J15="1", Ward!$A$2:$B$11, IF(J15="2", Ward!$C$2:$D$12, IF(J15="3", Ward!$E$2:$F$15, IF(J15="4", Ward!$G$2:$H$16, IF(J15="5", Ward!$I$2:$J$16, IF(J15="6", Ward!$K$2:$L$15, IF(J15="7", Ward!$M$2:$N$11, IF(J15="8", Ward!$O$2:$P$17, IF(J15="9", Ward!$Q$2:$R$14, IF(J15="10", Ward!$S$2:$T$16, IF(J15="11", Ward!$U$2:$V$17, IF(J15="12", Ward!$W$2:$X$12, IF(J15="Bình Chánh", Ward!$Y$2:$Z$17, IF(J15="Bình Tân", Ward!$AA$2:$AB$11, IF(J15="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J15="Cần Giờ", Ward!$AE$2:$AF$8, IF(J15="Củ Chi", Ward!$AG$2:$AH$22, IF(J15="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J15="Hóc Môn", Ward!$AK$2:$AL$13, IF(J15="Nhà Bè", Ward!$AM$2:$AN$8, IF(J15="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J15="Tân Bình", Ward!$AQ$2:$AR$16, IF(J15="Tân Phú", Ward!$AS$2:$AT$12, IF(J15="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2782,7 +2782,7 @@
         <f>IF(J16 &lt;&gt; "", VLOOKUP(J16, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W16" s="28" t="str">
+      <c r="W16" s="23" t="str">
         <f>IF(K16 &lt;&gt; "", VLOOKUP(K16, IF(J16="1", Ward!$A$2:$B$11, IF(J16="2", Ward!$C$2:$D$12, IF(J16="3", Ward!$E$2:$F$15, IF(J16="4", Ward!$G$2:$H$16, IF(J16="5", Ward!$I$2:$J$16, IF(J16="6", Ward!$K$2:$L$15, IF(J16="7", Ward!$M$2:$N$11, IF(J16="8", Ward!$O$2:$P$17, IF(J16="9", Ward!$Q$2:$R$14, IF(J16="10", Ward!$S$2:$T$16, IF(J16="11", Ward!$U$2:$V$17, IF(J16="12", Ward!$W$2:$X$12, IF(J16="Bình Chánh", Ward!$Y$2:$Z$17, IF(J16="Bình Tân", Ward!$AA$2:$AB$11, IF(J16="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J16="Cần Giờ", Ward!$AE$2:$AF$8, IF(J16="Củ Chi", Ward!$AG$2:$AH$22, IF(J16="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J16="Hóc Môn", Ward!$AK$2:$AL$13, IF(J16="Nhà Bè", Ward!$AM$2:$AN$8, IF(J16="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J16="Tân Bình", Ward!$AQ$2:$AR$16, IF(J16="Tân Phú", Ward!$AS$2:$AT$12, IF(J16="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2820,7 +2820,7 @@
         <f>IF(J17 &lt;&gt; "", VLOOKUP(J17, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W17" s="28" t="str">
+      <c r="W17" s="23" t="str">
         <f>IF(K17 &lt;&gt; "", VLOOKUP(K17, IF(J17="1", Ward!$A$2:$B$11, IF(J17="2", Ward!$C$2:$D$12, IF(J17="3", Ward!$E$2:$F$15, IF(J17="4", Ward!$G$2:$H$16, IF(J17="5", Ward!$I$2:$J$16, IF(J17="6", Ward!$K$2:$L$15, IF(J17="7", Ward!$M$2:$N$11, IF(J17="8", Ward!$O$2:$P$17, IF(J17="9", Ward!$Q$2:$R$14, IF(J17="10", Ward!$S$2:$T$16, IF(J17="11", Ward!$U$2:$V$17, IF(J17="12", Ward!$W$2:$X$12, IF(J17="Bình Chánh", Ward!$Y$2:$Z$17, IF(J17="Bình Tân", Ward!$AA$2:$AB$11, IF(J17="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J17="Cần Giờ", Ward!$AE$2:$AF$8, IF(J17="Củ Chi", Ward!$AG$2:$AH$22, IF(J17="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J17="Hóc Môn", Ward!$AK$2:$AL$13, IF(J17="Nhà Bè", Ward!$AM$2:$AN$8, IF(J17="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J17="Tân Bình", Ward!$AQ$2:$AR$16, IF(J17="Tân Phú", Ward!$AS$2:$AT$12, IF(J17="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2858,7 +2858,7 @@
         <f>IF(J18 &lt;&gt; "", VLOOKUP(J18, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W18" s="28" t="str">
+      <c r="W18" s="23" t="str">
         <f>IF(K18 &lt;&gt; "", VLOOKUP(K18, IF(J18="1", Ward!$A$2:$B$11, IF(J18="2", Ward!$C$2:$D$12, IF(J18="3", Ward!$E$2:$F$15, IF(J18="4", Ward!$G$2:$H$16, IF(J18="5", Ward!$I$2:$J$16, IF(J18="6", Ward!$K$2:$L$15, IF(J18="7", Ward!$M$2:$N$11, IF(J18="8", Ward!$O$2:$P$17, IF(J18="9", Ward!$Q$2:$R$14, IF(J18="10", Ward!$S$2:$T$16, IF(J18="11", Ward!$U$2:$V$17, IF(J18="12", Ward!$W$2:$X$12, IF(J18="Bình Chánh", Ward!$Y$2:$Z$17, IF(J18="Bình Tân", Ward!$AA$2:$AB$11, IF(J18="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J18="Cần Giờ", Ward!$AE$2:$AF$8, IF(J18="Củ Chi", Ward!$AG$2:$AH$22, IF(J18="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J18="Hóc Môn", Ward!$AK$2:$AL$13, IF(J18="Nhà Bè", Ward!$AM$2:$AN$8, IF(J18="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J18="Tân Bình", Ward!$AQ$2:$AR$16, IF(J18="Tân Phú", Ward!$AS$2:$AT$12, IF(J18="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2896,7 +2896,7 @@
         <f>IF(J19 &lt;&gt; "", VLOOKUP(J19, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W19" s="28" t="str">
+      <c r="W19" s="23" t="str">
         <f>IF(K19 &lt;&gt; "", VLOOKUP(K19, IF(J19="1", Ward!$A$2:$B$11, IF(J19="2", Ward!$C$2:$D$12, IF(J19="3", Ward!$E$2:$F$15, IF(J19="4", Ward!$G$2:$H$16, IF(J19="5", Ward!$I$2:$J$16, IF(J19="6", Ward!$K$2:$L$15, IF(J19="7", Ward!$M$2:$N$11, IF(J19="8", Ward!$O$2:$P$17, IF(J19="9", Ward!$Q$2:$R$14, IF(J19="10", Ward!$S$2:$T$16, IF(J19="11", Ward!$U$2:$V$17, IF(J19="12", Ward!$W$2:$X$12, IF(J19="Bình Chánh", Ward!$Y$2:$Z$17, IF(J19="Bình Tân", Ward!$AA$2:$AB$11, IF(J19="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J19="Cần Giờ", Ward!$AE$2:$AF$8, IF(J19="Củ Chi", Ward!$AG$2:$AH$22, IF(J19="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J19="Hóc Môn", Ward!$AK$2:$AL$13, IF(J19="Nhà Bè", Ward!$AM$2:$AN$8, IF(J19="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J19="Tân Bình", Ward!$AQ$2:$AR$16, IF(J19="Tân Phú", Ward!$AS$2:$AT$12, IF(J19="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2934,7 +2934,7 @@
         <f>IF(J20 &lt;&gt; "", VLOOKUP(J20, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W20" s="28" t="str">
+      <c r="W20" s="23" t="str">
         <f>IF(K20 &lt;&gt; "", VLOOKUP(K20, IF(J20="1", Ward!$A$2:$B$11, IF(J20="2", Ward!$C$2:$D$12, IF(J20="3", Ward!$E$2:$F$15, IF(J20="4", Ward!$G$2:$H$16, IF(J20="5", Ward!$I$2:$J$16, IF(J20="6", Ward!$K$2:$L$15, IF(J20="7", Ward!$M$2:$N$11, IF(J20="8", Ward!$O$2:$P$17, IF(J20="9", Ward!$Q$2:$R$14, IF(J20="10", Ward!$S$2:$T$16, IF(J20="11", Ward!$U$2:$V$17, IF(J20="12", Ward!$W$2:$X$12, IF(J20="Bình Chánh", Ward!$Y$2:$Z$17, IF(J20="Bình Tân", Ward!$AA$2:$AB$11, IF(J20="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J20="Cần Giờ", Ward!$AE$2:$AF$8, IF(J20="Củ Chi", Ward!$AG$2:$AH$22, IF(J20="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J20="Hóc Môn", Ward!$AK$2:$AL$13, IF(J20="Nhà Bè", Ward!$AM$2:$AN$8, IF(J20="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J20="Tân Bình", Ward!$AQ$2:$AR$16, IF(J20="Tân Phú", Ward!$AS$2:$AT$12, IF(J20="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -2972,7 +2972,7 @@
         <f>IF(J21 &lt;&gt; "", VLOOKUP(J21, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W21" s="28" t="str">
+      <c r="W21" s="23" t="str">
         <f>IF(K21 &lt;&gt; "", VLOOKUP(K21, IF(J21="1", Ward!$A$2:$B$11, IF(J21="2", Ward!$C$2:$D$12, IF(J21="3", Ward!$E$2:$F$15, IF(J21="4", Ward!$G$2:$H$16, IF(J21="5", Ward!$I$2:$J$16, IF(J21="6", Ward!$K$2:$L$15, IF(J21="7", Ward!$M$2:$N$11, IF(J21="8", Ward!$O$2:$P$17, IF(J21="9", Ward!$Q$2:$R$14, IF(J21="10", Ward!$S$2:$T$16, IF(J21="11", Ward!$U$2:$V$17, IF(J21="12", Ward!$W$2:$X$12, IF(J21="Bình Chánh", Ward!$Y$2:$Z$17, IF(J21="Bình Tân", Ward!$AA$2:$AB$11, IF(J21="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J21="Cần Giờ", Ward!$AE$2:$AF$8, IF(J21="Củ Chi", Ward!$AG$2:$AH$22, IF(J21="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J21="Hóc Môn", Ward!$AK$2:$AL$13, IF(J21="Nhà Bè", Ward!$AM$2:$AN$8, IF(J21="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J21="Tân Bình", Ward!$AQ$2:$AR$16, IF(J21="Tân Phú", Ward!$AS$2:$AT$12, IF(J21="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3010,7 +3010,7 @@
         <f>IF(J22 &lt;&gt; "", VLOOKUP(J22, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W22" s="28" t="str">
+      <c r="W22" s="23" t="str">
         <f>IF(K22 &lt;&gt; "", VLOOKUP(K22, IF(J22="1", Ward!$A$2:$B$11, IF(J22="2", Ward!$C$2:$D$12, IF(J22="3", Ward!$E$2:$F$15, IF(J22="4", Ward!$G$2:$H$16, IF(J22="5", Ward!$I$2:$J$16, IF(J22="6", Ward!$K$2:$L$15, IF(J22="7", Ward!$M$2:$N$11, IF(J22="8", Ward!$O$2:$P$17, IF(J22="9", Ward!$Q$2:$R$14, IF(J22="10", Ward!$S$2:$T$16, IF(J22="11", Ward!$U$2:$V$17, IF(J22="12", Ward!$W$2:$X$12, IF(J22="Bình Chánh", Ward!$Y$2:$Z$17, IF(J22="Bình Tân", Ward!$AA$2:$AB$11, IF(J22="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J22="Cần Giờ", Ward!$AE$2:$AF$8, IF(J22="Củ Chi", Ward!$AG$2:$AH$22, IF(J22="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J22="Hóc Môn", Ward!$AK$2:$AL$13, IF(J22="Nhà Bè", Ward!$AM$2:$AN$8, IF(J22="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J22="Tân Bình", Ward!$AQ$2:$AR$16, IF(J22="Tân Phú", Ward!$AS$2:$AT$12, IF(J22="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3048,7 +3048,7 @@
         <f>IF(J23 &lt;&gt; "", VLOOKUP(J23, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W23" s="28" t="str">
+      <c r="W23" s="23" t="str">
         <f>IF(K23 &lt;&gt; "", VLOOKUP(K23, IF(J23="1", Ward!$A$2:$B$11, IF(J23="2", Ward!$C$2:$D$12, IF(J23="3", Ward!$E$2:$F$15, IF(J23="4", Ward!$G$2:$H$16, IF(J23="5", Ward!$I$2:$J$16, IF(J23="6", Ward!$K$2:$L$15, IF(J23="7", Ward!$M$2:$N$11, IF(J23="8", Ward!$O$2:$P$17, IF(J23="9", Ward!$Q$2:$R$14, IF(J23="10", Ward!$S$2:$T$16, IF(J23="11", Ward!$U$2:$V$17, IF(J23="12", Ward!$W$2:$X$12, IF(J23="Bình Chánh", Ward!$Y$2:$Z$17, IF(J23="Bình Tân", Ward!$AA$2:$AB$11, IF(J23="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J23="Cần Giờ", Ward!$AE$2:$AF$8, IF(J23="Củ Chi", Ward!$AG$2:$AH$22, IF(J23="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J23="Hóc Môn", Ward!$AK$2:$AL$13, IF(J23="Nhà Bè", Ward!$AM$2:$AN$8, IF(J23="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J23="Tân Bình", Ward!$AQ$2:$AR$16, IF(J23="Tân Phú", Ward!$AS$2:$AT$12, IF(J23="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3086,7 +3086,7 @@
         <f>IF(J24 &lt;&gt; "", VLOOKUP(J24, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W24" s="28" t="str">
+      <c r="W24" s="23" t="str">
         <f>IF(K24 &lt;&gt; "", VLOOKUP(K24, IF(J24="1", Ward!$A$2:$B$11, IF(J24="2", Ward!$C$2:$D$12, IF(J24="3", Ward!$E$2:$F$15, IF(J24="4", Ward!$G$2:$H$16, IF(J24="5", Ward!$I$2:$J$16, IF(J24="6", Ward!$K$2:$L$15, IF(J24="7", Ward!$M$2:$N$11, IF(J24="8", Ward!$O$2:$P$17, IF(J24="9", Ward!$Q$2:$R$14, IF(J24="10", Ward!$S$2:$T$16, IF(J24="11", Ward!$U$2:$V$17, IF(J24="12", Ward!$W$2:$X$12, IF(J24="Bình Chánh", Ward!$Y$2:$Z$17, IF(J24="Bình Tân", Ward!$AA$2:$AB$11, IF(J24="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J24="Cần Giờ", Ward!$AE$2:$AF$8, IF(J24="Củ Chi", Ward!$AG$2:$AH$22, IF(J24="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J24="Hóc Môn", Ward!$AK$2:$AL$13, IF(J24="Nhà Bè", Ward!$AM$2:$AN$8, IF(J24="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J24="Tân Bình", Ward!$AQ$2:$AR$16, IF(J24="Tân Phú", Ward!$AS$2:$AT$12, IF(J24="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3124,7 +3124,7 @@
         <f>IF(J25 &lt;&gt; "", VLOOKUP(J25, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W25" s="28" t="str">
+      <c r="W25" s="23" t="str">
         <f>IF(K25 &lt;&gt; "", VLOOKUP(K25, IF(J25="1", Ward!$A$2:$B$11, IF(J25="2", Ward!$C$2:$D$12, IF(J25="3", Ward!$E$2:$F$15, IF(J25="4", Ward!$G$2:$H$16, IF(J25="5", Ward!$I$2:$J$16, IF(J25="6", Ward!$K$2:$L$15, IF(J25="7", Ward!$M$2:$N$11, IF(J25="8", Ward!$O$2:$P$17, IF(J25="9", Ward!$Q$2:$R$14, IF(J25="10", Ward!$S$2:$T$16, IF(J25="11", Ward!$U$2:$V$17, IF(J25="12", Ward!$W$2:$X$12, IF(J25="Bình Chánh", Ward!$Y$2:$Z$17, IF(J25="Bình Tân", Ward!$AA$2:$AB$11, IF(J25="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J25="Cần Giờ", Ward!$AE$2:$AF$8, IF(J25="Củ Chi", Ward!$AG$2:$AH$22, IF(J25="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J25="Hóc Môn", Ward!$AK$2:$AL$13, IF(J25="Nhà Bè", Ward!$AM$2:$AN$8, IF(J25="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J25="Tân Bình", Ward!$AQ$2:$AR$16, IF(J25="Tân Phú", Ward!$AS$2:$AT$12, IF(J25="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3162,7 +3162,7 @@
         <f>IF(J26 &lt;&gt; "", VLOOKUP(J26, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W26" s="28" t="str">
+      <c r="W26" s="23" t="str">
         <f>IF(K26 &lt;&gt; "", VLOOKUP(K26, IF(J26="1", Ward!$A$2:$B$11, IF(J26="2", Ward!$C$2:$D$12, IF(J26="3", Ward!$E$2:$F$15, IF(J26="4", Ward!$G$2:$H$16, IF(J26="5", Ward!$I$2:$J$16, IF(J26="6", Ward!$K$2:$L$15, IF(J26="7", Ward!$M$2:$N$11, IF(J26="8", Ward!$O$2:$P$17, IF(J26="9", Ward!$Q$2:$R$14, IF(J26="10", Ward!$S$2:$T$16, IF(J26="11", Ward!$U$2:$V$17, IF(J26="12", Ward!$W$2:$X$12, IF(J26="Bình Chánh", Ward!$Y$2:$Z$17, IF(J26="Bình Tân", Ward!$AA$2:$AB$11, IF(J26="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J26="Cần Giờ", Ward!$AE$2:$AF$8, IF(J26="Củ Chi", Ward!$AG$2:$AH$22, IF(J26="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J26="Hóc Môn", Ward!$AK$2:$AL$13, IF(J26="Nhà Bè", Ward!$AM$2:$AN$8, IF(J26="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J26="Tân Bình", Ward!$AQ$2:$AR$16, IF(J26="Tân Phú", Ward!$AS$2:$AT$12, IF(J26="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3200,7 +3200,7 @@
         <f>IF(J27 &lt;&gt; "", VLOOKUP(J27, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W27" s="28" t="str">
+      <c r="W27" s="23" t="str">
         <f>IF(K27 &lt;&gt; "", VLOOKUP(K27, IF(J27="1", Ward!$A$2:$B$11, IF(J27="2", Ward!$C$2:$D$12, IF(J27="3", Ward!$E$2:$F$15, IF(J27="4", Ward!$G$2:$H$16, IF(J27="5", Ward!$I$2:$J$16, IF(J27="6", Ward!$K$2:$L$15, IF(J27="7", Ward!$M$2:$N$11, IF(J27="8", Ward!$O$2:$P$17, IF(J27="9", Ward!$Q$2:$R$14, IF(J27="10", Ward!$S$2:$T$16, IF(J27="11", Ward!$U$2:$V$17, IF(J27="12", Ward!$W$2:$X$12, IF(J27="Bình Chánh", Ward!$Y$2:$Z$17, IF(J27="Bình Tân", Ward!$AA$2:$AB$11, IF(J27="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J27="Cần Giờ", Ward!$AE$2:$AF$8, IF(J27="Củ Chi", Ward!$AG$2:$AH$22, IF(J27="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J27="Hóc Môn", Ward!$AK$2:$AL$13, IF(J27="Nhà Bè", Ward!$AM$2:$AN$8, IF(J27="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J27="Tân Bình", Ward!$AQ$2:$AR$16, IF(J27="Tân Phú", Ward!$AS$2:$AT$12, IF(J27="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3238,7 +3238,7 @@
         <f>IF(J28 &lt;&gt; "", VLOOKUP(J28, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W28" s="28" t="str">
+      <c r="W28" s="23" t="str">
         <f>IF(K28 &lt;&gt; "", VLOOKUP(K28, IF(J28="1", Ward!$A$2:$B$11, IF(J28="2", Ward!$C$2:$D$12, IF(J28="3", Ward!$E$2:$F$15, IF(J28="4", Ward!$G$2:$H$16, IF(J28="5", Ward!$I$2:$J$16, IF(J28="6", Ward!$K$2:$L$15, IF(J28="7", Ward!$M$2:$N$11, IF(J28="8", Ward!$O$2:$P$17, IF(J28="9", Ward!$Q$2:$R$14, IF(J28="10", Ward!$S$2:$T$16, IF(J28="11", Ward!$U$2:$V$17, IF(J28="12", Ward!$W$2:$X$12, IF(J28="Bình Chánh", Ward!$Y$2:$Z$17, IF(J28="Bình Tân", Ward!$AA$2:$AB$11, IF(J28="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J28="Cần Giờ", Ward!$AE$2:$AF$8, IF(J28="Củ Chi", Ward!$AG$2:$AH$22, IF(J28="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J28="Hóc Môn", Ward!$AK$2:$AL$13, IF(J28="Nhà Bè", Ward!$AM$2:$AN$8, IF(J28="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J28="Tân Bình", Ward!$AQ$2:$AR$16, IF(J28="Tân Phú", Ward!$AS$2:$AT$12, IF(J28="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3276,7 +3276,7 @@
         <f>IF(J29 &lt;&gt; "", VLOOKUP(J29, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W29" s="28" t="str">
+      <c r="W29" s="23" t="str">
         <f>IF(K29 &lt;&gt; "", VLOOKUP(K29, IF(J29="1", Ward!$A$2:$B$11, IF(J29="2", Ward!$C$2:$D$12, IF(J29="3", Ward!$E$2:$F$15, IF(J29="4", Ward!$G$2:$H$16, IF(J29="5", Ward!$I$2:$J$16, IF(J29="6", Ward!$K$2:$L$15, IF(J29="7", Ward!$M$2:$N$11, IF(J29="8", Ward!$O$2:$P$17, IF(J29="9", Ward!$Q$2:$R$14, IF(J29="10", Ward!$S$2:$T$16, IF(J29="11", Ward!$U$2:$V$17, IF(J29="12", Ward!$W$2:$X$12, IF(J29="Bình Chánh", Ward!$Y$2:$Z$17, IF(J29="Bình Tân", Ward!$AA$2:$AB$11, IF(J29="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J29="Cần Giờ", Ward!$AE$2:$AF$8, IF(J29="Củ Chi", Ward!$AG$2:$AH$22, IF(J29="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J29="Hóc Môn", Ward!$AK$2:$AL$13, IF(J29="Nhà Bè", Ward!$AM$2:$AN$8, IF(J29="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J29="Tân Bình", Ward!$AQ$2:$AR$16, IF(J29="Tân Phú", Ward!$AS$2:$AT$12, IF(J29="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3314,7 +3314,7 @@
         <f>IF(J30 &lt;&gt; "", VLOOKUP(J30, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W30" s="28" t="str">
+      <c r="W30" s="23" t="str">
         <f>IF(K30 &lt;&gt; "", VLOOKUP(K30, IF(J30="1", Ward!$A$2:$B$11, IF(J30="2", Ward!$C$2:$D$12, IF(J30="3", Ward!$E$2:$F$15, IF(J30="4", Ward!$G$2:$H$16, IF(J30="5", Ward!$I$2:$J$16, IF(J30="6", Ward!$K$2:$L$15, IF(J30="7", Ward!$M$2:$N$11, IF(J30="8", Ward!$O$2:$P$17, IF(J30="9", Ward!$Q$2:$R$14, IF(J30="10", Ward!$S$2:$T$16, IF(J30="11", Ward!$U$2:$V$17, IF(J30="12", Ward!$W$2:$X$12, IF(J30="Bình Chánh", Ward!$Y$2:$Z$17, IF(J30="Bình Tân", Ward!$AA$2:$AB$11, IF(J30="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J30="Cần Giờ", Ward!$AE$2:$AF$8, IF(J30="Củ Chi", Ward!$AG$2:$AH$22, IF(J30="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J30="Hóc Môn", Ward!$AK$2:$AL$13, IF(J30="Nhà Bè", Ward!$AM$2:$AN$8, IF(J30="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J30="Tân Bình", Ward!$AQ$2:$AR$16, IF(J30="Tân Phú", Ward!$AS$2:$AT$12, IF(J30="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3352,7 +3352,7 @@
         <f>IF(J31 &lt;&gt; "", VLOOKUP(J31, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W31" s="28" t="str">
+      <c r="W31" s="23" t="str">
         <f>IF(K31 &lt;&gt; "", VLOOKUP(K31, IF(J31="1", Ward!$A$2:$B$11, IF(J31="2", Ward!$C$2:$D$12, IF(J31="3", Ward!$E$2:$F$15, IF(J31="4", Ward!$G$2:$H$16, IF(J31="5", Ward!$I$2:$J$16, IF(J31="6", Ward!$K$2:$L$15, IF(J31="7", Ward!$M$2:$N$11, IF(J31="8", Ward!$O$2:$P$17, IF(J31="9", Ward!$Q$2:$R$14, IF(J31="10", Ward!$S$2:$T$16, IF(J31="11", Ward!$U$2:$V$17, IF(J31="12", Ward!$W$2:$X$12, IF(J31="Bình Chánh", Ward!$Y$2:$Z$17, IF(J31="Bình Tân", Ward!$AA$2:$AB$11, IF(J31="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J31="Cần Giờ", Ward!$AE$2:$AF$8, IF(J31="Củ Chi", Ward!$AG$2:$AH$22, IF(J31="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J31="Hóc Môn", Ward!$AK$2:$AL$13, IF(J31="Nhà Bè", Ward!$AM$2:$AN$8, IF(J31="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J31="Tân Bình", Ward!$AQ$2:$AR$16, IF(J31="Tân Phú", Ward!$AS$2:$AT$12, IF(J31="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3390,7 +3390,7 @@
         <f>IF(J32 &lt;&gt; "", VLOOKUP(J32, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W32" s="28" t="str">
+      <c r="W32" s="23" t="str">
         <f>IF(K32 &lt;&gt; "", VLOOKUP(K32, IF(J32="1", Ward!$A$2:$B$11, IF(J32="2", Ward!$C$2:$D$12, IF(J32="3", Ward!$E$2:$F$15, IF(J32="4", Ward!$G$2:$H$16, IF(J32="5", Ward!$I$2:$J$16, IF(J32="6", Ward!$K$2:$L$15, IF(J32="7", Ward!$M$2:$N$11, IF(J32="8", Ward!$O$2:$P$17, IF(J32="9", Ward!$Q$2:$R$14, IF(J32="10", Ward!$S$2:$T$16, IF(J32="11", Ward!$U$2:$V$17, IF(J32="12", Ward!$W$2:$X$12, IF(J32="Bình Chánh", Ward!$Y$2:$Z$17, IF(J32="Bình Tân", Ward!$AA$2:$AB$11, IF(J32="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J32="Cần Giờ", Ward!$AE$2:$AF$8, IF(J32="Củ Chi", Ward!$AG$2:$AH$22, IF(J32="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J32="Hóc Môn", Ward!$AK$2:$AL$13, IF(J32="Nhà Bè", Ward!$AM$2:$AN$8, IF(J32="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J32="Tân Bình", Ward!$AQ$2:$AR$16, IF(J32="Tân Phú", Ward!$AS$2:$AT$12, IF(J32="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3428,7 +3428,7 @@
         <f>IF(J33 &lt;&gt; "", VLOOKUP(J33, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W33" s="28" t="str">
+      <c r="W33" s="23" t="str">
         <f>IF(K33 &lt;&gt; "", VLOOKUP(K33, IF(J33="1", Ward!$A$2:$B$11, IF(J33="2", Ward!$C$2:$D$12, IF(J33="3", Ward!$E$2:$F$15, IF(J33="4", Ward!$G$2:$H$16, IF(J33="5", Ward!$I$2:$J$16, IF(J33="6", Ward!$K$2:$L$15, IF(J33="7", Ward!$M$2:$N$11, IF(J33="8", Ward!$O$2:$P$17, IF(J33="9", Ward!$Q$2:$R$14, IF(J33="10", Ward!$S$2:$T$16, IF(J33="11", Ward!$U$2:$V$17, IF(J33="12", Ward!$W$2:$X$12, IF(J33="Bình Chánh", Ward!$Y$2:$Z$17, IF(J33="Bình Tân", Ward!$AA$2:$AB$11, IF(J33="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J33="Cần Giờ", Ward!$AE$2:$AF$8, IF(J33="Củ Chi", Ward!$AG$2:$AH$22, IF(J33="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J33="Hóc Môn", Ward!$AK$2:$AL$13, IF(J33="Nhà Bè", Ward!$AM$2:$AN$8, IF(J33="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J33="Tân Bình", Ward!$AQ$2:$AR$16, IF(J33="Tân Phú", Ward!$AS$2:$AT$12, IF(J33="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3466,7 +3466,7 @@
         <f>IF(J34 &lt;&gt; "", VLOOKUP(J34, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W34" s="28" t="str">
+      <c r="W34" s="23" t="str">
         <f>IF(K34 &lt;&gt; "", VLOOKUP(K34, IF(J34="1", Ward!$A$2:$B$11, IF(J34="2", Ward!$C$2:$D$12, IF(J34="3", Ward!$E$2:$F$15, IF(J34="4", Ward!$G$2:$H$16, IF(J34="5", Ward!$I$2:$J$16, IF(J34="6", Ward!$K$2:$L$15, IF(J34="7", Ward!$M$2:$N$11, IF(J34="8", Ward!$O$2:$P$17, IF(J34="9", Ward!$Q$2:$R$14, IF(J34="10", Ward!$S$2:$T$16, IF(J34="11", Ward!$U$2:$V$17, IF(J34="12", Ward!$W$2:$X$12, IF(J34="Bình Chánh", Ward!$Y$2:$Z$17, IF(J34="Bình Tân", Ward!$AA$2:$AB$11, IF(J34="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J34="Cần Giờ", Ward!$AE$2:$AF$8, IF(J34="Củ Chi", Ward!$AG$2:$AH$22, IF(J34="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J34="Hóc Môn", Ward!$AK$2:$AL$13, IF(J34="Nhà Bè", Ward!$AM$2:$AN$8, IF(J34="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J34="Tân Bình", Ward!$AQ$2:$AR$16, IF(J34="Tân Phú", Ward!$AS$2:$AT$12, IF(J34="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3504,7 +3504,7 @@
         <f>IF(J35 &lt;&gt; "", VLOOKUP(J35, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W35" s="28" t="str">
+      <c r="W35" s="23" t="str">
         <f>IF(K35 &lt;&gt; "", VLOOKUP(K35, IF(J35="1", Ward!$A$2:$B$11, IF(J35="2", Ward!$C$2:$D$12, IF(J35="3", Ward!$E$2:$F$15, IF(J35="4", Ward!$G$2:$H$16, IF(J35="5", Ward!$I$2:$J$16, IF(J35="6", Ward!$K$2:$L$15, IF(J35="7", Ward!$M$2:$N$11, IF(J35="8", Ward!$O$2:$P$17, IF(J35="9", Ward!$Q$2:$R$14, IF(J35="10", Ward!$S$2:$T$16, IF(J35="11", Ward!$U$2:$V$17, IF(J35="12", Ward!$W$2:$X$12, IF(J35="Bình Chánh", Ward!$Y$2:$Z$17, IF(J35="Bình Tân", Ward!$AA$2:$AB$11, IF(J35="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J35="Cần Giờ", Ward!$AE$2:$AF$8, IF(J35="Củ Chi", Ward!$AG$2:$AH$22, IF(J35="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J35="Hóc Môn", Ward!$AK$2:$AL$13, IF(J35="Nhà Bè", Ward!$AM$2:$AN$8, IF(J35="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J35="Tân Bình", Ward!$AQ$2:$AR$16, IF(J35="Tân Phú", Ward!$AS$2:$AT$12, IF(J35="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3542,7 +3542,7 @@
         <f>IF(J36 &lt;&gt; "", VLOOKUP(J36, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W36" s="28" t="str">
+      <c r="W36" s="23" t="str">
         <f>IF(K36 &lt;&gt; "", VLOOKUP(K36, IF(J36="1", Ward!$A$2:$B$11, IF(J36="2", Ward!$C$2:$D$12, IF(J36="3", Ward!$E$2:$F$15, IF(J36="4", Ward!$G$2:$H$16, IF(J36="5", Ward!$I$2:$J$16, IF(J36="6", Ward!$K$2:$L$15, IF(J36="7", Ward!$M$2:$N$11, IF(J36="8", Ward!$O$2:$P$17, IF(J36="9", Ward!$Q$2:$R$14, IF(J36="10", Ward!$S$2:$T$16, IF(J36="11", Ward!$U$2:$V$17, IF(J36="12", Ward!$W$2:$X$12, IF(J36="Bình Chánh", Ward!$Y$2:$Z$17, IF(J36="Bình Tân", Ward!$AA$2:$AB$11, IF(J36="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J36="Cần Giờ", Ward!$AE$2:$AF$8, IF(J36="Củ Chi", Ward!$AG$2:$AH$22, IF(J36="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J36="Hóc Môn", Ward!$AK$2:$AL$13, IF(J36="Nhà Bè", Ward!$AM$2:$AN$8, IF(J36="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J36="Tân Bình", Ward!$AQ$2:$AR$16, IF(J36="Tân Phú", Ward!$AS$2:$AT$12, IF(J36="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3580,7 +3580,7 @@
         <f>IF(J37 &lt;&gt; "", VLOOKUP(J37, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W37" s="28" t="str">
+      <c r="W37" s="23" t="str">
         <f>IF(K37 &lt;&gt; "", VLOOKUP(K37, IF(J37="1", Ward!$A$2:$B$11, IF(J37="2", Ward!$C$2:$D$12, IF(J37="3", Ward!$E$2:$F$15, IF(J37="4", Ward!$G$2:$H$16, IF(J37="5", Ward!$I$2:$J$16, IF(J37="6", Ward!$K$2:$L$15, IF(J37="7", Ward!$M$2:$N$11, IF(J37="8", Ward!$O$2:$P$17, IF(J37="9", Ward!$Q$2:$R$14, IF(J37="10", Ward!$S$2:$T$16, IF(J37="11", Ward!$U$2:$V$17, IF(J37="12", Ward!$W$2:$X$12, IF(J37="Bình Chánh", Ward!$Y$2:$Z$17, IF(J37="Bình Tân", Ward!$AA$2:$AB$11, IF(J37="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J37="Cần Giờ", Ward!$AE$2:$AF$8, IF(J37="Củ Chi", Ward!$AG$2:$AH$22, IF(J37="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J37="Hóc Môn", Ward!$AK$2:$AL$13, IF(J37="Nhà Bè", Ward!$AM$2:$AN$8, IF(J37="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J37="Tân Bình", Ward!$AQ$2:$AR$16, IF(J37="Tân Phú", Ward!$AS$2:$AT$12, IF(J37="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3618,7 +3618,7 @@
         <f>IF(J38 &lt;&gt; "", VLOOKUP(J38, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W38" s="28" t="str">
+      <c r="W38" s="23" t="str">
         <f>IF(K38 &lt;&gt; "", VLOOKUP(K38, IF(J38="1", Ward!$A$2:$B$11, IF(J38="2", Ward!$C$2:$D$12, IF(J38="3", Ward!$E$2:$F$15, IF(J38="4", Ward!$G$2:$H$16, IF(J38="5", Ward!$I$2:$J$16, IF(J38="6", Ward!$K$2:$L$15, IF(J38="7", Ward!$M$2:$N$11, IF(J38="8", Ward!$O$2:$P$17, IF(J38="9", Ward!$Q$2:$R$14, IF(J38="10", Ward!$S$2:$T$16, IF(J38="11", Ward!$U$2:$V$17, IF(J38="12", Ward!$W$2:$X$12, IF(J38="Bình Chánh", Ward!$Y$2:$Z$17, IF(J38="Bình Tân", Ward!$AA$2:$AB$11, IF(J38="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J38="Cần Giờ", Ward!$AE$2:$AF$8, IF(J38="Củ Chi", Ward!$AG$2:$AH$22, IF(J38="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J38="Hóc Môn", Ward!$AK$2:$AL$13, IF(J38="Nhà Bè", Ward!$AM$2:$AN$8, IF(J38="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J38="Tân Bình", Ward!$AQ$2:$AR$16, IF(J38="Tân Phú", Ward!$AS$2:$AT$12, IF(J38="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3656,7 +3656,7 @@
         <f>IF(J39 &lt;&gt; "", VLOOKUP(J39, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W39" s="28" t="str">
+      <c r="W39" s="23" t="str">
         <f>IF(K39 &lt;&gt; "", VLOOKUP(K39, IF(J39="1", Ward!$A$2:$B$11, IF(J39="2", Ward!$C$2:$D$12, IF(J39="3", Ward!$E$2:$F$15, IF(J39="4", Ward!$G$2:$H$16, IF(J39="5", Ward!$I$2:$J$16, IF(J39="6", Ward!$K$2:$L$15, IF(J39="7", Ward!$M$2:$N$11, IF(J39="8", Ward!$O$2:$P$17, IF(J39="9", Ward!$Q$2:$R$14, IF(J39="10", Ward!$S$2:$T$16, IF(J39="11", Ward!$U$2:$V$17, IF(J39="12", Ward!$W$2:$X$12, IF(J39="Bình Chánh", Ward!$Y$2:$Z$17, IF(J39="Bình Tân", Ward!$AA$2:$AB$11, IF(J39="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J39="Cần Giờ", Ward!$AE$2:$AF$8, IF(J39="Củ Chi", Ward!$AG$2:$AH$22, IF(J39="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J39="Hóc Môn", Ward!$AK$2:$AL$13, IF(J39="Nhà Bè", Ward!$AM$2:$AN$8, IF(J39="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J39="Tân Bình", Ward!$AQ$2:$AR$16, IF(J39="Tân Phú", Ward!$AS$2:$AT$12, IF(J39="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3694,7 +3694,7 @@
         <f>IF(J40 &lt;&gt; "", VLOOKUP(J40, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W40" s="28" t="str">
+      <c r="W40" s="23" t="str">
         <f>IF(K40 &lt;&gt; "", VLOOKUP(K40, IF(J40="1", Ward!$A$2:$B$11, IF(J40="2", Ward!$C$2:$D$12, IF(J40="3", Ward!$E$2:$F$15, IF(J40="4", Ward!$G$2:$H$16, IF(J40="5", Ward!$I$2:$J$16, IF(J40="6", Ward!$K$2:$L$15, IF(J40="7", Ward!$M$2:$N$11, IF(J40="8", Ward!$O$2:$P$17, IF(J40="9", Ward!$Q$2:$R$14, IF(J40="10", Ward!$S$2:$T$16, IF(J40="11", Ward!$U$2:$V$17, IF(J40="12", Ward!$W$2:$X$12, IF(J40="Bình Chánh", Ward!$Y$2:$Z$17, IF(J40="Bình Tân", Ward!$AA$2:$AB$11, IF(J40="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J40="Cần Giờ", Ward!$AE$2:$AF$8, IF(J40="Củ Chi", Ward!$AG$2:$AH$22, IF(J40="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J40="Hóc Môn", Ward!$AK$2:$AL$13, IF(J40="Nhà Bè", Ward!$AM$2:$AN$8, IF(J40="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J40="Tân Bình", Ward!$AQ$2:$AR$16, IF(J40="Tân Phú", Ward!$AS$2:$AT$12, IF(J40="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3732,7 +3732,7 @@
         <f>IF(J41 &lt;&gt; "", VLOOKUP(J41, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W41" s="28" t="str">
+      <c r="W41" s="23" t="str">
         <f>IF(K41 &lt;&gt; "", VLOOKUP(K41, IF(J41="1", Ward!$A$2:$B$11, IF(J41="2", Ward!$C$2:$D$12, IF(J41="3", Ward!$E$2:$F$15, IF(J41="4", Ward!$G$2:$H$16, IF(J41="5", Ward!$I$2:$J$16, IF(J41="6", Ward!$K$2:$L$15, IF(J41="7", Ward!$M$2:$N$11, IF(J41="8", Ward!$O$2:$P$17, IF(J41="9", Ward!$Q$2:$R$14, IF(J41="10", Ward!$S$2:$T$16, IF(J41="11", Ward!$U$2:$V$17, IF(J41="12", Ward!$W$2:$X$12, IF(J41="Bình Chánh", Ward!$Y$2:$Z$17, IF(J41="Bình Tân", Ward!$AA$2:$AB$11, IF(J41="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J41="Cần Giờ", Ward!$AE$2:$AF$8, IF(J41="Củ Chi", Ward!$AG$2:$AH$22, IF(J41="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J41="Hóc Môn", Ward!$AK$2:$AL$13, IF(J41="Nhà Bè", Ward!$AM$2:$AN$8, IF(J41="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J41="Tân Bình", Ward!$AQ$2:$AR$16, IF(J41="Tân Phú", Ward!$AS$2:$AT$12, IF(J41="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3770,7 +3770,7 @@
         <f>IF(J42 &lt;&gt; "", VLOOKUP(J42, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W42" s="28" t="str">
+      <c r="W42" s="23" t="str">
         <f>IF(K42 &lt;&gt; "", VLOOKUP(K42, IF(J42="1", Ward!$A$2:$B$11, IF(J42="2", Ward!$C$2:$D$12, IF(J42="3", Ward!$E$2:$F$15, IF(J42="4", Ward!$G$2:$H$16, IF(J42="5", Ward!$I$2:$J$16, IF(J42="6", Ward!$K$2:$L$15, IF(J42="7", Ward!$M$2:$N$11, IF(J42="8", Ward!$O$2:$P$17, IF(J42="9", Ward!$Q$2:$R$14, IF(J42="10", Ward!$S$2:$T$16, IF(J42="11", Ward!$U$2:$V$17, IF(J42="12", Ward!$W$2:$X$12, IF(J42="Bình Chánh", Ward!$Y$2:$Z$17, IF(J42="Bình Tân", Ward!$AA$2:$AB$11, IF(J42="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J42="Cần Giờ", Ward!$AE$2:$AF$8, IF(J42="Củ Chi", Ward!$AG$2:$AH$22, IF(J42="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J42="Hóc Môn", Ward!$AK$2:$AL$13, IF(J42="Nhà Bè", Ward!$AM$2:$AN$8, IF(J42="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J42="Tân Bình", Ward!$AQ$2:$AR$16, IF(J42="Tân Phú", Ward!$AS$2:$AT$12, IF(J42="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3808,7 +3808,7 @@
         <f>IF(J43 &lt;&gt; "", VLOOKUP(J43, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W43" s="28" t="str">
+      <c r="W43" s="23" t="str">
         <f>IF(K43 &lt;&gt; "", VLOOKUP(K43, IF(J43="1", Ward!$A$2:$B$11, IF(J43="2", Ward!$C$2:$D$12, IF(J43="3", Ward!$E$2:$F$15, IF(J43="4", Ward!$G$2:$H$16, IF(J43="5", Ward!$I$2:$J$16, IF(J43="6", Ward!$K$2:$L$15, IF(J43="7", Ward!$M$2:$N$11, IF(J43="8", Ward!$O$2:$P$17, IF(J43="9", Ward!$Q$2:$R$14, IF(J43="10", Ward!$S$2:$T$16, IF(J43="11", Ward!$U$2:$V$17, IF(J43="12", Ward!$W$2:$X$12, IF(J43="Bình Chánh", Ward!$Y$2:$Z$17, IF(J43="Bình Tân", Ward!$AA$2:$AB$11, IF(J43="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J43="Cần Giờ", Ward!$AE$2:$AF$8, IF(J43="Củ Chi", Ward!$AG$2:$AH$22, IF(J43="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J43="Hóc Môn", Ward!$AK$2:$AL$13, IF(J43="Nhà Bè", Ward!$AM$2:$AN$8, IF(J43="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J43="Tân Bình", Ward!$AQ$2:$AR$16, IF(J43="Tân Phú", Ward!$AS$2:$AT$12, IF(J43="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3846,7 +3846,7 @@
         <f>IF(J44 &lt;&gt; "", VLOOKUP(J44, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W44" s="28" t="str">
+      <c r="W44" s="23" t="str">
         <f>IF(K44 &lt;&gt; "", VLOOKUP(K44, IF(J44="1", Ward!$A$2:$B$11, IF(J44="2", Ward!$C$2:$D$12, IF(J44="3", Ward!$E$2:$F$15, IF(J44="4", Ward!$G$2:$H$16, IF(J44="5", Ward!$I$2:$J$16, IF(J44="6", Ward!$K$2:$L$15, IF(J44="7", Ward!$M$2:$N$11, IF(J44="8", Ward!$O$2:$P$17, IF(J44="9", Ward!$Q$2:$R$14, IF(J44="10", Ward!$S$2:$T$16, IF(J44="11", Ward!$U$2:$V$17, IF(J44="12", Ward!$W$2:$X$12, IF(J44="Bình Chánh", Ward!$Y$2:$Z$17, IF(J44="Bình Tân", Ward!$AA$2:$AB$11, IF(J44="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J44="Cần Giờ", Ward!$AE$2:$AF$8, IF(J44="Củ Chi", Ward!$AG$2:$AH$22, IF(J44="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J44="Hóc Môn", Ward!$AK$2:$AL$13, IF(J44="Nhà Bè", Ward!$AM$2:$AN$8, IF(J44="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J44="Tân Bình", Ward!$AQ$2:$AR$16, IF(J44="Tân Phú", Ward!$AS$2:$AT$12, IF(J44="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3884,7 +3884,7 @@
         <f>IF(J45 &lt;&gt; "", VLOOKUP(J45, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W45" s="28" t="str">
+      <c r="W45" s="23" t="str">
         <f>IF(K45 &lt;&gt; "", VLOOKUP(K45, IF(J45="1", Ward!$A$2:$B$11, IF(J45="2", Ward!$C$2:$D$12, IF(J45="3", Ward!$E$2:$F$15, IF(J45="4", Ward!$G$2:$H$16, IF(J45="5", Ward!$I$2:$J$16, IF(J45="6", Ward!$K$2:$L$15, IF(J45="7", Ward!$M$2:$N$11, IF(J45="8", Ward!$O$2:$P$17, IF(J45="9", Ward!$Q$2:$R$14, IF(J45="10", Ward!$S$2:$T$16, IF(J45="11", Ward!$U$2:$V$17, IF(J45="12", Ward!$W$2:$X$12, IF(J45="Bình Chánh", Ward!$Y$2:$Z$17, IF(J45="Bình Tân", Ward!$AA$2:$AB$11, IF(J45="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J45="Cần Giờ", Ward!$AE$2:$AF$8, IF(J45="Củ Chi", Ward!$AG$2:$AH$22, IF(J45="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J45="Hóc Môn", Ward!$AK$2:$AL$13, IF(J45="Nhà Bè", Ward!$AM$2:$AN$8, IF(J45="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J45="Tân Bình", Ward!$AQ$2:$AR$16, IF(J45="Tân Phú", Ward!$AS$2:$AT$12, IF(J45="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3922,7 +3922,7 @@
         <f>IF(J46 &lt;&gt; "", VLOOKUP(J46, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W46" s="28" t="str">
+      <c r="W46" s="23" t="str">
         <f>IF(K46 &lt;&gt; "", VLOOKUP(K46, IF(J46="1", Ward!$A$2:$B$11, IF(J46="2", Ward!$C$2:$D$12, IF(J46="3", Ward!$E$2:$F$15, IF(J46="4", Ward!$G$2:$H$16, IF(J46="5", Ward!$I$2:$J$16, IF(J46="6", Ward!$K$2:$L$15, IF(J46="7", Ward!$M$2:$N$11, IF(J46="8", Ward!$O$2:$P$17, IF(J46="9", Ward!$Q$2:$R$14, IF(J46="10", Ward!$S$2:$T$16, IF(J46="11", Ward!$U$2:$V$17, IF(J46="12", Ward!$W$2:$X$12, IF(J46="Bình Chánh", Ward!$Y$2:$Z$17, IF(J46="Bình Tân", Ward!$AA$2:$AB$11, IF(J46="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J46="Cần Giờ", Ward!$AE$2:$AF$8, IF(J46="Củ Chi", Ward!$AG$2:$AH$22, IF(J46="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J46="Hóc Môn", Ward!$AK$2:$AL$13, IF(J46="Nhà Bè", Ward!$AM$2:$AN$8, IF(J46="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J46="Tân Bình", Ward!$AQ$2:$AR$16, IF(J46="Tân Phú", Ward!$AS$2:$AT$12, IF(J46="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3960,7 +3960,7 @@
         <f>IF(J47 &lt;&gt; "", VLOOKUP(J47, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W47" s="28" t="str">
+      <c r="W47" s="23" t="str">
         <f>IF(K47 &lt;&gt; "", VLOOKUP(K47, IF(J47="1", Ward!$A$2:$B$11, IF(J47="2", Ward!$C$2:$D$12, IF(J47="3", Ward!$E$2:$F$15, IF(J47="4", Ward!$G$2:$H$16, IF(J47="5", Ward!$I$2:$J$16, IF(J47="6", Ward!$K$2:$L$15, IF(J47="7", Ward!$M$2:$N$11, IF(J47="8", Ward!$O$2:$P$17, IF(J47="9", Ward!$Q$2:$R$14, IF(J47="10", Ward!$S$2:$T$16, IF(J47="11", Ward!$U$2:$V$17, IF(J47="12", Ward!$W$2:$X$12, IF(J47="Bình Chánh", Ward!$Y$2:$Z$17, IF(J47="Bình Tân", Ward!$AA$2:$AB$11, IF(J47="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J47="Cần Giờ", Ward!$AE$2:$AF$8, IF(J47="Củ Chi", Ward!$AG$2:$AH$22, IF(J47="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J47="Hóc Môn", Ward!$AK$2:$AL$13, IF(J47="Nhà Bè", Ward!$AM$2:$AN$8, IF(J47="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J47="Tân Bình", Ward!$AQ$2:$AR$16, IF(J47="Tân Phú", Ward!$AS$2:$AT$12, IF(J47="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -3998,7 +3998,7 @@
         <f>IF(J48 &lt;&gt; "", VLOOKUP(J48, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W48" s="28" t="str">
+      <c r="W48" s="23" t="str">
         <f>IF(K48 &lt;&gt; "", VLOOKUP(K48, IF(J48="1", Ward!$A$2:$B$11, IF(J48="2", Ward!$C$2:$D$12, IF(J48="3", Ward!$E$2:$F$15, IF(J48="4", Ward!$G$2:$H$16, IF(J48="5", Ward!$I$2:$J$16, IF(J48="6", Ward!$K$2:$L$15, IF(J48="7", Ward!$M$2:$N$11, IF(J48="8", Ward!$O$2:$P$17, IF(J48="9", Ward!$Q$2:$R$14, IF(J48="10", Ward!$S$2:$T$16, IF(J48="11", Ward!$U$2:$V$17, IF(J48="12", Ward!$W$2:$X$12, IF(J48="Bình Chánh", Ward!$Y$2:$Z$17, IF(J48="Bình Tân", Ward!$AA$2:$AB$11, IF(J48="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J48="Cần Giờ", Ward!$AE$2:$AF$8, IF(J48="Củ Chi", Ward!$AG$2:$AH$22, IF(J48="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J48="Hóc Môn", Ward!$AK$2:$AL$13, IF(J48="Nhà Bè", Ward!$AM$2:$AN$8, IF(J48="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J48="Tân Bình", Ward!$AQ$2:$AR$16, IF(J48="Tân Phú", Ward!$AS$2:$AT$12, IF(J48="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4036,7 +4036,7 @@
         <f>IF(J49 &lt;&gt; "", VLOOKUP(J49, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W49" s="28" t="str">
+      <c r="W49" s="23" t="str">
         <f>IF(K49 &lt;&gt; "", VLOOKUP(K49, IF(J49="1", Ward!$A$2:$B$11, IF(J49="2", Ward!$C$2:$D$12, IF(J49="3", Ward!$E$2:$F$15, IF(J49="4", Ward!$G$2:$H$16, IF(J49="5", Ward!$I$2:$J$16, IF(J49="6", Ward!$K$2:$L$15, IF(J49="7", Ward!$M$2:$N$11, IF(J49="8", Ward!$O$2:$P$17, IF(J49="9", Ward!$Q$2:$R$14, IF(J49="10", Ward!$S$2:$T$16, IF(J49="11", Ward!$U$2:$V$17, IF(J49="12", Ward!$W$2:$X$12, IF(J49="Bình Chánh", Ward!$Y$2:$Z$17, IF(J49="Bình Tân", Ward!$AA$2:$AB$11, IF(J49="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J49="Cần Giờ", Ward!$AE$2:$AF$8, IF(J49="Củ Chi", Ward!$AG$2:$AH$22, IF(J49="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J49="Hóc Môn", Ward!$AK$2:$AL$13, IF(J49="Nhà Bè", Ward!$AM$2:$AN$8, IF(J49="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J49="Tân Bình", Ward!$AQ$2:$AR$16, IF(J49="Tân Phú", Ward!$AS$2:$AT$12, IF(J49="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4074,7 +4074,7 @@
         <f>IF(J50 &lt;&gt; "", VLOOKUP(J50, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W50" s="28" t="str">
+      <c r="W50" s="23" t="str">
         <f>IF(K50 &lt;&gt; "", VLOOKUP(K50, IF(J50="1", Ward!$A$2:$B$11, IF(J50="2", Ward!$C$2:$D$12, IF(J50="3", Ward!$E$2:$F$15, IF(J50="4", Ward!$G$2:$H$16, IF(J50="5", Ward!$I$2:$J$16, IF(J50="6", Ward!$K$2:$L$15, IF(J50="7", Ward!$M$2:$N$11, IF(J50="8", Ward!$O$2:$P$17, IF(J50="9", Ward!$Q$2:$R$14, IF(J50="10", Ward!$S$2:$T$16, IF(J50="11", Ward!$U$2:$V$17, IF(J50="12", Ward!$W$2:$X$12, IF(J50="Bình Chánh", Ward!$Y$2:$Z$17, IF(J50="Bình Tân", Ward!$AA$2:$AB$11, IF(J50="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J50="Cần Giờ", Ward!$AE$2:$AF$8, IF(J50="Củ Chi", Ward!$AG$2:$AH$22, IF(J50="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J50="Hóc Môn", Ward!$AK$2:$AL$13, IF(J50="Nhà Bè", Ward!$AM$2:$AN$8, IF(J50="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J50="Tân Bình", Ward!$AQ$2:$AR$16, IF(J50="Tân Phú", Ward!$AS$2:$AT$12, IF(J50="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4112,7 +4112,7 @@
         <f>IF(J51 &lt;&gt; "", VLOOKUP(J51, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W51" s="28" t="str">
+      <c r="W51" s="23" t="str">
         <f>IF(K51 &lt;&gt; "", VLOOKUP(K51, IF(J51="1", Ward!$A$2:$B$11, IF(J51="2", Ward!$C$2:$D$12, IF(J51="3", Ward!$E$2:$F$15, IF(J51="4", Ward!$G$2:$H$16, IF(J51="5", Ward!$I$2:$J$16, IF(J51="6", Ward!$K$2:$L$15, IF(J51="7", Ward!$M$2:$N$11, IF(J51="8", Ward!$O$2:$P$17, IF(J51="9", Ward!$Q$2:$R$14, IF(J51="10", Ward!$S$2:$T$16, IF(J51="11", Ward!$U$2:$V$17, IF(J51="12", Ward!$W$2:$X$12, IF(J51="Bình Chánh", Ward!$Y$2:$Z$17, IF(J51="Bình Tân", Ward!$AA$2:$AB$11, IF(J51="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J51="Cần Giờ", Ward!$AE$2:$AF$8, IF(J51="Củ Chi", Ward!$AG$2:$AH$22, IF(J51="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J51="Hóc Môn", Ward!$AK$2:$AL$13, IF(J51="Nhà Bè", Ward!$AM$2:$AN$8, IF(J51="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J51="Tân Bình", Ward!$AQ$2:$AR$16, IF(J51="Tân Phú", Ward!$AS$2:$AT$12, IF(J51="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4150,7 +4150,7 @@
         <f>IF(J52 &lt;&gt; "", VLOOKUP(J52, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W52" s="28" t="str">
+      <c r="W52" s="23" t="str">
         <f>IF(K52 &lt;&gt; "", VLOOKUP(K52, IF(J52="1", Ward!$A$2:$B$11, IF(J52="2", Ward!$C$2:$D$12, IF(J52="3", Ward!$E$2:$F$15, IF(J52="4", Ward!$G$2:$H$16, IF(J52="5", Ward!$I$2:$J$16, IF(J52="6", Ward!$K$2:$L$15, IF(J52="7", Ward!$M$2:$N$11, IF(J52="8", Ward!$O$2:$P$17, IF(J52="9", Ward!$Q$2:$R$14, IF(J52="10", Ward!$S$2:$T$16, IF(J52="11", Ward!$U$2:$V$17, IF(J52="12", Ward!$W$2:$X$12, IF(J52="Bình Chánh", Ward!$Y$2:$Z$17, IF(J52="Bình Tân", Ward!$AA$2:$AB$11, IF(J52="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J52="Cần Giờ", Ward!$AE$2:$AF$8, IF(J52="Củ Chi", Ward!$AG$2:$AH$22, IF(J52="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J52="Hóc Môn", Ward!$AK$2:$AL$13, IF(J52="Nhà Bè", Ward!$AM$2:$AN$8, IF(J52="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J52="Tân Bình", Ward!$AQ$2:$AR$16, IF(J52="Tân Phú", Ward!$AS$2:$AT$12, IF(J52="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4188,7 +4188,7 @@
         <f>IF(J53 &lt;&gt; "", VLOOKUP(J53, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W53" s="28" t="str">
+      <c r="W53" s="23" t="str">
         <f>IF(K53 &lt;&gt; "", VLOOKUP(K53, IF(J53="1", Ward!$A$2:$B$11, IF(J53="2", Ward!$C$2:$D$12, IF(J53="3", Ward!$E$2:$F$15, IF(J53="4", Ward!$G$2:$H$16, IF(J53="5", Ward!$I$2:$J$16, IF(J53="6", Ward!$K$2:$L$15, IF(J53="7", Ward!$M$2:$N$11, IF(J53="8", Ward!$O$2:$P$17, IF(J53="9", Ward!$Q$2:$R$14, IF(J53="10", Ward!$S$2:$T$16, IF(J53="11", Ward!$U$2:$V$17, IF(J53="12", Ward!$W$2:$X$12, IF(J53="Bình Chánh", Ward!$Y$2:$Z$17, IF(J53="Bình Tân", Ward!$AA$2:$AB$11, IF(J53="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J53="Cần Giờ", Ward!$AE$2:$AF$8, IF(J53="Củ Chi", Ward!$AG$2:$AH$22, IF(J53="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J53="Hóc Môn", Ward!$AK$2:$AL$13, IF(J53="Nhà Bè", Ward!$AM$2:$AN$8, IF(J53="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J53="Tân Bình", Ward!$AQ$2:$AR$16, IF(J53="Tân Phú", Ward!$AS$2:$AT$12, IF(J53="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4226,7 +4226,7 @@
         <f>IF(J54 &lt;&gt; "", VLOOKUP(J54, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W54" s="28" t="str">
+      <c r="W54" s="23" t="str">
         <f>IF(K54 &lt;&gt; "", VLOOKUP(K54, IF(J54="1", Ward!$A$2:$B$11, IF(J54="2", Ward!$C$2:$D$12, IF(J54="3", Ward!$E$2:$F$15, IF(J54="4", Ward!$G$2:$H$16, IF(J54="5", Ward!$I$2:$J$16, IF(J54="6", Ward!$K$2:$L$15, IF(J54="7", Ward!$M$2:$N$11, IF(J54="8", Ward!$O$2:$P$17, IF(J54="9", Ward!$Q$2:$R$14, IF(J54="10", Ward!$S$2:$T$16, IF(J54="11", Ward!$U$2:$V$17, IF(J54="12", Ward!$W$2:$X$12, IF(J54="Bình Chánh", Ward!$Y$2:$Z$17, IF(J54="Bình Tân", Ward!$AA$2:$AB$11, IF(J54="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J54="Cần Giờ", Ward!$AE$2:$AF$8, IF(J54="Củ Chi", Ward!$AG$2:$AH$22, IF(J54="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J54="Hóc Môn", Ward!$AK$2:$AL$13, IF(J54="Nhà Bè", Ward!$AM$2:$AN$8, IF(J54="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J54="Tân Bình", Ward!$AQ$2:$AR$16, IF(J54="Tân Phú", Ward!$AS$2:$AT$12, IF(J54="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4264,7 +4264,7 @@
         <f>IF(J55 &lt;&gt; "", VLOOKUP(J55, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W55" s="28" t="str">
+      <c r="W55" s="23" t="str">
         <f>IF(K55 &lt;&gt; "", VLOOKUP(K55, IF(J55="1", Ward!$A$2:$B$11, IF(J55="2", Ward!$C$2:$D$12, IF(J55="3", Ward!$E$2:$F$15, IF(J55="4", Ward!$G$2:$H$16, IF(J55="5", Ward!$I$2:$J$16, IF(J55="6", Ward!$K$2:$L$15, IF(J55="7", Ward!$M$2:$N$11, IF(J55="8", Ward!$O$2:$P$17, IF(J55="9", Ward!$Q$2:$R$14, IF(J55="10", Ward!$S$2:$T$16, IF(J55="11", Ward!$U$2:$V$17, IF(J55="12", Ward!$W$2:$X$12, IF(J55="Bình Chánh", Ward!$Y$2:$Z$17, IF(J55="Bình Tân", Ward!$AA$2:$AB$11, IF(J55="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J55="Cần Giờ", Ward!$AE$2:$AF$8, IF(J55="Củ Chi", Ward!$AG$2:$AH$22, IF(J55="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J55="Hóc Môn", Ward!$AK$2:$AL$13, IF(J55="Nhà Bè", Ward!$AM$2:$AN$8, IF(J55="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J55="Tân Bình", Ward!$AQ$2:$AR$16, IF(J55="Tân Phú", Ward!$AS$2:$AT$12, IF(J55="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4302,7 +4302,7 @@
         <f>IF(J56 &lt;&gt; "", VLOOKUP(J56, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W56" s="28" t="str">
+      <c r="W56" s="23" t="str">
         <f>IF(K56 &lt;&gt; "", VLOOKUP(K56, IF(J56="1", Ward!$A$2:$B$11, IF(J56="2", Ward!$C$2:$D$12, IF(J56="3", Ward!$E$2:$F$15, IF(J56="4", Ward!$G$2:$H$16, IF(J56="5", Ward!$I$2:$J$16, IF(J56="6", Ward!$K$2:$L$15, IF(J56="7", Ward!$M$2:$N$11, IF(J56="8", Ward!$O$2:$P$17, IF(J56="9", Ward!$Q$2:$R$14, IF(J56="10", Ward!$S$2:$T$16, IF(J56="11", Ward!$U$2:$V$17, IF(J56="12", Ward!$W$2:$X$12, IF(J56="Bình Chánh", Ward!$Y$2:$Z$17, IF(J56="Bình Tân", Ward!$AA$2:$AB$11, IF(J56="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J56="Cần Giờ", Ward!$AE$2:$AF$8, IF(J56="Củ Chi", Ward!$AG$2:$AH$22, IF(J56="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J56="Hóc Môn", Ward!$AK$2:$AL$13, IF(J56="Nhà Bè", Ward!$AM$2:$AN$8, IF(J56="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J56="Tân Bình", Ward!$AQ$2:$AR$16, IF(J56="Tân Phú", Ward!$AS$2:$AT$12, IF(J56="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4340,7 +4340,7 @@
         <f>IF(J57 &lt;&gt; "", VLOOKUP(J57, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W57" s="28" t="str">
+      <c r="W57" s="23" t="str">
         <f>IF(K57 &lt;&gt; "", VLOOKUP(K57, IF(J57="1", Ward!$A$2:$B$11, IF(J57="2", Ward!$C$2:$D$12, IF(J57="3", Ward!$E$2:$F$15, IF(J57="4", Ward!$G$2:$H$16, IF(J57="5", Ward!$I$2:$J$16, IF(J57="6", Ward!$K$2:$L$15, IF(J57="7", Ward!$M$2:$N$11, IF(J57="8", Ward!$O$2:$P$17, IF(J57="9", Ward!$Q$2:$R$14, IF(J57="10", Ward!$S$2:$T$16, IF(J57="11", Ward!$U$2:$V$17, IF(J57="12", Ward!$W$2:$X$12, IF(J57="Bình Chánh", Ward!$Y$2:$Z$17, IF(J57="Bình Tân", Ward!$AA$2:$AB$11, IF(J57="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J57="Cần Giờ", Ward!$AE$2:$AF$8, IF(J57="Củ Chi", Ward!$AG$2:$AH$22, IF(J57="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J57="Hóc Môn", Ward!$AK$2:$AL$13, IF(J57="Nhà Bè", Ward!$AM$2:$AN$8, IF(J57="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J57="Tân Bình", Ward!$AQ$2:$AR$16, IF(J57="Tân Phú", Ward!$AS$2:$AT$12, IF(J57="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4378,7 +4378,7 @@
         <f>IF(J58 &lt;&gt; "", VLOOKUP(J58, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W58" s="28" t="str">
+      <c r="W58" s="23" t="str">
         <f>IF(K58 &lt;&gt; "", VLOOKUP(K58, IF(J58="1", Ward!$A$2:$B$11, IF(J58="2", Ward!$C$2:$D$12, IF(J58="3", Ward!$E$2:$F$15, IF(J58="4", Ward!$G$2:$H$16, IF(J58="5", Ward!$I$2:$J$16, IF(J58="6", Ward!$K$2:$L$15, IF(J58="7", Ward!$M$2:$N$11, IF(J58="8", Ward!$O$2:$P$17, IF(J58="9", Ward!$Q$2:$R$14, IF(J58="10", Ward!$S$2:$T$16, IF(J58="11", Ward!$U$2:$V$17, IF(J58="12", Ward!$W$2:$X$12, IF(J58="Bình Chánh", Ward!$Y$2:$Z$17, IF(J58="Bình Tân", Ward!$AA$2:$AB$11, IF(J58="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J58="Cần Giờ", Ward!$AE$2:$AF$8, IF(J58="Củ Chi", Ward!$AG$2:$AH$22, IF(J58="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J58="Hóc Môn", Ward!$AK$2:$AL$13, IF(J58="Nhà Bè", Ward!$AM$2:$AN$8, IF(J58="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J58="Tân Bình", Ward!$AQ$2:$AR$16, IF(J58="Tân Phú", Ward!$AS$2:$AT$12, IF(J58="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4416,7 +4416,7 @@
         <f>IF(J59 &lt;&gt; "", VLOOKUP(J59, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W59" s="28" t="str">
+      <c r="W59" s="23" t="str">
         <f>IF(K59 &lt;&gt; "", VLOOKUP(K59, IF(J59="1", Ward!$A$2:$B$11, IF(J59="2", Ward!$C$2:$D$12, IF(J59="3", Ward!$E$2:$F$15, IF(J59="4", Ward!$G$2:$H$16, IF(J59="5", Ward!$I$2:$J$16, IF(J59="6", Ward!$K$2:$L$15, IF(J59="7", Ward!$M$2:$N$11, IF(J59="8", Ward!$O$2:$P$17, IF(J59="9", Ward!$Q$2:$R$14, IF(J59="10", Ward!$S$2:$T$16, IF(J59="11", Ward!$U$2:$V$17, IF(J59="12", Ward!$W$2:$X$12, IF(J59="Bình Chánh", Ward!$Y$2:$Z$17, IF(J59="Bình Tân", Ward!$AA$2:$AB$11, IF(J59="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J59="Cần Giờ", Ward!$AE$2:$AF$8, IF(J59="Củ Chi", Ward!$AG$2:$AH$22, IF(J59="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J59="Hóc Môn", Ward!$AK$2:$AL$13, IF(J59="Nhà Bè", Ward!$AM$2:$AN$8, IF(J59="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J59="Tân Bình", Ward!$AQ$2:$AR$16, IF(J59="Tân Phú", Ward!$AS$2:$AT$12, IF(J59="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4454,7 +4454,7 @@
         <f>IF(J60 &lt;&gt; "", VLOOKUP(J60, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W60" s="28" t="str">
+      <c r="W60" s="23" t="str">
         <f>IF(K60 &lt;&gt; "", VLOOKUP(K60, IF(J60="1", Ward!$A$2:$B$11, IF(J60="2", Ward!$C$2:$D$12, IF(J60="3", Ward!$E$2:$F$15, IF(J60="4", Ward!$G$2:$H$16, IF(J60="5", Ward!$I$2:$J$16, IF(J60="6", Ward!$K$2:$L$15, IF(J60="7", Ward!$M$2:$N$11, IF(J60="8", Ward!$O$2:$P$17, IF(J60="9", Ward!$Q$2:$R$14, IF(J60="10", Ward!$S$2:$T$16, IF(J60="11", Ward!$U$2:$V$17, IF(J60="12", Ward!$W$2:$X$12, IF(J60="Bình Chánh", Ward!$Y$2:$Z$17, IF(J60="Bình Tân", Ward!$AA$2:$AB$11, IF(J60="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J60="Cần Giờ", Ward!$AE$2:$AF$8, IF(J60="Củ Chi", Ward!$AG$2:$AH$22, IF(J60="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J60="Hóc Môn", Ward!$AK$2:$AL$13, IF(J60="Nhà Bè", Ward!$AM$2:$AN$8, IF(J60="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J60="Tân Bình", Ward!$AQ$2:$AR$16, IF(J60="Tân Phú", Ward!$AS$2:$AT$12, IF(J60="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4492,7 +4492,7 @@
         <f>IF(J61 &lt;&gt; "", VLOOKUP(J61, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W61" s="28" t="str">
+      <c r="W61" s="23" t="str">
         <f>IF(K61 &lt;&gt; "", VLOOKUP(K61, IF(J61="1", Ward!$A$2:$B$11, IF(J61="2", Ward!$C$2:$D$12, IF(J61="3", Ward!$E$2:$F$15, IF(J61="4", Ward!$G$2:$H$16, IF(J61="5", Ward!$I$2:$J$16, IF(J61="6", Ward!$K$2:$L$15, IF(J61="7", Ward!$M$2:$N$11, IF(J61="8", Ward!$O$2:$P$17, IF(J61="9", Ward!$Q$2:$R$14, IF(J61="10", Ward!$S$2:$T$16, IF(J61="11", Ward!$U$2:$V$17, IF(J61="12", Ward!$W$2:$X$12, IF(J61="Bình Chánh", Ward!$Y$2:$Z$17, IF(J61="Bình Tân", Ward!$AA$2:$AB$11, IF(J61="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J61="Cần Giờ", Ward!$AE$2:$AF$8, IF(J61="Củ Chi", Ward!$AG$2:$AH$22, IF(J61="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J61="Hóc Môn", Ward!$AK$2:$AL$13, IF(J61="Nhà Bè", Ward!$AM$2:$AN$8, IF(J61="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J61="Tân Bình", Ward!$AQ$2:$AR$16, IF(J61="Tân Phú", Ward!$AS$2:$AT$12, IF(J61="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4530,7 +4530,7 @@
         <f>IF(J62 &lt;&gt; "", VLOOKUP(J62, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W62" s="28" t="str">
+      <c r="W62" s="23" t="str">
         <f>IF(K62 &lt;&gt; "", VLOOKUP(K62, IF(J62="1", Ward!$A$2:$B$11, IF(J62="2", Ward!$C$2:$D$12, IF(J62="3", Ward!$E$2:$F$15, IF(J62="4", Ward!$G$2:$H$16, IF(J62="5", Ward!$I$2:$J$16, IF(J62="6", Ward!$K$2:$L$15, IF(J62="7", Ward!$M$2:$N$11, IF(J62="8", Ward!$O$2:$P$17, IF(J62="9", Ward!$Q$2:$R$14, IF(J62="10", Ward!$S$2:$T$16, IF(J62="11", Ward!$U$2:$V$17, IF(J62="12", Ward!$W$2:$X$12, IF(J62="Bình Chánh", Ward!$Y$2:$Z$17, IF(J62="Bình Tân", Ward!$AA$2:$AB$11, IF(J62="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J62="Cần Giờ", Ward!$AE$2:$AF$8, IF(J62="Củ Chi", Ward!$AG$2:$AH$22, IF(J62="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J62="Hóc Môn", Ward!$AK$2:$AL$13, IF(J62="Nhà Bè", Ward!$AM$2:$AN$8, IF(J62="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J62="Tân Bình", Ward!$AQ$2:$AR$16, IF(J62="Tân Phú", Ward!$AS$2:$AT$12, IF(J62="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4568,7 +4568,7 @@
         <f>IF(J63 &lt;&gt; "", VLOOKUP(J63, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W63" s="28" t="str">
+      <c r="W63" s="23" t="str">
         <f>IF(K63 &lt;&gt; "", VLOOKUP(K63, IF(J63="1", Ward!$A$2:$B$11, IF(J63="2", Ward!$C$2:$D$12, IF(J63="3", Ward!$E$2:$F$15, IF(J63="4", Ward!$G$2:$H$16, IF(J63="5", Ward!$I$2:$J$16, IF(J63="6", Ward!$K$2:$L$15, IF(J63="7", Ward!$M$2:$N$11, IF(J63="8", Ward!$O$2:$P$17, IF(J63="9", Ward!$Q$2:$R$14, IF(J63="10", Ward!$S$2:$T$16, IF(J63="11", Ward!$U$2:$V$17, IF(J63="12", Ward!$W$2:$X$12, IF(J63="Bình Chánh", Ward!$Y$2:$Z$17, IF(J63="Bình Tân", Ward!$AA$2:$AB$11, IF(J63="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J63="Cần Giờ", Ward!$AE$2:$AF$8, IF(J63="Củ Chi", Ward!$AG$2:$AH$22, IF(J63="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J63="Hóc Môn", Ward!$AK$2:$AL$13, IF(J63="Nhà Bè", Ward!$AM$2:$AN$8, IF(J63="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J63="Tân Bình", Ward!$AQ$2:$AR$16, IF(J63="Tân Phú", Ward!$AS$2:$AT$12, IF(J63="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4606,7 +4606,7 @@
         <f>IF(J64 &lt;&gt; "", VLOOKUP(J64, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W64" s="28" t="str">
+      <c r="W64" s="23" t="str">
         <f>IF(K64 &lt;&gt; "", VLOOKUP(K64, IF(J64="1", Ward!$A$2:$B$11, IF(J64="2", Ward!$C$2:$D$12, IF(J64="3", Ward!$E$2:$F$15, IF(J64="4", Ward!$G$2:$H$16, IF(J64="5", Ward!$I$2:$J$16, IF(J64="6", Ward!$K$2:$L$15, IF(J64="7", Ward!$M$2:$N$11, IF(J64="8", Ward!$O$2:$P$17, IF(J64="9", Ward!$Q$2:$R$14, IF(J64="10", Ward!$S$2:$T$16, IF(J64="11", Ward!$U$2:$V$17, IF(J64="12", Ward!$W$2:$X$12, IF(J64="Bình Chánh", Ward!$Y$2:$Z$17, IF(J64="Bình Tân", Ward!$AA$2:$AB$11, IF(J64="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J64="Cần Giờ", Ward!$AE$2:$AF$8, IF(J64="Củ Chi", Ward!$AG$2:$AH$22, IF(J64="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J64="Hóc Môn", Ward!$AK$2:$AL$13, IF(J64="Nhà Bè", Ward!$AM$2:$AN$8, IF(J64="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J64="Tân Bình", Ward!$AQ$2:$AR$16, IF(J64="Tân Phú", Ward!$AS$2:$AT$12, IF(J64="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4644,7 +4644,7 @@
         <f>IF(J65 &lt;&gt; "", VLOOKUP(J65, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W65" s="28" t="str">
+      <c r="W65" s="23" t="str">
         <f>IF(K65 &lt;&gt; "", VLOOKUP(K65, IF(J65="1", Ward!$A$2:$B$11, IF(J65="2", Ward!$C$2:$D$12, IF(J65="3", Ward!$E$2:$F$15, IF(J65="4", Ward!$G$2:$H$16, IF(J65="5", Ward!$I$2:$J$16, IF(J65="6", Ward!$K$2:$L$15, IF(J65="7", Ward!$M$2:$N$11, IF(J65="8", Ward!$O$2:$P$17, IF(J65="9", Ward!$Q$2:$R$14, IF(J65="10", Ward!$S$2:$T$16, IF(J65="11", Ward!$U$2:$V$17, IF(J65="12", Ward!$W$2:$X$12, IF(J65="Bình Chánh", Ward!$Y$2:$Z$17, IF(J65="Bình Tân", Ward!$AA$2:$AB$11, IF(J65="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J65="Cần Giờ", Ward!$AE$2:$AF$8, IF(J65="Củ Chi", Ward!$AG$2:$AH$22, IF(J65="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J65="Hóc Môn", Ward!$AK$2:$AL$13, IF(J65="Nhà Bè", Ward!$AM$2:$AN$8, IF(J65="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J65="Tân Bình", Ward!$AQ$2:$AR$16, IF(J65="Tân Phú", Ward!$AS$2:$AT$12, IF(J65="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4682,7 +4682,7 @@
         <f>IF(J66 &lt;&gt; "", VLOOKUP(J66, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W66" s="28" t="str">
+      <c r="W66" s="23" t="str">
         <f>IF(K66 &lt;&gt; "", VLOOKUP(K66, IF(J66="1", Ward!$A$2:$B$11, IF(J66="2", Ward!$C$2:$D$12, IF(J66="3", Ward!$E$2:$F$15, IF(J66="4", Ward!$G$2:$H$16, IF(J66="5", Ward!$I$2:$J$16, IF(J66="6", Ward!$K$2:$L$15, IF(J66="7", Ward!$M$2:$N$11, IF(J66="8", Ward!$O$2:$P$17, IF(J66="9", Ward!$Q$2:$R$14, IF(J66="10", Ward!$S$2:$T$16, IF(J66="11", Ward!$U$2:$V$17, IF(J66="12", Ward!$W$2:$X$12, IF(J66="Bình Chánh", Ward!$Y$2:$Z$17, IF(J66="Bình Tân", Ward!$AA$2:$AB$11, IF(J66="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J66="Cần Giờ", Ward!$AE$2:$AF$8, IF(J66="Củ Chi", Ward!$AG$2:$AH$22, IF(J66="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J66="Hóc Môn", Ward!$AK$2:$AL$13, IF(J66="Nhà Bè", Ward!$AM$2:$AN$8, IF(J66="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J66="Tân Bình", Ward!$AQ$2:$AR$16, IF(J66="Tân Phú", Ward!$AS$2:$AT$12, IF(J66="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4720,7 +4720,7 @@
         <f>IF(J67 &lt;&gt; "", VLOOKUP(J67, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W67" s="28" t="str">
+      <c r="W67" s="23" t="str">
         <f>IF(K67 &lt;&gt; "", VLOOKUP(K67, IF(J67="1", Ward!$A$2:$B$11, IF(J67="2", Ward!$C$2:$D$12, IF(J67="3", Ward!$E$2:$F$15, IF(J67="4", Ward!$G$2:$H$16, IF(J67="5", Ward!$I$2:$J$16, IF(J67="6", Ward!$K$2:$L$15, IF(J67="7", Ward!$M$2:$N$11, IF(J67="8", Ward!$O$2:$P$17, IF(J67="9", Ward!$Q$2:$R$14, IF(J67="10", Ward!$S$2:$T$16, IF(J67="11", Ward!$U$2:$V$17, IF(J67="12", Ward!$W$2:$X$12, IF(J67="Bình Chánh", Ward!$Y$2:$Z$17, IF(J67="Bình Tân", Ward!$AA$2:$AB$11, IF(J67="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J67="Cần Giờ", Ward!$AE$2:$AF$8, IF(J67="Củ Chi", Ward!$AG$2:$AH$22, IF(J67="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J67="Hóc Môn", Ward!$AK$2:$AL$13, IF(J67="Nhà Bè", Ward!$AM$2:$AN$8, IF(J67="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J67="Tân Bình", Ward!$AQ$2:$AR$16, IF(J67="Tân Phú", Ward!$AS$2:$AT$12, IF(J67="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4758,7 +4758,7 @@
         <f>IF(J68 &lt;&gt; "", VLOOKUP(J68, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W68" s="28" t="str">
+      <c r="W68" s="23" t="str">
         <f>IF(K68 &lt;&gt; "", VLOOKUP(K68, IF(J68="1", Ward!$A$2:$B$11, IF(J68="2", Ward!$C$2:$D$12, IF(J68="3", Ward!$E$2:$F$15, IF(J68="4", Ward!$G$2:$H$16, IF(J68="5", Ward!$I$2:$J$16, IF(J68="6", Ward!$K$2:$L$15, IF(J68="7", Ward!$M$2:$N$11, IF(J68="8", Ward!$O$2:$P$17, IF(J68="9", Ward!$Q$2:$R$14, IF(J68="10", Ward!$S$2:$T$16, IF(J68="11", Ward!$U$2:$V$17, IF(J68="12", Ward!$W$2:$X$12, IF(J68="Bình Chánh", Ward!$Y$2:$Z$17, IF(J68="Bình Tân", Ward!$AA$2:$AB$11, IF(J68="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J68="Cần Giờ", Ward!$AE$2:$AF$8, IF(J68="Củ Chi", Ward!$AG$2:$AH$22, IF(J68="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J68="Hóc Môn", Ward!$AK$2:$AL$13, IF(J68="Nhà Bè", Ward!$AM$2:$AN$8, IF(J68="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J68="Tân Bình", Ward!$AQ$2:$AR$16, IF(J68="Tân Phú", Ward!$AS$2:$AT$12, IF(J68="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4796,7 +4796,7 @@
         <f>IF(J69 &lt;&gt; "", VLOOKUP(J69, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W69" s="28" t="str">
+      <c r="W69" s="23" t="str">
         <f>IF(K69 &lt;&gt; "", VLOOKUP(K69, IF(J69="1", Ward!$A$2:$B$11, IF(J69="2", Ward!$C$2:$D$12, IF(J69="3", Ward!$E$2:$F$15, IF(J69="4", Ward!$G$2:$H$16, IF(J69="5", Ward!$I$2:$J$16, IF(J69="6", Ward!$K$2:$L$15, IF(J69="7", Ward!$M$2:$N$11, IF(J69="8", Ward!$O$2:$P$17, IF(J69="9", Ward!$Q$2:$R$14, IF(J69="10", Ward!$S$2:$T$16, IF(J69="11", Ward!$U$2:$V$17, IF(J69="12", Ward!$W$2:$X$12, IF(J69="Bình Chánh", Ward!$Y$2:$Z$17, IF(J69="Bình Tân", Ward!$AA$2:$AB$11, IF(J69="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J69="Cần Giờ", Ward!$AE$2:$AF$8, IF(J69="Củ Chi", Ward!$AG$2:$AH$22, IF(J69="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J69="Hóc Môn", Ward!$AK$2:$AL$13, IF(J69="Nhà Bè", Ward!$AM$2:$AN$8, IF(J69="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J69="Tân Bình", Ward!$AQ$2:$AR$16, IF(J69="Tân Phú", Ward!$AS$2:$AT$12, IF(J69="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4834,7 +4834,7 @@
         <f>IF(J70 &lt;&gt; "", VLOOKUP(J70, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W70" s="28" t="str">
+      <c r="W70" s="23" t="str">
         <f>IF(K70 &lt;&gt; "", VLOOKUP(K70, IF(J70="1", Ward!$A$2:$B$11, IF(J70="2", Ward!$C$2:$D$12, IF(J70="3", Ward!$E$2:$F$15, IF(J70="4", Ward!$G$2:$H$16, IF(J70="5", Ward!$I$2:$J$16, IF(J70="6", Ward!$K$2:$L$15, IF(J70="7", Ward!$M$2:$N$11, IF(J70="8", Ward!$O$2:$P$17, IF(J70="9", Ward!$Q$2:$R$14, IF(J70="10", Ward!$S$2:$T$16, IF(J70="11", Ward!$U$2:$V$17, IF(J70="12", Ward!$W$2:$X$12, IF(J70="Bình Chánh", Ward!$Y$2:$Z$17, IF(J70="Bình Tân", Ward!$AA$2:$AB$11, IF(J70="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J70="Cần Giờ", Ward!$AE$2:$AF$8, IF(J70="Củ Chi", Ward!$AG$2:$AH$22, IF(J70="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J70="Hóc Môn", Ward!$AK$2:$AL$13, IF(J70="Nhà Bè", Ward!$AM$2:$AN$8, IF(J70="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J70="Tân Bình", Ward!$AQ$2:$AR$16, IF(J70="Tân Phú", Ward!$AS$2:$AT$12, IF(J70="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4872,7 +4872,7 @@
         <f>IF(J71 &lt;&gt; "", VLOOKUP(J71, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W71" s="28" t="str">
+      <c r="W71" s="23" t="str">
         <f>IF(K71 &lt;&gt; "", VLOOKUP(K71, IF(J71="1", Ward!$A$2:$B$11, IF(J71="2", Ward!$C$2:$D$12, IF(J71="3", Ward!$E$2:$F$15, IF(J71="4", Ward!$G$2:$H$16, IF(J71="5", Ward!$I$2:$J$16, IF(J71="6", Ward!$K$2:$L$15, IF(J71="7", Ward!$M$2:$N$11, IF(J71="8", Ward!$O$2:$P$17, IF(J71="9", Ward!$Q$2:$R$14, IF(J71="10", Ward!$S$2:$T$16, IF(J71="11", Ward!$U$2:$V$17, IF(J71="12", Ward!$W$2:$X$12, IF(J71="Bình Chánh", Ward!$Y$2:$Z$17, IF(J71="Bình Tân", Ward!$AA$2:$AB$11, IF(J71="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J71="Cần Giờ", Ward!$AE$2:$AF$8, IF(J71="Củ Chi", Ward!$AG$2:$AH$22, IF(J71="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J71="Hóc Môn", Ward!$AK$2:$AL$13, IF(J71="Nhà Bè", Ward!$AM$2:$AN$8, IF(J71="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J71="Tân Bình", Ward!$AQ$2:$AR$16, IF(J71="Tân Phú", Ward!$AS$2:$AT$12, IF(J71="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4910,7 +4910,7 @@
         <f>IF(J72 &lt;&gt; "", VLOOKUP(J72, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W72" s="28" t="str">
+      <c r="W72" s="23" t="str">
         <f>IF(K72 &lt;&gt; "", VLOOKUP(K72, IF(J72="1", Ward!$A$2:$B$11, IF(J72="2", Ward!$C$2:$D$12, IF(J72="3", Ward!$E$2:$F$15, IF(J72="4", Ward!$G$2:$H$16, IF(J72="5", Ward!$I$2:$J$16, IF(J72="6", Ward!$K$2:$L$15, IF(J72="7", Ward!$M$2:$N$11, IF(J72="8", Ward!$O$2:$P$17, IF(J72="9", Ward!$Q$2:$R$14, IF(J72="10", Ward!$S$2:$T$16, IF(J72="11", Ward!$U$2:$V$17, IF(J72="12", Ward!$W$2:$X$12, IF(J72="Bình Chánh", Ward!$Y$2:$Z$17, IF(J72="Bình Tân", Ward!$AA$2:$AB$11, IF(J72="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J72="Cần Giờ", Ward!$AE$2:$AF$8, IF(J72="Củ Chi", Ward!$AG$2:$AH$22, IF(J72="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J72="Hóc Môn", Ward!$AK$2:$AL$13, IF(J72="Nhà Bè", Ward!$AM$2:$AN$8, IF(J72="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J72="Tân Bình", Ward!$AQ$2:$AR$16, IF(J72="Tân Phú", Ward!$AS$2:$AT$12, IF(J72="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4948,7 +4948,7 @@
         <f>IF(J73 &lt;&gt; "", VLOOKUP(J73, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W73" s="28" t="str">
+      <c r="W73" s="23" t="str">
         <f>IF(K73 &lt;&gt; "", VLOOKUP(K73, IF(J73="1", Ward!$A$2:$B$11, IF(J73="2", Ward!$C$2:$D$12, IF(J73="3", Ward!$E$2:$F$15, IF(J73="4", Ward!$G$2:$H$16, IF(J73="5", Ward!$I$2:$J$16, IF(J73="6", Ward!$K$2:$L$15, IF(J73="7", Ward!$M$2:$N$11, IF(J73="8", Ward!$O$2:$P$17, IF(J73="9", Ward!$Q$2:$R$14, IF(J73="10", Ward!$S$2:$T$16, IF(J73="11", Ward!$U$2:$V$17, IF(J73="12", Ward!$W$2:$X$12, IF(J73="Bình Chánh", Ward!$Y$2:$Z$17, IF(J73="Bình Tân", Ward!$AA$2:$AB$11, IF(J73="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J73="Cần Giờ", Ward!$AE$2:$AF$8, IF(J73="Củ Chi", Ward!$AG$2:$AH$22, IF(J73="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J73="Hóc Môn", Ward!$AK$2:$AL$13, IF(J73="Nhà Bè", Ward!$AM$2:$AN$8, IF(J73="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J73="Tân Bình", Ward!$AQ$2:$AR$16, IF(J73="Tân Phú", Ward!$AS$2:$AT$12, IF(J73="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -4986,7 +4986,7 @@
         <f>IF(J74 &lt;&gt; "", VLOOKUP(J74, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W74" s="28" t="str">
+      <c r="W74" s="23" t="str">
         <f>IF(K74 &lt;&gt; "", VLOOKUP(K74, IF(J74="1", Ward!$A$2:$B$11, IF(J74="2", Ward!$C$2:$D$12, IF(J74="3", Ward!$E$2:$F$15, IF(J74="4", Ward!$G$2:$H$16, IF(J74="5", Ward!$I$2:$J$16, IF(J74="6", Ward!$K$2:$L$15, IF(J74="7", Ward!$M$2:$N$11, IF(J74="8", Ward!$O$2:$P$17, IF(J74="9", Ward!$Q$2:$R$14, IF(J74="10", Ward!$S$2:$T$16, IF(J74="11", Ward!$U$2:$V$17, IF(J74="12", Ward!$W$2:$X$12, IF(J74="Bình Chánh", Ward!$Y$2:$Z$17, IF(J74="Bình Tân", Ward!$AA$2:$AB$11, IF(J74="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J74="Cần Giờ", Ward!$AE$2:$AF$8, IF(J74="Củ Chi", Ward!$AG$2:$AH$22, IF(J74="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J74="Hóc Môn", Ward!$AK$2:$AL$13, IF(J74="Nhà Bè", Ward!$AM$2:$AN$8, IF(J74="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J74="Tân Bình", Ward!$AQ$2:$AR$16, IF(J74="Tân Phú", Ward!$AS$2:$AT$12, IF(J74="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5024,7 +5024,7 @@
         <f>IF(J75 &lt;&gt; "", VLOOKUP(J75, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W75" s="28" t="str">
+      <c r="W75" s="23" t="str">
         <f>IF(K75 &lt;&gt; "", VLOOKUP(K75, IF(J75="1", Ward!$A$2:$B$11, IF(J75="2", Ward!$C$2:$D$12, IF(J75="3", Ward!$E$2:$F$15, IF(J75="4", Ward!$G$2:$H$16, IF(J75="5", Ward!$I$2:$J$16, IF(J75="6", Ward!$K$2:$L$15, IF(J75="7", Ward!$M$2:$N$11, IF(J75="8", Ward!$O$2:$P$17, IF(J75="9", Ward!$Q$2:$R$14, IF(J75="10", Ward!$S$2:$T$16, IF(J75="11", Ward!$U$2:$V$17, IF(J75="12", Ward!$W$2:$X$12, IF(J75="Bình Chánh", Ward!$Y$2:$Z$17, IF(J75="Bình Tân", Ward!$AA$2:$AB$11, IF(J75="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J75="Cần Giờ", Ward!$AE$2:$AF$8, IF(J75="Củ Chi", Ward!$AG$2:$AH$22, IF(J75="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J75="Hóc Môn", Ward!$AK$2:$AL$13, IF(J75="Nhà Bè", Ward!$AM$2:$AN$8, IF(J75="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J75="Tân Bình", Ward!$AQ$2:$AR$16, IF(J75="Tân Phú", Ward!$AS$2:$AT$12, IF(J75="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5062,7 +5062,7 @@
         <f>IF(J76 &lt;&gt; "", VLOOKUP(J76, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W76" s="28" t="str">
+      <c r="W76" s="23" t="str">
         <f>IF(K76 &lt;&gt; "", VLOOKUP(K76, IF(J76="1", Ward!$A$2:$B$11, IF(J76="2", Ward!$C$2:$D$12, IF(J76="3", Ward!$E$2:$F$15, IF(J76="4", Ward!$G$2:$H$16, IF(J76="5", Ward!$I$2:$J$16, IF(J76="6", Ward!$K$2:$L$15, IF(J76="7", Ward!$M$2:$N$11, IF(J76="8", Ward!$O$2:$P$17, IF(J76="9", Ward!$Q$2:$R$14, IF(J76="10", Ward!$S$2:$T$16, IF(J76="11", Ward!$U$2:$V$17, IF(J76="12", Ward!$W$2:$X$12, IF(J76="Bình Chánh", Ward!$Y$2:$Z$17, IF(J76="Bình Tân", Ward!$AA$2:$AB$11, IF(J76="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J76="Cần Giờ", Ward!$AE$2:$AF$8, IF(J76="Củ Chi", Ward!$AG$2:$AH$22, IF(J76="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J76="Hóc Môn", Ward!$AK$2:$AL$13, IF(J76="Nhà Bè", Ward!$AM$2:$AN$8, IF(J76="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J76="Tân Bình", Ward!$AQ$2:$AR$16, IF(J76="Tân Phú", Ward!$AS$2:$AT$12, IF(J76="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5100,7 +5100,7 @@
         <f>IF(J77 &lt;&gt; "", VLOOKUP(J77, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W77" s="28" t="str">
+      <c r="W77" s="23" t="str">
         <f>IF(K77 &lt;&gt; "", VLOOKUP(K77, IF(J77="1", Ward!$A$2:$B$11, IF(J77="2", Ward!$C$2:$D$12, IF(J77="3", Ward!$E$2:$F$15, IF(J77="4", Ward!$G$2:$H$16, IF(J77="5", Ward!$I$2:$J$16, IF(J77="6", Ward!$K$2:$L$15, IF(J77="7", Ward!$M$2:$N$11, IF(J77="8", Ward!$O$2:$P$17, IF(J77="9", Ward!$Q$2:$R$14, IF(J77="10", Ward!$S$2:$T$16, IF(J77="11", Ward!$U$2:$V$17, IF(J77="12", Ward!$W$2:$X$12, IF(J77="Bình Chánh", Ward!$Y$2:$Z$17, IF(J77="Bình Tân", Ward!$AA$2:$AB$11, IF(J77="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J77="Cần Giờ", Ward!$AE$2:$AF$8, IF(J77="Củ Chi", Ward!$AG$2:$AH$22, IF(J77="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J77="Hóc Môn", Ward!$AK$2:$AL$13, IF(J77="Nhà Bè", Ward!$AM$2:$AN$8, IF(J77="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J77="Tân Bình", Ward!$AQ$2:$AR$16, IF(J77="Tân Phú", Ward!$AS$2:$AT$12, IF(J77="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5138,7 +5138,7 @@
         <f>IF(J78 &lt;&gt; "", VLOOKUP(J78, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W78" s="28" t="str">
+      <c r="W78" s="23" t="str">
         <f>IF(K78 &lt;&gt; "", VLOOKUP(K78, IF(J78="1", Ward!$A$2:$B$11, IF(J78="2", Ward!$C$2:$D$12, IF(J78="3", Ward!$E$2:$F$15, IF(J78="4", Ward!$G$2:$H$16, IF(J78="5", Ward!$I$2:$J$16, IF(J78="6", Ward!$K$2:$L$15, IF(J78="7", Ward!$M$2:$N$11, IF(J78="8", Ward!$O$2:$P$17, IF(J78="9", Ward!$Q$2:$R$14, IF(J78="10", Ward!$S$2:$T$16, IF(J78="11", Ward!$U$2:$V$17, IF(J78="12", Ward!$W$2:$X$12, IF(J78="Bình Chánh", Ward!$Y$2:$Z$17, IF(J78="Bình Tân", Ward!$AA$2:$AB$11, IF(J78="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J78="Cần Giờ", Ward!$AE$2:$AF$8, IF(J78="Củ Chi", Ward!$AG$2:$AH$22, IF(J78="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J78="Hóc Môn", Ward!$AK$2:$AL$13, IF(J78="Nhà Bè", Ward!$AM$2:$AN$8, IF(J78="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J78="Tân Bình", Ward!$AQ$2:$AR$16, IF(J78="Tân Phú", Ward!$AS$2:$AT$12, IF(J78="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5176,7 +5176,7 @@
         <f>IF(J79 &lt;&gt; "", VLOOKUP(J79, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W79" s="28" t="str">
+      <c r="W79" s="23" t="str">
         <f>IF(K79 &lt;&gt; "", VLOOKUP(K79, IF(J79="1", Ward!$A$2:$B$11, IF(J79="2", Ward!$C$2:$D$12, IF(J79="3", Ward!$E$2:$F$15, IF(J79="4", Ward!$G$2:$H$16, IF(J79="5", Ward!$I$2:$J$16, IF(J79="6", Ward!$K$2:$L$15, IF(J79="7", Ward!$M$2:$N$11, IF(J79="8", Ward!$O$2:$P$17, IF(J79="9", Ward!$Q$2:$R$14, IF(J79="10", Ward!$S$2:$T$16, IF(J79="11", Ward!$U$2:$V$17, IF(J79="12", Ward!$W$2:$X$12, IF(J79="Bình Chánh", Ward!$Y$2:$Z$17, IF(J79="Bình Tân", Ward!$AA$2:$AB$11, IF(J79="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J79="Cần Giờ", Ward!$AE$2:$AF$8, IF(J79="Củ Chi", Ward!$AG$2:$AH$22, IF(J79="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J79="Hóc Môn", Ward!$AK$2:$AL$13, IF(J79="Nhà Bè", Ward!$AM$2:$AN$8, IF(J79="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J79="Tân Bình", Ward!$AQ$2:$AR$16, IF(J79="Tân Phú", Ward!$AS$2:$AT$12, IF(J79="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5214,7 +5214,7 @@
         <f>IF(J80 &lt;&gt; "", VLOOKUP(J80, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W80" s="28" t="str">
+      <c r="W80" s="23" t="str">
         <f>IF(K80 &lt;&gt; "", VLOOKUP(K80, IF(J80="1", Ward!$A$2:$B$11, IF(J80="2", Ward!$C$2:$D$12, IF(J80="3", Ward!$E$2:$F$15, IF(J80="4", Ward!$G$2:$H$16, IF(J80="5", Ward!$I$2:$J$16, IF(J80="6", Ward!$K$2:$L$15, IF(J80="7", Ward!$M$2:$N$11, IF(J80="8", Ward!$O$2:$P$17, IF(J80="9", Ward!$Q$2:$R$14, IF(J80="10", Ward!$S$2:$T$16, IF(J80="11", Ward!$U$2:$V$17, IF(J80="12", Ward!$W$2:$X$12, IF(J80="Bình Chánh", Ward!$Y$2:$Z$17, IF(J80="Bình Tân", Ward!$AA$2:$AB$11, IF(J80="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J80="Cần Giờ", Ward!$AE$2:$AF$8, IF(J80="Củ Chi", Ward!$AG$2:$AH$22, IF(J80="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J80="Hóc Môn", Ward!$AK$2:$AL$13, IF(J80="Nhà Bè", Ward!$AM$2:$AN$8, IF(J80="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J80="Tân Bình", Ward!$AQ$2:$AR$16, IF(J80="Tân Phú", Ward!$AS$2:$AT$12, IF(J80="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5252,7 +5252,7 @@
         <f>IF(J81 &lt;&gt; "", VLOOKUP(J81, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W81" s="28" t="str">
+      <c r="W81" s="23" t="str">
         <f>IF(K81 &lt;&gt; "", VLOOKUP(K81, IF(J81="1", Ward!$A$2:$B$11, IF(J81="2", Ward!$C$2:$D$12, IF(J81="3", Ward!$E$2:$F$15, IF(J81="4", Ward!$G$2:$H$16, IF(J81="5", Ward!$I$2:$J$16, IF(J81="6", Ward!$K$2:$L$15, IF(J81="7", Ward!$M$2:$N$11, IF(J81="8", Ward!$O$2:$P$17, IF(J81="9", Ward!$Q$2:$R$14, IF(J81="10", Ward!$S$2:$T$16, IF(J81="11", Ward!$U$2:$V$17, IF(J81="12", Ward!$W$2:$X$12, IF(J81="Bình Chánh", Ward!$Y$2:$Z$17, IF(J81="Bình Tân", Ward!$AA$2:$AB$11, IF(J81="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J81="Cần Giờ", Ward!$AE$2:$AF$8, IF(J81="Củ Chi", Ward!$AG$2:$AH$22, IF(J81="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J81="Hóc Môn", Ward!$AK$2:$AL$13, IF(J81="Nhà Bè", Ward!$AM$2:$AN$8, IF(J81="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J81="Tân Bình", Ward!$AQ$2:$AR$16, IF(J81="Tân Phú", Ward!$AS$2:$AT$12, IF(J81="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5290,7 +5290,7 @@
         <f>IF(J82 &lt;&gt; "", VLOOKUP(J82, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W82" s="28" t="str">
+      <c r="W82" s="23" t="str">
         <f>IF(K82 &lt;&gt; "", VLOOKUP(K82, IF(J82="1", Ward!$A$2:$B$11, IF(J82="2", Ward!$C$2:$D$12, IF(J82="3", Ward!$E$2:$F$15, IF(J82="4", Ward!$G$2:$H$16, IF(J82="5", Ward!$I$2:$J$16, IF(J82="6", Ward!$K$2:$L$15, IF(J82="7", Ward!$M$2:$N$11, IF(J82="8", Ward!$O$2:$P$17, IF(J82="9", Ward!$Q$2:$R$14, IF(J82="10", Ward!$S$2:$T$16, IF(J82="11", Ward!$U$2:$V$17, IF(J82="12", Ward!$W$2:$X$12, IF(J82="Bình Chánh", Ward!$Y$2:$Z$17, IF(J82="Bình Tân", Ward!$AA$2:$AB$11, IF(J82="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J82="Cần Giờ", Ward!$AE$2:$AF$8, IF(J82="Củ Chi", Ward!$AG$2:$AH$22, IF(J82="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J82="Hóc Môn", Ward!$AK$2:$AL$13, IF(J82="Nhà Bè", Ward!$AM$2:$AN$8, IF(J82="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J82="Tân Bình", Ward!$AQ$2:$AR$16, IF(J82="Tân Phú", Ward!$AS$2:$AT$12, IF(J82="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5328,7 +5328,7 @@
         <f>IF(J83 &lt;&gt; "", VLOOKUP(J83, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W83" s="28" t="str">
+      <c r="W83" s="23" t="str">
         <f>IF(K83 &lt;&gt; "", VLOOKUP(K83, IF(J83="1", Ward!$A$2:$B$11, IF(J83="2", Ward!$C$2:$D$12, IF(J83="3", Ward!$E$2:$F$15, IF(J83="4", Ward!$G$2:$H$16, IF(J83="5", Ward!$I$2:$J$16, IF(J83="6", Ward!$K$2:$L$15, IF(J83="7", Ward!$M$2:$N$11, IF(J83="8", Ward!$O$2:$P$17, IF(J83="9", Ward!$Q$2:$R$14, IF(J83="10", Ward!$S$2:$T$16, IF(J83="11", Ward!$U$2:$V$17, IF(J83="12", Ward!$W$2:$X$12, IF(J83="Bình Chánh", Ward!$Y$2:$Z$17, IF(J83="Bình Tân", Ward!$AA$2:$AB$11, IF(J83="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J83="Cần Giờ", Ward!$AE$2:$AF$8, IF(J83="Củ Chi", Ward!$AG$2:$AH$22, IF(J83="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J83="Hóc Môn", Ward!$AK$2:$AL$13, IF(J83="Nhà Bè", Ward!$AM$2:$AN$8, IF(J83="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J83="Tân Bình", Ward!$AQ$2:$AR$16, IF(J83="Tân Phú", Ward!$AS$2:$AT$12, IF(J83="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5366,7 +5366,7 @@
         <f>IF(J84 &lt;&gt; "", VLOOKUP(J84, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W84" s="28" t="str">
+      <c r="W84" s="23" t="str">
         <f>IF(K84 &lt;&gt; "", VLOOKUP(K84, IF(J84="1", Ward!$A$2:$B$11, IF(J84="2", Ward!$C$2:$D$12, IF(J84="3", Ward!$E$2:$F$15, IF(J84="4", Ward!$G$2:$H$16, IF(J84="5", Ward!$I$2:$J$16, IF(J84="6", Ward!$K$2:$L$15, IF(J84="7", Ward!$M$2:$N$11, IF(J84="8", Ward!$O$2:$P$17, IF(J84="9", Ward!$Q$2:$R$14, IF(J84="10", Ward!$S$2:$T$16, IF(J84="11", Ward!$U$2:$V$17, IF(J84="12", Ward!$W$2:$X$12, IF(J84="Bình Chánh", Ward!$Y$2:$Z$17, IF(J84="Bình Tân", Ward!$AA$2:$AB$11, IF(J84="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J84="Cần Giờ", Ward!$AE$2:$AF$8, IF(J84="Củ Chi", Ward!$AG$2:$AH$22, IF(J84="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J84="Hóc Môn", Ward!$AK$2:$AL$13, IF(J84="Nhà Bè", Ward!$AM$2:$AN$8, IF(J84="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J84="Tân Bình", Ward!$AQ$2:$AR$16, IF(J84="Tân Phú", Ward!$AS$2:$AT$12, IF(J84="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5404,7 +5404,7 @@
         <f>IF(J85 &lt;&gt; "", VLOOKUP(J85, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W85" s="28" t="str">
+      <c r="W85" s="23" t="str">
         <f>IF(K85 &lt;&gt; "", VLOOKUP(K85, IF(J85="1", Ward!$A$2:$B$11, IF(J85="2", Ward!$C$2:$D$12, IF(J85="3", Ward!$E$2:$F$15, IF(J85="4", Ward!$G$2:$H$16, IF(J85="5", Ward!$I$2:$J$16, IF(J85="6", Ward!$K$2:$L$15, IF(J85="7", Ward!$M$2:$N$11, IF(J85="8", Ward!$O$2:$P$17, IF(J85="9", Ward!$Q$2:$R$14, IF(J85="10", Ward!$S$2:$T$16, IF(J85="11", Ward!$U$2:$V$17, IF(J85="12", Ward!$W$2:$X$12, IF(J85="Bình Chánh", Ward!$Y$2:$Z$17, IF(J85="Bình Tân", Ward!$AA$2:$AB$11, IF(J85="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J85="Cần Giờ", Ward!$AE$2:$AF$8, IF(J85="Củ Chi", Ward!$AG$2:$AH$22, IF(J85="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J85="Hóc Môn", Ward!$AK$2:$AL$13, IF(J85="Nhà Bè", Ward!$AM$2:$AN$8, IF(J85="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J85="Tân Bình", Ward!$AQ$2:$AR$16, IF(J85="Tân Phú", Ward!$AS$2:$AT$12, IF(J85="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5442,7 +5442,7 @@
         <f>IF(J86 &lt;&gt; "", VLOOKUP(J86, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W86" s="28" t="str">
+      <c r="W86" s="23" t="str">
         <f>IF(K86 &lt;&gt; "", VLOOKUP(K86, IF(J86="1", Ward!$A$2:$B$11, IF(J86="2", Ward!$C$2:$D$12, IF(J86="3", Ward!$E$2:$F$15, IF(J86="4", Ward!$G$2:$H$16, IF(J86="5", Ward!$I$2:$J$16, IF(J86="6", Ward!$K$2:$L$15, IF(J86="7", Ward!$M$2:$N$11, IF(J86="8", Ward!$O$2:$P$17, IF(J86="9", Ward!$Q$2:$R$14, IF(J86="10", Ward!$S$2:$T$16, IF(J86="11", Ward!$U$2:$V$17, IF(J86="12", Ward!$W$2:$X$12, IF(J86="Bình Chánh", Ward!$Y$2:$Z$17, IF(J86="Bình Tân", Ward!$AA$2:$AB$11, IF(J86="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J86="Cần Giờ", Ward!$AE$2:$AF$8, IF(J86="Củ Chi", Ward!$AG$2:$AH$22, IF(J86="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J86="Hóc Môn", Ward!$AK$2:$AL$13, IF(J86="Nhà Bè", Ward!$AM$2:$AN$8, IF(J86="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J86="Tân Bình", Ward!$AQ$2:$AR$16, IF(J86="Tân Phú", Ward!$AS$2:$AT$12, IF(J86="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5480,7 +5480,7 @@
         <f>IF(J87 &lt;&gt; "", VLOOKUP(J87, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W87" s="28" t="str">
+      <c r="W87" s="23" t="str">
         <f>IF(K87 &lt;&gt; "", VLOOKUP(K87, IF(J87="1", Ward!$A$2:$B$11, IF(J87="2", Ward!$C$2:$D$12, IF(J87="3", Ward!$E$2:$F$15, IF(J87="4", Ward!$G$2:$H$16, IF(J87="5", Ward!$I$2:$J$16, IF(J87="6", Ward!$K$2:$L$15, IF(J87="7", Ward!$M$2:$N$11, IF(J87="8", Ward!$O$2:$P$17, IF(J87="9", Ward!$Q$2:$R$14, IF(J87="10", Ward!$S$2:$T$16, IF(J87="11", Ward!$U$2:$V$17, IF(J87="12", Ward!$W$2:$X$12, IF(J87="Bình Chánh", Ward!$Y$2:$Z$17, IF(J87="Bình Tân", Ward!$AA$2:$AB$11, IF(J87="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J87="Cần Giờ", Ward!$AE$2:$AF$8, IF(J87="Củ Chi", Ward!$AG$2:$AH$22, IF(J87="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J87="Hóc Môn", Ward!$AK$2:$AL$13, IF(J87="Nhà Bè", Ward!$AM$2:$AN$8, IF(J87="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J87="Tân Bình", Ward!$AQ$2:$AR$16, IF(J87="Tân Phú", Ward!$AS$2:$AT$12, IF(J87="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5518,7 +5518,7 @@
         <f>IF(J88 &lt;&gt; "", VLOOKUP(J88, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W88" s="28" t="str">
+      <c r="W88" s="23" t="str">
         <f>IF(K88 &lt;&gt; "", VLOOKUP(K88, IF(J88="1", Ward!$A$2:$B$11, IF(J88="2", Ward!$C$2:$D$12, IF(J88="3", Ward!$E$2:$F$15, IF(J88="4", Ward!$G$2:$H$16, IF(J88="5", Ward!$I$2:$J$16, IF(J88="6", Ward!$K$2:$L$15, IF(J88="7", Ward!$M$2:$N$11, IF(J88="8", Ward!$O$2:$P$17, IF(J88="9", Ward!$Q$2:$R$14, IF(J88="10", Ward!$S$2:$T$16, IF(J88="11", Ward!$U$2:$V$17, IF(J88="12", Ward!$W$2:$X$12, IF(J88="Bình Chánh", Ward!$Y$2:$Z$17, IF(J88="Bình Tân", Ward!$AA$2:$AB$11, IF(J88="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J88="Cần Giờ", Ward!$AE$2:$AF$8, IF(J88="Củ Chi", Ward!$AG$2:$AH$22, IF(J88="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J88="Hóc Môn", Ward!$AK$2:$AL$13, IF(J88="Nhà Bè", Ward!$AM$2:$AN$8, IF(J88="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J88="Tân Bình", Ward!$AQ$2:$AR$16, IF(J88="Tân Phú", Ward!$AS$2:$AT$12, IF(J88="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5556,7 +5556,7 @@
         <f>IF(J89 &lt;&gt; "", VLOOKUP(J89, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W89" s="28" t="str">
+      <c r="W89" s="23" t="str">
         <f>IF(K89 &lt;&gt; "", VLOOKUP(K89, IF(J89="1", Ward!$A$2:$B$11, IF(J89="2", Ward!$C$2:$D$12, IF(J89="3", Ward!$E$2:$F$15, IF(J89="4", Ward!$G$2:$H$16, IF(J89="5", Ward!$I$2:$J$16, IF(J89="6", Ward!$K$2:$L$15, IF(J89="7", Ward!$M$2:$N$11, IF(J89="8", Ward!$O$2:$P$17, IF(J89="9", Ward!$Q$2:$R$14, IF(J89="10", Ward!$S$2:$T$16, IF(J89="11", Ward!$U$2:$V$17, IF(J89="12", Ward!$W$2:$X$12, IF(J89="Bình Chánh", Ward!$Y$2:$Z$17, IF(J89="Bình Tân", Ward!$AA$2:$AB$11, IF(J89="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J89="Cần Giờ", Ward!$AE$2:$AF$8, IF(J89="Củ Chi", Ward!$AG$2:$AH$22, IF(J89="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J89="Hóc Môn", Ward!$AK$2:$AL$13, IF(J89="Nhà Bè", Ward!$AM$2:$AN$8, IF(J89="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J89="Tân Bình", Ward!$AQ$2:$AR$16, IF(J89="Tân Phú", Ward!$AS$2:$AT$12, IF(J89="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5594,7 +5594,7 @@
         <f>IF(J90 &lt;&gt; "", VLOOKUP(J90, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W90" s="28" t="str">
+      <c r="W90" s="23" t="str">
         <f>IF(K90 &lt;&gt; "", VLOOKUP(K90, IF(J90="1", Ward!$A$2:$B$11, IF(J90="2", Ward!$C$2:$D$12, IF(J90="3", Ward!$E$2:$F$15, IF(J90="4", Ward!$G$2:$H$16, IF(J90="5", Ward!$I$2:$J$16, IF(J90="6", Ward!$K$2:$L$15, IF(J90="7", Ward!$M$2:$N$11, IF(J90="8", Ward!$O$2:$P$17, IF(J90="9", Ward!$Q$2:$R$14, IF(J90="10", Ward!$S$2:$T$16, IF(J90="11", Ward!$U$2:$V$17, IF(J90="12", Ward!$W$2:$X$12, IF(J90="Bình Chánh", Ward!$Y$2:$Z$17, IF(J90="Bình Tân", Ward!$AA$2:$AB$11, IF(J90="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J90="Cần Giờ", Ward!$AE$2:$AF$8, IF(J90="Củ Chi", Ward!$AG$2:$AH$22, IF(J90="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J90="Hóc Môn", Ward!$AK$2:$AL$13, IF(J90="Nhà Bè", Ward!$AM$2:$AN$8, IF(J90="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J90="Tân Bình", Ward!$AQ$2:$AR$16, IF(J90="Tân Phú", Ward!$AS$2:$AT$12, IF(J90="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5632,7 +5632,7 @@
         <f>IF(J91 &lt;&gt; "", VLOOKUP(J91, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W91" s="28" t="str">
+      <c r="W91" s="23" t="str">
         <f>IF(K91 &lt;&gt; "", VLOOKUP(K91, IF(J91="1", Ward!$A$2:$B$11, IF(J91="2", Ward!$C$2:$D$12, IF(J91="3", Ward!$E$2:$F$15, IF(J91="4", Ward!$G$2:$H$16, IF(J91="5", Ward!$I$2:$J$16, IF(J91="6", Ward!$K$2:$L$15, IF(J91="7", Ward!$M$2:$N$11, IF(J91="8", Ward!$O$2:$P$17, IF(J91="9", Ward!$Q$2:$R$14, IF(J91="10", Ward!$S$2:$T$16, IF(J91="11", Ward!$U$2:$V$17, IF(J91="12", Ward!$W$2:$X$12, IF(J91="Bình Chánh", Ward!$Y$2:$Z$17, IF(J91="Bình Tân", Ward!$AA$2:$AB$11, IF(J91="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J91="Cần Giờ", Ward!$AE$2:$AF$8, IF(J91="Củ Chi", Ward!$AG$2:$AH$22, IF(J91="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J91="Hóc Môn", Ward!$AK$2:$AL$13, IF(J91="Nhà Bè", Ward!$AM$2:$AN$8, IF(J91="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J91="Tân Bình", Ward!$AQ$2:$AR$16, IF(J91="Tân Phú", Ward!$AS$2:$AT$12, IF(J91="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5670,7 +5670,7 @@
         <f>IF(J92 &lt;&gt; "", VLOOKUP(J92, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W92" s="28" t="str">
+      <c r="W92" s="23" t="str">
         <f>IF(K92 &lt;&gt; "", VLOOKUP(K92, IF(J92="1", Ward!$A$2:$B$11, IF(J92="2", Ward!$C$2:$D$12, IF(J92="3", Ward!$E$2:$F$15, IF(J92="4", Ward!$G$2:$H$16, IF(J92="5", Ward!$I$2:$J$16, IF(J92="6", Ward!$K$2:$L$15, IF(J92="7", Ward!$M$2:$N$11, IF(J92="8", Ward!$O$2:$P$17, IF(J92="9", Ward!$Q$2:$R$14, IF(J92="10", Ward!$S$2:$T$16, IF(J92="11", Ward!$U$2:$V$17, IF(J92="12", Ward!$W$2:$X$12, IF(J92="Bình Chánh", Ward!$Y$2:$Z$17, IF(J92="Bình Tân", Ward!$AA$2:$AB$11, IF(J92="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J92="Cần Giờ", Ward!$AE$2:$AF$8, IF(J92="Củ Chi", Ward!$AG$2:$AH$22, IF(J92="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J92="Hóc Môn", Ward!$AK$2:$AL$13, IF(J92="Nhà Bè", Ward!$AM$2:$AN$8, IF(J92="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J92="Tân Bình", Ward!$AQ$2:$AR$16, IF(J92="Tân Phú", Ward!$AS$2:$AT$12, IF(J92="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5708,7 +5708,7 @@
         <f>IF(J93 &lt;&gt; "", VLOOKUP(J93, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W93" s="28" t="str">
+      <c r="W93" s="23" t="str">
         <f>IF(K93 &lt;&gt; "", VLOOKUP(K93, IF(J93="1", Ward!$A$2:$B$11, IF(J93="2", Ward!$C$2:$D$12, IF(J93="3", Ward!$E$2:$F$15, IF(J93="4", Ward!$G$2:$H$16, IF(J93="5", Ward!$I$2:$J$16, IF(J93="6", Ward!$K$2:$L$15, IF(J93="7", Ward!$M$2:$N$11, IF(J93="8", Ward!$O$2:$P$17, IF(J93="9", Ward!$Q$2:$R$14, IF(J93="10", Ward!$S$2:$T$16, IF(J93="11", Ward!$U$2:$V$17, IF(J93="12", Ward!$W$2:$X$12, IF(J93="Bình Chánh", Ward!$Y$2:$Z$17, IF(J93="Bình Tân", Ward!$AA$2:$AB$11, IF(J93="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J93="Cần Giờ", Ward!$AE$2:$AF$8, IF(J93="Củ Chi", Ward!$AG$2:$AH$22, IF(J93="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J93="Hóc Môn", Ward!$AK$2:$AL$13, IF(J93="Nhà Bè", Ward!$AM$2:$AN$8, IF(J93="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J93="Tân Bình", Ward!$AQ$2:$AR$16, IF(J93="Tân Phú", Ward!$AS$2:$AT$12, IF(J93="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5746,7 +5746,7 @@
         <f>IF(J94 &lt;&gt; "", VLOOKUP(J94, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W94" s="28" t="str">
+      <c r="W94" s="23" t="str">
         <f>IF(K94 &lt;&gt; "", VLOOKUP(K94, IF(J94="1", Ward!$A$2:$B$11, IF(J94="2", Ward!$C$2:$D$12, IF(J94="3", Ward!$E$2:$F$15, IF(J94="4", Ward!$G$2:$H$16, IF(J94="5", Ward!$I$2:$J$16, IF(J94="6", Ward!$K$2:$L$15, IF(J94="7", Ward!$M$2:$N$11, IF(J94="8", Ward!$O$2:$P$17, IF(J94="9", Ward!$Q$2:$R$14, IF(J94="10", Ward!$S$2:$T$16, IF(J94="11", Ward!$U$2:$V$17, IF(J94="12", Ward!$W$2:$X$12, IF(J94="Bình Chánh", Ward!$Y$2:$Z$17, IF(J94="Bình Tân", Ward!$AA$2:$AB$11, IF(J94="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J94="Cần Giờ", Ward!$AE$2:$AF$8, IF(J94="Củ Chi", Ward!$AG$2:$AH$22, IF(J94="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J94="Hóc Môn", Ward!$AK$2:$AL$13, IF(J94="Nhà Bè", Ward!$AM$2:$AN$8, IF(J94="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J94="Tân Bình", Ward!$AQ$2:$AR$16, IF(J94="Tân Phú", Ward!$AS$2:$AT$12, IF(J94="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5784,7 +5784,7 @@
         <f>IF(J95 &lt;&gt; "", VLOOKUP(J95, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W95" s="28" t="str">
+      <c r="W95" s="23" t="str">
         <f>IF(K95 &lt;&gt; "", VLOOKUP(K95, IF(J95="1", Ward!$A$2:$B$11, IF(J95="2", Ward!$C$2:$D$12, IF(J95="3", Ward!$E$2:$F$15, IF(J95="4", Ward!$G$2:$H$16, IF(J95="5", Ward!$I$2:$J$16, IF(J95="6", Ward!$K$2:$L$15, IF(J95="7", Ward!$M$2:$N$11, IF(J95="8", Ward!$O$2:$P$17, IF(J95="9", Ward!$Q$2:$R$14, IF(J95="10", Ward!$S$2:$T$16, IF(J95="11", Ward!$U$2:$V$17, IF(J95="12", Ward!$W$2:$X$12, IF(J95="Bình Chánh", Ward!$Y$2:$Z$17, IF(J95="Bình Tân", Ward!$AA$2:$AB$11, IF(J95="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J95="Cần Giờ", Ward!$AE$2:$AF$8, IF(J95="Củ Chi", Ward!$AG$2:$AH$22, IF(J95="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J95="Hóc Môn", Ward!$AK$2:$AL$13, IF(J95="Nhà Bè", Ward!$AM$2:$AN$8, IF(J95="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J95="Tân Bình", Ward!$AQ$2:$AR$16, IF(J95="Tân Phú", Ward!$AS$2:$AT$12, IF(J95="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5822,7 +5822,7 @@
         <f>IF(J96 &lt;&gt; "", VLOOKUP(J96, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W96" s="28" t="str">
+      <c r="W96" s="23" t="str">
         <f>IF(K96 &lt;&gt; "", VLOOKUP(K96, IF(J96="1", Ward!$A$2:$B$11, IF(J96="2", Ward!$C$2:$D$12, IF(J96="3", Ward!$E$2:$F$15, IF(J96="4", Ward!$G$2:$H$16, IF(J96="5", Ward!$I$2:$J$16, IF(J96="6", Ward!$K$2:$L$15, IF(J96="7", Ward!$M$2:$N$11, IF(J96="8", Ward!$O$2:$P$17, IF(J96="9", Ward!$Q$2:$R$14, IF(J96="10", Ward!$S$2:$T$16, IF(J96="11", Ward!$U$2:$V$17, IF(J96="12", Ward!$W$2:$X$12, IF(J96="Bình Chánh", Ward!$Y$2:$Z$17, IF(J96="Bình Tân", Ward!$AA$2:$AB$11, IF(J96="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J96="Cần Giờ", Ward!$AE$2:$AF$8, IF(J96="Củ Chi", Ward!$AG$2:$AH$22, IF(J96="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J96="Hóc Môn", Ward!$AK$2:$AL$13, IF(J96="Nhà Bè", Ward!$AM$2:$AN$8, IF(J96="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J96="Tân Bình", Ward!$AQ$2:$AR$16, IF(J96="Tân Phú", Ward!$AS$2:$AT$12, IF(J96="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5860,7 +5860,7 @@
         <f>IF(J97 &lt;&gt; "", VLOOKUP(J97, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W97" s="28" t="str">
+      <c r="W97" s="23" t="str">
         <f>IF(K97 &lt;&gt; "", VLOOKUP(K97, IF(J97="1", Ward!$A$2:$B$11, IF(J97="2", Ward!$C$2:$D$12, IF(J97="3", Ward!$E$2:$F$15, IF(J97="4", Ward!$G$2:$H$16, IF(J97="5", Ward!$I$2:$J$16, IF(J97="6", Ward!$K$2:$L$15, IF(J97="7", Ward!$M$2:$N$11, IF(J97="8", Ward!$O$2:$P$17, IF(J97="9", Ward!$Q$2:$R$14, IF(J97="10", Ward!$S$2:$T$16, IF(J97="11", Ward!$U$2:$V$17, IF(J97="12", Ward!$W$2:$X$12, IF(J97="Bình Chánh", Ward!$Y$2:$Z$17, IF(J97="Bình Tân", Ward!$AA$2:$AB$11, IF(J97="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J97="Cần Giờ", Ward!$AE$2:$AF$8, IF(J97="Củ Chi", Ward!$AG$2:$AH$22, IF(J97="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J97="Hóc Môn", Ward!$AK$2:$AL$13, IF(J97="Nhà Bè", Ward!$AM$2:$AN$8, IF(J97="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J97="Tân Bình", Ward!$AQ$2:$AR$16, IF(J97="Tân Phú", Ward!$AS$2:$AT$12, IF(J97="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5898,7 +5898,7 @@
         <f>IF(J98 &lt;&gt; "", VLOOKUP(J98, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W98" s="28" t="str">
+      <c r="W98" s="23" t="str">
         <f>IF(K98 &lt;&gt; "", VLOOKUP(K98, IF(J98="1", Ward!$A$2:$B$11, IF(J98="2", Ward!$C$2:$D$12, IF(J98="3", Ward!$E$2:$F$15, IF(J98="4", Ward!$G$2:$H$16, IF(J98="5", Ward!$I$2:$J$16, IF(J98="6", Ward!$K$2:$L$15, IF(J98="7", Ward!$M$2:$N$11, IF(J98="8", Ward!$O$2:$P$17, IF(J98="9", Ward!$Q$2:$R$14, IF(J98="10", Ward!$S$2:$T$16, IF(J98="11", Ward!$U$2:$V$17, IF(J98="12", Ward!$W$2:$X$12, IF(J98="Bình Chánh", Ward!$Y$2:$Z$17, IF(J98="Bình Tân", Ward!$AA$2:$AB$11, IF(J98="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J98="Cần Giờ", Ward!$AE$2:$AF$8, IF(J98="Củ Chi", Ward!$AG$2:$AH$22, IF(J98="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J98="Hóc Môn", Ward!$AK$2:$AL$13, IF(J98="Nhà Bè", Ward!$AM$2:$AN$8, IF(J98="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J98="Tân Bình", Ward!$AQ$2:$AR$16, IF(J98="Tân Phú", Ward!$AS$2:$AT$12, IF(J98="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5936,7 +5936,7 @@
         <f>IF(J99 &lt;&gt; "", VLOOKUP(J99, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W99" s="28" t="str">
+      <c r="W99" s="23" t="str">
         <f>IF(K99 &lt;&gt; "", VLOOKUP(K99, IF(J99="1", Ward!$A$2:$B$11, IF(J99="2", Ward!$C$2:$D$12, IF(J99="3", Ward!$E$2:$F$15, IF(J99="4", Ward!$G$2:$H$16, IF(J99="5", Ward!$I$2:$J$16, IF(J99="6", Ward!$K$2:$L$15, IF(J99="7", Ward!$M$2:$N$11, IF(J99="8", Ward!$O$2:$P$17, IF(J99="9", Ward!$Q$2:$R$14, IF(J99="10", Ward!$S$2:$T$16, IF(J99="11", Ward!$U$2:$V$17, IF(J99="12", Ward!$W$2:$X$12, IF(J99="Bình Chánh", Ward!$Y$2:$Z$17, IF(J99="Bình Tân", Ward!$AA$2:$AB$11, IF(J99="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J99="Cần Giờ", Ward!$AE$2:$AF$8, IF(J99="Củ Chi", Ward!$AG$2:$AH$22, IF(J99="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J99="Hóc Môn", Ward!$AK$2:$AL$13, IF(J99="Nhà Bè", Ward!$AM$2:$AN$8, IF(J99="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J99="Tân Bình", Ward!$AQ$2:$AR$16, IF(J99="Tân Phú", Ward!$AS$2:$AT$12, IF(J99="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -5974,7 +5974,7 @@
         <f>IF(J100 &lt;&gt; "", VLOOKUP(J100, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W100" s="28" t="str">
+      <c r="W100" s="23" t="str">
         <f>IF(K100 &lt;&gt; "", VLOOKUP(K100, IF(J100="1", Ward!$A$2:$B$11, IF(J100="2", Ward!$C$2:$D$12, IF(J100="3", Ward!$E$2:$F$15, IF(J100="4", Ward!$G$2:$H$16, IF(J100="5", Ward!$I$2:$J$16, IF(J100="6", Ward!$K$2:$L$15, IF(J100="7", Ward!$M$2:$N$11, IF(J100="8", Ward!$O$2:$P$17, IF(J100="9", Ward!$Q$2:$R$14, IF(J100="10", Ward!$S$2:$T$16, IF(J100="11", Ward!$U$2:$V$17, IF(J100="12", Ward!$W$2:$X$12, IF(J100="Bình Chánh", Ward!$Y$2:$Z$17, IF(J100="Bình Tân", Ward!$AA$2:$AB$11, IF(J100="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J100="Cần Giờ", Ward!$AE$2:$AF$8, IF(J100="Củ Chi", Ward!$AG$2:$AH$22, IF(J100="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J100="Hóc Môn", Ward!$AK$2:$AL$13, IF(J100="Nhà Bè", Ward!$AM$2:$AN$8, IF(J100="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J100="Tân Bình", Ward!$AQ$2:$AR$16, IF(J100="Tân Phú", Ward!$AS$2:$AT$12, IF(J100="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6012,7 +6012,7 @@
         <f>IF(J101 &lt;&gt; "", VLOOKUP(J101, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W101" s="28" t="str">
+      <c r="W101" s="23" t="str">
         <f>IF(K101 &lt;&gt; "", VLOOKUP(K101, IF(J101="1", Ward!$A$2:$B$11, IF(J101="2", Ward!$C$2:$D$12, IF(J101="3", Ward!$E$2:$F$15, IF(J101="4", Ward!$G$2:$H$16, IF(J101="5", Ward!$I$2:$J$16, IF(J101="6", Ward!$K$2:$L$15, IF(J101="7", Ward!$M$2:$N$11, IF(J101="8", Ward!$O$2:$P$17, IF(J101="9", Ward!$Q$2:$R$14, IF(J101="10", Ward!$S$2:$T$16, IF(J101="11", Ward!$U$2:$V$17, IF(J101="12", Ward!$W$2:$X$12, IF(J101="Bình Chánh", Ward!$Y$2:$Z$17, IF(J101="Bình Tân", Ward!$AA$2:$AB$11, IF(J101="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J101="Cần Giờ", Ward!$AE$2:$AF$8, IF(J101="Củ Chi", Ward!$AG$2:$AH$22, IF(J101="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J101="Hóc Môn", Ward!$AK$2:$AL$13, IF(J101="Nhà Bè", Ward!$AM$2:$AN$8, IF(J101="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J101="Tân Bình", Ward!$AQ$2:$AR$16, IF(J101="Tân Phú", Ward!$AS$2:$AT$12, IF(J101="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6050,7 +6050,7 @@
         <f>IF(J102 &lt;&gt; "", VLOOKUP(J102, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W102" s="28" t="str">
+      <c r="W102" s="23" t="str">
         <f>IF(K102 &lt;&gt; "", VLOOKUP(K102, IF(J102="1", Ward!$A$2:$B$11, IF(J102="2", Ward!$C$2:$D$12, IF(J102="3", Ward!$E$2:$F$15, IF(J102="4", Ward!$G$2:$H$16, IF(J102="5", Ward!$I$2:$J$16, IF(J102="6", Ward!$K$2:$L$15, IF(J102="7", Ward!$M$2:$N$11, IF(J102="8", Ward!$O$2:$P$17, IF(J102="9", Ward!$Q$2:$R$14, IF(J102="10", Ward!$S$2:$T$16, IF(J102="11", Ward!$U$2:$V$17, IF(J102="12", Ward!$W$2:$X$12, IF(J102="Bình Chánh", Ward!$Y$2:$Z$17, IF(J102="Bình Tân", Ward!$AA$2:$AB$11, IF(J102="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J102="Cần Giờ", Ward!$AE$2:$AF$8, IF(J102="Củ Chi", Ward!$AG$2:$AH$22, IF(J102="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J102="Hóc Môn", Ward!$AK$2:$AL$13, IF(J102="Nhà Bè", Ward!$AM$2:$AN$8, IF(J102="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J102="Tân Bình", Ward!$AQ$2:$AR$16, IF(J102="Tân Phú", Ward!$AS$2:$AT$12, IF(J102="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6088,7 +6088,7 @@
         <f>IF(J103 &lt;&gt; "", VLOOKUP(J103, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W103" s="28" t="str">
+      <c r="W103" s="23" t="str">
         <f>IF(K103 &lt;&gt; "", VLOOKUP(K103, IF(J103="1", Ward!$A$2:$B$11, IF(J103="2", Ward!$C$2:$D$12, IF(J103="3", Ward!$E$2:$F$15, IF(J103="4", Ward!$G$2:$H$16, IF(J103="5", Ward!$I$2:$J$16, IF(J103="6", Ward!$K$2:$L$15, IF(J103="7", Ward!$M$2:$N$11, IF(J103="8", Ward!$O$2:$P$17, IF(J103="9", Ward!$Q$2:$R$14, IF(J103="10", Ward!$S$2:$T$16, IF(J103="11", Ward!$U$2:$V$17, IF(J103="12", Ward!$W$2:$X$12, IF(J103="Bình Chánh", Ward!$Y$2:$Z$17, IF(J103="Bình Tân", Ward!$AA$2:$AB$11, IF(J103="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J103="Cần Giờ", Ward!$AE$2:$AF$8, IF(J103="Củ Chi", Ward!$AG$2:$AH$22, IF(J103="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J103="Hóc Môn", Ward!$AK$2:$AL$13, IF(J103="Nhà Bè", Ward!$AM$2:$AN$8, IF(J103="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J103="Tân Bình", Ward!$AQ$2:$AR$16, IF(J103="Tân Phú", Ward!$AS$2:$AT$12, IF(J103="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6126,7 +6126,7 @@
         <f>IF(J104 &lt;&gt; "", VLOOKUP(J104, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W104" s="28" t="str">
+      <c r="W104" s="23" t="str">
         <f>IF(K104 &lt;&gt; "", VLOOKUP(K104, IF(J104="1", Ward!$A$2:$B$11, IF(J104="2", Ward!$C$2:$D$12, IF(J104="3", Ward!$E$2:$F$15, IF(J104="4", Ward!$G$2:$H$16, IF(J104="5", Ward!$I$2:$J$16, IF(J104="6", Ward!$K$2:$L$15, IF(J104="7", Ward!$M$2:$N$11, IF(J104="8", Ward!$O$2:$P$17, IF(J104="9", Ward!$Q$2:$R$14, IF(J104="10", Ward!$S$2:$T$16, IF(J104="11", Ward!$U$2:$V$17, IF(J104="12", Ward!$W$2:$X$12, IF(J104="Bình Chánh", Ward!$Y$2:$Z$17, IF(J104="Bình Tân", Ward!$AA$2:$AB$11, IF(J104="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J104="Cần Giờ", Ward!$AE$2:$AF$8, IF(J104="Củ Chi", Ward!$AG$2:$AH$22, IF(J104="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J104="Hóc Môn", Ward!$AK$2:$AL$13, IF(J104="Nhà Bè", Ward!$AM$2:$AN$8, IF(J104="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J104="Tân Bình", Ward!$AQ$2:$AR$16, IF(J104="Tân Phú", Ward!$AS$2:$AT$12, IF(J104="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6164,7 +6164,7 @@
         <f>IF(J105 &lt;&gt; "", VLOOKUP(J105, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W105" s="28" t="str">
+      <c r="W105" s="23" t="str">
         <f>IF(K105 &lt;&gt; "", VLOOKUP(K105, IF(J105="1", Ward!$A$2:$B$11, IF(J105="2", Ward!$C$2:$D$12, IF(J105="3", Ward!$E$2:$F$15, IF(J105="4", Ward!$G$2:$H$16, IF(J105="5", Ward!$I$2:$J$16, IF(J105="6", Ward!$K$2:$L$15, IF(J105="7", Ward!$M$2:$N$11, IF(J105="8", Ward!$O$2:$P$17, IF(J105="9", Ward!$Q$2:$R$14, IF(J105="10", Ward!$S$2:$T$16, IF(J105="11", Ward!$U$2:$V$17, IF(J105="12", Ward!$W$2:$X$12, IF(J105="Bình Chánh", Ward!$Y$2:$Z$17, IF(J105="Bình Tân", Ward!$AA$2:$AB$11, IF(J105="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J105="Cần Giờ", Ward!$AE$2:$AF$8, IF(J105="Củ Chi", Ward!$AG$2:$AH$22, IF(J105="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J105="Hóc Môn", Ward!$AK$2:$AL$13, IF(J105="Nhà Bè", Ward!$AM$2:$AN$8, IF(J105="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J105="Tân Bình", Ward!$AQ$2:$AR$16, IF(J105="Tân Phú", Ward!$AS$2:$AT$12, IF(J105="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6202,7 +6202,7 @@
         <f>IF(J106 &lt;&gt; "", VLOOKUP(J106, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W106" s="28" t="str">
+      <c r="W106" s="23" t="str">
         <f>IF(K106 &lt;&gt; "", VLOOKUP(K106, IF(J106="1", Ward!$A$2:$B$11, IF(J106="2", Ward!$C$2:$D$12, IF(J106="3", Ward!$E$2:$F$15, IF(J106="4", Ward!$G$2:$H$16, IF(J106="5", Ward!$I$2:$J$16, IF(J106="6", Ward!$K$2:$L$15, IF(J106="7", Ward!$M$2:$N$11, IF(J106="8", Ward!$O$2:$P$17, IF(J106="9", Ward!$Q$2:$R$14, IF(J106="10", Ward!$S$2:$T$16, IF(J106="11", Ward!$U$2:$V$17, IF(J106="12", Ward!$W$2:$X$12, IF(J106="Bình Chánh", Ward!$Y$2:$Z$17, IF(J106="Bình Tân", Ward!$AA$2:$AB$11, IF(J106="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J106="Cần Giờ", Ward!$AE$2:$AF$8, IF(J106="Củ Chi", Ward!$AG$2:$AH$22, IF(J106="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J106="Hóc Môn", Ward!$AK$2:$AL$13, IF(J106="Nhà Bè", Ward!$AM$2:$AN$8, IF(J106="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J106="Tân Bình", Ward!$AQ$2:$AR$16, IF(J106="Tân Phú", Ward!$AS$2:$AT$12, IF(J106="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6240,7 +6240,7 @@
         <f>IF(J107 &lt;&gt; "", VLOOKUP(J107, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W107" s="28" t="str">
+      <c r="W107" s="23" t="str">
         <f>IF(K107 &lt;&gt; "", VLOOKUP(K107, IF(J107="1", Ward!$A$2:$B$11, IF(J107="2", Ward!$C$2:$D$12, IF(J107="3", Ward!$E$2:$F$15, IF(J107="4", Ward!$G$2:$H$16, IF(J107="5", Ward!$I$2:$J$16, IF(J107="6", Ward!$K$2:$L$15, IF(J107="7", Ward!$M$2:$N$11, IF(J107="8", Ward!$O$2:$P$17, IF(J107="9", Ward!$Q$2:$R$14, IF(J107="10", Ward!$S$2:$T$16, IF(J107="11", Ward!$U$2:$V$17, IF(J107="12", Ward!$W$2:$X$12, IF(J107="Bình Chánh", Ward!$Y$2:$Z$17, IF(J107="Bình Tân", Ward!$AA$2:$AB$11, IF(J107="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J107="Cần Giờ", Ward!$AE$2:$AF$8, IF(J107="Củ Chi", Ward!$AG$2:$AH$22, IF(J107="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J107="Hóc Môn", Ward!$AK$2:$AL$13, IF(J107="Nhà Bè", Ward!$AM$2:$AN$8, IF(J107="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J107="Tân Bình", Ward!$AQ$2:$AR$16, IF(J107="Tân Phú", Ward!$AS$2:$AT$12, IF(J107="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6278,7 +6278,7 @@
         <f>IF(J108 &lt;&gt; "", VLOOKUP(J108, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W108" s="28" t="str">
+      <c r="W108" s="23" t="str">
         <f>IF(K108 &lt;&gt; "", VLOOKUP(K108, IF(J108="1", Ward!$A$2:$B$11, IF(J108="2", Ward!$C$2:$D$12, IF(J108="3", Ward!$E$2:$F$15, IF(J108="4", Ward!$G$2:$H$16, IF(J108="5", Ward!$I$2:$J$16, IF(J108="6", Ward!$K$2:$L$15, IF(J108="7", Ward!$M$2:$N$11, IF(J108="8", Ward!$O$2:$P$17, IF(J108="9", Ward!$Q$2:$R$14, IF(J108="10", Ward!$S$2:$T$16, IF(J108="11", Ward!$U$2:$V$17, IF(J108="12", Ward!$W$2:$X$12, IF(J108="Bình Chánh", Ward!$Y$2:$Z$17, IF(J108="Bình Tân", Ward!$AA$2:$AB$11, IF(J108="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J108="Cần Giờ", Ward!$AE$2:$AF$8, IF(J108="Củ Chi", Ward!$AG$2:$AH$22, IF(J108="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J108="Hóc Môn", Ward!$AK$2:$AL$13, IF(J108="Nhà Bè", Ward!$AM$2:$AN$8, IF(J108="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J108="Tân Bình", Ward!$AQ$2:$AR$16, IF(J108="Tân Phú", Ward!$AS$2:$AT$12, IF(J108="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6316,7 +6316,7 @@
         <f>IF(J109 &lt;&gt; "", VLOOKUP(J109, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W109" s="28" t="str">
+      <c r="W109" s="23" t="str">
         <f>IF(K109 &lt;&gt; "", VLOOKUP(K109, IF(J109="1", Ward!$A$2:$B$11, IF(J109="2", Ward!$C$2:$D$12, IF(J109="3", Ward!$E$2:$F$15, IF(J109="4", Ward!$G$2:$H$16, IF(J109="5", Ward!$I$2:$J$16, IF(J109="6", Ward!$K$2:$L$15, IF(J109="7", Ward!$M$2:$N$11, IF(J109="8", Ward!$O$2:$P$17, IF(J109="9", Ward!$Q$2:$R$14, IF(J109="10", Ward!$S$2:$T$16, IF(J109="11", Ward!$U$2:$V$17, IF(J109="12", Ward!$W$2:$X$12, IF(J109="Bình Chánh", Ward!$Y$2:$Z$17, IF(J109="Bình Tân", Ward!$AA$2:$AB$11, IF(J109="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J109="Cần Giờ", Ward!$AE$2:$AF$8, IF(J109="Củ Chi", Ward!$AG$2:$AH$22, IF(J109="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J109="Hóc Môn", Ward!$AK$2:$AL$13, IF(J109="Nhà Bè", Ward!$AM$2:$AN$8, IF(J109="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J109="Tân Bình", Ward!$AQ$2:$AR$16, IF(J109="Tân Phú", Ward!$AS$2:$AT$12, IF(J109="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6354,7 +6354,7 @@
         <f>IF(J110 &lt;&gt; "", VLOOKUP(J110, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W110" s="28" t="str">
+      <c r="W110" s="23" t="str">
         <f>IF(K110 &lt;&gt; "", VLOOKUP(K110, IF(J110="1", Ward!$A$2:$B$11, IF(J110="2", Ward!$C$2:$D$12, IF(J110="3", Ward!$E$2:$F$15, IF(J110="4", Ward!$G$2:$H$16, IF(J110="5", Ward!$I$2:$J$16, IF(J110="6", Ward!$K$2:$L$15, IF(J110="7", Ward!$M$2:$N$11, IF(J110="8", Ward!$O$2:$P$17, IF(J110="9", Ward!$Q$2:$R$14, IF(J110="10", Ward!$S$2:$T$16, IF(J110="11", Ward!$U$2:$V$17, IF(J110="12", Ward!$W$2:$X$12, IF(J110="Bình Chánh", Ward!$Y$2:$Z$17, IF(J110="Bình Tân", Ward!$AA$2:$AB$11, IF(J110="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J110="Cần Giờ", Ward!$AE$2:$AF$8, IF(J110="Củ Chi", Ward!$AG$2:$AH$22, IF(J110="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J110="Hóc Môn", Ward!$AK$2:$AL$13, IF(J110="Nhà Bè", Ward!$AM$2:$AN$8, IF(J110="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J110="Tân Bình", Ward!$AQ$2:$AR$16, IF(J110="Tân Phú", Ward!$AS$2:$AT$12, IF(J110="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6392,7 +6392,7 @@
         <f>IF(J111 &lt;&gt; "", VLOOKUP(J111, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W111" s="28" t="str">
+      <c r="W111" s="23" t="str">
         <f>IF(K111 &lt;&gt; "", VLOOKUP(K111, IF(J111="1", Ward!$A$2:$B$11, IF(J111="2", Ward!$C$2:$D$12, IF(J111="3", Ward!$E$2:$F$15, IF(J111="4", Ward!$G$2:$H$16, IF(J111="5", Ward!$I$2:$J$16, IF(J111="6", Ward!$K$2:$L$15, IF(J111="7", Ward!$M$2:$N$11, IF(J111="8", Ward!$O$2:$P$17, IF(J111="9", Ward!$Q$2:$R$14, IF(J111="10", Ward!$S$2:$T$16, IF(J111="11", Ward!$U$2:$V$17, IF(J111="12", Ward!$W$2:$X$12, IF(J111="Bình Chánh", Ward!$Y$2:$Z$17, IF(J111="Bình Tân", Ward!$AA$2:$AB$11, IF(J111="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J111="Cần Giờ", Ward!$AE$2:$AF$8, IF(J111="Củ Chi", Ward!$AG$2:$AH$22, IF(J111="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J111="Hóc Môn", Ward!$AK$2:$AL$13, IF(J111="Nhà Bè", Ward!$AM$2:$AN$8, IF(J111="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J111="Tân Bình", Ward!$AQ$2:$AR$16, IF(J111="Tân Phú", Ward!$AS$2:$AT$12, IF(J111="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6430,7 +6430,7 @@
         <f>IF(J112 &lt;&gt; "", VLOOKUP(J112, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W112" s="28" t="str">
+      <c r="W112" s="23" t="str">
         <f>IF(K112 &lt;&gt; "", VLOOKUP(K112, IF(J112="1", Ward!$A$2:$B$11, IF(J112="2", Ward!$C$2:$D$12, IF(J112="3", Ward!$E$2:$F$15, IF(J112="4", Ward!$G$2:$H$16, IF(J112="5", Ward!$I$2:$J$16, IF(J112="6", Ward!$K$2:$L$15, IF(J112="7", Ward!$M$2:$N$11, IF(J112="8", Ward!$O$2:$P$17, IF(J112="9", Ward!$Q$2:$R$14, IF(J112="10", Ward!$S$2:$T$16, IF(J112="11", Ward!$U$2:$V$17, IF(J112="12", Ward!$W$2:$X$12, IF(J112="Bình Chánh", Ward!$Y$2:$Z$17, IF(J112="Bình Tân", Ward!$AA$2:$AB$11, IF(J112="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J112="Cần Giờ", Ward!$AE$2:$AF$8, IF(J112="Củ Chi", Ward!$AG$2:$AH$22, IF(J112="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J112="Hóc Môn", Ward!$AK$2:$AL$13, IF(J112="Nhà Bè", Ward!$AM$2:$AN$8, IF(J112="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J112="Tân Bình", Ward!$AQ$2:$AR$16, IF(J112="Tân Phú", Ward!$AS$2:$AT$12, IF(J112="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6468,7 +6468,7 @@
         <f>IF(J113 &lt;&gt; "", VLOOKUP(J113, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W113" s="28" t="str">
+      <c r="W113" s="23" t="str">
         <f>IF(K113 &lt;&gt; "", VLOOKUP(K113, IF(J113="1", Ward!$A$2:$B$11, IF(J113="2", Ward!$C$2:$D$12, IF(J113="3", Ward!$E$2:$F$15, IF(J113="4", Ward!$G$2:$H$16, IF(J113="5", Ward!$I$2:$J$16, IF(J113="6", Ward!$K$2:$L$15, IF(J113="7", Ward!$M$2:$N$11, IF(J113="8", Ward!$O$2:$P$17, IF(J113="9", Ward!$Q$2:$R$14, IF(J113="10", Ward!$S$2:$T$16, IF(J113="11", Ward!$U$2:$V$17, IF(J113="12", Ward!$W$2:$X$12, IF(J113="Bình Chánh", Ward!$Y$2:$Z$17, IF(J113="Bình Tân", Ward!$AA$2:$AB$11, IF(J113="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J113="Cần Giờ", Ward!$AE$2:$AF$8, IF(J113="Củ Chi", Ward!$AG$2:$AH$22, IF(J113="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J113="Hóc Môn", Ward!$AK$2:$AL$13, IF(J113="Nhà Bè", Ward!$AM$2:$AN$8, IF(J113="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J113="Tân Bình", Ward!$AQ$2:$AR$16, IF(J113="Tân Phú", Ward!$AS$2:$AT$12, IF(J113="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6506,7 +6506,7 @@
         <f>IF(J114 &lt;&gt; "", VLOOKUP(J114, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W114" s="28" t="str">
+      <c r="W114" s="23" t="str">
         <f>IF(K114 &lt;&gt; "", VLOOKUP(K114, IF(J114="1", Ward!$A$2:$B$11, IF(J114="2", Ward!$C$2:$D$12, IF(J114="3", Ward!$E$2:$F$15, IF(J114="4", Ward!$G$2:$H$16, IF(J114="5", Ward!$I$2:$J$16, IF(J114="6", Ward!$K$2:$L$15, IF(J114="7", Ward!$M$2:$N$11, IF(J114="8", Ward!$O$2:$P$17, IF(J114="9", Ward!$Q$2:$R$14, IF(J114="10", Ward!$S$2:$T$16, IF(J114="11", Ward!$U$2:$V$17, IF(J114="12", Ward!$W$2:$X$12, IF(J114="Bình Chánh", Ward!$Y$2:$Z$17, IF(J114="Bình Tân", Ward!$AA$2:$AB$11, IF(J114="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J114="Cần Giờ", Ward!$AE$2:$AF$8, IF(J114="Củ Chi", Ward!$AG$2:$AH$22, IF(J114="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J114="Hóc Môn", Ward!$AK$2:$AL$13, IF(J114="Nhà Bè", Ward!$AM$2:$AN$8, IF(J114="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J114="Tân Bình", Ward!$AQ$2:$AR$16, IF(J114="Tân Phú", Ward!$AS$2:$AT$12, IF(J114="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6544,7 +6544,7 @@
         <f>IF(J115 &lt;&gt; "", VLOOKUP(J115, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W115" s="28" t="str">
+      <c r="W115" s="23" t="str">
         <f>IF(K115 &lt;&gt; "", VLOOKUP(K115, IF(J115="1", Ward!$A$2:$B$11, IF(J115="2", Ward!$C$2:$D$12, IF(J115="3", Ward!$E$2:$F$15, IF(J115="4", Ward!$G$2:$H$16, IF(J115="5", Ward!$I$2:$J$16, IF(J115="6", Ward!$K$2:$L$15, IF(J115="7", Ward!$M$2:$N$11, IF(J115="8", Ward!$O$2:$P$17, IF(J115="9", Ward!$Q$2:$R$14, IF(J115="10", Ward!$S$2:$T$16, IF(J115="11", Ward!$U$2:$V$17, IF(J115="12", Ward!$W$2:$X$12, IF(J115="Bình Chánh", Ward!$Y$2:$Z$17, IF(J115="Bình Tân", Ward!$AA$2:$AB$11, IF(J115="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J115="Cần Giờ", Ward!$AE$2:$AF$8, IF(J115="Củ Chi", Ward!$AG$2:$AH$22, IF(J115="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J115="Hóc Môn", Ward!$AK$2:$AL$13, IF(J115="Nhà Bè", Ward!$AM$2:$AN$8, IF(J115="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J115="Tân Bình", Ward!$AQ$2:$AR$16, IF(J115="Tân Phú", Ward!$AS$2:$AT$12, IF(J115="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6582,7 +6582,7 @@
         <f>IF(J116 &lt;&gt; "", VLOOKUP(J116, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W116" s="28" t="str">
+      <c r="W116" s="23" t="str">
         <f>IF(K116 &lt;&gt; "", VLOOKUP(K116, IF(J116="1", Ward!$A$2:$B$11, IF(J116="2", Ward!$C$2:$D$12, IF(J116="3", Ward!$E$2:$F$15, IF(J116="4", Ward!$G$2:$H$16, IF(J116="5", Ward!$I$2:$J$16, IF(J116="6", Ward!$K$2:$L$15, IF(J116="7", Ward!$M$2:$N$11, IF(J116="8", Ward!$O$2:$P$17, IF(J116="9", Ward!$Q$2:$R$14, IF(J116="10", Ward!$S$2:$T$16, IF(J116="11", Ward!$U$2:$V$17, IF(J116="12", Ward!$W$2:$X$12, IF(J116="Bình Chánh", Ward!$Y$2:$Z$17, IF(J116="Bình Tân", Ward!$AA$2:$AB$11, IF(J116="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J116="Cần Giờ", Ward!$AE$2:$AF$8, IF(J116="Củ Chi", Ward!$AG$2:$AH$22, IF(J116="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J116="Hóc Môn", Ward!$AK$2:$AL$13, IF(J116="Nhà Bè", Ward!$AM$2:$AN$8, IF(J116="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J116="Tân Bình", Ward!$AQ$2:$AR$16, IF(J116="Tân Phú", Ward!$AS$2:$AT$12, IF(J116="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6620,7 +6620,7 @@
         <f>IF(J117 &lt;&gt; "", VLOOKUP(J117, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W117" s="28" t="str">
+      <c r="W117" s="23" t="str">
         <f>IF(K117 &lt;&gt; "", VLOOKUP(K117, IF(J117="1", Ward!$A$2:$B$11, IF(J117="2", Ward!$C$2:$D$12, IF(J117="3", Ward!$E$2:$F$15, IF(J117="4", Ward!$G$2:$H$16, IF(J117="5", Ward!$I$2:$J$16, IF(J117="6", Ward!$K$2:$L$15, IF(J117="7", Ward!$M$2:$N$11, IF(J117="8", Ward!$O$2:$P$17, IF(J117="9", Ward!$Q$2:$R$14, IF(J117="10", Ward!$S$2:$T$16, IF(J117="11", Ward!$U$2:$V$17, IF(J117="12", Ward!$W$2:$X$12, IF(J117="Bình Chánh", Ward!$Y$2:$Z$17, IF(J117="Bình Tân", Ward!$AA$2:$AB$11, IF(J117="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J117="Cần Giờ", Ward!$AE$2:$AF$8, IF(J117="Củ Chi", Ward!$AG$2:$AH$22, IF(J117="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J117="Hóc Môn", Ward!$AK$2:$AL$13, IF(J117="Nhà Bè", Ward!$AM$2:$AN$8, IF(J117="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J117="Tân Bình", Ward!$AQ$2:$AR$16, IF(J117="Tân Phú", Ward!$AS$2:$AT$12, IF(J117="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6658,7 +6658,7 @@
         <f>IF(J118 &lt;&gt; "", VLOOKUP(J118, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W118" s="28" t="str">
+      <c r="W118" s="23" t="str">
         <f>IF(K118 &lt;&gt; "", VLOOKUP(K118, IF(J118="1", Ward!$A$2:$B$11, IF(J118="2", Ward!$C$2:$D$12, IF(J118="3", Ward!$E$2:$F$15, IF(J118="4", Ward!$G$2:$H$16, IF(J118="5", Ward!$I$2:$J$16, IF(J118="6", Ward!$K$2:$L$15, IF(J118="7", Ward!$M$2:$N$11, IF(J118="8", Ward!$O$2:$P$17, IF(J118="9", Ward!$Q$2:$R$14, IF(J118="10", Ward!$S$2:$T$16, IF(J118="11", Ward!$U$2:$V$17, IF(J118="12", Ward!$W$2:$X$12, IF(J118="Bình Chánh", Ward!$Y$2:$Z$17, IF(J118="Bình Tân", Ward!$AA$2:$AB$11, IF(J118="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J118="Cần Giờ", Ward!$AE$2:$AF$8, IF(J118="Củ Chi", Ward!$AG$2:$AH$22, IF(J118="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J118="Hóc Môn", Ward!$AK$2:$AL$13, IF(J118="Nhà Bè", Ward!$AM$2:$AN$8, IF(J118="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J118="Tân Bình", Ward!$AQ$2:$AR$16, IF(J118="Tân Phú", Ward!$AS$2:$AT$12, IF(J118="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6696,7 +6696,7 @@
         <f>IF(J119 &lt;&gt; "", VLOOKUP(J119, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W119" s="28" t="str">
+      <c r="W119" s="23" t="str">
         <f>IF(K119 &lt;&gt; "", VLOOKUP(K119, IF(J119="1", Ward!$A$2:$B$11, IF(J119="2", Ward!$C$2:$D$12, IF(J119="3", Ward!$E$2:$F$15, IF(J119="4", Ward!$G$2:$H$16, IF(J119="5", Ward!$I$2:$J$16, IF(J119="6", Ward!$K$2:$L$15, IF(J119="7", Ward!$M$2:$N$11, IF(J119="8", Ward!$O$2:$P$17, IF(J119="9", Ward!$Q$2:$R$14, IF(J119="10", Ward!$S$2:$T$16, IF(J119="11", Ward!$U$2:$V$17, IF(J119="12", Ward!$W$2:$X$12, IF(J119="Bình Chánh", Ward!$Y$2:$Z$17, IF(J119="Bình Tân", Ward!$AA$2:$AB$11, IF(J119="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J119="Cần Giờ", Ward!$AE$2:$AF$8, IF(J119="Củ Chi", Ward!$AG$2:$AH$22, IF(J119="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J119="Hóc Môn", Ward!$AK$2:$AL$13, IF(J119="Nhà Bè", Ward!$AM$2:$AN$8, IF(J119="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J119="Tân Bình", Ward!$AQ$2:$AR$16, IF(J119="Tân Phú", Ward!$AS$2:$AT$12, IF(J119="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6734,7 +6734,7 @@
         <f>IF(J120 &lt;&gt; "", VLOOKUP(J120, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W120" s="28" t="str">
+      <c r="W120" s="23" t="str">
         <f>IF(K120 &lt;&gt; "", VLOOKUP(K120, IF(J120="1", Ward!$A$2:$B$11, IF(J120="2", Ward!$C$2:$D$12, IF(J120="3", Ward!$E$2:$F$15, IF(J120="4", Ward!$G$2:$H$16, IF(J120="5", Ward!$I$2:$J$16, IF(J120="6", Ward!$K$2:$L$15, IF(J120="7", Ward!$M$2:$N$11, IF(J120="8", Ward!$O$2:$P$17, IF(J120="9", Ward!$Q$2:$R$14, IF(J120="10", Ward!$S$2:$T$16, IF(J120="11", Ward!$U$2:$V$17, IF(J120="12", Ward!$W$2:$X$12, IF(J120="Bình Chánh", Ward!$Y$2:$Z$17, IF(J120="Bình Tân", Ward!$AA$2:$AB$11, IF(J120="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J120="Cần Giờ", Ward!$AE$2:$AF$8, IF(J120="Củ Chi", Ward!$AG$2:$AH$22, IF(J120="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J120="Hóc Môn", Ward!$AK$2:$AL$13, IF(J120="Nhà Bè", Ward!$AM$2:$AN$8, IF(J120="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J120="Tân Bình", Ward!$AQ$2:$AR$16, IF(J120="Tân Phú", Ward!$AS$2:$AT$12, IF(J120="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6772,7 +6772,7 @@
         <f>IF(J121 &lt;&gt; "", VLOOKUP(J121, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W121" s="28" t="str">
+      <c r="W121" s="23" t="str">
         <f>IF(K121 &lt;&gt; "", VLOOKUP(K121, IF(J121="1", Ward!$A$2:$B$11, IF(J121="2", Ward!$C$2:$D$12, IF(J121="3", Ward!$E$2:$F$15, IF(J121="4", Ward!$G$2:$H$16, IF(J121="5", Ward!$I$2:$J$16, IF(J121="6", Ward!$K$2:$L$15, IF(J121="7", Ward!$M$2:$N$11, IF(J121="8", Ward!$O$2:$P$17, IF(J121="9", Ward!$Q$2:$R$14, IF(J121="10", Ward!$S$2:$T$16, IF(J121="11", Ward!$U$2:$V$17, IF(J121="12", Ward!$W$2:$X$12, IF(J121="Bình Chánh", Ward!$Y$2:$Z$17, IF(J121="Bình Tân", Ward!$AA$2:$AB$11, IF(J121="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J121="Cần Giờ", Ward!$AE$2:$AF$8, IF(J121="Củ Chi", Ward!$AG$2:$AH$22, IF(J121="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J121="Hóc Môn", Ward!$AK$2:$AL$13, IF(J121="Nhà Bè", Ward!$AM$2:$AN$8, IF(J121="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J121="Tân Bình", Ward!$AQ$2:$AR$16, IF(J121="Tân Phú", Ward!$AS$2:$AT$12, IF(J121="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6810,7 +6810,7 @@
         <f>IF(J122 &lt;&gt; "", VLOOKUP(J122, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W122" s="28" t="str">
+      <c r="W122" s="23" t="str">
         <f>IF(K122 &lt;&gt; "", VLOOKUP(K122, IF(J122="1", Ward!$A$2:$B$11, IF(J122="2", Ward!$C$2:$D$12, IF(J122="3", Ward!$E$2:$F$15, IF(J122="4", Ward!$G$2:$H$16, IF(J122="5", Ward!$I$2:$J$16, IF(J122="6", Ward!$K$2:$L$15, IF(J122="7", Ward!$M$2:$N$11, IF(J122="8", Ward!$O$2:$P$17, IF(J122="9", Ward!$Q$2:$R$14, IF(J122="10", Ward!$S$2:$T$16, IF(J122="11", Ward!$U$2:$V$17, IF(J122="12", Ward!$W$2:$X$12, IF(J122="Bình Chánh", Ward!$Y$2:$Z$17, IF(J122="Bình Tân", Ward!$AA$2:$AB$11, IF(J122="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J122="Cần Giờ", Ward!$AE$2:$AF$8, IF(J122="Củ Chi", Ward!$AG$2:$AH$22, IF(J122="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J122="Hóc Môn", Ward!$AK$2:$AL$13, IF(J122="Nhà Bè", Ward!$AM$2:$AN$8, IF(J122="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J122="Tân Bình", Ward!$AQ$2:$AR$16, IF(J122="Tân Phú", Ward!$AS$2:$AT$12, IF(J122="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6848,7 +6848,7 @@
         <f>IF(J123 &lt;&gt; "", VLOOKUP(J123, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W123" s="28" t="str">
+      <c r="W123" s="23" t="str">
         <f>IF(K123 &lt;&gt; "", VLOOKUP(K123, IF(J123="1", Ward!$A$2:$B$11, IF(J123="2", Ward!$C$2:$D$12, IF(J123="3", Ward!$E$2:$F$15, IF(J123="4", Ward!$G$2:$H$16, IF(J123="5", Ward!$I$2:$J$16, IF(J123="6", Ward!$K$2:$L$15, IF(J123="7", Ward!$M$2:$N$11, IF(J123="8", Ward!$O$2:$P$17, IF(J123="9", Ward!$Q$2:$R$14, IF(J123="10", Ward!$S$2:$T$16, IF(J123="11", Ward!$U$2:$V$17, IF(J123="12", Ward!$W$2:$X$12, IF(J123="Bình Chánh", Ward!$Y$2:$Z$17, IF(J123="Bình Tân", Ward!$AA$2:$AB$11, IF(J123="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J123="Cần Giờ", Ward!$AE$2:$AF$8, IF(J123="Củ Chi", Ward!$AG$2:$AH$22, IF(J123="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J123="Hóc Môn", Ward!$AK$2:$AL$13, IF(J123="Nhà Bè", Ward!$AM$2:$AN$8, IF(J123="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J123="Tân Bình", Ward!$AQ$2:$AR$16, IF(J123="Tân Phú", Ward!$AS$2:$AT$12, IF(J123="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6886,7 +6886,7 @@
         <f>IF(J124 &lt;&gt; "", VLOOKUP(J124, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W124" s="28" t="str">
+      <c r="W124" s="23" t="str">
         <f>IF(K124 &lt;&gt; "", VLOOKUP(K124, IF(J124="1", Ward!$A$2:$B$11, IF(J124="2", Ward!$C$2:$D$12, IF(J124="3", Ward!$E$2:$F$15, IF(J124="4", Ward!$G$2:$H$16, IF(J124="5", Ward!$I$2:$J$16, IF(J124="6", Ward!$K$2:$L$15, IF(J124="7", Ward!$M$2:$N$11, IF(J124="8", Ward!$O$2:$P$17, IF(J124="9", Ward!$Q$2:$R$14, IF(J124="10", Ward!$S$2:$T$16, IF(J124="11", Ward!$U$2:$V$17, IF(J124="12", Ward!$W$2:$X$12, IF(J124="Bình Chánh", Ward!$Y$2:$Z$17, IF(J124="Bình Tân", Ward!$AA$2:$AB$11, IF(J124="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J124="Cần Giờ", Ward!$AE$2:$AF$8, IF(J124="Củ Chi", Ward!$AG$2:$AH$22, IF(J124="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J124="Hóc Môn", Ward!$AK$2:$AL$13, IF(J124="Nhà Bè", Ward!$AM$2:$AN$8, IF(J124="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J124="Tân Bình", Ward!$AQ$2:$AR$16, IF(J124="Tân Phú", Ward!$AS$2:$AT$12, IF(J124="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6924,7 +6924,7 @@
         <f>IF(J125 &lt;&gt; "", VLOOKUP(J125, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W125" s="28" t="str">
+      <c r="W125" s="23" t="str">
         <f>IF(K125 &lt;&gt; "", VLOOKUP(K125, IF(J125="1", Ward!$A$2:$B$11, IF(J125="2", Ward!$C$2:$D$12, IF(J125="3", Ward!$E$2:$F$15, IF(J125="4", Ward!$G$2:$H$16, IF(J125="5", Ward!$I$2:$J$16, IF(J125="6", Ward!$K$2:$L$15, IF(J125="7", Ward!$M$2:$N$11, IF(J125="8", Ward!$O$2:$P$17, IF(J125="9", Ward!$Q$2:$R$14, IF(J125="10", Ward!$S$2:$T$16, IF(J125="11", Ward!$U$2:$V$17, IF(J125="12", Ward!$W$2:$X$12, IF(J125="Bình Chánh", Ward!$Y$2:$Z$17, IF(J125="Bình Tân", Ward!$AA$2:$AB$11, IF(J125="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J125="Cần Giờ", Ward!$AE$2:$AF$8, IF(J125="Củ Chi", Ward!$AG$2:$AH$22, IF(J125="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J125="Hóc Môn", Ward!$AK$2:$AL$13, IF(J125="Nhà Bè", Ward!$AM$2:$AN$8, IF(J125="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J125="Tân Bình", Ward!$AQ$2:$AR$16, IF(J125="Tân Phú", Ward!$AS$2:$AT$12, IF(J125="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -6962,7 +6962,7 @@
         <f>IF(J126 &lt;&gt; "", VLOOKUP(J126, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W126" s="28" t="str">
+      <c r="W126" s="23" t="str">
         <f>IF(K126 &lt;&gt; "", VLOOKUP(K126, IF(J126="1", Ward!$A$2:$B$11, IF(J126="2", Ward!$C$2:$D$12, IF(J126="3", Ward!$E$2:$F$15, IF(J126="4", Ward!$G$2:$H$16, IF(J126="5", Ward!$I$2:$J$16, IF(J126="6", Ward!$K$2:$L$15, IF(J126="7", Ward!$M$2:$N$11, IF(J126="8", Ward!$O$2:$P$17, IF(J126="9", Ward!$Q$2:$R$14, IF(J126="10", Ward!$S$2:$T$16, IF(J126="11", Ward!$U$2:$V$17, IF(J126="12", Ward!$W$2:$X$12, IF(J126="Bình Chánh", Ward!$Y$2:$Z$17, IF(J126="Bình Tân", Ward!$AA$2:$AB$11, IF(J126="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J126="Cần Giờ", Ward!$AE$2:$AF$8, IF(J126="Củ Chi", Ward!$AG$2:$AH$22, IF(J126="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J126="Hóc Môn", Ward!$AK$2:$AL$13, IF(J126="Nhà Bè", Ward!$AM$2:$AN$8, IF(J126="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J126="Tân Bình", Ward!$AQ$2:$AR$16, IF(J126="Tân Phú", Ward!$AS$2:$AT$12, IF(J126="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7000,7 +7000,7 @@
         <f>IF(J127 &lt;&gt; "", VLOOKUP(J127, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W127" s="28" t="str">
+      <c r="W127" s="23" t="str">
         <f>IF(K127 &lt;&gt; "", VLOOKUP(K127, IF(J127="1", Ward!$A$2:$B$11, IF(J127="2", Ward!$C$2:$D$12, IF(J127="3", Ward!$E$2:$F$15, IF(J127="4", Ward!$G$2:$H$16, IF(J127="5", Ward!$I$2:$J$16, IF(J127="6", Ward!$K$2:$L$15, IF(J127="7", Ward!$M$2:$N$11, IF(J127="8", Ward!$O$2:$P$17, IF(J127="9", Ward!$Q$2:$R$14, IF(J127="10", Ward!$S$2:$T$16, IF(J127="11", Ward!$U$2:$V$17, IF(J127="12", Ward!$W$2:$X$12, IF(J127="Bình Chánh", Ward!$Y$2:$Z$17, IF(J127="Bình Tân", Ward!$AA$2:$AB$11, IF(J127="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J127="Cần Giờ", Ward!$AE$2:$AF$8, IF(J127="Củ Chi", Ward!$AG$2:$AH$22, IF(J127="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J127="Hóc Môn", Ward!$AK$2:$AL$13, IF(J127="Nhà Bè", Ward!$AM$2:$AN$8, IF(J127="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J127="Tân Bình", Ward!$AQ$2:$AR$16, IF(J127="Tân Phú", Ward!$AS$2:$AT$12, IF(J127="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7038,7 +7038,7 @@
         <f>IF(J128 &lt;&gt; "", VLOOKUP(J128, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W128" s="28" t="str">
+      <c r="W128" s="23" t="str">
         <f>IF(K128 &lt;&gt; "", VLOOKUP(K128, IF(J128="1", Ward!$A$2:$B$11, IF(J128="2", Ward!$C$2:$D$12, IF(J128="3", Ward!$E$2:$F$15, IF(J128="4", Ward!$G$2:$H$16, IF(J128="5", Ward!$I$2:$J$16, IF(J128="6", Ward!$K$2:$L$15, IF(J128="7", Ward!$M$2:$N$11, IF(J128="8", Ward!$O$2:$P$17, IF(J128="9", Ward!$Q$2:$R$14, IF(J128="10", Ward!$S$2:$T$16, IF(J128="11", Ward!$U$2:$V$17, IF(J128="12", Ward!$W$2:$X$12, IF(J128="Bình Chánh", Ward!$Y$2:$Z$17, IF(J128="Bình Tân", Ward!$AA$2:$AB$11, IF(J128="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J128="Cần Giờ", Ward!$AE$2:$AF$8, IF(J128="Củ Chi", Ward!$AG$2:$AH$22, IF(J128="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J128="Hóc Môn", Ward!$AK$2:$AL$13, IF(J128="Nhà Bè", Ward!$AM$2:$AN$8, IF(J128="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J128="Tân Bình", Ward!$AQ$2:$AR$16, IF(J128="Tân Phú", Ward!$AS$2:$AT$12, IF(J128="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7076,7 +7076,7 @@
         <f>IF(J129 &lt;&gt; "", VLOOKUP(J129, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W129" s="28" t="str">
+      <c r="W129" s="23" t="str">
         <f>IF(K129 &lt;&gt; "", VLOOKUP(K129, IF(J129="1", Ward!$A$2:$B$11, IF(J129="2", Ward!$C$2:$D$12, IF(J129="3", Ward!$E$2:$F$15, IF(J129="4", Ward!$G$2:$H$16, IF(J129="5", Ward!$I$2:$J$16, IF(J129="6", Ward!$K$2:$L$15, IF(J129="7", Ward!$M$2:$N$11, IF(J129="8", Ward!$O$2:$P$17, IF(J129="9", Ward!$Q$2:$R$14, IF(J129="10", Ward!$S$2:$T$16, IF(J129="11", Ward!$U$2:$V$17, IF(J129="12", Ward!$W$2:$X$12, IF(J129="Bình Chánh", Ward!$Y$2:$Z$17, IF(J129="Bình Tân", Ward!$AA$2:$AB$11, IF(J129="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J129="Cần Giờ", Ward!$AE$2:$AF$8, IF(J129="Củ Chi", Ward!$AG$2:$AH$22, IF(J129="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J129="Hóc Môn", Ward!$AK$2:$AL$13, IF(J129="Nhà Bè", Ward!$AM$2:$AN$8, IF(J129="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J129="Tân Bình", Ward!$AQ$2:$AR$16, IF(J129="Tân Phú", Ward!$AS$2:$AT$12, IF(J129="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7114,7 +7114,7 @@
         <f>IF(J130 &lt;&gt; "", VLOOKUP(J130, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W130" s="28" t="str">
+      <c r="W130" s="23" t="str">
         <f>IF(K130 &lt;&gt; "", VLOOKUP(K130, IF(J130="1", Ward!$A$2:$B$11, IF(J130="2", Ward!$C$2:$D$12, IF(J130="3", Ward!$E$2:$F$15, IF(J130="4", Ward!$G$2:$H$16, IF(J130="5", Ward!$I$2:$J$16, IF(J130="6", Ward!$K$2:$L$15, IF(J130="7", Ward!$M$2:$N$11, IF(J130="8", Ward!$O$2:$P$17, IF(J130="9", Ward!$Q$2:$R$14, IF(J130="10", Ward!$S$2:$T$16, IF(J130="11", Ward!$U$2:$V$17, IF(J130="12", Ward!$W$2:$X$12, IF(J130="Bình Chánh", Ward!$Y$2:$Z$17, IF(J130="Bình Tân", Ward!$AA$2:$AB$11, IF(J130="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J130="Cần Giờ", Ward!$AE$2:$AF$8, IF(J130="Củ Chi", Ward!$AG$2:$AH$22, IF(J130="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J130="Hóc Môn", Ward!$AK$2:$AL$13, IF(J130="Nhà Bè", Ward!$AM$2:$AN$8, IF(J130="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J130="Tân Bình", Ward!$AQ$2:$AR$16, IF(J130="Tân Phú", Ward!$AS$2:$AT$12, IF(J130="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7152,7 +7152,7 @@
         <f>IF(J131 &lt;&gt; "", VLOOKUP(J131, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W131" s="28" t="str">
+      <c r="W131" s="23" t="str">
         <f>IF(K131 &lt;&gt; "", VLOOKUP(K131, IF(J131="1", Ward!$A$2:$B$11, IF(J131="2", Ward!$C$2:$D$12, IF(J131="3", Ward!$E$2:$F$15, IF(J131="4", Ward!$G$2:$H$16, IF(J131="5", Ward!$I$2:$J$16, IF(J131="6", Ward!$K$2:$L$15, IF(J131="7", Ward!$M$2:$N$11, IF(J131="8", Ward!$O$2:$P$17, IF(J131="9", Ward!$Q$2:$R$14, IF(J131="10", Ward!$S$2:$T$16, IF(J131="11", Ward!$U$2:$V$17, IF(J131="12", Ward!$W$2:$X$12, IF(J131="Bình Chánh", Ward!$Y$2:$Z$17, IF(J131="Bình Tân", Ward!$AA$2:$AB$11, IF(J131="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J131="Cần Giờ", Ward!$AE$2:$AF$8, IF(J131="Củ Chi", Ward!$AG$2:$AH$22, IF(J131="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J131="Hóc Môn", Ward!$AK$2:$AL$13, IF(J131="Nhà Bè", Ward!$AM$2:$AN$8, IF(J131="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J131="Tân Bình", Ward!$AQ$2:$AR$16, IF(J131="Tân Phú", Ward!$AS$2:$AT$12, IF(J131="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7190,7 +7190,7 @@
         <f>IF(J132 &lt;&gt; "", VLOOKUP(J132, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W132" s="28" t="str">
+      <c r="W132" s="23" t="str">
         <f>IF(K132 &lt;&gt; "", VLOOKUP(K132, IF(J132="1", Ward!$A$2:$B$11, IF(J132="2", Ward!$C$2:$D$12, IF(J132="3", Ward!$E$2:$F$15, IF(J132="4", Ward!$G$2:$H$16, IF(J132="5", Ward!$I$2:$J$16, IF(J132="6", Ward!$K$2:$L$15, IF(J132="7", Ward!$M$2:$N$11, IF(J132="8", Ward!$O$2:$P$17, IF(J132="9", Ward!$Q$2:$R$14, IF(J132="10", Ward!$S$2:$T$16, IF(J132="11", Ward!$U$2:$V$17, IF(J132="12", Ward!$W$2:$X$12, IF(J132="Bình Chánh", Ward!$Y$2:$Z$17, IF(J132="Bình Tân", Ward!$AA$2:$AB$11, IF(J132="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J132="Cần Giờ", Ward!$AE$2:$AF$8, IF(J132="Củ Chi", Ward!$AG$2:$AH$22, IF(J132="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J132="Hóc Môn", Ward!$AK$2:$AL$13, IF(J132="Nhà Bè", Ward!$AM$2:$AN$8, IF(J132="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J132="Tân Bình", Ward!$AQ$2:$AR$16, IF(J132="Tân Phú", Ward!$AS$2:$AT$12, IF(J132="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7228,7 +7228,7 @@
         <f>IF(J133 &lt;&gt; "", VLOOKUP(J133, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W133" s="28" t="str">
+      <c r="W133" s="23" t="str">
         <f>IF(K133 &lt;&gt; "", VLOOKUP(K133, IF(J133="1", Ward!$A$2:$B$11, IF(J133="2", Ward!$C$2:$D$12, IF(J133="3", Ward!$E$2:$F$15, IF(J133="4", Ward!$G$2:$H$16, IF(J133="5", Ward!$I$2:$J$16, IF(J133="6", Ward!$K$2:$L$15, IF(J133="7", Ward!$M$2:$N$11, IF(J133="8", Ward!$O$2:$P$17, IF(J133="9", Ward!$Q$2:$R$14, IF(J133="10", Ward!$S$2:$T$16, IF(J133="11", Ward!$U$2:$V$17, IF(J133="12", Ward!$W$2:$X$12, IF(J133="Bình Chánh", Ward!$Y$2:$Z$17, IF(J133="Bình Tân", Ward!$AA$2:$AB$11, IF(J133="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J133="Cần Giờ", Ward!$AE$2:$AF$8, IF(J133="Củ Chi", Ward!$AG$2:$AH$22, IF(J133="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J133="Hóc Môn", Ward!$AK$2:$AL$13, IF(J133="Nhà Bè", Ward!$AM$2:$AN$8, IF(J133="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J133="Tân Bình", Ward!$AQ$2:$AR$16, IF(J133="Tân Phú", Ward!$AS$2:$AT$12, IF(J133="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7266,7 +7266,7 @@
         <f>IF(J134 &lt;&gt; "", VLOOKUP(J134, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W134" s="28" t="str">
+      <c r="W134" s="23" t="str">
         <f>IF(K134 &lt;&gt; "", VLOOKUP(K134, IF(J134="1", Ward!$A$2:$B$11, IF(J134="2", Ward!$C$2:$D$12, IF(J134="3", Ward!$E$2:$F$15, IF(J134="4", Ward!$G$2:$H$16, IF(J134="5", Ward!$I$2:$J$16, IF(J134="6", Ward!$K$2:$L$15, IF(J134="7", Ward!$M$2:$N$11, IF(J134="8", Ward!$O$2:$P$17, IF(J134="9", Ward!$Q$2:$R$14, IF(J134="10", Ward!$S$2:$T$16, IF(J134="11", Ward!$U$2:$V$17, IF(J134="12", Ward!$W$2:$X$12, IF(J134="Bình Chánh", Ward!$Y$2:$Z$17, IF(J134="Bình Tân", Ward!$AA$2:$AB$11, IF(J134="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J134="Cần Giờ", Ward!$AE$2:$AF$8, IF(J134="Củ Chi", Ward!$AG$2:$AH$22, IF(J134="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J134="Hóc Môn", Ward!$AK$2:$AL$13, IF(J134="Nhà Bè", Ward!$AM$2:$AN$8, IF(J134="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J134="Tân Bình", Ward!$AQ$2:$AR$16, IF(J134="Tân Phú", Ward!$AS$2:$AT$12, IF(J134="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7304,7 +7304,7 @@
         <f>IF(J135 &lt;&gt; "", VLOOKUP(J135, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W135" s="28" t="str">
+      <c r="W135" s="23" t="str">
         <f>IF(K135 &lt;&gt; "", VLOOKUP(K135, IF(J135="1", Ward!$A$2:$B$11, IF(J135="2", Ward!$C$2:$D$12, IF(J135="3", Ward!$E$2:$F$15, IF(J135="4", Ward!$G$2:$H$16, IF(J135="5", Ward!$I$2:$J$16, IF(J135="6", Ward!$K$2:$L$15, IF(J135="7", Ward!$M$2:$N$11, IF(J135="8", Ward!$O$2:$P$17, IF(J135="9", Ward!$Q$2:$R$14, IF(J135="10", Ward!$S$2:$T$16, IF(J135="11", Ward!$U$2:$V$17, IF(J135="12", Ward!$W$2:$X$12, IF(J135="Bình Chánh", Ward!$Y$2:$Z$17, IF(J135="Bình Tân", Ward!$AA$2:$AB$11, IF(J135="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J135="Cần Giờ", Ward!$AE$2:$AF$8, IF(J135="Củ Chi", Ward!$AG$2:$AH$22, IF(J135="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J135="Hóc Môn", Ward!$AK$2:$AL$13, IF(J135="Nhà Bè", Ward!$AM$2:$AN$8, IF(J135="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J135="Tân Bình", Ward!$AQ$2:$AR$16, IF(J135="Tân Phú", Ward!$AS$2:$AT$12, IF(J135="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7342,7 +7342,7 @@
         <f>IF(J136 &lt;&gt; "", VLOOKUP(J136, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W136" s="28" t="str">
+      <c r="W136" s="23" t="str">
         <f>IF(K136 &lt;&gt; "", VLOOKUP(K136, IF(J136="1", Ward!$A$2:$B$11, IF(J136="2", Ward!$C$2:$D$12, IF(J136="3", Ward!$E$2:$F$15, IF(J136="4", Ward!$G$2:$H$16, IF(J136="5", Ward!$I$2:$J$16, IF(J136="6", Ward!$K$2:$L$15, IF(J136="7", Ward!$M$2:$N$11, IF(J136="8", Ward!$O$2:$P$17, IF(J136="9", Ward!$Q$2:$R$14, IF(J136="10", Ward!$S$2:$T$16, IF(J136="11", Ward!$U$2:$V$17, IF(J136="12", Ward!$W$2:$X$12, IF(J136="Bình Chánh", Ward!$Y$2:$Z$17, IF(J136="Bình Tân", Ward!$AA$2:$AB$11, IF(J136="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J136="Cần Giờ", Ward!$AE$2:$AF$8, IF(J136="Củ Chi", Ward!$AG$2:$AH$22, IF(J136="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J136="Hóc Môn", Ward!$AK$2:$AL$13, IF(J136="Nhà Bè", Ward!$AM$2:$AN$8, IF(J136="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J136="Tân Bình", Ward!$AQ$2:$AR$16, IF(J136="Tân Phú", Ward!$AS$2:$AT$12, IF(J136="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7380,7 +7380,7 @@
         <f>IF(J137 &lt;&gt; "", VLOOKUP(J137, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W137" s="28" t="str">
+      <c r="W137" s="23" t="str">
         <f>IF(K137 &lt;&gt; "", VLOOKUP(K137, IF(J137="1", Ward!$A$2:$B$11, IF(J137="2", Ward!$C$2:$D$12, IF(J137="3", Ward!$E$2:$F$15, IF(J137="4", Ward!$G$2:$H$16, IF(J137="5", Ward!$I$2:$J$16, IF(J137="6", Ward!$K$2:$L$15, IF(J137="7", Ward!$M$2:$N$11, IF(J137="8", Ward!$O$2:$P$17, IF(J137="9", Ward!$Q$2:$R$14, IF(J137="10", Ward!$S$2:$T$16, IF(J137="11", Ward!$U$2:$V$17, IF(J137="12", Ward!$W$2:$X$12, IF(J137="Bình Chánh", Ward!$Y$2:$Z$17, IF(J137="Bình Tân", Ward!$AA$2:$AB$11, IF(J137="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J137="Cần Giờ", Ward!$AE$2:$AF$8, IF(J137="Củ Chi", Ward!$AG$2:$AH$22, IF(J137="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J137="Hóc Môn", Ward!$AK$2:$AL$13, IF(J137="Nhà Bè", Ward!$AM$2:$AN$8, IF(J137="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J137="Tân Bình", Ward!$AQ$2:$AR$16, IF(J137="Tân Phú", Ward!$AS$2:$AT$12, IF(J137="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7418,7 +7418,7 @@
         <f>IF(J138 &lt;&gt; "", VLOOKUP(J138, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W138" s="28" t="str">
+      <c r="W138" s="23" t="str">
         <f>IF(K138 &lt;&gt; "", VLOOKUP(K138, IF(J138="1", Ward!$A$2:$B$11, IF(J138="2", Ward!$C$2:$D$12, IF(J138="3", Ward!$E$2:$F$15, IF(J138="4", Ward!$G$2:$H$16, IF(J138="5", Ward!$I$2:$J$16, IF(J138="6", Ward!$K$2:$L$15, IF(J138="7", Ward!$M$2:$N$11, IF(J138="8", Ward!$O$2:$P$17, IF(J138="9", Ward!$Q$2:$R$14, IF(J138="10", Ward!$S$2:$T$16, IF(J138="11", Ward!$U$2:$V$17, IF(J138="12", Ward!$W$2:$X$12, IF(J138="Bình Chánh", Ward!$Y$2:$Z$17, IF(J138="Bình Tân", Ward!$AA$2:$AB$11, IF(J138="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J138="Cần Giờ", Ward!$AE$2:$AF$8, IF(J138="Củ Chi", Ward!$AG$2:$AH$22, IF(J138="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J138="Hóc Môn", Ward!$AK$2:$AL$13, IF(J138="Nhà Bè", Ward!$AM$2:$AN$8, IF(J138="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J138="Tân Bình", Ward!$AQ$2:$AR$16, IF(J138="Tân Phú", Ward!$AS$2:$AT$12, IF(J138="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7456,7 +7456,7 @@
         <f>IF(J139 &lt;&gt; "", VLOOKUP(J139, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W139" s="28" t="str">
+      <c r="W139" s="23" t="str">
         <f>IF(K139 &lt;&gt; "", VLOOKUP(K139, IF(J139="1", Ward!$A$2:$B$11, IF(J139="2", Ward!$C$2:$D$12, IF(J139="3", Ward!$E$2:$F$15, IF(J139="4", Ward!$G$2:$H$16, IF(J139="5", Ward!$I$2:$J$16, IF(J139="6", Ward!$K$2:$L$15, IF(J139="7", Ward!$M$2:$N$11, IF(J139="8", Ward!$O$2:$P$17, IF(J139="9", Ward!$Q$2:$R$14, IF(J139="10", Ward!$S$2:$T$16, IF(J139="11", Ward!$U$2:$V$17, IF(J139="12", Ward!$W$2:$X$12, IF(J139="Bình Chánh", Ward!$Y$2:$Z$17, IF(J139="Bình Tân", Ward!$AA$2:$AB$11, IF(J139="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J139="Cần Giờ", Ward!$AE$2:$AF$8, IF(J139="Củ Chi", Ward!$AG$2:$AH$22, IF(J139="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J139="Hóc Môn", Ward!$AK$2:$AL$13, IF(J139="Nhà Bè", Ward!$AM$2:$AN$8, IF(J139="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J139="Tân Bình", Ward!$AQ$2:$AR$16, IF(J139="Tân Phú", Ward!$AS$2:$AT$12, IF(J139="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7494,7 +7494,7 @@
         <f>IF(J140 &lt;&gt; "", VLOOKUP(J140, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W140" s="28" t="str">
+      <c r="W140" s="23" t="str">
         <f>IF(K140 &lt;&gt; "", VLOOKUP(K140, IF(J140="1", Ward!$A$2:$B$11, IF(J140="2", Ward!$C$2:$D$12, IF(J140="3", Ward!$E$2:$F$15, IF(J140="4", Ward!$G$2:$H$16, IF(J140="5", Ward!$I$2:$J$16, IF(J140="6", Ward!$K$2:$L$15, IF(J140="7", Ward!$M$2:$N$11, IF(J140="8", Ward!$O$2:$P$17, IF(J140="9", Ward!$Q$2:$R$14, IF(J140="10", Ward!$S$2:$T$16, IF(J140="11", Ward!$U$2:$V$17, IF(J140="12", Ward!$W$2:$X$12, IF(J140="Bình Chánh", Ward!$Y$2:$Z$17, IF(J140="Bình Tân", Ward!$AA$2:$AB$11, IF(J140="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J140="Cần Giờ", Ward!$AE$2:$AF$8, IF(J140="Củ Chi", Ward!$AG$2:$AH$22, IF(J140="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J140="Hóc Môn", Ward!$AK$2:$AL$13, IF(J140="Nhà Bè", Ward!$AM$2:$AN$8, IF(J140="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J140="Tân Bình", Ward!$AQ$2:$AR$16, IF(J140="Tân Phú", Ward!$AS$2:$AT$12, IF(J140="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7532,7 +7532,7 @@
         <f>IF(J141 &lt;&gt; "", VLOOKUP(J141, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W141" s="28" t="str">
+      <c r="W141" s="23" t="str">
         <f>IF(K141 &lt;&gt; "", VLOOKUP(K141, IF(J141="1", Ward!$A$2:$B$11, IF(J141="2", Ward!$C$2:$D$12, IF(J141="3", Ward!$E$2:$F$15, IF(J141="4", Ward!$G$2:$H$16, IF(J141="5", Ward!$I$2:$J$16, IF(J141="6", Ward!$K$2:$L$15, IF(J141="7", Ward!$M$2:$N$11, IF(J141="8", Ward!$O$2:$P$17, IF(J141="9", Ward!$Q$2:$R$14, IF(J141="10", Ward!$S$2:$T$16, IF(J141="11", Ward!$U$2:$V$17, IF(J141="12", Ward!$W$2:$X$12, IF(J141="Bình Chánh", Ward!$Y$2:$Z$17, IF(J141="Bình Tân", Ward!$AA$2:$AB$11, IF(J141="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J141="Cần Giờ", Ward!$AE$2:$AF$8, IF(J141="Củ Chi", Ward!$AG$2:$AH$22, IF(J141="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J141="Hóc Môn", Ward!$AK$2:$AL$13, IF(J141="Nhà Bè", Ward!$AM$2:$AN$8, IF(J141="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J141="Tân Bình", Ward!$AQ$2:$AR$16, IF(J141="Tân Phú", Ward!$AS$2:$AT$12, IF(J141="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7570,7 +7570,7 @@
         <f>IF(J142 &lt;&gt; "", VLOOKUP(J142, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W142" s="28" t="str">
+      <c r="W142" s="23" t="str">
         <f>IF(K142 &lt;&gt; "", VLOOKUP(K142, IF(J142="1", Ward!$A$2:$B$11, IF(J142="2", Ward!$C$2:$D$12, IF(J142="3", Ward!$E$2:$F$15, IF(J142="4", Ward!$G$2:$H$16, IF(J142="5", Ward!$I$2:$J$16, IF(J142="6", Ward!$K$2:$L$15, IF(J142="7", Ward!$M$2:$N$11, IF(J142="8", Ward!$O$2:$P$17, IF(J142="9", Ward!$Q$2:$R$14, IF(J142="10", Ward!$S$2:$T$16, IF(J142="11", Ward!$U$2:$V$17, IF(J142="12", Ward!$W$2:$X$12, IF(J142="Bình Chánh", Ward!$Y$2:$Z$17, IF(J142="Bình Tân", Ward!$AA$2:$AB$11, IF(J142="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J142="Cần Giờ", Ward!$AE$2:$AF$8, IF(J142="Củ Chi", Ward!$AG$2:$AH$22, IF(J142="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J142="Hóc Môn", Ward!$AK$2:$AL$13, IF(J142="Nhà Bè", Ward!$AM$2:$AN$8, IF(J142="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J142="Tân Bình", Ward!$AQ$2:$AR$16, IF(J142="Tân Phú", Ward!$AS$2:$AT$12, IF(J142="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7608,7 +7608,7 @@
         <f>IF(J143 &lt;&gt; "", VLOOKUP(J143, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W143" s="28" t="str">
+      <c r="W143" s="23" t="str">
         <f>IF(K143 &lt;&gt; "", VLOOKUP(K143, IF(J143="1", Ward!$A$2:$B$11, IF(J143="2", Ward!$C$2:$D$12, IF(J143="3", Ward!$E$2:$F$15, IF(J143="4", Ward!$G$2:$H$16, IF(J143="5", Ward!$I$2:$J$16, IF(J143="6", Ward!$K$2:$L$15, IF(J143="7", Ward!$M$2:$N$11, IF(J143="8", Ward!$O$2:$P$17, IF(J143="9", Ward!$Q$2:$R$14, IF(J143="10", Ward!$S$2:$T$16, IF(J143="11", Ward!$U$2:$V$17, IF(J143="12", Ward!$W$2:$X$12, IF(J143="Bình Chánh", Ward!$Y$2:$Z$17, IF(J143="Bình Tân", Ward!$AA$2:$AB$11, IF(J143="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J143="Cần Giờ", Ward!$AE$2:$AF$8, IF(J143="Củ Chi", Ward!$AG$2:$AH$22, IF(J143="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J143="Hóc Môn", Ward!$AK$2:$AL$13, IF(J143="Nhà Bè", Ward!$AM$2:$AN$8, IF(J143="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J143="Tân Bình", Ward!$AQ$2:$AR$16, IF(J143="Tân Phú", Ward!$AS$2:$AT$12, IF(J143="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7646,7 +7646,7 @@
         <f>IF(J144 &lt;&gt; "", VLOOKUP(J144, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W144" s="28" t="str">
+      <c r="W144" s="23" t="str">
         <f>IF(K144 &lt;&gt; "", VLOOKUP(K144, IF(J144="1", Ward!$A$2:$B$11, IF(J144="2", Ward!$C$2:$D$12, IF(J144="3", Ward!$E$2:$F$15, IF(J144="4", Ward!$G$2:$H$16, IF(J144="5", Ward!$I$2:$J$16, IF(J144="6", Ward!$K$2:$L$15, IF(J144="7", Ward!$M$2:$N$11, IF(J144="8", Ward!$O$2:$P$17, IF(J144="9", Ward!$Q$2:$R$14, IF(J144="10", Ward!$S$2:$T$16, IF(J144="11", Ward!$U$2:$V$17, IF(J144="12", Ward!$W$2:$X$12, IF(J144="Bình Chánh", Ward!$Y$2:$Z$17, IF(J144="Bình Tân", Ward!$AA$2:$AB$11, IF(J144="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J144="Cần Giờ", Ward!$AE$2:$AF$8, IF(J144="Củ Chi", Ward!$AG$2:$AH$22, IF(J144="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J144="Hóc Môn", Ward!$AK$2:$AL$13, IF(J144="Nhà Bè", Ward!$AM$2:$AN$8, IF(J144="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J144="Tân Bình", Ward!$AQ$2:$AR$16, IF(J144="Tân Phú", Ward!$AS$2:$AT$12, IF(J144="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7684,7 +7684,7 @@
         <f>IF(J145 &lt;&gt; "", VLOOKUP(J145, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W145" s="28" t="str">
+      <c r="W145" s="23" t="str">
         <f>IF(K145 &lt;&gt; "", VLOOKUP(K145, IF(J145="1", Ward!$A$2:$B$11, IF(J145="2", Ward!$C$2:$D$12, IF(J145="3", Ward!$E$2:$F$15, IF(J145="4", Ward!$G$2:$H$16, IF(J145="5", Ward!$I$2:$J$16, IF(J145="6", Ward!$K$2:$L$15, IF(J145="7", Ward!$M$2:$N$11, IF(J145="8", Ward!$O$2:$P$17, IF(J145="9", Ward!$Q$2:$R$14, IF(J145="10", Ward!$S$2:$T$16, IF(J145="11", Ward!$U$2:$V$17, IF(J145="12", Ward!$W$2:$X$12, IF(J145="Bình Chánh", Ward!$Y$2:$Z$17, IF(J145="Bình Tân", Ward!$AA$2:$AB$11, IF(J145="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J145="Cần Giờ", Ward!$AE$2:$AF$8, IF(J145="Củ Chi", Ward!$AG$2:$AH$22, IF(J145="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J145="Hóc Môn", Ward!$AK$2:$AL$13, IF(J145="Nhà Bè", Ward!$AM$2:$AN$8, IF(J145="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J145="Tân Bình", Ward!$AQ$2:$AR$16, IF(J145="Tân Phú", Ward!$AS$2:$AT$12, IF(J145="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7722,7 +7722,7 @@
         <f>IF(J146 &lt;&gt; "", VLOOKUP(J146, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W146" s="28" t="str">
+      <c r="W146" s="23" t="str">
         <f>IF(K146 &lt;&gt; "", VLOOKUP(K146, IF(J146="1", Ward!$A$2:$B$11, IF(J146="2", Ward!$C$2:$D$12, IF(J146="3", Ward!$E$2:$F$15, IF(J146="4", Ward!$G$2:$H$16, IF(J146="5", Ward!$I$2:$J$16, IF(J146="6", Ward!$K$2:$L$15, IF(J146="7", Ward!$M$2:$N$11, IF(J146="8", Ward!$O$2:$P$17, IF(J146="9", Ward!$Q$2:$R$14, IF(J146="10", Ward!$S$2:$T$16, IF(J146="11", Ward!$U$2:$V$17, IF(J146="12", Ward!$W$2:$X$12, IF(J146="Bình Chánh", Ward!$Y$2:$Z$17, IF(J146="Bình Tân", Ward!$AA$2:$AB$11, IF(J146="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J146="Cần Giờ", Ward!$AE$2:$AF$8, IF(J146="Củ Chi", Ward!$AG$2:$AH$22, IF(J146="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J146="Hóc Môn", Ward!$AK$2:$AL$13, IF(J146="Nhà Bè", Ward!$AM$2:$AN$8, IF(J146="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J146="Tân Bình", Ward!$AQ$2:$AR$16, IF(J146="Tân Phú", Ward!$AS$2:$AT$12, IF(J146="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7760,7 +7760,7 @@
         <f>IF(J147 &lt;&gt; "", VLOOKUP(J147, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W147" s="28" t="str">
+      <c r="W147" s="23" t="str">
         <f>IF(K147 &lt;&gt; "", VLOOKUP(K147, IF(J147="1", Ward!$A$2:$B$11, IF(J147="2", Ward!$C$2:$D$12, IF(J147="3", Ward!$E$2:$F$15, IF(J147="4", Ward!$G$2:$H$16, IF(J147="5", Ward!$I$2:$J$16, IF(J147="6", Ward!$K$2:$L$15, IF(J147="7", Ward!$M$2:$N$11, IF(J147="8", Ward!$O$2:$P$17, IF(J147="9", Ward!$Q$2:$R$14, IF(J147="10", Ward!$S$2:$T$16, IF(J147="11", Ward!$U$2:$V$17, IF(J147="12", Ward!$W$2:$X$12, IF(J147="Bình Chánh", Ward!$Y$2:$Z$17, IF(J147="Bình Tân", Ward!$AA$2:$AB$11, IF(J147="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J147="Cần Giờ", Ward!$AE$2:$AF$8, IF(J147="Củ Chi", Ward!$AG$2:$AH$22, IF(J147="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J147="Hóc Môn", Ward!$AK$2:$AL$13, IF(J147="Nhà Bè", Ward!$AM$2:$AN$8, IF(J147="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J147="Tân Bình", Ward!$AQ$2:$AR$16, IF(J147="Tân Phú", Ward!$AS$2:$AT$12, IF(J147="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7798,7 +7798,7 @@
         <f>IF(J148 &lt;&gt; "", VLOOKUP(J148, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W148" s="28" t="str">
+      <c r="W148" s="23" t="str">
         <f>IF(K148 &lt;&gt; "", VLOOKUP(K148, IF(J148="1", Ward!$A$2:$B$11, IF(J148="2", Ward!$C$2:$D$12, IF(J148="3", Ward!$E$2:$F$15, IF(J148="4", Ward!$G$2:$H$16, IF(J148="5", Ward!$I$2:$J$16, IF(J148="6", Ward!$K$2:$L$15, IF(J148="7", Ward!$M$2:$N$11, IF(J148="8", Ward!$O$2:$P$17, IF(J148="9", Ward!$Q$2:$R$14, IF(J148="10", Ward!$S$2:$T$16, IF(J148="11", Ward!$U$2:$V$17, IF(J148="12", Ward!$W$2:$X$12, IF(J148="Bình Chánh", Ward!$Y$2:$Z$17, IF(J148="Bình Tân", Ward!$AA$2:$AB$11, IF(J148="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J148="Cần Giờ", Ward!$AE$2:$AF$8, IF(J148="Củ Chi", Ward!$AG$2:$AH$22, IF(J148="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J148="Hóc Môn", Ward!$AK$2:$AL$13, IF(J148="Nhà Bè", Ward!$AM$2:$AN$8, IF(J148="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J148="Tân Bình", Ward!$AQ$2:$AR$16, IF(J148="Tân Phú", Ward!$AS$2:$AT$12, IF(J148="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7836,7 +7836,7 @@
         <f>IF(J149 &lt;&gt; "", VLOOKUP(J149, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W149" s="28" t="str">
+      <c r="W149" s="23" t="str">
         <f>IF(K149 &lt;&gt; "", VLOOKUP(K149, IF(J149="1", Ward!$A$2:$B$11, IF(J149="2", Ward!$C$2:$D$12, IF(J149="3", Ward!$E$2:$F$15, IF(J149="4", Ward!$G$2:$H$16, IF(J149="5", Ward!$I$2:$J$16, IF(J149="6", Ward!$K$2:$L$15, IF(J149="7", Ward!$M$2:$N$11, IF(J149="8", Ward!$O$2:$P$17, IF(J149="9", Ward!$Q$2:$R$14, IF(J149="10", Ward!$S$2:$T$16, IF(J149="11", Ward!$U$2:$V$17, IF(J149="12", Ward!$W$2:$X$12, IF(J149="Bình Chánh", Ward!$Y$2:$Z$17, IF(J149="Bình Tân", Ward!$AA$2:$AB$11, IF(J149="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J149="Cần Giờ", Ward!$AE$2:$AF$8, IF(J149="Củ Chi", Ward!$AG$2:$AH$22, IF(J149="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J149="Hóc Môn", Ward!$AK$2:$AL$13, IF(J149="Nhà Bè", Ward!$AM$2:$AN$8, IF(J149="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J149="Tân Bình", Ward!$AQ$2:$AR$16, IF(J149="Tân Phú", Ward!$AS$2:$AT$12, IF(J149="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7874,7 +7874,7 @@
         <f>IF(J150 &lt;&gt; "", VLOOKUP(J150, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W150" s="28" t="str">
+      <c r="W150" s="23" t="str">
         <f>IF(K150 &lt;&gt; "", VLOOKUP(K150, IF(J150="1", Ward!$A$2:$B$11, IF(J150="2", Ward!$C$2:$D$12, IF(J150="3", Ward!$E$2:$F$15, IF(J150="4", Ward!$G$2:$H$16, IF(J150="5", Ward!$I$2:$J$16, IF(J150="6", Ward!$K$2:$L$15, IF(J150="7", Ward!$M$2:$N$11, IF(J150="8", Ward!$O$2:$P$17, IF(J150="9", Ward!$Q$2:$R$14, IF(J150="10", Ward!$S$2:$T$16, IF(J150="11", Ward!$U$2:$V$17, IF(J150="12", Ward!$W$2:$X$12, IF(J150="Bình Chánh", Ward!$Y$2:$Z$17, IF(J150="Bình Tân", Ward!$AA$2:$AB$11, IF(J150="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J150="Cần Giờ", Ward!$AE$2:$AF$8, IF(J150="Củ Chi", Ward!$AG$2:$AH$22, IF(J150="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J150="Hóc Môn", Ward!$AK$2:$AL$13, IF(J150="Nhà Bè", Ward!$AM$2:$AN$8, IF(J150="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J150="Tân Bình", Ward!$AQ$2:$AR$16, IF(J150="Tân Phú", Ward!$AS$2:$AT$12, IF(J150="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7912,7 +7912,7 @@
         <f>IF(J151 &lt;&gt; "", VLOOKUP(J151, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W151" s="28" t="str">
+      <c r="W151" s="23" t="str">
         <f>IF(K151 &lt;&gt; "", VLOOKUP(K151, IF(J151="1", Ward!$A$2:$B$11, IF(J151="2", Ward!$C$2:$D$12, IF(J151="3", Ward!$E$2:$F$15, IF(J151="4", Ward!$G$2:$H$16, IF(J151="5", Ward!$I$2:$J$16, IF(J151="6", Ward!$K$2:$L$15, IF(J151="7", Ward!$M$2:$N$11, IF(J151="8", Ward!$O$2:$P$17, IF(J151="9", Ward!$Q$2:$R$14, IF(J151="10", Ward!$S$2:$T$16, IF(J151="11", Ward!$U$2:$V$17, IF(J151="12", Ward!$W$2:$X$12, IF(J151="Bình Chánh", Ward!$Y$2:$Z$17, IF(J151="Bình Tân", Ward!$AA$2:$AB$11, IF(J151="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J151="Cần Giờ", Ward!$AE$2:$AF$8, IF(J151="Củ Chi", Ward!$AG$2:$AH$22, IF(J151="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J151="Hóc Môn", Ward!$AK$2:$AL$13, IF(J151="Nhà Bè", Ward!$AM$2:$AN$8, IF(J151="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J151="Tân Bình", Ward!$AQ$2:$AR$16, IF(J151="Tân Phú", Ward!$AS$2:$AT$12, IF(J151="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7950,7 +7950,7 @@
         <f>IF(J152 &lt;&gt; "", VLOOKUP(J152, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W152" s="28" t="str">
+      <c r="W152" s="23" t="str">
         <f>IF(K152 &lt;&gt; "", VLOOKUP(K152, IF(J152="1", Ward!$A$2:$B$11, IF(J152="2", Ward!$C$2:$D$12, IF(J152="3", Ward!$E$2:$F$15, IF(J152="4", Ward!$G$2:$H$16, IF(J152="5", Ward!$I$2:$J$16, IF(J152="6", Ward!$K$2:$L$15, IF(J152="7", Ward!$M$2:$N$11, IF(J152="8", Ward!$O$2:$P$17, IF(J152="9", Ward!$Q$2:$R$14, IF(J152="10", Ward!$S$2:$T$16, IF(J152="11", Ward!$U$2:$V$17, IF(J152="12", Ward!$W$2:$X$12, IF(J152="Bình Chánh", Ward!$Y$2:$Z$17, IF(J152="Bình Tân", Ward!$AA$2:$AB$11, IF(J152="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J152="Cần Giờ", Ward!$AE$2:$AF$8, IF(J152="Củ Chi", Ward!$AG$2:$AH$22, IF(J152="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J152="Hóc Môn", Ward!$AK$2:$AL$13, IF(J152="Nhà Bè", Ward!$AM$2:$AN$8, IF(J152="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J152="Tân Bình", Ward!$AQ$2:$AR$16, IF(J152="Tân Phú", Ward!$AS$2:$AT$12, IF(J152="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -7988,7 +7988,7 @@
         <f>IF(J153 &lt;&gt; "", VLOOKUP(J153, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W153" s="28" t="str">
+      <c r="W153" s="23" t="str">
         <f>IF(K153 &lt;&gt; "", VLOOKUP(K153, IF(J153="1", Ward!$A$2:$B$11, IF(J153="2", Ward!$C$2:$D$12, IF(J153="3", Ward!$E$2:$F$15, IF(J153="4", Ward!$G$2:$H$16, IF(J153="5", Ward!$I$2:$J$16, IF(J153="6", Ward!$K$2:$L$15, IF(J153="7", Ward!$M$2:$N$11, IF(J153="8", Ward!$O$2:$P$17, IF(J153="9", Ward!$Q$2:$R$14, IF(J153="10", Ward!$S$2:$T$16, IF(J153="11", Ward!$U$2:$V$17, IF(J153="12", Ward!$W$2:$X$12, IF(J153="Bình Chánh", Ward!$Y$2:$Z$17, IF(J153="Bình Tân", Ward!$AA$2:$AB$11, IF(J153="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J153="Cần Giờ", Ward!$AE$2:$AF$8, IF(J153="Củ Chi", Ward!$AG$2:$AH$22, IF(J153="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J153="Hóc Môn", Ward!$AK$2:$AL$13, IF(J153="Nhà Bè", Ward!$AM$2:$AN$8, IF(J153="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J153="Tân Bình", Ward!$AQ$2:$AR$16, IF(J153="Tân Phú", Ward!$AS$2:$AT$12, IF(J153="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8026,7 +8026,7 @@
         <f>IF(J154 &lt;&gt; "", VLOOKUP(J154, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W154" s="28" t="str">
+      <c r="W154" s="23" t="str">
         <f>IF(K154 &lt;&gt; "", VLOOKUP(K154, IF(J154="1", Ward!$A$2:$B$11, IF(J154="2", Ward!$C$2:$D$12, IF(J154="3", Ward!$E$2:$F$15, IF(J154="4", Ward!$G$2:$H$16, IF(J154="5", Ward!$I$2:$J$16, IF(J154="6", Ward!$K$2:$L$15, IF(J154="7", Ward!$M$2:$N$11, IF(J154="8", Ward!$O$2:$P$17, IF(J154="9", Ward!$Q$2:$R$14, IF(J154="10", Ward!$S$2:$T$16, IF(J154="11", Ward!$U$2:$V$17, IF(J154="12", Ward!$W$2:$X$12, IF(J154="Bình Chánh", Ward!$Y$2:$Z$17, IF(J154="Bình Tân", Ward!$AA$2:$AB$11, IF(J154="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J154="Cần Giờ", Ward!$AE$2:$AF$8, IF(J154="Củ Chi", Ward!$AG$2:$AH$22, IF(J154="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J154="Hóc Môn", Ward!$AK$2:$AL$13, IF(J154="Nhà Bè", Ward!$AM$2:$AN$8, IF(J154="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J154="Tân Bình", Ward!$AQ$2:$AR$16, IF(J154="Tân Phú", Ward!$AS$2:$AT$12, IF(J154="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8064,7 +8064,7 @@
         <f>IF(J155 &lt;&gt; "", VLOOKUP(J155, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W155" s="28" t="str">
+      <c r="W155" s="23" t="str">
         <f>IF(K155 &lt;&gt; "", VLOOKUP(K155, IF(J155="1", Ward!$A$2:$B$11, IF(J155="2", Ward!$C$2:$D$12, IF(J155="3", Ward!$E$2:$F$15, IF(J155="4", Ward!$G$2:$H$16, IF(J155="5", Ward!$I$2:$J$16, IF(J155="6", Ward!$K$2:$L$15, IF(J155="7", Ward!$M$2:$N$11, IF(J155="8", Ward!$O$2:$P$17, IF(J155="9", Ward!$Q$2:$R$14, IF(J155="10", Ward!$S$2:$T$16, IF(J155="11", Ward!$U$2:$V$17, IF(J155="12", Ward!$W$2:$X$12, IF(J155="Bình Chánh", Ward!$Y$2:$Z$17, IF(J155="Bình Tân", Ward!$AA$2:$AB$11, IF(J155="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J155="Cần Giờ", Ward!$AE$2:$AF$8, IF(J155="Củ Chi", Ward!$AG$2:$AH$22, IF(J155="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J155="Hóc Môn", Ward!$AK$2:$AL$13, IF(J155="Nhà Bè", Ward!$AM$2:$AN$8, IF(J155="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J155="Tân Bình", Ward!$AQ$2:$AR$16, IF(J155="Tân Phú", Ward!$AS$2:$AT$12, IF(J155="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8102,7 +8102,7 @@
         <f>IF(J156 &lt;&gt; "", VLOOKUP(J156, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W156" s="28" t="str">
+      <c r="W156" s="23" t="str">
         <f>IF(K156 &lt;&gt; "", VLOOKUP(K156, IF(J156="1", Ward!$A$2:$B$11, IF(J156="2", Ward!$C$2:$D$12, IF(J156="3", Ward!$E$2:$F$15, IF(J156="4", Ward!$G$2:$H$16, IF(J156="5", Ward!$I$2:$J$16, IF(J156="6", Ward!$K$2:$L$15, IF(J156="7", Ward!$M$2:$N$11, IF(J156="8", Ward!$O$2:$P$17, IF(J156="9", Ward!$Q$2:$R$14, IF(J156="10", Ward!$S$2:$T$16, IF(J156="11", Ward!$U$2:$V$17, IF(J156="12", Ward!$W$2:$X$12, IF(J156="Bình Chánh", Ward!$Y$2:$Z$17, IF(J156="Bình Tân", Ward!$AA$2:$AB$11, IF(J156="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J156="Cần Giờ", Ward!$AE$2:$AF$8, IF(J156="Củ Chi", Ward!$AG$2:$AH$22, IF(J156="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J156="Hóc Môn", Ward!$AK$2:$AL$13, IF(J156="Nhà Bè", Ward!$AM$2:$AN$8, IF(J156="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J156="Tân Bình", Ward!$AQ$2:$AR$16, IF(J156="Tân Phú", Ward!$AS$2:$AT$12, IF(J156="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8140,7 +8140,7 @@
         <f>IF(J157 &lt;&gt; "", VLOOKUP(J157, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W157" s="28" t="str">
+      <c r="W157" s="23" t="str">
         <f>IF(K157 &lt;&gt; "", VLOOKUP(K157, IF(J157="1", Ward!$A$2:$B$11, IF(J157="2", Ward!$C$2:$D$12, IF(J157="3", Ward!$E$2:$F$15, IF(J157="4", Ward!$G$2:$H$16, IF(J157="5", Ward!$I$2:$J$16, IF(J157="6", Ward!$K$2:$L$15, IF(J157="7", Ward!$M$2:$N$11, IF(J157="8", Ward!$O$2:$P$17, IF(J157="9", Ward!$Q$2:$R$14, IF(J157="10", Ward!$S$2:$T$16, IF(J157="11", Ward!$U$2:$V$17, IF(J157="12", Ward!$W$2:$X$12, IF(J157="Bình Chánh", Ward!$Y$2:$Z$17, IF(J157="Bình Tân", Ward!$AA$2:$AB$11, IF(J157="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J157="Cần Giờ", Ward!$AE$2:$AF$8, IF(J157="Củ Chi", Ward!$AG$2:$AH$22, IF(J157="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J157="Hóc Môn", Ward!$AK$2:$AL$13, IF(J157="Nhà Bè", Ward!$AM$2:$AN$8, IF(J157="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J157="Tân Bình", Ward!$AQ$2:$AR$16, IF(J157="Tân Phú", Ward!$AS$2:$AT$12, IF(J157="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8178,7 +8178,7 @@
         <f>IF(J158 &lt;&gt; "", VLOOKUP(J158, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W158" s="28" t="str">
+      <c r="W158" s="23" t="str">
         <f>IF(K158 &lt;&gt; "", VLOOKUP(K158, IF(J158="1", Ward!$A$2:$B$11, IF(J158="2", Ward!$C$2:$D$12, IF(J158="3", Ward!$E$2:$F$15, IF(J158="4", Ward!$G$2:$H$16, IF(J158="5", Ward!$I$2:$J$16, IF(J158="6", Ward!$K$2:$L$15, IF(J158="7", Ward!$M$2:$N$11, IF(J158="8", Ward!$O$2:$P$17, IF(J158="9", Ward!$Q$2:$R$14, IF(J158="10", Ward!$S$2:$T$16, IF(J158="11", Ward!$U$2:$V$17, IF(J158="12", Ward!$W$2:$X$12, IF(J158="Bình Chánh", Ward!$Y$2:$Z$17, IF(J158="Bình Tân", Ward!$AA$2:$AB$11, IF(J158="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J158="Cần Giờ", Ward!$AE$2:$AF$8, IF(J158="Củ Chi", Ward!$AG$2:$AH$22, IF(J158="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J158="Hóc Môn", Ward!$AK$2:$AL$13, IF(J158="Nhà Bè", Ward!$AM$2:$AN$8, IF(J158="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J158="Tân Bình", Ward!$AQ$2:$AR$16, IF(J158="Tân Phú", Ward!$AS$2:$AT$12, IF(J158="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8216,7 +8216,7 @@
         <f>IF(J159 &lt;&gt; "", VLOOKUP(J159, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W159" s="28" t="str">
+      <c r="W159" s="23" t="str">
         <f>IF(K159 &lt;&gt; "", VLOOKUP(K159, IF(J159="1", Ward!$A$2:$B$11, IF(J159="2", Ward!$C$2:$D$12, IF(J159="3", Ward!$E$2:$F$15, IF(J159="4", Ward!$G$2:$H$16, IF(J159="5", Ward!$I$2:$J$16, IF(J159="6", Ward!$K$2:$L$15, IF(J159="7", Ward!$M$2:$N$11, IF(J159="8", Ward!$O$2:$P$17, IF(J159="9", Ward!$Q$2:$R$14, IF(J159="10", Ward!$S$2:$T$16, IF(J159="11", Ward!$U$2:$V$17, IF(J159="12", Ward!$W$2:$X$12, IF(J159="Bình Chánh", Ward!$Y$2:$Z$17, IF(J159="Bình Tân", Ward!$AA$2:$AB$11, IF(J159="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J159="Cần Giờ", Ward!$AE$2:$AF$8, IF(J159="Củ Chi", Ward!$AG$2:$AH$22, IF(J159="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J159="Hóc Môn", Ward!$AK$2:$AL$13, IF(J159="Nhà Bè", Ward!$AM$2:$AN$8, IF(J159="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J159="Tân Bình", Ward!$AQ$2:$AR$16, IF(J159="Tân Phú", Ward!$AS$2:$AT$12, IF(J159="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8254,7 +8254,7 @@
         <f>IF(J160 &lt;&gt; "", VLOOKUP(J160, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W160" s="28" t="str">
+      <c r="W160" s="23" t="str">
         <f>IF(K160 &lt;&gt; "", VLOOKUP(K160, IF(J160="1", Ward!$A$2:$B$11, IF(J160="2", Ward!$C$2:$D$12, IF(J160="3", Ward!$E$2:$F$15, IF(J160="4", Ward!$G$2:$H$16, IF(J160="5", Ward!$I$2:$J$16, IF(J160="6", Ward!$K$2:$L$15, IF(J160="7", Ward!$M$2:$N$11, IF(J160="8", Ward!$O$2:$P$17, IF(J160="9", Ward!$Q$2:$R$14, IF(J160="10", Ward!$S$2:$T$16, IF(J160="11", Ward!$U$2:$V$17, IF(J160="12", Ward!$W$2:$X$12, IF(J160="Bình Chánh", Ward!$Y$2:$Z$17, IF(J160="Bình Tân", Ward!$AA$2:$AB$11, IF(J160="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J160="Cần Giờ", Ward!$AE$2:$AF$8, IF(J160="Củ Chi", Ward!$AG$2:$AH$22, IF(J160="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J160="Hóc Môn", Ward!$AK$2:$AL$13, IF(J160="Nhà Bè", Ward!$AM$2:$AN$8, IF(J160="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J160="Tân Bình", Ward!$AQ$2:$AR$16, IF(J160="Tân Phú", Ward!$AS$2:$AT$12, IF(J160="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8292,7 +8292,7 @@
         <f>IF(J161 &lt;&gt; "", VLOOKUP(J161, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W161" s="28" t="str">
+      <c r="W161" s="23" t="str">
         <f>IF(K161 &lt;&gt; "", VLOOKUP(K161, IF(J161="1", Ward!$A$2:$B$11, IF(J161="2", Ward!$C$2:$D$12, IF(J161="3", Ward!$E$2:$F$15, IF(J161="4", Ward!$G$2:$H$16, IF(J161="5", Ward!$I$2:$J$16, IF(J161="6", Ward!$K$2:$L$15, IF(J161="7", Ward!$M$2:$N$11, IF(J161="8", Ward!$O$2:$P$17, IF(J161="9", Ward!$Q$2:$R$14, IF(J161="10", Ward!$S$2:$T$16, IF(J161="11", Ward!$U$2:$V$17, IF(J161="12", Ward!$W$2:$X$12, IF(J161="Bình Chánh", Ward!$Y$2:$Z$17, IF(J161="Bình Tân", Ward!$AA$2:$AB$11, IF(J161="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J161="Cần Giờ", Ward!$AE$2:$AF$8, IF(J161="Củ Chi", Ward!$AG$2:$AH$22, IF(J161="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J161="Hóc Môn", Ward!$AK$2:$AL$13, IF(J161="Nhà Bè", Ward!$AM$2:$AN$8, IF(J161="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J161="Tân Bình", Ward!$AQ$2:$AR$16, IF(J161="Tân Phú", Ward!$AS$2:$AT$12, IF(J161="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8330,7 +8330,7 @@
         <f>IF(J162 &lt;&gt; "", VLOOKUP(J162, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W162" s="28" t="str">
+      <c r="W162" s="23" t="str">
         <f>IF(K162 &lt;&gt; "", VLOOKUP(K162, IF(J162="1", Ward!$A$2:$B$11, IF(J162="2", Ward!$C$2:$D$12, IF(J162="3", Ward!$E$2:$F$15, IF(J162="4", Ward!$G$2:$H$16, IF(J162="5", Ward!$I$2:$J$16, IF(J162="6", Ward!$K$2:$L$15, IF(J162="7", Ward!$M$2:$N$11, IF(J162="8", Ward!$O$2:$P$17, IF(J162="9", Ward!$Q$2:$R$14, IF(J162="10", Ward!$S$2:$T$16, IF(J162="11", Ward!$U$2:$V$17, IF(J162="12", Ward!$W$2:$X$12, IF(J162="Bình Chánh", Ward!$Y$2:$Z$17, IF(J162="Bình Tân", Ward!$AA$2:$AB$11, IF(J162="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J162="Cần Giờ", Ward!$AE$2:$AF$8, IF(J162="Củ Chi", Ward!$AG$2:$AH$22, IF(J162="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J162="Hóc Môn", Ward!$AK$2:$AL$13, IF(J162="Nhà Bè", Ward!$AM$2:$AN$8, IF(J162="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J162="Tân Bình", Ward!$AQ$2:$AR$16, IF(J162="Tân Phú", Ward!$AS$2:$AT$12, IF(J162="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8368,7 +8368,7 @@
         <f>IF(J163 &lt;&gt; "", VLOOKUP(J163, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W163" s="28" t="str">
+      <c r="W163" s="23" t="str">
         <f>IF(K163 &lt;&gt; "", VLOOKUP(K163, IF(J163="1", Ward!$A$2:$B$11, IF(J163="2", Ward!$C$2:$D$12, IF(J163="3", Ward!$E$2:$F$15, IF(J163="4", Ward!$G$2:$H$16, IF(J163="5", Ward!$I$2:$J$16, IF(J163="6", Ward!$K$2:$L$15, IF(J163="7", Ward!$M$2:$N$11, IF(J163="8", Ward!$O$2:$P$17, IF(J163="9", Ward!$Q$2:$R$14, IF(J163="10", Ward!$S$2:$T$16, IF(J163="11", Ward!$U$2:$V$17, IF(J163="12", Ward!$W$2:$X$12, IF(J163="Bình Chánh", Ward!$Y$2:$Z$17, IF(J163="Bình Tân", Ward!$AA$2:$AB$11, IF(J163="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J163="Cần Giờ", Ward!$AE$2:$AF$8, IF(J163="Củ Chi", Ward!$AG$2:$AH$22, IF(J163="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J163="Hóc Môn", Ward!$AK$2:$AL$13, IF(J163="Nhà Bè", Ward!$AM$2:$AN$8, IF(J163="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J163="Tân Bình", Ward!$AQ$2:$AR$16, IF(J163="Tân Phú", Ward!$AS$2:$AT$12, IF(J163="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8406,7 +8406,7 @@
         <f>IF(J164 &lt;&gt; "", VLOOKUP(J164, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W164" s="28" t="str">
+      <c r="W164" s="23" t="str">
         <f>IF(K164 &lt;&gt; "", VLOOKUP(K164, IF(J164="1", Ward!$A$2:$B$11, IF(J164="2", Ward!$C$2:$D$12, IF(J164="3", Ward!$E$2:$F$15, IF(J164="4", Ward!$G$2:$H$16, IF(J164="5", Ward!$I$2:$J$16, IF(J164="6", Ward!$K$2:$L$15, IF(J164="7", Ward!$M$2:$N$11, IF(J164="8", Ward!$O$2:$P$17, IF(J164="9", Ward!$Q$2:$R$14, IF(J164="10", Ward!$S$2:$T$16, IF(J164="11", Ward!$U$2:$V$17, IF(J164="12", Ward!$W$2:$X$12, IF(J164="Bình Chánh", Ward!$Y$2:$Z$17, IF(J164="Bình Tân", Ward!$AA$2:$AB$11, IF(J164="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J164="Cần Giờ", Ward!$AE$2:$AF$8, IF(J164="Củ Chi", Ward!$AG$2:$AH$22, IF(J164="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J164="Hóc Môn", Ward!$AK$2:$AL$13, IF(J164="Nhà Bè", Ward!$AM$2:$AN$8, IF(J164="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J164="Tân Bình", Ward!$AQ$2:$AR$16, IF(J164="Tân Phú", Ward!$AS$2:$AT$12, IF(J164="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8444,7 +8444,7 @@
         <f>IF(J165 &lt;&gt; "", VLOOKUP(J165, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W165" s="28" t="str">
+      <c r="W165" s="23" t="str">
         <f>IF(K165 &lt;&gt; "", VLOOKUP(K165, IF(J165="1", Ward!$A$2:$B$11, IF(J165="2", Ward!$C$2:$D$12, IF(J165="3", Ward!$E$2:$F$15, IF(J165="4", Ward!$G$2:$H$16, IF(J165="5", Ward!$I$2:$J$16, IF(J165="6", Ward!$K$2:$L$15, IF(J165="7", Ward!$M$2:$N$11, IF(J165="8", Ward!$O$2:$P$17, IF(J165="9", Ward!$Q$2:$R$14, IF(J165="10", Ward!$S$2:$T$16, IF(J165="11", Ward!$U$2:$V$17, IF(J165="12", Ward!$W$2:$X$12, IF(J165="Bình Chánh", Ward!$Y$2:$Z$17, IF(J165="Bình Tân", Ward!$AA$2:$AB$11, IF(J165="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J165="Cần Giờ", Ward!$AE$2:$AF$8, IF(J165="Củ Chi", Ward!$AG$2:$AH$22, IF(J165="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J165="Hóc Môn", Ward!$AK$2:$AL$13, IF(J165="Nhà Bè", Ward!$AM$2:$AN$8, IF(J165="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J165="Tân Bình", Ward!$AQ$2:$AR$16, IF(J165="Tân Phú", Ward!$AS$2:$AT$12, IF(J165="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8482,7 +8482,7 @@
         <f>IF(J166 &lt;&gt; "", VLOOKUP(J166, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W166" s="28" t="str">
+      <c r="W166" s="23" t="str">
         <f>IF(K166 &lt;&gt; "", VLOOKUP(K166, IF(J166="1", Ward!$A$2:$B$11, IF(J166="2", Ward!$C$2:$D$12, IF(J166="3", Ward!$E$2:$F$15, IF(J166="4", Ward!$G$2:$H$16, IF(J166="5", Ward!$I$2:$J$16, IF(J166="6", Ward!$K$2:$L$15, IF(J166="7", Ward!$M$2:$N$11, IF(J166="8", Ward!$O$2:$P$17, IF(J166="9", Ward!$Q$2:$R$14, IF(J166="10", Ward!$S$2:$T$16, IF(J166="11", Ward!$U$2:$V$17, IF(J166="12", Ward!$W$2:$X$12, IF(J166="Bình Chánh", Ward!$Y$2:$Z$17, IF(J166="Bình Tân", Ward!$AA$2:$AB$11, IF(J166="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J166="Cần Giờ", Ward!$AE$2:$AF$8, IF(J166="Củ Chi", Ward!$AG$2:$AH$22, IF(J166="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J166="Hóc Môn", Ward!$AK$2:$AL$13, IF(J166="Nhà Bè", Ward!$AM$2:$AN$8, IF(J166="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J166="Tân Bình", Ward!$AQ$2:$AR$16, IF(J166="Tân Phú", Ward!$AS$2:$AT$12, IF(J166="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8520,7 +8520,7 @@
         <f>IF(J167 &lt;&gt; "", VLOOKUP(J167, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W167" s="28" t="str">
+      <c r="W167" s="23" t="str">
         <f>IF(K167 &lt;&gt; "", VLOOKUP(K167, IF(J167="1", Ward!$A$2:$B$11, IF(J167="2", Ward!$C$2:$D$12, IF(J167="3", Ward!$E$2:$F$15, IF(J167="4", Ward!$G$2:$H$16, IF(J167="5", Ward!$I$2:$J$16, IF(J167="6", Ward!$K$2:$L$15, IF(J167="7", Ward!$M$2:$N$11, IF(J167="8", Ward!$O$2:$P$17, IF(J167="9", Ward!$Q$2:$R$14, IF(J167="10", Ward!$S$2:$T$16, IF(J167="11", Ward!$U$2:$V$17, IF(J167="12", Ward!$W$2:$X$12, IF(J167="Bình Chánh", Ward!$Y$2:$Z$17, IF(J167="Bình Tân", Ward!$AA$2:$AB$11, IF(J167="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J167="Cần Giờ", Ward!$AE$2:$AF$8, IF(J167="Củ Chi", Ward!$AG$2:$AH$22, IF(J167="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J167="Hóc Môn", Ward!$AK$2:$AL$13, IF(J167="Nhà Bè", Ward!$AM$2:$AN$8, IF(J167="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J167="Tân Bình", Ward!$AQ$2:$AR$16, IF(J167="Tân Phú", Ward!$AS$2:$AT$12, IF(J167="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8558,7 +8558,7 @@
         <f>IF(J168 &lt;&gt; "", VLOOKUP(J168, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W168" s="28" t="str">
+      <c r="W168" s="23" t="str">
         <f>IF(K168 &lt;&gt; "", VLOOKUP(K168, IF(J168="1", Ward!$A$2:$B$11, IF(J168="2", Ward!$C$2:$D$12, IF(J168="3", Ward!$E$2:$F$15, IF(J168="4", Ward!$G$2:$H$16, IF(J168="5", Ward!$I$2:$J$16, IF(J168="6", Ward!$K$2:$L$15, IF(J168="7", Ward!$M$2:$N$11, IF(J168="8", Ward!$O$2:$P$17, IF(J168="9", Ward!$Q$2:$R$14, IF(J168="10", Ward!$S$2:$T$16, IF(J168="11", Ward!$U$2:$V$17, IF(J168="12", Ward!$W$2:$X$12, IF(J168="Bình Chánh", Ward!$Y$2:$Z$17, IF(J168="Bình Tân", Ward!$AA$2:$AB$11, IF(J168="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J168="Cần Giờ", Ward!$AE$2:$AF$8, IF(J168="Củ Chi", Ward!$AG$2:$AH$22, IF(J168="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J168="Hóc Môn", Ward!$AK$2:$AL$13, IF(J168="Nhà Bè", Ward!$AM$2:$AN$8, IF(J168="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J168="Tân Bình", Ward!$AQ$2:$AR$16, IF(J168="Tân Phú", Ward!$AS$2:$AT$12, IF(J168="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8596,7 +8596,7 @@
         <f>IF(J169 &lt;&gt; "", VLOOKUP(J169, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W169" s="28" t="str">
+      <c r="W169" s="23" t="str">
         <f>IF(K169 &lt;&gt; "", VLOOKUP(K169, IF(J169="1", Ward!$A$2:$B$11, IF(J169="2", Ward!$C$2:$D$12, IF(J169="3", Ward!$E$2:$F$15, IF(J169="4", Ward!$G$2:$H$16, IF(J169="5", Ward!$I$2:$J$16, IF(J169="6", Ward!$K$2:$L$15, IF(J169="7", Ward!$M$2:$N$11, IF(J169="8", Ward!$O$2:$P$17, IF(J169="9", Ward!$Q$2:$R$14, IF(J169="10", Ward!$S$2:$T$16, IF(J169="11", Ward!$U$2:$V$17, IF(J169="12", Ward!$W$2:$X$12, IF(J169="Bình Chánh", Ward!$Y$2:$Z$17, IF(J169="Bình Tân", Ward!$AA$2:$AB$11, IF(J169="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J169="Cần Giờ", Ward!$AE$2:$AF$8, IF(J169="Củ Chi", Ward!$AG$2:$AH$22, IF(J169="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J169="Hóc Môn", Ward!$AK$2:$AL$13, IF(J169="Nhà Bè", Ward!$AM$2:$AN$8, IF(J169="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J169="Tân Bình", Ward!$AQ$2:$AR$16, IF(J169="Tân Phú", Ward!$AS$2:$AT$12, IF(J169="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8634,7 +8634,7 @@
         <f>IF(J170 &lt;&gt; "", VLOOKUP(J170, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W170" s="28" t="str">
+      <c r="W170" s="23" t="str">
         <f>IF(K170 &lt;&gt; "", VLOOKUP(K170, IF(J170="1", Ward!$A$2:$B$11, IF(J170="2", Ward!$C$2:$D$12, IF(J170="3", Ward!$E$2:$F$15, IF(J170="4", Ward!$G$2:$H$16, IF(J170="5", Ward!$I$2:$J$16, IF(J170="6", Ward!$K$2:$L$15, IF(J170="7", Ward!$M$2:$N$11, IF(J170="8", Ward!$O$2:$P$17, IF(J170="9", Ward!$Q$2:$R$14, IF(J170="10", Ward!$S$2:$T$16, IF(J170="11", Ward!$U$2:$V$17, IF(J170="12", Ward!$W$2:$X$12, IF(J170="Bình Chánh", Ward!$Y$2:$Z$17, IF(J170="Bình Tân", Ward!$AA$2:$AB$11, IF(J170="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J170="Cần Giờ", Ward!$AE$2:$AF$8, IF(J170="Củ Chi", Ward!$AG$2:$AH$22, IF(J170="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J170="Hóc Môn", Ward!$AK$2:$AL$13, IF(J170="Nhà Bè", Ward!$AM$2:$AN$8, IF(J170="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J170="Tân Bình", Ward!$AQ$2:$AR$16, IF(J170="Tân Phú", Ward!$AS$2:$AT$12, IF(J170="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8672,7 +8672,7 @@
         <f>IF(J171 &lt;&gt; "", VLOOKUP(J171, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W171" s="28" t="str">
+      <c r="W171" s="23" t="str">
         <f>IF(K171 &lt;&gt; "", VLOOKUP(K171, IF(J171="1", Ward!$A$2:$B$11, IF(J171="2", Ward!$C$2:$D$12, IF(J171="3", Ward!$E$2:$F$15, IF(J171="4", Ward!$G$2:$H$16, IF(J171="5", Ward!$I$2:$J$16, IF(J171="6", Ward!$K$2:$L$15, IF(J171="7", Ward!$M$2:$N$11, IF(J171="8", Ward!$O$2:$P$17, IF(J171="9", Ward!$Q$2:$R$14, IF(J171="10", Ward!$S$2:$T$16, IF(J171="11", Ward!$U$2:$V$17, IF(J171="12", Ward!$W$2:$X$12, IF(J171="Bình Chánh", Ward!$Y$2:$Z$17, IF(J171="Bình Tân", Ward!$AA$2:$AB$11, IF(J171="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J171="Cần Giờ", Ward!$AE$2:$AF$8, IF(J171="Củ Chi", Ward!$AG$2:$AH$22, IF(J171="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J171="Hóc Môn", Ward!$AK$2:$AL$13, IF(J171="Nhà Bè", Ward!$AM$2:$AN$8, IF(J171="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J171="Tân Bình", Ward!$AQ$2:$AR$16, IF(J171="Tân Phú", Ward!$AS$2:$AT$12, IF(J171="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8710,7 +8710,7 @@
         <f>IF(J172 &lt;&gt; "", VLOOKUP(J172, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W172" s="28" t="str">
+      <c r="W172" s="23" t="str">
         <f>IF(K172 &lt;&gt; "", VLOOKUP(K172, IF(J172="1", Ward!$A$2:$B$11, IF(J172="2", Ward!$C$2:$D$12, IF(J172="3", Ward!$E$2:$F$15, IF(J172="4", Ward!$G$2:$H$16, IF(J172="5", Ward!$I$2:$J$16, IF(J172="6", Ward!$K$2:$L$15, IF(J172="7", Ward!$M$2:$N$11, IF(J172="8", Ward!$O$2:$P$17, IF(J172="9", Ward!$Q$2:$R$14, IF(J172="10", Ward!$S$2:$T$16, IF(J172="11", Ward!$U$2:$V$17, IF(J172="12", Ward!$W$2:$X$12, IF(J172="Bình Chánh", Ward!$Y$2:$Z$17, IF(J172="Bình Tân", Ward!$AA$2:$AB$11, IF(J172="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J172="Cần Giờ", Ward!$AE$2:$AF$8, IF(J172="Củ Chi", Ward!$AG$2:$AH$22, IF(J172="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J172="Hóc Môn", Ward!$AK$2:$AL$13, IF(J172="Nhà Bè", Ward!$AM$2:$AN$8, IF(J172="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J172="Tân Bình", Ward!$AQ$2:$AR$16, IF(J172="Tân Phú", Ward!$AS$2:$AT$12, IF(J172="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8748,7 +8748,7 @@
         <f>IF(J173 &lt;&gt; "", VLOOKUP(J173, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W173" s="28" t="str">
+      <c r="W173" s="23" t="str">
         <f>IF(K173 &lt;&gt; "", VLOOKUP(K173, IF(J173="1", Ward!$A$2:$B$11, IF(J173="2", Ward!$C$2:$D$12, IF(J173="3", Ward!$E$2:$F$15, IF(J173="4", Ward!$G$2:$H$16, IF(J173="5", Ward!$I$2:$J$16, IF(J173="6", Ward!$K$2:$L$15, IF(J173="7", Ward!$M$2:$N$11, IF(J173="8", Ward!$O$2:$P$17, IF(J173="9", Ward!$Q$2:$R$14, IF(J173="10", Ward!$S$2:$T$16, IF(J173="11", Ward!$U$2:$V$17, IF(J173="12", Ward!$W$2:$X$12, IF(J173="Bình Chánh", Ward!$Y$2:$Z$17, IF(J173="Bình Tân", Ward!$AA$2:$AB$11, IF(J173="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J173="Cần Giờ", Ward!$AE$2:$AF$8, IF(J173="Củ Chi", Ward!$AG$2:$AH$22, IF(J173="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J173="Hóc Môn", Ward!$AK$2:$AL$13, IF(J173="Nhà Bè", Ward!$AM$2:$AN$8, IF(J173="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J173="Tân Bình", Ward!$AQ$2:$AR$16, IF(J173="Tân Phú", Ward!$AS$2:$AT$12, IF(J173="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8786,7 +8786,7 @@
         <f>IF(J174 &lt;&gt; "", VLOOKUP(J174, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W174" s="28" t="str">
+      <c r="W174" s="23" t="str">
         <f>IF(K174 &lt;&gt; "", VLOOKUP(K174, IF(J174="1", Ward!$A$2:$B$11, IF(J174="2", Ward!$C$2:$D$12, IF(J174="3", Ward!$E$2:$F$15, IF(J174="4", Ward!$G$2:$H$16, IF(J174="5", Ward!$I$2:$J$16, IF(J174="6", Ward!$K$2:$L$15, IF(J174="7", Ward!$M$2:$N$11, IF(J174="8", Ward!$O$2:$P$17, IF(J174="9", Ward!$Q$2:$R$14, IF(J174="10", Ward!$S$2:$T$16, IF(J174="11", Ward!$U$2:$V$17, IF(J174="12", Ward!$W$2:$X$12, IF(J174="Bình Chánh", Ward!$Y$2:$Z$17, IF(J174="Bình Tân", Ward!$AA$2:$AB$11, IF(J174="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J174="Cần Giờ", Ward!$AE$2:$AF$8, IF(J174="Củ Chi", Ward!$AG$2:$AH$22, IF(J174="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J174="Hóc Môn", Ward!$AK$2:$AL$13, IF(J174="Nhà Bè", Ward!$AM$2:$AN$8, IF(J174="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J174="Tân Bình", Ward!$AQ$2:$AR$16, IF(J174="Tân Phú", Ward!$AS$2:$AT$12, IF(J174="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8824,7 +8824,7 @@
         <f>IF(J175 &lt;&gt; "", VLOOKUP(J175, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W175" s="28" t="str">
+      <c r="W175" s="23" t="str">
         <f>IF(K175 &lt;&gt; "", VLOOKUP(K175, IF(J175="1", Ward!$A$2:$B$11, IF(J175="2", Ward!$C$2:$D$12, IF(J175="3", Ward!$E$2:$F$15, IF(J175="4", Ward!$G$2:$H$16, IF(J175="5", Ward!$I$2:$J$16, IF(J175="6", Ward!$K$2:$L$15, IF(J175="7", Ward!$M$2:$N$11, IF(J175="8", Ward!$O$2:$P$17, IF(J175="9", Ward!$Q$2:$R$14, IF(J175="10", Ward!$S$2:$T$16, IF(J175="11", Ward!$U$2:$V$17, IF(J175="12", Ward!$W$2:$X$12, IF(J175="Bình Chánh", Ward!$Y$2:$Z$17, IF(J175="Bình Tân", Ward!$AA$2:$AB$11, IF(J175="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J175="Cần Giờ", Ward!$AE$2:$AF$8, IF(J175="Củ Chi", Ward!$AG$2:$AH$22, IF(J175="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J175="Hóc Môn", Ward!$AK$2:$AL$13, IF(J175="Nhà Bè", Ward!$AM$2:$AN$8, IF(J175="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J175="Tân Bình", Ward!$AQ$2:$AR$16, IF(J175="Tân Phú", Ward!$AS$2:$AT$12, IF(J175="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8862,7 +8862,7 @@
         <f>IF(J176 &lt;&gt; "", VLOOKUP(J176, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W176" s="28" t="str">
+      <c r="W176" s="23" t="str">
         <f>IF(K176 &lt;&gt; "", VLOOKUP(K176, IF(J176="1", Ward!$A$2:$B$11, IF(J176="2", Ward!$C$2:$D$12, IF(J176="3", Ward!$E$2:$F$15, IF(J176="4", Ward!$G$2:$H$16, IF(J176="5", Ward!$I$2:$J$16, IF(J176="6", Ward!$K$2:$L$15, IF(J176="7", Ward!$M$2:$N$11, IF(J176="8", Ward!$O$2:$P$17, IF(J176="9", Ward!$Q$2:$R$14, IF(J176="10", Ward!$S$2:$T$16, IF(J176="11", Ward!$U$2:$V$17, IF(J176="12", Ward!$W$2:$X$12, IF(J176="Bình Chánh", Ward!$Y$2:$Z$17, IF(J176="Bình Tân", Ward!$AA$2:$AB$11, IF(J176="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J176="Cần Giờ", Ward!$AE$2:$AF$8, IF(J176="Củ Chi", Ward!$AG$2:$AH$22, IF(J176="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J176="Hóc Môn", Ward!$AK$2:$AL$13, IF(J176="Nhà Bè", Ward!$AM$2:$AN$8, IF(J176="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J176="Tân Bình", Ward!$AQ$2:$AR$16, IF(J176="Tân Phú", Ward!$AS$2:$AT$12, IF(J176="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8900,7 +8900,7 @@
         <f>IF(J177 &lt;&gt; "", VLOOKUP(J177, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W177" s="28" t="str">
+      <c r="W177" s="23" t="str">
         <f>IF(K177 &lt;&gt; "", VLOOKUP(K177, IF(J177="1", Ward!$A$2:$B$11, IF(J177="2", Ward!$C$2:$D$12, IF(J177="3", Ward!$E$2:$F$15, IF(J177="4", Ward!$G$2:$H$16, IF(J177="5", Ward!$I$2:$J$16, IF(J177="6", Ward!$K$2:$L$15, IF(J177="7", Ward!$M$2:$N$11, IF(J177="8", Ward!$O$2:$P$17, IF(J177="9", Ward!$Q$2:$R$14, IF(J177="10", Ward!$S$2:$T$16, IF(J177="11", Ward!$U$2:$V$17, IF(J177="12", Ward!$W$2:$X$12, IF(J177="Bình Chánh", Ward!$Y$2:$Z$17, IF(J177="Bình Tân", Ward!$AA$2:$AB$11, IF(J177="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J177="Cần Giờ", Ward!$AE$2:$AF$8, IF(J177="Củ Chi", Ward!$AG$2:$AH$22, IF(J177="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J177="Hóc Môn", Ward!$AK$2:$AL$13, IF(J177="Nhà Bè", Ward!$AM$2:$AN$8, IF(J177="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J177="Tân Bình", Ward!$AQ$2:$AR$16, IF(J177="Tân Phú", Ward!$AS$2:$AT$12, IF(J177="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8938,7 +8938,7 @@
         <f>IF(J178 &lt;&gt; "", VLOOKUP(J178, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W178" s="28" t="str">
+      <c r="W178" s="23" t="str">
         <f>IF(K178 &lt;&gt; "", VLOOKUP(K178, IF(J178="1", Ward!$A$2:$B$11, IF(J178="2", Ward!$C$2:$D$12, IF(J178="3", Ward!$E$2:$F$15, IF(J178="4", Ward!$G$2:$H$16, IF(J178="5", Ward!$I$2:$J$16, IF(J178="6", Ward!$K$2:$L$15, IF(J178="7", Ward!$M$2:$N$11, IF(J178="8", Ward!$O$2:$P$17, IF(J178="9", Ward!$Q$2:$R$14, IF(J178="10", Ward!$S$2:$T$16, IF(J178="11", Ward!$U$2:$V$17, IF(J178="12", Ward!$W$2:$X$12, IF(J178="Bình Chánh", Ward!$Y$2:$Z$17, IF(J178="Bình Tân", Ward!$AA$2:$AB$11, IF(J178="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J178="Cần Giờ", Ward!$AE$2:$AF$8, IF(J178="Củ Chi", Ward!$AG$2:$AH$22, IF(J178="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J178="Hóc Môn", Ward!$AK$2:$AL$13, IF(J178="Nhà Bè", Ward!$AM$2:$AN$8, IF(J178="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J178="Tân Bình", Ward!$AQ$2:$AR$16, IF(J178="Tân Phú", Ward!$AS$2:$AT$12, IF(J178="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -8976,7 +8976,7 @@
         <f>IF(J179 &lt;&gt; "", VLOOKUP(J179, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W179" s="28" t="str">
+      <c r="W179" s="23" t="str">
         <f>IF(K179 &lt;&gt; "", VLOOKUP(K179, IF(J179="1", Ward!$A$2:$B$11, IF(J179="2", Ward!$C$2:$D$12, IF(J179="3", Ward!$E$2:$F$15, IF(J179="4", Ward!$G$2:$H$16, IF(J179="5", Ward!$I$2:$J$16, IF(J179="6", Ward!$K$2:$L$15, IF(J179="7", Ward!$M$2:$N$11, IF(J179="8", Ward!$O$2:$P$17, IF(J179="9", Ward!$Q$2:$R$14, IF(J179="10", Ward!$S$2:$T$16, IF(J179="11", Ward!$U$2:$V$17, IF(J179="12", Ward!$W$2:$X$12, IF(J179="Bình Chánh", Ward!$Y$2:$Z$17, IF(J179="Bình Tân", Ward!$AA$2:$AB$11, IF(J179="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J179="Cần Giờ", Ward!$AE$2:$AF$8, IF(J179="Củ Chi", Ward!$AG$2:$AH$22, IF(J179="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J179="Hóc Môn", Ward!$AK$2:$AL$13, IF(J179="Nhà Bè", Ward!$AM$2:$AN$8, IF(J179="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J179="Tân Bình", Ward!$AQ$2:$AR$16, IF(J179="Tân Phú", Ward!$AS$2:$AT$12, IF(J179="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9014,7 +9014,7 @@
         <f>IF(J180 &lt;&gt; "", VLOOKUP(J180, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W180" s="28" t="str">
+      <c r="W180" s="23" t="str">
         <f>IF(K180 &lt;&gt; "", VLOOKUP(K180, IF(J180="1", Ward!$A$2:$B$11, IF(J180="2", Ward!$C$2:$D$12, IF(J180="3", Ward!$E$2:$F$15, IF(J180="4", Ward!$G$2:$H$16, IF(J180="5", Ward!$I$2:$J$16, IF(J180="6", Ward!$K$2:$L$15, IF(J180="7", Ward!$M$2:$N$11, IF(J180="8", Ward!$O$2:$P$17, IF(J180="9", Ward!$Q$2:$R$14, IF(J180="10", Ward!$S$2:$T$16, IF(J180="11", Ward!$U$2:$V$17, IF(J180="12", Ward!$W$2:$X$12, IF(J180="Bình Chánh", Ward!$Y$2:$Z$17, IF(J180="Bình Tân", Ward!$AA$2:$AB$11, IF(J180="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J180="Cần Giờ", Ward!$AE$2:$AF$8, IF(J180="Củ Chi", Ward!$AG$2:$AH$22, IF(J180="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J180="Hóc Môn", Ward!$AK$2:$AL$13, IF(J180="Nhà Bè", Ward!$AM$2:$AN$8, IF(J180="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J180="Tân Bình", Ward!$AQ$2:$AR$16, IF(J180="Tân Phú", Ward!$AS$2:$AT$12, IF(J180="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9052,7 +9052,7 @@
         <f>IF(J181 &lt;&gt; "", VLOOKUP(J181, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W181" s="28" t="str">
+      <c r="W181" s="23" t="str">
         <f>IF(K181 &lt;&gt; "", VLOOKUP(K181, IF(J181="1", Ward!$A$2:$B$11, IF(J181="2", Ward!$C$2:$D$12, IF(J181="3", Ward!$E$2:$F$15, IF(J181="4", Ward!$G$2:$H$16, IF(J181="5", Ward!$I$2:$J$16, IF(J181="6", Ward!$K$2:$L$15, IF(J181="7", Ward!$M$2:$N$11, IF(J181="8", Ward!$O$2:$P$17, IF(J181="9", Ward!$Q$2:$R$14, IF(J181="10", Ward!$S$2:$T$16, IF(J181="11", Ward!$U$2:$V$17, IF(J181="12", Ward!$W$2:$X$12, IF(J181="Bình Chánh", Ward!$Y$2:$Z$17, IF(J181="Bình Tân", Ward!$AA$2:$AB$11, IF(J181="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J181="Cần Giờ", Ward!$AE$2:$AF$8, IF(J181="Củ Chi", Ward!$AG$2:$AH$22, IF(J181="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J181="Hóc Môn", Ward!$AK$2:$AL$13, IF(J181="Nhà Bè", Ward!$AM$2:$AN$8, IF(J181="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J181="Tân Bình", Ward!$AQ$2:$AR$16, IF(J181="Tân Phú", Ward!$AS$2:$AT$12, IF(J181="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9090,7 +9090,7 @@
         <f>IF(J182 &lt;&gt; "", VLOOKUP(J182, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W182" s="28" t="str">
+      <c r="W182" s="23" t="str">
         <f>IF(K182 &lt;&gt; "", VLOOKUP(K182, IF(J182="1", Ward!$A$2:$B$11, IF(J182="2", Ward!$C$2:$D$12, IF(J182="3", Ward!$E$2:$F$15, IF(J182="4", Ward!$G$2:$H$16, IF(J182="5", Ward!$I$2:$J$16, IF(J182="6", Ward!$K$2:$L$15, IF(J182="7", Ward!$M$2:$N$11, IF(J182="8", Ward!$O$2:$P$17, IF(J182="9", Ward!$Q$2:$R$14, IF(J182="10", Ward!$S$2:$T$16, IF(J182="11", Ward!$U$2:$V$17, IF(J182="12", Ward!$W$2:$X$12, IF(J182="Bình Chánh", Ward!$Y$2:$Z$17, IF(J182="Bình Tân", Ward!$AA$2:$AB$11, IF(J182="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J182="Cần Giờ", Ward!$AE$2:$AF$8, IF(J182="Củ Chi", Ward!$AG$2:$AH$22, IF(J182="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J182="Hóc Môn", Ward!$AK$2:$AL$13, IF(J182="Nhà Bè", Ward!$AM$2:$AN$8, IF(J182="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J182="Tân Bình", Ward!$AQ$2:$AR$16, IF(J182="Tân Phú", Ward!$AS$2:$AT$12, IF(J182="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9128,7 +9128,7 @@
         <f>IF(J183 &lt;&gt; "", VLOOKUP(J183, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W183" s="28" t="str">
+      <c r="W183" s="23" t="str">
         <f>IF(K183 &lt;&gt; "", VLOOKUP(K183, IF(J183="1", Ward!$A$2:$B$11, IF(J183="2", Ward!$C$2:$D$12, IF(J183="3", Ward!$E$2:$F$15, IF(J183="4", Ward!$G$2:$H$16, IF(J183="5", Ward!$I$2:$J$16, IF(J183="6", Ward!$K$2:$L$15, IF(J183="7", Ward!$M$2:$N$11, IF(J183="8", Ward!$O$2:$P$17, IF(J183="9", Ward!$Q$2:$R$14, IF(J183="10", Ward!$S$2:$T$16, IF(J183="11", Ward!$U$2:$V$17, IF(J183="12", Ward!$W$2:$X$12, IF(J183="Bình Chánh", Ward!$Y$2:$Z$17, IF(J183="Bình Tân", Ward!$AA$2:$AB$11, IF(J183="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J183="Cần Giờ", Ward!$AE$2:$AF$8, IF(J183="Củ Chi", Ward!$AG$2:$AH$22, IF(J183="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J183="Hóc Môn", Ward!$AK$2:$AL$13, IF(J183="Nhà Bè", Ward!$AM$2:$AN$8, IF(J183="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J183="Tân Bình", Ward!$AQ$2:$AR$16, IF(J183="Tân Phú", Ward!$AS$2:$AT$12, IF(J183="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9166,7 +9166,7 @@
         <f>IF(J184 &lt;&gt; "", VLOOKUP(J184, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W184" s="28" t="str">
+      <c r="W184" s="23" t="str">
         <f>IF(K184 &lt;&gt; "", VLOOKUP(K184, IF(J184="1", Ward!$A$2:$B$11, IF(J184="2", Ward!$C$2:$D$12, IF(J184="3", Ward!$E$2:$F$15, IF(J184="4", Ward!$G$2:$H$16, IF(J184="5", Ward!$I$2:$J$16, IF(J184="6", Ward!$K$2:$L$15, IF(J184="7", Ward!$M$2:$N$11, IF(J184="8", Ward!$O$2:$P$17, IF(J184="9", Ward!$Q$2:$R$14, IF(J184="10", Ward!$S$2:$T$16, IF(J184="11", Ward!$U$2:$V$17, IF(J184="12", Ward!$W$2:$X$12, IF(J184="Bình Chánh", Ward!$Y$2:$Z$17, IF(J184="Bình Tân", Ward!$AA$2:$AB$11, IF(J184="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J184="Cần Giờ", Ward!$AE$2:$AF$8, IF(J184="Củ Chi", Ward!$AG$2:$AH$22, IF(J184="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J184="Hóc Môn", Ward!$AK$2:$AL$13, IF(J184="Nhà Bè", Ward!$AM$2:$AN$8, IF(J184="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J184="Tân Bình", Ward!$AQ$2:$AR$16, IF(J184="Tân Phú", Ward!$AS$2:$AT$12, IF(J184="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9204,7 +9204,7 @@
         <f>IF(J185 &lt;&gt; "", VLOOKUP(J185, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W185" s="28" t="str">
+      <c r="W185" s="23" t="str">
         <f>IF(K185 &lt;&gt; "", VLOOKUP(K185, IF(J185="1", Ward!$A$2:$B$11, IF(J185="2", Ward!$C$2:$D$12, IF(J185="3", Ward!$E$2:$F$15, IF(J185="4", Ward!$G$2:$H$16, IF(J185="5", Ward!$I$2:$J$16, IF(J185="6", Ward!$K$2:$L$15, IF(J185="7", Ward!$M$2:$N$11, IF(J185="8", Ward!$O$2:$P$17, IF(J185="9", Ward!$Q$2:$R$14, IF(J185="10", Ward!$S$2:$T$16, IF(J185="11", Ward!$U$2:$V$17, IF(J185="12", Ward!$W$2:$X$12, IF(J185="Bình Chánh", Ward!$Y$2:$Z$17, IF(J185="Bình Tân", Ward!$AA$2:$AB$11, IF(J185="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J185="Cần Giờ", Ward!$AE$2:$AF$8, IF(J185="Củ Chi", Ward!$AG$2:$AH$22, IF(J185="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J185="Hóc Môn", Ward!$AK$2:$AL$13, IF(J185="Nhà Bè", Ward!$AM$2:$AN$8, IF(J185="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J185="Tân Bình", Ward!$AQ$2:$AR$16, IF(J185="Tân Phú", Ward!$AS$2:$AT$12, IF(J185="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9242,7 +9242,7 @@
         <f>IF(J186 &lt;&gt; "", VLOOKUP(J186, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W186" s="28" t="str">
+      <c r="W186" s="23" t="str">
         <f>IF(K186 &lt;&gt; "", VLOOKUP(K186, IF(J186="1", Ward!$A$2:$B$11, IF(J186="2", Ward!$C$2:$D$12, IF(J186="3", Ward!$E$2:$F$15, IF(J186="4", Ward!$G$2:$H$16, IF(J186="5", Ward!$I$2:$J$16, IF(J186="6", Ward!$K$2:$L$15, IF(J186="7", Ward!$M$2:$N$11, IF(J186="8", Ward!$O$2:$P$17, IF(J186="9", Ward!$Q$2:$R$14, IF(J186="10", Ward!$S$2:$T$16, IF(J186="11", Ward!$U$2:$V$17, IF(J186="12", Ward!$W$2:$X$12, IF(J186="Bình Chánh", Ward!$Y$2:$Z$17, IF(J186="Bình Tân", Ward!$AA$2:$AB$11, IF(J186="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J186="Cần Giờ", Ward!$AE$2:$AF$8, IF(J186="Củ Chi", Ward!$AG$2:$AH$22, IF(J186="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J186="Hóc Môn", Ward!$AK$2:$AL$13, IF(J186="Nhà Bè", Ward!$AM$2:$AN$8, IF(J186="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J186="Tân Bình", Ward!$AQ$2:$AR$16, IF(J186="Tân Phú", Ward!$AS$2:$AT$12, IF(J186="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9280,7 +9280,7 @@
         <f>IF(J187 &lt;&gt; "", VLOOKUP(J187, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W187" s="28" t="str">
+      <c r="W187" s="23" t="str">
         <f>IF(K187 &lt;&gt; "", VLOOKUP(K187, IF(J187="1", Ward!$A$2:$B$11, IF(J187="2", Ward!$C$2:$D$12, IF(J187="3", Ward!$E$2:$F$15, IF(J187="4", Ward!$G$2:$H$16, IF(J187="5", Ward!$I$2:$J$16, IF(J187="6", Ward!$K$2:$L$15, IF(J187="7", Ward!$M$2:$N$11, IF(J187="8", Ward!$O$2:$P$17, IF(J187="9", Ward!$Q$2:$R$14, IF(J187="10", Ward!$S$2:$T$16, IF(J187="11", Ward!$U$2:$V$17, IF(J187="12", Ward!$W$2:$X$12, IF(J187="Bình Chánh", Ward!$Y$2:$Z$17, IF(J187="Bình Tân", Ward!$AA$2:$AB$11, IF(J187="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J187="Cần Giờ", Ward!$AE$2:$AF$8, IF(J187="Củ Chi", Ward!$AG$2:$AH$22, IF(J187="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J187="Hóc Môn", Ward!$AK$2:$AL$13, IF(J187="Nhà Bè", Ward!$AM$2:$AN$8, IF(J187="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J187="Tân Bình", Ward!$AQ$2:$AR$16, IF(J187="Tân Phú", Ward!$AS$2:$AT$12, IF(J187="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9318,7 +9318,7 @@
         <f>IF(J188 &lt;&gt; "", VLOOKUP(J188, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W188" s="28" t="str">
+      <c r="W188" s="23" t="str">
         <f>IF(K188 &lt;&gt; "", VLOOKUP(K188, IF(J188="1", Ward!$A$2:$B$11, IF(J188="2", Ward!$C$2:$D$12, IF(J188="3", Ward!$E$2:$F$15, IF(J188="4", Ward!$G$2:$H$16, IF(J188="5", Ward!$I$2:$J$16, IF(J188="6", Ward!$K$2:$L$15, IF(J188="7", Ward!$M$2:$N$11, IF(J188="8", Ward!$O$2:$P$17, IF(J188="9", Ward!$Q$2:$R$14, IF(J188="10", Ward!$S$2:$T$16, IF(J188="11", Ward!$U$2:$V$17, IF(J188="12", Ward!$W$2:$X$12, IF(J188="Bình Chánh", Ward!$Y$2:$Z$17, IF(J188="Bình Tân", Ward!$AA$2:$AB$11, IF(J188="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J188="Cần Giờ", Ward!$AE$2:$AF$8, IF(J188="Củ Chi", Ward!$AG$2:$AH$22, IF(J188="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J188="Hóc Môn", Ward!$AK$2:$AL$13, IF(J188="Nhà Bè", Ward!$AM$2:$AN$8, IF(J188="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J188="Tân Bình", Ward!$AQ$2:$AR$16, IF(J188="Tân Phú", Ward!$AS$2:$AT$12, IF(J188="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9356,7 +9356,7 @@
         <f>IF(J189 &lt;&gt; "", VLOOKUP(J189, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W189" s="28" t="str">
+      <c r="W189" s="23" t="str">
         <f>IF(K189 &lt;&gt; "", VLOOKUP(K189, IF(J189="1", Ward!$A$2:$B$11, IF(J189="2", Ward!$C$2:$D$12, IF(J189="3", Ward!$E$2:$F$15, IF(J189="4", Ward!$G$2:$H$16, IF(J189="5", Ward!$I$2:$J$16, IF(J189="6", Ward!$K$2:$L$15, IF(J189="7", Ward!$M$2:$N$11, IF(J189="8", Ward!$O$2:$P$17, IF(J189="9", Ward!$Q$2:$R$14, IF(J189="10", Ward!$S$2:$T$16, IF(J189="11", Ward!$U$2:$V$17, IF(J189="12", Ward!$W$2:$X$12, IF(J189="Bình Chánh", Ward!$Y$2:$Z$17, IF(J189="Bình Tân", Ward!$AA$2:$AB$11, IF(J189="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J189="Cần Giờ", Ward!$AE$2:$AF$8, IF(J189="Củ Chi", Ward!$AG$2:$AH$22, IF(J189="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J189="Hóc Môn", Ward!$AK$2:$AL$13, IF(J189="Nhà Bè", Ward!$AM$2:$AN$8, IF(J189="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J189="Tân Bình", Ward!$AQ$2:$AR$16, IF(J189="Tân Phú", Ward!$AS$2:$AT$12, IF(J189="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9394,7 +9394,7 @@
         <f>IF(J190 &lt;&gt; "", VLOOKUP(J190, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W190" s="28" t="str">
+      <c r="W190" s="23" t="str">
         <f>IF(K190 &lt;&gt; "", VLOOKUP(K190, IF(J190="1", Ward!$A$2:$B$11, IF(J190="2", Ward!$C$2:$D$12, IF(J190="3", Ward!$E$2:$F$15, IF(J190="4", Ward!$G$2:$H$16, IF(J190="5", Ward!$I$2:$J$16, IF(J190="6", Ward!$K$2:$L$15, IF(J190="7", Ward!$M$2:$N$11, IF(J190="8", Ward!$O$2:$P$17, IF(J190="9", Ward!$Q$2:$R$14, IF(J190="10", Ward!$S$2:$T$16, IF(J190="11", Ward!$U$2:$V$17, IF(J190="12", Ward!$W$2:$X$12, IF(J190="Bình Chánh", Ward!$Y$2:$Z$17, IF(J190="Bình Tân", Ward!$AA$2:$AB$11, IF(J190="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J190="Cần Giờ", Ward!$AE$2:$AF$8, IF(J190="Củ Chi", Ward!$AG$2:$AH$22, IF(J190="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J190="Hóc Môn", Ward!$AK$2:$AL$13, IF(J190="Nhà Bè", Ward!$AM$2:$AN$8, IF(J190="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J190="Tân Bình", Ward!$AQ$2:$AR$16, IF(J190="Tân Phú", Ward!$AS$2:$AT$12, IF(J190="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9432,7 +9432,7 @@
         <f>IF(J191 &lt;&gt; "", VLOOKUP(J191, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W191" s="28" t="str">
+      <c r="W191" s="23" t="str">
         <f>IF(K191 &lt;&gt; "", VLOOKUP(K191, IF(J191="1", Ward!$A$2:$B$11, IF(J191="2", Ward!$C$2:$D$12, IF(J191="3", Ward!$E$2:$F$15, IF(J191="4", Ward!$G$2:$H$16, IF(J191="5", Ward!$I$2:$J$16, IF(J191="6", Ward!$K$2:$L$15, IF(J191="7", Ward!$M$2:$N$11, IF(J191="8", Ward!$O$2:$P$17, IF(J191="9", Ward!$Q$2:$R$14, IF(J191="10", Ward!$S$2:$T$16, IF(J191="11", Ward!$U$2:$V$17, IF(J191="12", Ward!$W$2:$X$12, IF(J191="Bình Chánh", Ward!$Y$2:$Z$17, IF(J191="Bình Tân", Ward!$AA$2:$AB$11, IF(J191="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J191="Cần Giờ", Ward!$AE$2:$AF$8, IF(J191="Củ Chi", Ward!$AG$2:$AH$22, IF(J191="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J191="Hóc Môn", Ward!$AK$2:$AL$13, IF(J191="Nhà Bè", Ward!$AM$2:$AN$8, IF(J191="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J191="Tân Bình", Ward!$AQ$2:$AR$16, IF(J191="Tân Phú", Ward!$AS$2:$AT$12, IF(J191="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9470,7 +9470,7 @@
         <f>IF(J192 &lt;&gt; "", VLOOKUP(J192, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W192" s="28" t="str">
+      <c r="W192" s="23" t="str">
         <f>IF(K192 &lt;&gt; "", VLOOKUP(K192, IF(J192="1", Ward!$A$2:$B$11, IF(J192="2", Ward!$C$2:$D$12, IF(J192="3", Ward!$E$2:$F$15, IF(J192="4", Ward!$G$2:$H$16, IF(J192="5", Ward!$I$2:$J$16, IF(J192="6", Ward!$K$2:$L$15, IF(J192="7", Ward!$M$2:$N$11, IF(J192="8", Ward!$O$2:$P$17, IF(J192="9", Ward!$Q$2:$R$14, IF(J192="10", Ward!$S$2:$T$16, IF(J192="11", Ward!$U$2:$V$17, IF(J192="12", Ward!$W$2:$X$12, IF(J192="Bình Chánh", Ward!$Y$2:$Z$17, IF(J192="Bình Tân", Ward!$AA$2:$AB$11, IF(J192="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J192="Cần Giờ", Ward!$AE$2:$AF$8, IF(J192="Củ Chi", Ward!$AG$2:$AH$22, IF(J192="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J192="Hóc Môn", Ward!$AK$2:$AL$13, IF(J192="Nhà Bè", Ward!$AM$2:$AN$8, IF(J192="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J192="Tân Bình", Ward!$AQ$2:$AR$16, IF(J192="Tân Phú", Ward!$AS$2:$AT$12, IF(J192="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9508,7 +9508,7 @@
         <f>IF(J193 &lt;&gt; "", VLOOKUP(J193, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W193" s="28" t="str">
+      <c r="W193" s="23" t="str">
         <f>IF(K193 &lt;&gt; "", VLOOKUP(K193, IF(J193="1", Ward!$A$2:$B$11, IF(J193="2", Ward!$C$2:$D$12, IF(J193="3", Ward!$E$2:$F$15, IF(J193="4", Ward!$G$2:$H$16, IF(J193="5", Ward!$I$2:$J$16, IF(J193="6", Ward!$K$2:$L$15, IF(J193="7", Ward!$M$2:$N$11, IF(J193="8", Ward!$O$2:$P$17, IF(J193="9", Ward!$Q$2:$R$14, IF(J193="10", Ward!$S$2:$T$16, IF(J193="11", Ward!$U$2:$V$17, IF(J193="12", Ward!$W$2:$X$12, IF(J193="Bình Chánh", Ward!$Y$2:$Z$17, IF(J193="Bình Tân", Ward!$AA$2:$AB$11, IF(J193="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J193="Cần Giờ", Ward!$AE$2:$AF$8, IF(J193="Củ Chi", Ward!$AG$2:$AH$22, IF(J193="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J193="Hóc Môn", Ward!$AK$2:$AL$13, IF(J193="Nhà Bè", Ward!$AM$2:$AN$8, IF(J193="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J193="Tân Bình", Ward!$AQ$2:$AR$16, IF(J193="Tân Phú", Ward!$AS$2:$AT$12, IF(J193="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9546,7 +9546,7 @@
         <f>IF(J194 &lt;&gt; "", VLOOKUP(J194, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W194" s="28" t="str">
+      <c r="W194" s="23" t="str">
         <f>IF(K194 &lt;&gt; "", VLOOKUP(K194, IF(J194="1", Ward!$A$2:$B$11, IF(J194="2", Ward!$C$2:$D$12, IF(J194="3", Ward!$E$2:$F$15, IF(J194="4", Ward!$G$2:$H$16, IF(J194="5", Ward!$I$2:$J$16, IF(J194="6", Ward!$K$2:$L$15, IF(J194="7", Ward!$M$2:$N$11, IF(J194="8", Ward!$O$2:$P$17, IF(J194="9", Ward!$Q$2:$R$14, IF(J194="10", Ward!$S$2:$T$16, IF(J194="11", Ward!$U$2:$V$17, IF(J194="12", Ward!$W$2:$X$12, IF(J194="Bình Chánh", Ward!$Y$2:$Z$17, IF(J194="Bình Tân", Ward!$AA$2:$AB$11, IF(J194="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J194="Cần Giờ", Ward!$AE$2:$AF$8, IF(J194="Củ Chi", Ward!$AG$2:$AH$22, IF(J194="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J194="Hóc Môn", Ward!$AK$2:$AL$13, IF(J194="Nhà Bè", Ward!$AM$2:$AN$8, IF(J194="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J194="Tân Bình", Ward!$AQ$2:$AR$16, IF(J194="Tân Phú", Ward!$AS$2:$AT$12, IF(J194="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9584,7 +9584,7 @@
         <f>IF(J195 &lt;&gt; "", VLOOKUP(J195, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W195" s="28" t="str">
+      <c r="W195" s="23" t="str">
         <f>IF(K195 &lt;&gt; "", VLOOKUP(K195, IF(J195="1", Ward!$A$2:$B$11, IF(J195="2", Ward!$C$2:$D$12, IF(J195="3", Ward!$E$2:$F$15, IF(J195="4", Ward!$G$2:$H$16, IF(J195="5", Ward!$I$2:$J$16, IF(J195="6", Ward!$K$2:$L$15, IF(J195="7", Ward!$M$2:$N$11, IF(J195="8", Ward!$O$2:$P$17, IF(J195="9", Ward!$Q$2:$R$14, IF(J195="10", Ward!$S$2:$T$16, IF(J195="11", Ward!$U$2:$V$17, IF(J195="12", Ward!$W$2:$X$12, IF(J195="Bình Chánh", Ward!$Y$2:$Z$17, IF(J195="Bình Tân", Ward!$AA$2:$AB$11, IF(J195="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J195="Cần Giờ", Ward!$AE$2:$AF$8, IF(J195="Củ Chi", Ward!$AG$2:$AH$22, IF(J195="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J195="Hóc Môn", Ward!$AK$2:$AL$13, IF(J195="Nhà Bè", Ward!$AM$2:$AN$8, IF(J195="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J195="Tân Bình", Ward!$AQ$2:$AR$16, IF(J195="Tân Phú", Ward!$AS$2:$AT$12, IF(J195="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9622,7 +9622,7 @@
         <f>IF(J196 &lt;&gt; "", VLOOKUP(J196, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W196" s="28" t="str">
+      <c r="W196" s="23" t="str">
         <f>IF(K196 &lt;&gt; "", VLOOKUP(K196, IF(J196="1", Ward!$A$2:$B$11, IF(J196="2", Ward!$C$2:$D$12, IF(J196="3", Ward!$E$2:$F$15, IF(J196="4", Ward!$G$2:$H$16, IF(J196="5", Ward!$I$2:$J$16, IF(J196="6", Ward!$K$2:$L$15, IF(J196="7", Ward!$M$2:$N$11, IF(J196="8", Ward!$O$2:$P$17, IF(J196="9", Ward!$Q$2:$R$14, IF(J196="10", Ward!$S$2:$T$16, IF(J196="11", Ward!$U$2:$V$17, IF(J196="12", Ward!$W$2:$X$12, IF(J196="Bình Chánh", Ward!$Y$2:$Z$17, IF(J196="Bình Tân", Ward!$AA$2:$AB$11, IF(J196="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J196="Cần Giờ", Ward!$AE$2:$AF$8, IF(J196="Củ Chi", Ward!$AG$2:$AH$22, IF(J196="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J196="Hóc Môn", Ward!$AK$2:$AL$13, IF(J196="Nhà Bè", Ward!$AM$2:$AN$8, IF(J196="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J196="Tân Bình", Ward!$AQ$2:$AR$16, IF(J196="Tân Phú", Ward!$AS$2:$AT$12, IF(J196="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9660,7 +9660,7 @@
         <f>IF(J197 &lt;&gt; "", VLOOKUP(J197, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W197" s="28" t="str">
+      <c r="W197" s="23" t="str">
         <f>IF(K197 &lt;&gt; "", VLOOKUP(K197, IF(J197="1", Ward!$A$2:$B$11, IF(J197="2", Ward!$C$2:$D$12, IF(J197="3", Ward!$E$2:$F$15, IF(J197="4", Ward!$G$2:$H$16, IF(J197="5", Ward!$I$2:$J$16, IF(J197="6", Ward!$K$2:$L$15, IF(J197="7", Ward!$M$2:$N$11, IF(J197="8", Ward!$O$2:$P$17, IF(J197="9", Ward!$Q$2:$R$14, IF(J197="10", Ward!$S$2:$T$16, IF(J197="11", Ward!$U$2:$V$17, IF(J197="12", Ward!$W$2:$X$12, IF(J197="Bình Chánh", Ward!$Y$2:$Z$17, IF(J197="Bình Tân", Ward!$AA$2:$AB$11, IF(J197="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J197="Cần Giờ", Ward!$AE$2:$AF$8, IF(J197="Củ Chi", Ward!$AG$2:$AH$22, IF(J197="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J197="Hóc Môn", Ward!$AK$2:$AL$13, IF(J197="Nhà Bè", Ward!$AM$2:$AN$8, IF(J197="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J197="Tân Bình", Ward!$AQ$2:$AR$16, IF(J197="Tân Phú", Ward!$AS$2:$AT$12, IF(J197="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9698,7 +9698,7 @@
         <f>IF(J198 &lt;&gt; "", VLOOKUP(J198, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W198" s="28" t="str">
+      <c r="W198" s="23" t="str">
         <f>IF(K198 &lt;&gt; "", VLOOKUP(K198, IF(J198="1", Ward!$A$2:$B$11, IF(J198="2", Ward!$C$2:$D$12, IF(J198="3", Ward!$E$2:$F$15, IF(J198="4", Ward!$G$2:$H$16, IF(J198="5", Ward!$I$2:$J$16, IF(J198="6", Ward!$K$2:$L$15, IF(J198="7", Ward!$M$2:$N$11, IF(J198="8", Ward!$O$2:$P$17, IF(J198="9", Ward!$Q$2:$R$14, IF(J198="10", Ward!$S$2:$T$16, IF(J198="11", Ward!$U$2:$V$17, IF(J198="12", Ward!$W$2:$X$12, IF(J198="Bình Chánh", Ward!$Y$2:$Z$17, IF(J198="Bình Tân", Ward!$AA$2:$AB$11, IF(J198="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J198="Cần Giờ", Ward!$AE$2:$AF$8, IF(J198="Củ Chi", Ward!$AG$2:$AH$22, IF(J198="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J198="Hóc Môn", Ward!$AK$2:$AL$13, IF(J198="Nhà Bè", Ward!$AM$2:$AN$8, IF(J198="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J198="Tân Bình", Ward!$AQ$2:$AR$16, IF(J198="Tân Phú", Ward!$AS$2:$AT$12, IF(J198="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9736,7 +9736,7 @@
         <f>IF(J199 &lt;&gt; "", VLOOKUP(J199, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W199" s="28" t="str">
+      <c r="W199" s="23" t="str">
         <f>IF(K199 &lt;&gt; "", VLOOKUP(K199, IF(J199="1", Ward!$A$2:$B$11, IF(J199="2", Ward!$C$2:$D$12, IF(J199="3", Ward!$E$2:$F$15, IF(J199="4", Ward!$G$2:$H$16, IF(J199="5", Ward!$I$2:$J$16, IF(J199="6", Ward!$K$2:$L$15, IF(J199="7", Ward!$M$2:$N$11, IF(J199="8", Ward!$O$2:$P$17, IF(J199="9", Ward!$Q$2:$R$14, IF(J199="10", Ward!$S$2:$T$16, IF(J199="11", Ward!$U$2:$V$17, IF(J199="12", Ward!$W$2:$X$12, IF(J199="Bình Chánh", Ward!$Y$2:$Z$17, IF(J199="Bình Tân", Ward!$AA$2:$AB$11, IF(J199="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J199="Cần Giờ", Ward!$AE$2:$AF$8, IF(J199="Củ Chi", Ward!$AG$2:$AH$22, IF(J199="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J199="Hóc Môn", Ward!$AK$2:$AL$13, IF(J199="Nhà Bè", Ward!$AM$2:$AN$8, IF(J199="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J199="Tân Bình", Ward!$AQ$2:$AR$16, IF(J199="Tân Phú", Ward!$AS$2:$AT$12, IF(J199="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9774,7 +9774,7 @@
         <f>IF(J200 &lt;&gt; "", VLOOKUP(J200, District!$A$1:$B$25, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="W200" s="28" t="str">
+      <c r="W200" s="23" t="str">
         <f>IF(K200 &lt;&gt; "", VLOOKUP(K200, IF(J200="1", Ward!$A$2:$B$11, IF(J200="2", Ward!$C$2:$D$12, IF(J200="3", Ward!$E$2:$F$15, IF(J200="4", Ward!$G$2:$H$16, IF(J200="5", Ward!$I$2:$J$16, IF(J200="6", Ward!$K$2:$L$15, IF(J200="7", Ward!$M$2:$N$11, IF(J200="8", Ward!$O$2:$P$17, IF(J200="9", Ward!$Q$2:$R$14, IF(J200="10", Ward!$S$2:$T$16, IF(J200="11", Ward!$U$2:$V$17, IF(J200="12", Ward!$W$2:$X$12, IF(J200="Bình Chánh", Ward!$Y$2:$Z$17, IF(J200="Bình Tân", Ward!$AA$2:$AB$11, IF(J200="Bình Thạnh", Ward!$AC$2:$AD$21, IF(J200="Cần Giờ", Ward!$AE$2:$AF$8, IF(J200="Củ Chi", Ward!$AG$2:$AH$22, IF(J200="Gò Vấp", Ward!$AI$2:$AJ$17, IF(J200="Hóc Môn", Ward!$AK$2:$AL$13, IF(J200="Nhà Bè", Ward!$AM$2:$AN$8, IF(J200="Phú Nhuận", Ward!$AO$2:$AP$16, IF(J200="Tân Bình", Ward!$AQ$2:$AR$16, IF(J200="Tân Phú", Ward!$AS$2:$AT$12, IF(J200="Thủ Đức", Ward!$AU$2:$AV$13)))))))))))))))))))))))), 2, FALSE), "")</f>
         <v/>
       </c>
@@ -9784,7 +9784,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="7">
+  <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I200">
       <formula1>CityList</formula1>
     </dataValidation>
@@ -9805,6 +9805,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B200">
       <formula1>HospitalTypeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E200">
+      <formula1>"True, False"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9830,7 +9833,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9866,7 +9869,7 @@
         <v>13</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -10122,145 +10125,145 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G1" s="6">
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="I1" s="6">
         <v>5</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="K1" s="6">
         <v>6</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="M1" s="6">
         <v>7</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="O1" s="6">
         <v>8</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="Q1" s="6">
         <v>9</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="S1" s="6" t="s">
         <v>15</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="U1" s="6">
         <v>11</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="W1" s="6">
         <v>12</v>
       </c>
       <c r="X1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="Y1" s="6" t="s">
         <v>26</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="AA1" s="6" t="s">
         <v>27</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="AC1" s="6" t="s">
         <v>28</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="AE1" s="6" t="s">
         <v>29</v>
       </c>
       <c r="AF1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="AG1" s="6" t="s">
         <v>30</v>
       </c>
       <c r="AH1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="AI1" s="6" t="s">
         <v>31</v>
       </c>
       <c r="AJ1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="AK1" s="6" t="s">
         <v>32</v>
       </c>
       <c r="AL1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="AM1" s="6" t="s">
         <v>33</v>
       </c>
       <c r="AN1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="AO1" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AP1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="AQ1" s="6" t="s">
         <v>35</v>
       </c>
       <c r="AR1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="AS1" s="6" t="s">
         <v>36</v>
       </c>
       <c r="AT1" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="AU1" s="6" t="s">
         <v>37</v>
       </c>
       <c r="AV1" s="7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.25">
@@ -10280,25 +10283,25 @@
         <v>180</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>180</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>180</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>180</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="M2" s="8" t="s">
         <v>12</v>
@@ -10310,7 +10313,7 @@
         <v>180</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="Q2" s="8" t="s">
         <v>75</v>
@@ -10322,13 +10325,13 @@
         <v>180</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="U2" s="8" t="s">
         <v>180</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="W2" s="8" t="s">
         <v>100</v>
@@ -10352,7 +10355,7 @@
         <v>180</v>
       </c>
       <c r="AD2" s="8" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="AE2" s="8" t="s">
         <v>79</v>
@@ -10370,7 +10373,7 @@
         <v>180</v>
       </c>
       <c r="AJ2" s="8" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="AK2" s="8" t="s">
         <v>165</v>
@@ -10388,13 +10391,13 @@
         <v>180</v>
       </c>
       <c r="AP2" s="8" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="AQ2" s="8" t="s">
         <v>180</v>
       </c>
       <c r="AR2" s="8" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="AS2" s="8" t="s">
         <v>152</v>
@@ -10426,25 +10429,25 @@
         <v>181</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>181</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>181</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>181</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>145</v>
@@ -10456,7 +10459,7 @@
         <v>181</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="Q3" s="8" t="s">
         <v>41</v>
@@ -10468,13 +10471,13 @@
         <v>181</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="U3" s="8" t="s">
         <v>181</v>
       </c>
       <c r="V3" s="8" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="W3" s="8" t="s">
         <v>147</v>
@@ -10498,7 +10501,7 @@
         <v>181</v>
       </c>
       <c r="AD3" s="8" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="AE3" s="8" t="s">
         <v>55</v>
@@ -10516,7 +10519,7 @@
         <v>182</v>
       </c>
       <c r="AJ3" s="8" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AK3" s="8" t="s">
         <v>81</v>
@@ -10534,13 +10537,13 @@
         <v>181</v>
       </c>
       <c r="AP3" s="8" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="AQ3" s="8" t="s">
         <v>181</v>
       </c>
       <c r="AR3" s="8" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="AS3" s="8" t="s">
         <v>141</v>
@@ -10572,25 +10575,25 @@
         <v>182</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>182</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>182</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>182</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="M4" s="8" t="s">
         <v>111</v>
@@ -10602,7 +10605,7 @@
         <v>182</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="Q4" s="8" t="s">
         <v>146</v>
@@ -10614,13 +10617,13 @@
         <v>182</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="U4" s="8" t="s">
         <v>182</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="W4" s="8" t="s">
         <v>64</v>
@@ -10644,7 +10647,7 @@
         <v>182</v>
       </c>
       <c r="AD4" s="8" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="AE4" s="8" t="s">
         <v>45</v>
@@ -10662,7 +10665,7 @@
         <v>183</v>
       </c>
       <c r="AJ4" s="8" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="AK4" s="8" t="s">
         <v>32</v>
@@ -10680,13 +10683,13 @@
         <v>182</v>
       </c>
       <c r="AP4" s="8" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="AQ4" s="8" t="s">
         <v>182</v>
       </c>
       <c r="AR4" s="8" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="AS4" s="8" t="s">
         <v>120</v>
@@ -10718,25 +10721,25 @@
         <v>183</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>183</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>183</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="K5" s="8" t="s">
         <v>183</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="M5" s="8" t="s">
         <v>74</v>
@@ -10748,7 +10751,7 @@
         <v>183</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="Q5" s="8" t="s">
         <v>51</v>
@@ -10760,13 +10763,13 @@
         <v>183</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="U5" s="8" t="s">
         <v>183</v>
       </c>
       <c r="V5" s="8" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="W5" s="8" t="s">
         <v>88</v>
@@ -10790,7 +10793,7 @@
         <v>184</v>
       </c>
       <c r="AD5" s="8" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="AE5" s="8" t="s">
         <v>103</v>
@@ -10808,7 +10811,7 @@
         <v>184</v>
       </c>
       <c r="AJ5" s="8" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="AK5" s="8" t="s">
         <v>68</v>
@@ -10826,13 +10829,13 @@
         <v>183</v>
       </c>
       <c r="AP5" s="8" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="AQ5" s="8" t="s">
         <v>183</v>
       </c>
       <c r="AR5" s="8" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="AS5" s="8" t="s">
         <v>107</v>
@@ -10864,25 +10867,25 @@
         <v>184</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>184</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>184</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>184</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>63</v>
@@ -10894,7 +10897,7 @@
         <v>184</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="Q6" s="8" t="s">
         <v>155</v>
@@ -10906,13 +10909,13 @@
         <v>184</v>
       </c>
       <c r="T6" s="8" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="U6" s="8" t="s">
         <v>184</v>
       </c>
       <c r="V6" s="8" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="W6" s="8" t="s">
         <v>136</v>
@@ -10936,7 +10939,7 @@
         <v>185</v>
       </c>
       <c r="AD6" s="8" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="AE6" s="8" t="s">
         <v>116</v>
@@ -10954,7 +10957,7 @@
         <v>186</v>
       </c>
       <c r="AJ6" s="8" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="AK6" s="8" t="s">
         <v>57</v>
@@ -10972,13 +10975,13 @@
         <v>184</v>
       </c>
       <c r="AP6" s="8" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="AQ6" s="8" t="s">
         <v>184</v>
       </c>
       <c r="AR6" s="8" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="AS6" s="8" t="s">
         <v>130</v>
@@ -11010,25 +11013,25 @@
         <v>185</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>185</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>185</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>185</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="M7" s="8" t="s">
         <v>134</v>
@@ -11040,7 +11043,7 @@
         <v>185</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="Q7" s="8" t="s">
         <v>167</v>
@@ -11052,13 +11055,13 @@
         <v>185</v>
       </c>
       <c r="T7" s="8" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="U7" s="8" t="s">
         <v>185</v>
       </c>
       <c r="V7" s="8" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="W7" s="8" t="s">
         <v>113</v>
@@ -11082,7 +11085,7 @@
         <v>186</v>
       </c>
       <c r="AD7" s="8" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="AE7" s="8" t="s">
         <v>67</v>
@@ -11100,7 +11103,7 @@
         <v>15</v>
       </c>
       <c r="AJ7" s="8" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="AK7" s="8" t="s">
         <v>93</v>
@@ -11118,13 +11121,13 @@
         <v>186</v>
       </c>
       <c r="AP7" s="8" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="AQ7" s="8" t="s">
         <v>185</v>
       </c>
       <c r="AR7" s="8" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="AS7" s="8" t="s">
         <v>70</v>
@@ -11156,25 +11159,25 @@
         <v>186</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>187</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>186</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="K8" s="8" t="s">
         <v>186</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="M8" s="8" t="s">
         <v>36</v>
@@ -11186,7 +11189,7 @@
         <v>186</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="Q8" s="8" t="s">
         <v>162</v>
@@ -11198,13 +11201,13 @@
         <v>186</v>
       </c>
       <c r="T8" s="8" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="U8" s="8" t="s">
         <v>186</v>
       </c>
       <c r="V8" s="8" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="W8" s="8" t="s">
         <v>156</v>
@@ -11228,7 +11231,7 @@
         <v>16</v>
       </c>
       <c r="AD8" s="8" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="AE8" s="8" t="s">
         <v>91</v>
@@ -11246,7 +11249,7 @@
         <v>16</v>
       </c>
       <c r="AJ8" s="8" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="AK8" s="8" t="s">
         <v>129</v>
@@ -11264,13 +11267,13 @@
         <v>187</v>
       </c>
       <c r="AP8" s="8" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="AQ8" s="8" t="s">
         <v>186</v>
       </c>
       <c r="AR8" s="8" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="AS8" s="8" t="s">
         <v>83</v>
@@ -11302,25 +11305,25 @@
         <v>187</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>188</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>187</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="K9" s="8" t="s">
         <v>187</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="M9" s="8" t="s">
         <v>98</v>
@@ -11332,7 +11335,7 @@
         <v>187</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="Q9" s="8" t="s">
         <v>124</v>
@@ -11344,13 +11347,13 @@
         <v>187</v>
       </c>
       <c r="T9" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="U9" s="8" t="s">
         <v>187</v>
       </c>
       <c r="V9" s="8" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="W9" s="8" t="s">
         <v>52</v>
@@ -11374,7 +11377,7 @@
         <v>17</v>
       </c>
       <c r="AD9" s="8" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="AE9" s="8"/>
       <c r="AF9" s="8"/>
@@ -11388,7 +11391,7 @@
         <v>17</v>
       </c>
       <c r="AJ9" s="8" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="AK9" s="8" t="s">
         <v>105</v>
@@ -11402,13 +11405,13 @@
         <v>188</v>
       </c>
       <c r="AP9" s="8" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="AQ9" s="8" t="s">
         <v>187</v>
       </c>
       <c r="AR9" s="8" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="AS9" s="8" t="s">
         <v>46</v>
@@ -11440,25 +11443,25 @@
         <v>188</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>188</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>188</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="M10" s="8" t="s">
         <v>40</v>
@@ -11470,7 +11473,7 @@
         <v>188</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="Q10" s="8" t="s">
         <v>112</v>
@@ -11482,13 +11485,13 @@
         <v>188</v>
       </c>
       <c r="T10" s="8" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="U10" s="8" t="s">
         <v>188</v>
       </c>
       <c r="V10" s="8" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="W10" s="8" t="s">
         <v>42</v>
@@ -11512,7 +11515,7 @@
         <v>189</v>
       </c>
       <c r="AD10" s="8" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="AE10" s="8"/>
       <c r="AF10" s="8"/>
@@ -11526,7 +11529,7 @@
         <v>189</v>
       </c>
       <c r="AJ10" s="8" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="AK10" s="8" t="s">
         <v>151</v>
@@ -11540,13 +11543,13 @@
         <v>15</v>
       </c>
       <c r="AP10" s="8" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="AQ10" s="8" t="s">
         <v>188</v>
       </c>
       <c r="AR10" s="8" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="AS10" s="8" t="s">
         <v>95</v>
@@ -11578,25 +11581,25 @@
         <v>15</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>15</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="M11" s="8" t="s">
         <v>50</v>
@@ -11608,7 +11611,7 @@
         <v>15</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="Q11" s="8" t="s">
         <v>36</v>
@@ -11620,13 +11623,13 @@
         <v>15</v>
       </c>
       <c r="T11" s="8" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="U11" s="8" t="s">
         <v>15</v>
       </c>
       <c r="V11" s="8" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="W11" s="8" t="s">
         <v>76</v>
@@ -11650,7 +11653,7 @@
         <v>190</v>
       </c>
       <c r="AD11" s="8" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="AE11" s="8"/>
       <c r="AF11" s="8"/>
@@ -11664,7 +11667,7 @@
         <v>190</v>
       </c>
       <c r="AJ11" s="8" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="AK11" s="8" t="s">
         <v>140</v>
@@ -11678,13 +11681,13 @@
         <v>16</v>
       </c>
       <c r="AP11" s="8" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="AQ11" s="8" t="s">
         <v>15</v>
       </c>
       <c r="AR11" s="8" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="AS11" s="8" t="s">
         <v>160</v>
@@ -11712,25 +11715,25 @@
         <v>16</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>189</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>16</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>16</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
@@ -11738,7 +11741,7 @@
         <v>16</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="Q12" s="8" t="s">
         <v>87</v>
@@ -11750,13 +11753,13 @@
         <v>16</v>
       </c>
       <c r="T12" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="U12" s="8" t="s">
         <v>16</v>
       </c>
       <c r="V12" s="8" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="W12" s="8" t="s">
         <v>125</v>
@@ -11776,7 +11779,7 @@
         <v>191</v>
       </c>
       <c r="AD12" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="AE12" s="8"/>
       <c r="AF12" s="8"/>
@@ -11790,7 +11793,7 @@
         <v>191</v>
       </c>
       <c r="AJ12" s="8" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="AK12" s="8" t="s">
         <v>118</v>
@@ -11804,13 +11807,13 @@
         <v>17</v>
       </c>
       <c r="AP12" s="8" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="AQ12" s="8" t="s">
         <v>16</v>
       </c>
       <c r="AR12" s="8" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="AS12" s="8" t="s">
         <v>59</v>
@@ -11834,25 +11837,25 @@
         <v>17</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>190</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>17</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>17</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
@@ -11860,7 +11863,7 @@
         <v>17</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="Q13" s="8" t="s">
         <v>99</v>
@@ -11872,13 +11875,13 @@
         <v>17</v>
       </c>
       <c r="T13" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="U13" s="8" t="s">
         <v>17</v>
       </c>
       <c r="V13" s="8" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="W13" s="8"/>
       <c r="X13" s="8"/>
@@ -11894,7 +11897,7 @@
         <v>194</v>
       </c>
       <c r="AD13" s="8" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="AE13" s="8"/>
       <c r="AF13" s="8"/>
@@ -11908,7 +11911,7 @@
         <v>192</v>
       </c>
       <c r="AJ13" s="8" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="AK13" s="8" t="s">
         <v>159</v>
@@ -11922,13 +11925,13 @@
         <v>189</v>
       </c>
       <c r="AP13" s="8" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="AQ13" s="8" t="s">
         <v>17</v>
       </c>
       <c r="AR13" s="8" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="AS13" s="8"/>
       <c r="AT13" s="8"/>
@@ -11948,25 +11951,25 @@
         <v>189</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>191</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>189</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>189</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
@@ -11974,7 +11977,7 @@
         <v>189</v>
       </c>
       <c r="P14" s="8" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="Q14" s="8" t="s">
         <v>135</v>
@@ -11986,13 +11989,13 @@
         <v>189</v>
       </c>
       <c r="T14" s="8" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="U14" s="8" t="s">
         <v>189</v>
       </c>
       <c r="V14" s="8" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="W14" s="8"/>
       <c r="X14" s="8"/>
@@ -12008,7 +12011,7 @@
         <v>195</v>
       </c>
       <c r="AD14" s="8" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="AE14" s="8"/>
       <c r="AF14" s="8"/>
@@ -12022,7 +12025,7 @@
         <v>194</v>
       </c>
       <c r="AJ14" s="8" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="AK14" s="8"/>
       <c r="AL14" s="8"/>
@@ -12032,13 +12035,13 @@
         <v>190</v>
       </c>
       <c r="AP14" s="8" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="AQ14" s="8" t="s">
         <v>189</v>
       </c>
       <c r="AR14" s="8" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="AS14" s="8"/>
       <c r="AT14" s="8"/>
@@ -12054,25 +12057,25 @@
         <v>190</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>192</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>190</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>190</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
@@ -12080,7 +12083,7 @@
         <v>190</v>
       </c>
       <c r="P15" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
@@ -12088,13 +12091,13 @@
         <v>190</v>
       </c>
       <c r="T15" s="8" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="U15" s="8" t="s">
         <v>190</v>
       </c>
       <c r="V15" s="8" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="W15" s="8"/>
       <c r="X15" s="8"/>
@@ -12110,7 +12113,7 @@
         <v>196</v>
       </c>
       <c r="AD15" s="8" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="AE15" s="8"/>
       <c r="AF15" s="8"/>
@@ -12124,7 +12127,7 @@
         <v>22</v>
       </c>
       <c r="AJ15" s="8" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="AK15" s="8"/>
       <c r="AL15" s="8"/>
@@ -12134,13 +12137,13 @@
         <v>191</v>
       </c>
       <c r="AP15" s="8" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="AQ15" s="8" t="s">
         <v>190</v>
       </c>
       <c r="AR15" s="8" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="AS15" s="8"/>
       <c r="AT15" s="8"/>
@@ -12158,13 +12161,13 @@
         <v>193</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>191</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
@@ -12174,7 +12177,7 @@
         <v>191</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
@@ -12182,13 +12185,13 @@
         <v>191</v>
       </c>
       <c r="T16" s="8" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="U16" s="8" t="s">
         <v>191</v>
       </c>
       <c r="V16" s="8" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="W16" s="8"/>
       <c r="X16" s="8"/>
@@ -12204,7 +12207,7 @@
         <v>197</v>
       </c>
       <c r="AD16" s="8" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="AE16" s="8"/>
       <c r="AF16" s="8"/>
@@ -12218,7 +12221,7 @@
         <v>24</v>
       </c>
       <c r="AJ16" s="8" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="AK16" s="8"/>
       <c r="AL16" s="8"/>
@@ -12228,13 +12231,13 @@
         <v>194</v>
       </c>
       <c r="AP16" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AQ16" s="8" t="s">
         <v>191</v>
       </c>
       <c r="AR16" s="8" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="AS16" s="8"/>
       <c r="AT16" s="8"/>
@@ -12260,7 +12263,7 @@
         <v>192</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
@@ -12270,7 +12273,7 @@
         <v>192</v>
       </c>
       <c r="V17" s="8" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="W17" s="8"/>
       <c r="X17" s="8"/>
@@ -12286,7 +12289,7 @@
         <v>198</v>
       </c>
       <c r="AD17" s="8" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="AE17" s="8"/>
       <c r="AF17" s="8"/>
@@ -12300,7 +12303,7 @@
         <v>25</v>
       </c>
       <c r="AJ17" s="8" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="AK17" s="8"/>
       <c r="AL17" s="8"/>
@@ -12348,7 +12351,7 @@
         <v>199</v>
       </c>
       <c r="AD18" s="8" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="AE18" s="8"/>
       <c r="AF18" s="8"/>
@@ -12406,7 +12409,7 @@
         <v>200</v>
       </c>
       <c r="AD19" s="8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="AE19" s="8"/>
       <c r="AF19" s="8"/>
@@ -12464,7 +12467,7 @@
         <v>201</v>
       </c>
       <c r="AD20" s="8" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="AE20" s="8"/>
       <c r="AF20" s="8"/>
@@ -12522,7 +12525,7 @@
         <v>202</v>
       </c>
       <c r="AD21" s="8" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="AE21" s="8"/>
       <c r="AF21" s="8"/>
@@ -12624,15 +12627,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -12640,7 +12643,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B3" s="9">
         <v>2</v>
@@ -12648,7 +12651,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B4" s="9">
         <v>3</v>
@@ -12656,7 +12659,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B5" s="9">
         <v>4</v>
@@ -12664,7 +12667,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B6" s="9">
         <v>5</v>
@@ -12672,7 +12675,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B7" s="9">
         <v>6</v>
@@ -12680,7 +12683,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B8" s="9">
         <v>7</v>
@@ -12688,7 +12691,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B9" s="9">
         <v>8</v>
@@ -12696,7 +12699,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B10" s="9">
         <v>9</v>
@@ -12704,7 +12707,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B11" s="9">
         <v>10</v>
@@ -12712,7 +12715,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B12" s="9">
         <v>11</v>
@@ -12720,7 +12723,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B13" s="9">
         <v>12</v>
@@ -12728,7 +12731,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B14" s="9">
         <v>13</v>
@@ -12736,7 +12739,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B15" s="9">
         <v>14</v>
@@ -12744,7 +12747,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B16" s="9">
         <v>15</v>
@@ -12752,7 +12755,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B17" s="9">
         <v>16</v>
@@ -12760,7 +12763,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B18" s="9">
         <v>29</v>
@@ -12768,7 +12771,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B19" s="9">
         <v>17</v>
@@ -12776,7 +12779,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B20" s="9">
         <v>18</v>
@@ -12784,7 +12787,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B21" s="9">
         <v>19</v>
@@ -12792,7 +12795,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B22" s="9">
         <v>20</v>
@@ -12800,7 +12803,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B23" s="9">
         <v>21</v>
@@ -12808,7 +12811,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B24" s="9">
         <v>22</v>
@@ -12816,7 +12819,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B25" s="9">
         <v>23</v>
@@ -12824,7 +12827,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B26" s="9">
         <v>24</v>
@@ -12832,7 +12835,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B27" s="9">
         <v>25</v>
@@ -12840,7 +12843,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B28" s="9">
         <v>26</v>
@@ -12848,7 +12851,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B29" s="9">
         <v>27</v>
@@ -12856,7 +12859,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B30" s="9">
         <v>28</v>
@@ -12864,7 +12867,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B31" s="9">
         <v>31</v>
@@ -12872,7 +12875,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B32" s="9">
         <v>30</v>
@@ -12880,7 +12883,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B33" s="9">
         <v>32</v>
@@ -12888,7 +12891,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B34" s="9">
         <v>33</v>
@@ -12896,7 +12899,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B35" s="9">
         <v>34</v>
@@ -12904,7 +12907,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B36" s="9">
         <v>35</v>
@@ -12912,7 +12915,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B37" s="9">
         <v>36</v>
@@ -12920,7 +12923,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B38" s="9">
         <v>37</v>
@@ -12928,7 +12931,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B39" s="9">
         <v>38</v>
@@ -12936,7 +12939,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B40" s="9">
         <v>39</v>
@@ -12944,7 +12947,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B41" s="9">
         <v>40</v>
@@ -12952,7 +12955,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B42" s="9">
         <v>41</v>
@@ -12960,7 +12963,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B43" s="9">
         <v>42</v>
@@ -12968,7 +12971,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B44" s="9">
         <v>43</v>
@@ -12976,7 +12979,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B45" s="9">
         <v>44</v>
@@ -12984,7 +12987,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B46" s="9">
         <v>45</v>
@@ -12992,7 +12995,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B47" s="9">
         <v>46</v>
@@ -13000,7 +13003,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B48" s="9">
         <v>47</v>
@@ -13008,7 +13011,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B49" s="9">
         <v>48</v>
@@ -13016,7 +13019,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B50" s="9">
         <v>49</v>
@@ -13024,7 +13027,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B51" s="9">
         <v>50</v>
@@ -13032,7 +13035,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B52" s="9">
         <v>51</v>
@@ -13040,7 +13043,7 @@
     </row>
     <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B53" s="10">
         <v>52</v>
@@ -13067,15 +13070,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -13083,7 +13086,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B3" s="9">
         <v>2</v>
@@ -13091,7 +13094,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B4" s="9">
         <v>3</v>
@@ -13099,7 +13102,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B5" s="9">
         <v>4</v>
@@ -13107,7 +13110,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B6" s="9">
         <v>5</v>
@@ -13115,7 +13118,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B7" s="9">
         <v>6</v>
@@ -13123,7 +13126,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B8" s="9">
         <v>7</v>
@@ -13131,7 +13134,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B9" s="9">
         <v>8</v>
@@ -13139,7 +13142,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B10" s="9">
         <v>9</v>
@@ -13147,7 +13150,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B11" s="9">
         <v>10</v>
@@ -13155,7 +13158,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B12" s="9">
         <v>11</v>
@@ -13163,7 +13166,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B13" s="9">
         <v>12</v>
@@ -13171,7 +13174,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B14" s="9">
         <v>13</v>
@@ -13179,7 +13182,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B15" s="9">
         <v>14</v>
@@ -13187,7 +13190,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B16" s="9">
         <v>15</v>
@@ -13195,7 +13198,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B17" s="9">
         <v>16</v>
@@ -13203,7 +13206,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B18" s="9">
         <v>17</v>
@@ -13211,7 +13214,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B19" s="9">
         <v>18</v>
@@ -13219,7 +13222,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B20" s="9">
         <v>19</v>
@@ -13227,7 +13230,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B21" s="9">
         <v>20</v>
@@ -13235,7 +13238,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B22" s="9">
         <v>21</v>
@@ -13243,7 +13246,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B23" s="9">
         <v>22</v>
@@ -13251,7 +13254,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B24" s="9">
         <v>23</v>
@@ -13259,7 +13262,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B25" s="9">
         <v>24</v>
@@ -13267,7 +13270,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B26" s="9">
         <v>25</v>
@@ -13275,7 +13278,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B27" s="9">
         <v>26</v>
@@ -13283,7 +13286,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B28" s="9">
         <v>27</v>
@@ -13291,7 +13294,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B29" s="9">
         <v>28</v>
@@ -13299,7 +13302,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B30" s="9">
         <v>29</v>
@@ -13307,7 +13310,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B31" s="9">
         <v>30</v>
@@ -13315,7 +13318,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B32" s="9">
         <v>31</v>
@@ -13323,7 +13326,7 @@
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B33" s="10">
         <v>32</v>
@@ -13348,15 +13351,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -13364,7 +13367,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B3" s="9">
         <v>2</v>
@@ -13372,7 +13375,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B4" s="9">
         <v>3</v>
@@ -13380,7 +13383,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B5" s="9">
         <v>4</v>
@@ -13388,7 +13391,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B6" s="9">
         <v>5</v>
@@ -13396,7 +13399,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B7" s="9">
         <v>6</v>
@@ -13404,7 +13407,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B8" s="9">
         <v>7</v>
@@ -13412,7 +13415,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B9" s="9">
         <v>8</v>
@@ -13420,7 +13423,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B10" s="9">
         <v>9</v>
@@ -13428,7 +13431,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B11" s="9">
         <v>10</v>
@@ -13436,7 +13439,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B12" s="9">
         <v>11</v>
@@ -13444,7 +13447,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B13" s="9">
         <v>12</v>
@@ -13452,7 +13455,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B14" s="9">
         <v>13</v>
@@ -13460,7 +13463,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B15" s="9">
         <v>14</v>
@@ -13468,7 +13471,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B16" s="9">
         <v>15</v>
@@ -13476,7 +13479,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B17" s="9">
         <v>16</v>
@@ -13484,7 +13487,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B18" s="9">
         <v>17</v>
@@ -13492,7 +13495,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B19" s="9">
         <v>18</v>
@@ -13500,7 +13503,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B20" s="9">
         <v>19</v>
@@ -13508,7 +13511,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B21" s="9">
         <v>20</v>
@@ -13516,7 +13519,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B22" s="9">
         <v>21</v>
@@ -13524,7 +13527,7 @@
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B23" s="10">
         <v>22</v>
@@ -13551,12 +13554,12 @@
         <v>1</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -13564,7 +13567,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="B3" s="9">
         <v>3</v>
@@ -13572,7 +13575,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="B4" s="9">
         <v>7</v>
@@ -13580,7 +13583,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="B5" s="9">
         <v>8</v>
@@ -13588,7 +13591,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="B6" s="9">
         <v>2</v>
@@ -13596,7 +13599,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="B7" s="9">
         <v>6</v>
@@ -13604,7 +13607,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="B8" s="9">
         <v>4</v>
@@ -13612,7 +13615,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="B9" s="10">
         <v>5</v>

</xml_diff>